<commit_message>
added all manufacturing PMI to Sep 23
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68559227-5DD5-4FDA-B5B8-5F793B961EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244F50E3-7A11-4631-8DEF-C67B4D53D8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sorted countries" sheetId="2" r:id="rId2"/>
+    <sheet name="Detailed indices" sheetId="3" r:id="rId2"/>
+    <sheet name="Sorted countries" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="72">
   <si>
     <t>United States</t>
   </si>
@@ -250,13 +251,16 @@
   </si>
   <si>
     <t>34 countries &gt;= 2012</t>
+  </si>
+  <si>
+    <t>32 from 2012 + 3 from 2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +304,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,8 +366,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -374,19 +390,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -396,11 +399,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -414,30 +418,49 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -751,11 +774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H33" sqref="H33"/>
+      <selection pane="topRight" activeCell="H51" sqref="H51:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,12 +788,12 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
@@ -792,16 +815,15 @@
       <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="22" t="s">
+      <c r="J1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="23"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>57</v>
       </c>
@@ -811,33 +833,25 @@
       <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="18" t="s">
+      <c r="K2" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="18" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -849,16 +863,15 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="16">
+      <c r="I4" s="29">
         <v>1999</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L4" s="18"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -870,18 +883,17 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="16">
+      <c r="I5" s="29">
         <v>2008</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="15">
+      <c r="J5" s="26">
         <v>2019</v>
       </c>
-      <c r="L5" s="18">
+      <c r="K5" s="16">
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -893,16 +905,15 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="16">
+      <c r="I6" s="29">
         <v>2008</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="15">
+      <c r="J6" s="26">
         <v>2008</v>
       </c>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -914,16 +925,13 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="17">
-        <v>2021</v>
-      </c>
-      <c r="J7" s="24">
-        <v>2012</v>
-      </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="18"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I7" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -935,16 +943,15 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="16">
+      <c r="I8" s="29">
         <v>2008</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="15">
+      <c r="J8" s="26">
         <v>2008</v>
       </c>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -955,16 +962,15 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="24">
-        <v>2012</v>
-      </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="18">
+      <c r="I9" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="16">
         <v>2014</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -976,16 +982,15 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="16">
+      <c r="I10" s="29">
         <v>2008</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="15">
+      <c r="J10" s="26">
         <v>2008</v>
       </c>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -997,20 +1002,17 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="17">
+      <c r="I11" s="30">
+        <v>41426</v>
+      </c>
+      <c r="J11" s="26">
         <v>2018</v>
       </c>
-      <c r="J11" s="25">
-        <v>41426</v>
-      </c>
-      <c r="K11" s="15">
-        <v>2018</v>
-      </c>
-      <c r="L11" s="18">
+      <c r="K11" s="16">
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1021,14 +1023,13 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="25">
+      <c r="I12" s="30">
         <v>41548</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="18"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="26"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1044,14 +1045,13 @@
         <v>2001</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="25" t="s">
+      <c r="I13" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="18"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="26"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1067,16 +1067,15 @@
         <v>1999</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="16">
+      <c r="I14" s="29">
         <v>1999</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="15">
+      <c r="J14" s="26">
         <v>2006</v>
       </c>
-      <c r="L14" s="18"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1088,17 +1087,16 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L15" s="18"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="I15" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J15" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="10">
@@ -1107,14 +1105,13 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="I16" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I16" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J16" s="26"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1126,17 +1123,16 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L17" s="18"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="I17" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J17" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="8">
@@ -1144,14 +1140,13 @@
       </c>
       <c r="D18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="I18" s="16">
+      <c r="I18" s="29">
         <v>1999</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="26"/>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1167,12 +1162,11 @@
         <v>2001</v>
       </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="26"/>
       <c r="J19" s="26"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1183,12 +1177,11 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="26"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1204,14 +1197,13 @@
         <v>1999</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="16">
+      <c r="I21" s="29">
         <v>2004</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="26"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1222,14 +1214,13 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="24">
-        <v>2012</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="18"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I22" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1240,16 +1231,15 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L23" s="18"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I23" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J23" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1265,16 +1255,15 @@
         <v>2001</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="24">
-        <v>2012</v>
-      </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="18">
+      <c r="I24" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J24" s="26"/>
+      <c r="K24" s="16">
         <v>2008</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1285,14 +1274,13 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="18"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I25" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J25" s="26"/>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1308,30 +1296,27 @@
         <v>2010</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="26"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="18"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="5"/>
@@ -1341,33 +1326,32 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="16">
+      <c r="H29" s="34"/>
+      <c r="I29" s="29">
         <v>2005</v>
       </c>
-      <c r="J29" s="18"/>
-      <c r="K29" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="J29" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="8">
         <v>21</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="I30" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="H30" s="26"/>
+      <c r="I30" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J30" s="26"/>
+      <c r="K30" s="16"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="5"/>
@@ -1377,18 +1361,17 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J31" s="18"/>
-      <c r="K31" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="H31" s="34"/>
+      <c r="I31" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J31" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="5"/>
@@ -1398,16 +1381,15 @@
       <c r="D32" s="2"/>
       <c r="E32" s="4"/>
       <c r="F32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="H32" s="29"/>
+      <c r="I32" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J32" s="26"/>
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="5"/>
@@ -1417,18 +1399,17 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J33" s="18"/>
-      <c r="K33" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="H33" s="35"/>
+      <c r="I33" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J33" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B34" s="5"/>
@@ -1438,16 +1419,15 @@
       <c r="D34" s="2"/>
       <c r="E34" s="4"/>
       <c r="F34" s="2"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="18">
-        <v>2012</v>
-      </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="H34" s="34"/>
+      <c r="I34" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J34" s="26"/>
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="5"/>
@@ -1462,16 +1442,15 @@
       <c r="G35">
         <v>1999</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J35" s="18"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="H35" s="29"/>
+      <c r="I35" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J35" s="26"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="5"/>
@@ -1481,16 +1460,15 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="18"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="H36" s="29"/>
+      <c r="I36" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J36" s="26"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="8">
@@ -1499,15 +1477,13 @@
       <c r="D37" s="2"/>
       <c r="E37" s="4"/>
       <c r="F37" s="2"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="26">
-        <v>2016</v>
-      </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="18"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="5"/>
@@ -1517,16 +1493,15 @@
       <c r="D38" s="2"/>
       <c r="E38" s="4"/>
       <c r="F38" s="2"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="18"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="H38" s="34"/>
+      <c r="I38" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J38" s="26"/>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="10">
@@ -1535,15 +1510,13 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="26">
-        <v>2015</v>
-      </c>
-      <c r="K39" s="15"/>
-      <c r="L39" s="18"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="10">
@@ -1553,15 +1526,13 @@
       <c r="G40">
         <v>2004</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="26">
-        <v>2012</v>
-      </c>
-      <c r="K40" s="15"/>
-      <c r="L40" s="18"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="11">
@@ -1571,15 +1542,13 @@
       <c r="G41">
         <v>2001</v>
       </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="26">
-        <v>2017</v>
-      </c>
-      <c r="K41" s="15"/>
-      <c r="L41" s="18"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="11">
@@ -1589,13 +1558,13 @@
       <c r="G42">
         <v>2010</v>
       </c>
-      <c r="I42" s="15"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
       <c r="J42" s="26"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="19"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="K42" s="17"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="5"/>
@@ -1605,17 +1574,14 @@
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="2"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="17">
-        <v>2015</v>
-      </c>
-      <c r="J43" s="18">
-        <v>2012</v>
-      </c>
-      <c r="K43" s="15"/>
-      <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H43" s="31"/>
+      <c r="I43" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J43" s="26"/>
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>36</v>
       </c>
@@ -1625,15 +1591,13 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="18">
-        <v>2018</v>
-      </c>
-      <c r="K44" s="15"/>
-      <c r="L44" s="18"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="8">
@@ -1644,15 +1608,14 @@
       <c r="G45">
         <v>1999</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J45" s="18"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H45" s="29"/>
+      <c r="I45" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J45" s="26"/>
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
@@ -1664,14 +1627,13 @@
       <c r="F46" s="4">
         <v>2002</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="15"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="26"/>
       <c r="J46" s="26"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="K46" s="16"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="11">
@@ -1680,16 +1642,15 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J47" s="18"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="18"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="H47" s="29"/>
+      <c r="I47" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J47" s="26"/>
+      <c r="K47" s="16"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
         <v>40</v>
       </c>
       <c r="C48" s="11">
@@ -1700,12 +1661,12 @@
       <c r="G48">
         <v>2011</v>
       </c>
-      <c r="I48" s="15"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
       <c r="J48" s="26"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
@@ -1717,15 +1678,14 @@
       <c r="G49">
         <v>2011</v>
       </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="16">
+      <c r="H49" s="29"/>
+      <c r="I49" s="29">
         <v>1999</v>
       </c>
-      <c r="J49" s="18"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J49" s="26"/>
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>47</v>
       </c>
@@ -1737,16 +1697,15 @@
       <c r="G50">
         <v>1999</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="18">
-        <v>2012</v>
-      </c>
-      <c r="K50" s="15"/>
-      <c r="L50" s="18"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="H50" s="29"/>
+      <c r="I50" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J50" s="26"/>
+      <c r="K50" s="16"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
         <v>42</v>
       </c>
       <c r="C51" s="11">
@@ -1756,15 +1715,13 @@
       <c r="G51">
         <v>1999</v>
       </c>
-      <c r="I51" s="15"/>
-      <c r="J51" s="26">
-        <v>2013</v>
-      </c>
-      <c r="K51" s="15"/>
-      <c r="L51" s="18"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="16"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
         <v>43</v>
       </c>
       <c r="C52" s="11">
@@ -1778,33 +1735,30 @@
       <c r="G52">
         <v>2000</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="18">
-        <v>2015</v>
-      </c>
-      <c r="K52" s="15"/>
-      <c r="L52" s="18"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H52" s="31"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C53" s="9"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="18"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C54" s="9"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="18"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B55" s="5"/>
@@ -1814,13 +1768,12 @@
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="15"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="26"/>
       <c r="J55" s="26"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="18"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K55" s="16"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>45</v>
       </c>
@@ -1836,38 +1789,33 @@
       <c r="G56">
         <v>1999</v>
       </c>
-      <c r="H56" s="13"/>
-      <c r="I56" s="16">
-        <v>2012</v>
-      </c>
-      <c r="J56" s="18"/>
-      <c r="K56" s="15">
-        <v>2012</v>
-      </c>
-      <c r="L56" s="18"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I57" s="15"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="18"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I58" s="20" t="s">
+      <c r="H56" s="34"/>
+      <c r="I56" s="29">
+        <v>2012</v>
+      </c>
+      <c r="J56" s="26">
+        <v>2012</v>
+      </c>
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="16"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I58" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="J58" s="21"/>
-      <c r="K58" s="20" t="s">
+      <c r="J58" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="L58" s="21"/>
+      <c r="K58" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1875,6 +1823,518 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1999</v>
+      </c>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2008</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2008</v>
+      </c>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2008</v>
+      </c>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2008</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="15">
+        <v>2018</v>
+      </c>
+      <c r="C11" s="19">
+        <v>41426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="19">
+        <v>41548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14">
+        <v>1999</v>
+      </c>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="14">
+        <v>1999</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="20"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="14">
+        <v>2004</v>
+      </c>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="14">
+        <v>2005</v>
+      </c>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C30" s="16"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="20">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C38" s="16"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="20">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="20">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="20">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="20"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="15">
+        <v>2015</v>
+      </c>
+      <c r="C43" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="20">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C45" s="16"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="13"/>
+      <c r="C46" s="20"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C47" s="16"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="20"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="14">
+        <v>1999</v>
+      </c>
+      <c r="C49" s="16"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="13"/>
+      <c r="C50" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="20">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="20">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+      <c r="C53" s="16"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="16"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="20"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="14">
+        <v>2012</v>
+      </c>
+      <c r="C56" s="16"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="13"/>
+      <c r="C57" s="16"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B58:C58"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32A262C-BF3B-4D84-B60A-8947EF3BFC30}">
   <dimension ref="A1:A48"/>
   <sheetViews>

</xml_diff>

<commit_message>
corrected Brazil and added more GDP indicators
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C97C7D3-8FA4-4743-B5C9-650F35D77853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6641E967-29C5-4BBF-B24A-4239D6D8FD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="16200" yWindow="0" windowWidth="12705" windowHeight="15585" activeTab="1" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
   <si>
     <t>United States</t>
   </si>
@@ -340,10 +340,37 @@
     <t>Quaterly</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
     <t>rate YoY</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>GDP YoY</t>
+  </si>
+  <si>
+    <t>GDP QoQ</t>
+  </si>
+  <si>
+    <t>2003 to 2021</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Growth YoY</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>GDP per</t>
+  </si>
+  <si>
+    <t>Capita</t>
+  </si>
+  <si>
+    <t>2010 to 2020</t>
   </si>
 </sst>
 </file>
@@ -500,7 +527,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -536,6 +563,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,22 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -888,9 +909,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H65" sqref="H65"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,10 +941,10 @@
       <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="32" t="s">
         <v>46</v>
       </c>
       <c r="I1" s="21" t="s">
@@ -1401,7 +1422,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="4"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="44"/>
+      <c r="H27" s="31"/>
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1431,7 +1452,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="46"/>
+      <c r="H30" s="33"/>
       <c r="I30" s="2">
         <v>2005</v>
       </c>
@@ -1466,7 +1487,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="46"/>
+      <c r="H32" s="33"/>
       <c r="I32" s="2">
         <v>2012</v>
       </c>
@@ -1494,7 +1515,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="7">
@@ -1504,7 +1525,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="47"/>
+      <c r="H34" s="42"/>
       <c r="I34" s="2">
         <v>2012</v>
       </c>
@@ -1524,7 +1545,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="2"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="47"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="2">
         <v>2012</v>
       </c>
@@ -1546,7 +1567,7 @@
       <c r="G36" s="16">
         <v>1999</v>
       </c>
-      <c r="H36" s="44"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="2">
         <v>2012</v>
       </c>
@@ -1596,7 +1617,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="2"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="46"/>
+      <c r="H39" s="33"/>
       <c r="I39" s="2">
         <v>2012</v>
       </c>
@@ -1670,7 +1691,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="2"/>
       <c r="G44" s="16"/>
-      <c r="H44" s="44"/>
+      <c r="H44" s="31"/>
       <c r="I44" s="2">
         <v>2012</v>
       </c>
@@ -1821,7 +1842,7 @@
       <c r="G53" s="16">
         <v>2000</v>
       </c>
-      <c r="H53" s="44"/>
+      <c r="H53" s="31"/>
       <c r="J53" s="16"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -1851,7 +1872,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="16"/>
-      <c r="H56" s="48"/>
+      <c r="H56" s="35"/>
       <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -1870,7 +1891,7 @@
       <c r="G57" s="16">
         <v>1999</v>
       </c>
-      <c r="H57" s="47"/>
+      <c r="H57" s="34"/>
       <c r="I57" s="2">
         <v>2012</v>
       </c>
@@ -1901,11 +1922,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T55" sqref="T55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,25 +1943,24 @@
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B1" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="28"/>
+      <c r="E1" s="37"/>
       <c r="I1" s="13"/>
-      <c r="J1" s="37"/>
       <c r="K1" s="16"/>
       <c r="M1" s="16"/>
       <c r="Q1" s="16"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
@@ -1953,47 +1973,59 @@
       <c r="E2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" t="s">
         <v>90</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" t="s">
         <v>92</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" t="s">
         <v>94</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="R2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>107</v>
+      </c>
+      <c r="V2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -2004,47 +2036,59 @@
       <c r="E3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" t="s">
         <v>88</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" s="33" t="s">
+      <c r="N3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" t="s">
         <v>95</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="R3" s="33" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U3" t="s">
+        <v>106</v>
+      </c>
+      <c r="V3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2060,7 +2104,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="38"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="18"/>
       <c r="L4" s="2"/>
       <c r="M4" s="18"/>
@@ -2069,8 +2113,12 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2088,21 +2136,27 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="39">
+      <c r="J5" s="4">
         <v>2002</v>
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="2"/>
       <c r="M5" s="18"/>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="28" t="s">
         <v>91</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="4">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2118,7 +2172,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="38"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="18"/>
       <c r="L6" s="2"/>
       <c r="M6" s="18"/>
@@ -2127,8 +2181,12 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="18"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2140,10 +2198,10 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="35"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="2"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="38"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="18"/>
       <c r="L7" s="2"/>
       <c r="M7" s="18"/>
@@ -2152,8 +2210,12 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2169,7 +2231,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="38"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="18"/>
       <c r="L8" s="2"/>
       <c r="M8" s="18"/>
@@ -2178,8 +2240,12 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2192,11 +2258,11 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="35"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="38"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="35"/>
+      <c r="L9" s="28"/>
       <c r="M9" s="18"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -2205,8 +2271,12 @@
       </c>
       <c r="Q9" s="18"/>
       <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2222,7 +2292,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="38"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="18"/>
       <c r="L10" s="2"/>
       <c r="M10" s="18"/>
@@ -2231,8 +2301,12 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2252,17 +2326,21 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="14"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="18"/>
       <c r="L11" s="2"/>
       <c r="M11" s="18"/>
-      <c r="N11" s="35"/>
+      <c r="N11" s="28"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="35"/>
+      <c r="P11" s="28"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -2273,9 +2351,9 @@
       <c r="E12" s="16"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="35"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="18"/>
       <c r="L12" s="2"/>
       <c r="M12" s="18"/>
@@ -2286,8 +2364,12 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2298,9 +2380,9 @@
       <c r="E13" s="16"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="35"/>
+      <c r="H13" s="28"/>
       <c r="I13" s="14"/>
-      <c r="J13" s="38"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="18"/>
       <c r="L13" s="2"/>
       <c r="M13" s="18"/>
@@ -2311,8 +2393,12 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2326,11 +2412,11 @@
       <c r="E14" s="16"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="42" t="s">
+      <c r="H14" s="28"/>
+      <c r="I14" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="18"/>
       <c r="L14" s="2"/>
       <c r="M14" s="18"/>
@@ -2339,8 +2425,12 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -2356,7 +2446,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="14"/>
-      <c r="J15" s="38"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="18"/>
       <c r="L15" s="2"/>
       <c r="M15" s="18"/>
@@ -2365,8 +2455,12 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>15</v>
       </c>
@@ -2376,13 +2470,12 @@
       <c r="C16" s="16"/>
       <c r="E16" s="16"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="34"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="27"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -2398,7 +2491,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="38"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="18"/>
       <c r="L17" s="2"/>
       <c r="M17" s="18"/>
@@ -2407,8 +2500,12 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>21</v>
       </c>
@@ -2418,13 +2515,12 @@
       <c r="C18" s="16"/>
       <c r="E18" s="16"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="37"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="34"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="27"/>
       <c r="Q18" s="16"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -2433,9 +2529,9 @@
       <c r="E19" s="16"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="35"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="14"/>
-      <c r="J19" s="38"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="18"/>
       <c r="L19" s="2"/>
       <c r="M19" s="18"/>
@@ -2444,8 +2540,12 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -2454,9 +2554,9 @@
       <c r="E20" s="16"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="35"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="14"/>
-      <c r="J20" s="38"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="18"/>
       <c r="L20" s="2"/>
       <c r="M20" s="18"/>
@@ -2467,8 +2567,12 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -2478,10 +2582,10 @@
       <c r="C21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="14"/>
-      <c r="J21" s="38"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="18"/>
       <c r="L21" s="2"/>
       <c r="M21" s="18"/>
@@ -2490,8 +2594,12 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2504,9 +2612,9 @@
       <c r="G22" s="4">
         <v>2011</v>
       </c>
-      <c r="H22" s="35"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="38"/>
+      <c r="J22" s="2"/>
       <c r="K22" s="18"/>
       <c r="L22" s="4">
         <v>2012</v>
@@ -2517,8 +2625,12 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2532,9 +2644,9 @@
       <c r="E23" s="16"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="35"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="38"/>
+      <c r="J23" s="2"/>
       <c r="K23" s="18"/>
       <c r="L23" s="2"/>
       <c r="M23" s="18"/>
@@ -2545,8 +2657,12 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2559,19 +2675,23 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="38"/>
+      <c r="J24" s="2"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="35"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="18"/>
-      <c r="N24" s="35"/>
+      <c r="N24" s="28"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="35"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="2"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -2582,9 +2702,9 @@
       <c r="E25" s="16"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="35"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="38"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="18"/>
       <c r="L25" s="2"/>
       <c r="M25" s="18"/>
@@ -2593,8 +2713,12 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="2"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -2603,9 +2727,9 @@
       <c r="E26" s="16"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="35"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="14"/>
-      <c r="J26" s="38"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="18"/>
       <c r="L26" s="2"/>
       <c r="M26" s="18"/>
@@ -2614,44 +2738,51 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="2"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="14">
         <v>2012</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="2">
         <v>2012</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="35"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="14"/>
-      <c r="J27" s="38"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="35"/>
+      <c r="L27" s="28"/>
       <c r="M27" s="20"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="20"/>
-      <c r="R27" s="35"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28" s="13"/>
       <c r="C28" s="16"/>
       <c r="E28" s="16"/>
       <c r="I28" s="13"/>
-      <c r="J28" s="37"/>
       <c r="K28" s="16"/>
       <c r="M28" s="16"/>
       <c r="Q28" s="16"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -2659,12 +2790,11 @@
       <c r="C29" s="17"/>
       <c r="E29" s="16"/>
       <c r="I29" s="13"/>
-      <c r="J29" s="37"/>
       <c r="K29" s="16"/>
       <c r="M29" s="16"/>
       <c r="Q29" s="16"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2682,19 +2812,25 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="14"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="44">
+      <c r="J30" s="2"/>
+      <c r="K30" s="31">
         <v>2014</v>
       </c>
-      <c r="L30" s="35"/>
+      <c r="L30" s="28"/>
       <c r="M30" s="20"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="35"/>
+      <c r="P30" s="28"/>
       <c r="Q30" s="20"/>
       <c r="R30" s="2"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="4">
+        <v>2011</v>
+      </c>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>24</v>
       </c>
@@ -2704,12 +2840,11 @@
       <c r="C31" s="16"/>
       <c r="E31" s="16"/>
       <c r="I31" s="13"/>
-      <c r="J31" s="37"/>
       <c r="K31" s="16"/>
       <c r="M31" s="16"/>
       <c r="Q31" s="16"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2724,28 +2859,32 @@
       <c r="F32" s="4">
         <v>2000</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="28" t="s">
         <v>76</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="14"/>
-      <c r="J32" s="39">
+      <c r="J32" s="4">
         <v>2011</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="31">
         <v>2011</v>
       </c>
-      <c r="L32" s="35"/>
+      <c r="L32" s="28"/>
       <c r="M32" s="20"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="44">
+      <c r="Q32" s="31">
         <v>2012</v>
       </c>
       <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="28"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2758,8 +2897,8 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="14"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="44">
+      <c r="J33" s="2"/>
+      <c r="K33" s="31">
         <v>2000</v>
       </c>
       <c r="L33" s="2"/>
@@ -2769,10 +2908,14 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="2"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="B34" s="14">
         <v>2012</v>
@@ -2782,21 +2925,25 @@
         <v>2012</v>
       </c>
       <c r="E34" s="16"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="35"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="28"/>
       <c r="M34" s="20"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="35"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="28"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
@@ -2805,25 +2952,33 @@
         <v>2012</v>
       </c>
       <c r="E35" s="16"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="40"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="28"/>
       <c r="K35" s="20"/>
-      <c r="L35" s="35"/>
+      <c r="L35" s="28"/>
       <c r="M35" s="20"/>
       <c r="N35" s="2"/>
       <c r="O35" s="4">
         <v>2006</v>
       </c>
-      <c r="P35" s="35"/>
+      <c r="P35" s="28"/>
       <c r="Q35" s="20"/>
       <c r="R35" s="4">
         <v>2011</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="4">
+        <v>2010</v>
+      </c>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
@@ -2836,17 +2991,23 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="14"/>
-      <c r="J36" s="38"/>
+      <c r="J36" s="2"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="35"/>
+      <c r="L36" s="28"/>
       <c r="M36" s="20"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="35"/>
+      <c r="P36" s="28"/>
       <c r="Q36" s="18"/>
       <c r="R36" s="2"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -2861,8 +3022,8 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="14"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="44">
+      <c r="J37" s="2"/>
+      <c r="K37" s="31">
         <v>2001</v>
       </c>
       <c r="L37" s="2"/>
@@ -2871,11 +3032,17 @@
       <c r="O37" s="4">
         <v>2006</v>
       </c>
-      <c r="P37" s="35"/>
+      <c r="P37" s="28"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>31</v>
       </c>
@@ -2885,12 +3052,11 @@
       </c>
       <c r="E38" s="16"/>
       <c r="I38" s="13"/>
-      <c r="J38" s="37"/>
       <c r="K38" s="16"/>
       <c r="M38" s="16"/>
       <c r="Q38" s="16"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
@@ -2907,21 +3073,25 @@
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="14"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="44">
-        <v>2012</v>
-      </c>
-      <c r="L39" s="35"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="31">
+        <v>2012</v>
+      </c>
+      <c r="L39" s="28"/>
       <c r="M39" s="20"/>
       <c r="N39" s="2"/>
       <c r="O39" s="4">
         <v>2004</v>
       </c>
-      <c r="P39" s="35"/>
+      <c r="P39" s="28"/>
       <c r="Q39" s="18"/>
       <c r="R39" s="2"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="28"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>33</v>
       </c>
@@ -2931,12 +3101,11 @@
       </c>
       <c r="E40" s="16"/>
       <c r="I40" s="13"/>
-      <c r="J40" s="37"/>
       <c r="K40" s="16"/>
       <c r="M40" s="16"/>
       <c r="Q40" s="16"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>49</v>
       </c>
@@ -2946,12 +3115,11 @@
       </c>
       <c r="E41" s="16"/>
       <c r="I41" s="13"/>
-      <c r="J41" s="37"/>
       <c r="K41" s="16"/>
       <c r="M41" s="16"/>
       <c r="Q41" s="16"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>34</v>
       </c>
@@ -2961,12 +3129,11 @@
       </c>
       <c r="E42" s="16"/>
       <c r="I42" s="13"/>
-      <c r="J42" s="37"/>
       <c r="K42" s="16"/>
       <c r="M42" s="16"/>
       <c r="Q42" s="16"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>35</v>
       </c>
@@ -2974,12 +3141,11 @@
       <c r="C43" s="20"/>
       <c r="E43" s="17"/>
       <c r="I43" s="13"/>
-      <c r="J43" s="37"/>
       <c r="K43" s="16"/>
       <c r="M43" s="16"/>
       <c r="Q43" s="16"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -2996,14 +3162,14 @@
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="14"/>
-      <c r="J44" s="40" t="s">
+      <c r="J44" s="28" t="s">
         <v>82</v>
       </c>
       <c r="K44" s="20"/>
       <c r="L44" s="4">
         <v>2005</v>
       </c>
-      <c r="M44" s="44">
+      <c r="M44" s="31">
         <v>2005</v>
       </c>
       <c r="N44" s="2"/>
@@ -3011,8 +3177,12 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="18"/>
       <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="28"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
@@ -3022,12 +3192,11 @@
       </c>
       <c r="E45" s="16"/>
       <c r="I45" s="13"/>
-      <c r="J45" s="37"/>
       <c r="K45" s="16"/>
       <c r="M45" s="16"/>
       <c r="Q45" s="16"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -3040,10 +3209,10 @@
       <c r="G46" s="4">
         <v>2001</v>
       </c>
-      <c r="H46" s="35"/>
+      <c r="H46" s="28"/>
       <c r="I46" s="14"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="44">
+      <c r="J46" s="2"/>
+      <c r="K46" s="31">
         <v>2001</v>
       </c>
       <c r="L46" s="2"/>
@@ -3055,8 +3224,12 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="18"/>
       <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
@@ -3069,10 +3242,10 @@
       <c r="G47" s="4">
         <v>2002</v>
       </c>
-      <c r="H47" s="35"/>
+      <c r="H47" s="28"/>
       <c r="I47" s="14"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="44">
+      <c r="J47" s="2"/>
+      <c r="K47" s="31">
         <v>2004</v>
       </c>
       <c r="L47" s="2"/>
@@ -3084,8 +3257,12 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="18"/>
       <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
@@ -3096,9 +3273,9 @@
       <c r="E48" s="16"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="35"/>
+      <c r="H48" s="28"/>
       <c r="I48" s="14"/>
-      <c r="J48" s="38"/>
+      <c r="J48" s="2"/>
       <c r="K48" s="18"/>
       <c r="L48" s="2"/>
       <c r="M48" s="18"/>
@@ -3109,8 +3286,12 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="18"/>
       <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>40</v>
       </c>
@@ -3118,12 +3299,11 @@
       <c r="C49" s="20"/>
       <c r="E49" s="16"/>
       <c r="I49" s="13"/>
-      <c r="J49" s="37"/>
       <c r="K49" s="16"/>
       <c r="M49" s="16"/>
       <c r="Q49" s="16"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -3134,9 +3314,9 @@
       <c r="E50" s="16"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="35"/>
+      <c r="H50" s="28"/>
       <c r="I50" s="14"/>
-      <c r="J50" s="38"/>
+      <c r="J50" s="2"/>
       <c r="K50" s="18"/>
       <c r="L50" s="2"/>
       <c r="M50" s="18"/>
@@ -3145,8 +3325,12 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="18"/>
       <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
@@ -3157,10 +3341,10 @@
       <c r="E51" s="16"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="35"/>
+      <c r="H51" s="28"/>
       <c r="I51" s="14"/>
-      <c r="J51" s="38"/>
-      <c r="K51" s="44">
+      <c r="J51" s="2"/>
+      <c r="K51" s="31">
         <v>2000</v>
       </c>
       <c r="L51" s="2"/>
@@ -3170,8 +3354,12 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="2"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>42</v>
       </c>
@@ -3181,12 +3369,11 @@
       </c>
       <c r="E52" s="16"/>
       <c r="I52" s="13"/>
-      <c r="J52" s="37"/>
       <c r="K52" s="16"/>
       <c r="M52" s="16"/>
       <c r="Q52" s="16"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>43</v>
       </c>
@@ -3199,41 +3386,52 @@
       <c r="G53" s="4">
         <v>2001</v>
       </c>
-      <c r="H53" s="35"/>
+      <c r="H53" s="28"/>
       <c r="I53" s="14"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="44">
+      <c r="J53" s="2"/>
+      <c r="K53" s="31">
         <v>2003</v>
       </c>
       <c r="L53" s="4">
         <v>2007</v>
       </c>
-      <c r="M53" s="44">
+      <c r="M53" s="31">
         <v>2007</v>
       </c>
       <c r="N53" s="2"/>
-      <c r="O53" s="39">
+      <c r="O53" s="4">
         <v>2005</v>
       </c>
       <c r="P53" s="2"/>
-      <c r="Q53" s="44">
+      <c r="Q53" s="31">
         <v>2006</v>
       </c>
-      <c r="R53" s="39">
+      <c r="R53" s="4">
         <v>2006</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S53" s="4">
+        <v>2005</v>
+      </c>
+      <c r="T53" s="4">
+        <v>2006</v>
+      </c>
+      <c r="U53" s="4">
+        <v>2006</v>
+      </c>
+      <c r="V53" s="4">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B54" s="13"/>
       <c r="C54" s="16"/>
       <c r="E54" s="16"/>
       <c r="I54" s="13"/>
-      <c r="J54" s="37"/>
       <c r="K54" s="16"/>
       <c r="M54" s="16"/>
       <c r="Q54" s="16"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
@@ -3241,25 +3439,24 @@
       <c r="C55" s="16"/>
       <c r="E55" s="16"/>
       <c r="I55" s="13"/>
-      <c r="J55" s="37"/>
       <c r="K55" s="16"/>
       <c r="M55" s="16"/>
       <c r="Q55" s="16"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="20"/>
       <c r="E56" s="16"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="42"/>
-      <c r="J56" s="40"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="28"/>
       <c r="K56" s="20"/>
-      <c r="L56" s="35"/>
+      <c r="L56" s="28"/>
       <c r="M56" s="20"/>
       <c r="N56" s="4">
         <v>2017</v>
@@ -3267,11 +3464,19 @@
       <c r="O56" s="4">
         <v>2006</v>
       </c>
-      <c r="P56" s="35"/>
+      <c r="P56" s="28"/>
       <c r="Q56" s="20"/>
       <c r="R56" s="2"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56" s="2"/>
+      <c r="T56" s="4">
+        <v>2005</v>
+      </c>
+      <c r="U56" s="4">
+        <v>2005</v>
+      </c>
+      <c r="V56" s="28"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -3283,60 +3488,69 @@
         <v>2012</v>
       </c>
       <c r="E57" s="16"/>
-      <c r="F57" s="35" t="s">
+      <c r="F57" s="28" t="s">
         <v>74</v>
       </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="42" t="s">
+      <c r="H57" s="28"/>
+      <c r="I57" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J57" s="40" t="s">
+      <c r="J57" s="28" t="s">
         <v>74</v>
       </c>
       <c r="K57" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L57" s="35"/>
+      <c r="L57" s="28"/>
       <c r="M57" s="20"/>
-      <c r="N57" s="35" t="s">
+      <c r="N57" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="O57" s="35" t="s">
+      <c r="O57" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="P57" s="35" t="s">
+      <c r="P57" s="28" t="s">
         <v>91</v>
       </c>
       <c r="Q57" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="R57" s="35" t="s">
+      <c r="R57" s="28" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="T57" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="U57" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="V57" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58" s="13"/>
       <c r="C58" s="16"/>
       <c r="E58" s="16"/>
       <c r="I58" s="13"/>
-      <c r="J58" s="37"/>
       <c r="K58" s="16"/>
       <c r="M58" s="16"/>
       <c r="Q58" s="16"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="29" t="s">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B59" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="32" t="s">
+      <c r="C59" s="39"/>
+      <c r="D59" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="30"/>
+      <c r="E59" s="39"/>
       <c r="H59" s="16"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
       <c r="K59" s="16"/>
       <c r="M59" s="16"/>
       <c r="Q59" s="16"/>

</xml_diff>

<commit_message>
updated BIS central bank rates
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482CFCB7-D6CD-49C0-B26D-5B31FE33A2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A08DD2D-B774-45DA-9A93-BB477EA09992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="141">
   <si>
     <t>United States</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>Residential Buildings</t>
+  </si>
+  <si>
+    <t>Central Bank</t>
+  </si>
+  <si>
+    <t>Policy Rates</t>
   </si>
 </sst>
 </file>
@@ -611,7 +617,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -654,6 +660,9 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -672,19 +681,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1003,9 +1003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C47" sqref="C47:C53"/>
+      <selection pane="topRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1314,7 @@
       <c r="C16" s="10">
         <v>40</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="13"/>
@@ -1437,7 +1437,7 @@
       <c r="C23" s="8">
         <v>26</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="13"/>
@@ -1479,7 +1479,7 @@
       <c r="C25" s="12">
         <v>31</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="13"/>
@@ -1598,7 +1598,9 @@
         <v>12</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="20">
+        <v>36281</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="13"/>
       <c r="H33" s="15"/>
@@ -1636,7 +1638,9 @@
         <v>18</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>2000</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="13"/>
       <c r="H35" s="30"/>
@@ -1693,7 +1697,9 @@
         <v>27</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="4"/>
+      <c r="E38" s="4">
+        <v>2000</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
@@ -1708,7 +1714,9 @@
         <v>16</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4">
+        <v>2005</v>
+      </c>
       <c r="F39" s="2"/>
       <c r="G39" s="13"/>
       <c r="H39" s="29"/>
@@ -1766,7 +1774,7 @@
       <c r="C43" s="11">
         <v>57</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="4"/>
       <c r="G43" s="13">
         <v>2010</v>
       </c>
@@ -1782,7 +1790,9 @@
         <v>19</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="4"/>
+      <c r="E44" s="4">
+        <v>2002</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="13"/>
       <c r="H44" s="27"/>
@@ -1846,8 +1856,10 @@
       <c r="C48" s="11">
         <v>53</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4">
+        <v>2001</v>
+      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="13"/>
       <c r="H48" s="15"/>
@@ -1864,7 +1876,9 @@
         <v>48</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="4"/>
+      <c r="E49" s="4">
+        <v>2003</v>
+      </c>
       <c r="G49" s="13">
         <v>2011</v>
       </c>
@@ -1962,7 +1976,7 @@
       <c r="C56" s="8">
         <v>23</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="4"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="13"/>
@@ -2016,11 +2030,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:AI59"/>
+  <dimension ref="A1:AJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL13" sqref="AL13"/>
+      <selection pane="topRight" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,89 +2047,92 @@
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="13" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="13"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" style="40" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="13" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="11.7109375" customWidth="1"/>
-    <col min="29" max="29" width="11.7109375" style="13" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" style="13" customWidth="1"/>
-    <col min="32" max="32" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" style="13" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.7109375" style="13" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" style="13" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="34" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="34" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="34" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="34" t="s">
+      <c r="O1" s="40"/>
+      <c r="P1" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="34" t="s">
+      <c r="Q1" s="41"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="34" t="s">
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="18" t="s">
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AG1" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2142,13 +2159,13 @@
       <c r="J2" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" t="s">
         <v>107</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" t="s">
         <v>117</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="M2" s="13" t="s">
         <v>117</v>
       </c>
       <c r="N2" t="s">
@@ -2166,60 +2183,62 @@
       <c r="R2" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" t="s">
         <v>79</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="40" t="s">
+      <c r="V2" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="49" t="s">
+      <c r="W2" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="50" t="s">
+      <c r="X2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>92</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>104</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>106</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>125</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>127</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AD2" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>93</v>
       </c>
-      <c r="AF2" s="40" t="s">
+      <c r="AG2" t="s">
         <v>95</v>
       </c>
-      <c r="AG2" s="49" t="s">
+      <c r="AH2" t="s">
         <v>130</v>
       </c>
-      <c r="AH2" s="49" t="s">
+      <c r="AI2" t="s">
         <v>133</v>
       </c>
-      <c r="AI2" s="49" t="s">
+      <c r="AJ2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="40"/>
       <c r="C3" s="13" t="s">
         <v>66</v>
       </c>
@@ -2241,13 +2260,13 @@
       <c r="J3" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" t="s">
         <v>114</v>
       </c>
-      <c r="M3" s="50" t="s">
+      <c r="M3" s="13" t="s">
         <v>118</v>
       </c>
       <c r="N3" t="s">
@@ -2262,60 +2281,63 @@
       <c r="Q3" t="s">
         <v>124</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" t="s">
+        <v>140</v>
+      </c>
+      <c r="T3" t="s">
         <v>80</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>84</v>
       </c>
-      <c r="U3" s="40" t="s">
+      <c r="V3" t="s">
         <v>84</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="W3" t="s">
         <v>121</v>
       </c>
-      <c r="W3" s="50" t="s">
+      <c r="X3" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>129</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>105</v>
       </c>
       <c r="Z3" t="s">
         <v>105</v>
       </c>
       <c r="AA3" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="AB3" t="s">
         <v>126</v>
       </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AC3" t="s">
         <v>126</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE3" t="s">
         <v>94</v>
       </c>
-      <c r="AF3" s="40" t="s">
+      <c r="AG3" t="s">
         <v>96</v>
       </c>
-      <c r="AG3" s="49" t="s">
+      <c r="AH3" t="s">
         <v>131</v>
       </c>
-      <c r="AH3" s="49" t="s">
+      <c r="AI3" t="s">
         <v>134</v>
       </c>
-      <c r="AI3" s="49" t="s">
+      <c r="AJ3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="2">
         <v>1999</v>
       </c>
       <c r="D4" s="2">
@@ -2326,7 +2348,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="41"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="15"/>
       <c r="N4" s="2"/>
@@ -2334,28 +2356,29 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="15"/>
-      <c r="S4" s="41"/>
+      <c r="S4" s="2"/>
       <c r="T4" s="2"/>
-      <c r="U4" s="41"/>
+      <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="2"/>
-      <c r="AF4" s="41"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="25"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="25"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="2">
         <v>2008</v>
       </c>
       <c r="D5" s="4">
@@ -2369,7 +2392,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="42">
+      <c r="K5" s="4">
         <v>2007</v>
       </c>
       <c r="L5" s="2"/>
@@ -2385,30 +2408,31 @@
       <c r="R5" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="S5" s="41"/>
-      <c r="T5" s="4">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="4">
         <v>2002</v>
       </c>
-      <c r="U5" s="41"/>
       <c r="V5" s="2"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="15"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="2"/>
-      <c r="AF5" s="41"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="25"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="25"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="2">
         <v>2008</v>
       </c>
       <c r="D6" s="2">
@@ -2419,7 +2443,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="41"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="15"/>
       <c r="N6" s="2"/>
@@ -2427,28 +2451,29 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="15"/>
-      <c r="S6" s="41"/>
+      <c r="S6" s="2"/>
       <c r="T6" s="2"/>
-      <c r="U6" s="41"/>
+      <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="15"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="2"/>
-      <c r="AF6" s="41"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
-      <c r="AI6" s="25"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="25"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="4">
         <v>2021</v>
       </c>
       <c r="C7" s="15">
@@ -2459,7 +2484,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="41"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="15"/>
       <c r="N7" s="2"/>
@@ -2467,28 +2492,29 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="15"/>
-      <c r="S7" s="41"/>
+      <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="U7" s="41"/>
+      <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="15"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="2"/>
-      <c r="AF7" s="41"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="2">
         <v>2008</v>
       </c>
       <c r="D8" s="2">
@@ -2499,7 +2525,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="41"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="15"/>
       <c r="N8" s="2"/>
@@ -2507,28 +2533,28 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="15"/>
-      <c r="S8" s="41"/>
+      <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="17"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="2"/>
-      <c r="AF8" s="41"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="2"/>
       <c r="AG8" s="2"/>
-      <c r="AH8" s="25"/>
-      <c r="AI8" s="2"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="40"/>
       <c r="C9" s="15">
         <v>2012</v>
       </c>
@@ -2540,7 +2566,7 @@
       <c r="H9" s="17"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="41"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="15"/>
       <c r="N9" s="25"/>
@@ -2548,30 +2574,31 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="15"/>
-      <c r="S9" s="41"/>
+      <c r="S9" s="2"/>
       <c r="T9" s="2"/>
-      <c r="U9" s="41"/>
+      <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="15"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="4">
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="4">
         <v>2011</v>
       </c>
-      <c r="AF9" s="41"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
-      <c r="AI9" s="25"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="25"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="2">
         <v>2008</v>
       </c>
       <c r="D10" s="2">
@@ -2582,7 +2609,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="41"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="15"/>
       <c r="N10" s="2"/>
@@ -2590,28 +2617,29 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="15"/>
-      <c r="S10" s="41"/>
+      <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="17"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="2"/>
-      <c r="AF10" s="41"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="2"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="4">
         <v>2018</v>
       </c>
       <c r="C11" s="16">
@@ -2628,7 +2656,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="41"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="15"/>
       <c r="N11" s="2"/>
@@ -2636,28 +2664,28 @@
       <c r="P11" s="25"/>
       <c r="Q11" s="25"/>
       <c r="R11" s="17"/>
-      <c r="S11" s="41"/>
+      <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="41"/>
+      <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="15"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="25"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="25"/>
-      <c r="AH11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="25"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="25"/>
       <c r="AI11" s="2"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="40"/>
       <c r="C12" s="16">
         <v>41548</v>
       </c>
@@ -2666,7 +2694,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="41"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="15"/>
       <c r="N12" s="2"/>
@@ -2674,32 +2702,32 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="15"/>
-      <c r="S12" s="41"/>
+      <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="4">
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="4">
         <v>2003</v>
       </c>
-      <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="2"/>
-      <c r="AF12" s="41"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
-      <c r="AI12" s="25" t="s">
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="40"/>
       <c r="C13" s="16" t="s">
         <v>65</v>
       </c>
@@ -2708,7 +2736,7 @@
       <c r="H13" s="17"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="41"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="15"/>
       <c r="N13" s="2"/>
@@ -2716,30 +2744,31 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="15"/>
-      <c r="S13" s="41"/>
+      <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="41"/>
+      <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="4">
+      <c r="W13" s="2"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="4">
         <v>2005</v>
       </c>
-      <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="2"/>
-      <c r="AF13" s="41"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
-      <c r="AI13" s="25"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="25"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="2">
         <v>1999</v>
       </c>
       <c r="D14" s="2">
@@ -2750,7 +2779,7 @@
       <c r="H14" s="17"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="41"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="15"/>
       <c r="N14" s="2"/>
@@ -2758,30 +2787,31 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="15"/>
-      <c r="S14" s="46" t="s">
+      <c r="S14" s="2"/>
+      <c r="T14" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="T14" s="2"/>
-      <c r="U14" s="41"/>
+      <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="15"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="2"/>
-      <c r="AF14" s="41"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="2">
         <v>2012</v>
       </c>
       <c r="D15" s="2">
@@ -2792,7 +2822,7 @@
       <c r="H15" s="15"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="41"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="15"/>
       <c r="N15" s="2"/>
@@ -2800,41 +2830,41 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="15"/>
-      <c r="S15" s="41"/>
+      <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="17"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="2"/>
-      <c r="AF15" s="41"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="AJ15" s="2"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="41">
-        <v>2012</v>
-      </c>
-      <c r="L16"/>
+      <c r="B16" s="2">
+        <v>2012</v>
+      </c>
       <c r="N16" s="26"/>
       <c r="O16" s="24"/>
-      <c r="S16" s="40"/>
-      <c r="U16" s="47"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S16" s="2"/>
+      <c r="V16" s="26"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="2">
         <v>2012</v>
       </c>
       <c r="D17" s="2">
@@ -2845,7 +2875,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="41"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="15"/>
       <c r="N17" s="2"/>
@@ -2853,47 +2883,45 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="15"/>
-      <c r="S17" s="41"/>
+      <c r="S17" s="2"/>
       <c r="T17" s="2"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="17"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="2"/>
-      <c r="AF17" s="41"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
-      <c r="AI17" s="25"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="25"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="2">
         <v>1999</v>
       </c>
-      <c r="L18"/>
       <c r="N18" s="26"/>
       <c r="O18" s="24"/>
-      <c r="S18" s="40"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="40"/>
       <c r="C19" s="17"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="17"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="41"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="15"/>
       <c r="N19" s="2"/>
@@ -2901,35 +2929,35 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="15"/>
-      <c r="S19" s="41"/>
+      <c r="S19" s="2"/>
       <c r="T19" s="2"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="17"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="2"/>
-      <c r="AF19" s="41"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ19" s="2"/>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="40"/>
       <c r="C20" s="17"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="17"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="41"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="15"/>
       <c r="N20" s="2"/>
@@ -2937,30 +2965,31 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="15"/>
-      <c r="S20" s="41"/>
+      <c r="S20" s="2"/>
       <c r="T20" s="2"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="4">
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="4">
         <v>2003</v>
       </c>
-      <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="2"/>
-      <c r="AF20" s="41"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ20" s="2"/>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="2">
         <v>2004</v>
       </c>
       <c r="F21" s="2"/>
@@ -2968,7 +2997,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="41"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="15"/>
       <c r="N21" s="2"/>
@@ -2976,28 +3005,28 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="15"/>
-      <c r="S21" s="41"/>
+      <c r="S21" s="2"/>
       <c r="T21" s="2"/>
-      <c r="U21" s="41"/>
+      <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="15"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="2"/>
-      <c r="AF21" s="41"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ21" s="2"/>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="40"/>
       <c r="C22" s="15">
         <v>2012</v>
       </c>
@@ -3008,7 +3037,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="41"/>
+      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="15"/>
       <c r="N22" s="4">
@@ -3018,30 +3047,31 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="15"/>
-      <c r="S22" s="41"/>
+      <c r="S22" s="2"/>
       <c r="T22" s="2"/>
-      <c r="U22" s="41"/>
+      <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="15"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="2"/>
-      <c r="AF22" s="41"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="2"/>
       <c r="AG22" s="2"/>
-      <c r="AH22" s="4">
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="4">
         <v>2004</v>
       </c>
-      <c r="AI22" s="2"/>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ22" s="2"/>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="41">
+      <c r="B23" s="2">
         <v>2012</v>
       </c>
       <c r="D23" s="2">
@@ -3052,7 +3082,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="41"/>
+      <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="15"/>
       <c r="N23" s="2"/>
@@ -3060,32 +3090,32 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="15"/>
-      <c r="S23" s="41"/>
+      <c r="S23" s="2"/>
       <c r="T23" s="2"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="17"/>
-      <c r="X23" s="4">
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="4">
         <v>2002</v>
       </c>
-      <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="2"/>
-      <c r="AF23" s="41"/>
-      <c r="AG23" s="4">
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="4">
         <v>2000</v>
       </c>
-      <c r="AH23" s="2"/>
-      <c r="AI23" s="25"/>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="25"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="40"/>
       <c r="C24" s="15">
         <v>2012</v>
       </c>
@@ -3097,7 +3127,7 @@
       <c r="H24" s="17"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="41"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="15"/>
       <c r="N24" s="25"/>
@@ -3105,30 +3135,31 @@
       <c r="P24" s="25"/>
       <c r="Q24" s="25"/>
       <c r="R24" s="17"/>
-      <c r="S24" s="41"/>
+      <c r="S24" s="2"/>
       <c r="T24" s="2"/>
-      <c r="U24" s="41"/>
+      <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="17" t="s">
+      <c r="W24" s="2"/>
+      <c r="X24" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="25"/>
-      <c r="AF24" s="41"/>
-      <c r="AG24" s="25"/>
-      <c r="AH24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="25"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="25"/>
       <c r="AI24" s="2"/>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ24" s="2"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="41">
+      <c r="B25" s="2">
         <v>2012</v>
       </c>
       <c r="F25" s="2"/>
@@ -3136,7 +3167,7 @@
       <c r="H25" s="17"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="41"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="15"/>
       <c r="N25" s="2"/>
@@ -3144,35 +3175,35 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="15"/>
-      <c r="S25" s="41"/>
+      <c r="S25" s="2"/>
       <c r="T25" s="2"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="17"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="2"/>
-      <c r="AF25" s="41"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
-      <c r="AI25" s="25"/>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="25"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="40"/>
       <c r="C26" s="17"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="17"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="41"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="15"/>
       <c r="N26" s="2"/>
@@ -3180,28 +3211,29 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="15"/>
-      <c r="S26" s="41"/>
+      <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-      <c r="U26" s="41"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="25"/>
+      <c r="X26" s="17"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
-      <c r="AC26" s="15"/>
-      <c r="AD26" s="2"/>
-      <c r="AF26" s="41"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ26" s="2"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="41">
+      <c r="B27" s="2">
         <v>2012</v>
       </c>
       <c r="C27" s="24"/>
@@ -3213,7 +3245,7 @@
       <c r="H27" s="17"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
-      <c r="K27" s="46"/>
+      <c r="K27" s="25"/>
       <c r="L27" s="2"/>
       <c r="M27" s="15"/>
       <c r="N27" s="25"/>
@@ -3221,44 +3253,37 @@
       <c r="P27" s="25"/>
       <c r="Q27" s="25"/>
       <c r="R27" s="17"/>
-      <c r="S27" s="41"/>
+      <c r="S27" s="2"/>
       <c r="T27" s="2"/>
-      <c r="U27" s="41"/>
+      <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="25"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="15"/>
       <c r="Y27" s="25"/>
       <c r="Z27" s="25"/>
       <c r="AA27" s="25"/>
       <c r="AB27" s="25"/>
-      <c r="AC27" s="17"/>
-      <c r="AD27" s="2"/>
-      <c r="AF27" s="46"/>
-      <c r="AG27" s="2"/>
-      <c r="AH27" s="25" t="s">
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="2"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="AI27" s="2"/>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B28" s="40"/>
-      <c r="L28"/>
-      <c r="S28" s="40"/>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ27" s="2"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="40"/>
       <c r="C29" s="14"/>
-      <c r="L29"/>
-      <c r="S29" s="40"/>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B30" s="2">
         <v>2005</v>
       </c>
       <c r="D30" s="2">
@@ -3273,7 +3298,7 @@
       <c r="J30" s="4">
         <v>2011</v>
       </c>
-      <c r="K30" s="46"/>
+      <c r="K30" s="25"/>
       <c r="L30" s="2"/>
       <c r="M30" s="15"/>
       <c r="N30" s="25"/>
@@ -3281,42 +3306,41 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="15"/>
-      <c r="S30" s="41"/>
+      <c r="S30" s="2"/>
       <c r="T30" s="2"/>
-      <c r="U30" s="42">
+      <c r="U30" s="2"/>
+      <c r="V30" s="4">
         <v>2014</v>
       </c>
-      <c r="V30" s="2"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="25"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="2"/>
       <c r="Z30" s="25"/>
-      <c r="AA30" s="2"/>
+      <c r="AA30" s="25"/>
       <c r="AB30" s="2"/>
-      <c r="AC30" s="15"/>
-      <c r="AD30" s="25"/>
-      <c r="AF30" s="46"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="25"/>
       <c r="AG30" s="25"/>
-      <c r="AH30" s="25" t="s">
+      <c r="AH30" s="25"/>
+      <c r="AI30" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="AI30" s="25"/>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="AJ30" s="25"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="41">
-        <v>2012</v>
-      </c>
-      <c r="L31"/>
-      <c r="S31" s="40"/>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="41">
+      <c r="B32" s="2">
         <v>2012</v>
       </c>
       <c r="D32" s="2">
@@ -3331,7 +3355,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="46"/>
+      <c r="K32" s="25"/>
       <c r="L32" s="25" t="s">
         <v>81</v>
       </c>
@@ -3343,36 +3367,37 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="15"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="4">
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="4">
         <v>2011</v>
       </c>
-      <c r="U32" s="42">
+      <c r="V32" s="4">
         <v>2011</v>
       </c>
-      <c r="V32" s="2"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="15"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
-      <c r="AC32" s="15"/>
-      <c r="AD32" s="2"/>
-      <c r="AF32" s="42">
-        <v>2012</v>
-      </c>
-      <c r="AG32" s="25"/>
-      <c r="AH32" s="25" t="s">
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="15"/>
+      <c r="AE32" s="2"/>
+      <c r="AG32" s="4">
+        <v>2012</v>
+      </c>
+      <c r="AH32" s="25"/>
+      <c r="AI32" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="AI32" s="25"/>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ32" s="25"/>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="41">
+      <c r="B33" s="2">
         <v>2012</v>
       </c>
       <c r="F33" s="2"/>
@@ -3380,7 +3405,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="41"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="15"/>
       <c r="N33" s="2"/>
@@ -3388,32 +3413,35 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="15"/>
-      <c r="S33" s="41"/>
+      <c r="S33" s="20">
+        <v>36281</v>
+      </c>
       <c r="T33" s="2"/>
-      <c r="U33" s="42">
+      <c r="U33" s="2"/>
+      <c r="V33" s="4">
         <v>2000</v>
       </c>
-      <c r="V33" s="2"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="15"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
-      <c r="AC33" s="15"/>
-      <c r="AD33" s="2"/>
-      <c r="AF33" s="41"/>
-      <c r="AG33" s="25"/>
-      <c r="AH33" s="2"/>
-      <c r="AI33" s="25" t="s">
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="15"/>
+      <c r="AE33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="25"/>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="41">
+      <c r="B34" s="2">
         <v>2012</v>
       </c>
       <c r="D34" s="2">
@@ -3424,7 +3452,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="46"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="25" t="s">
         <v>81</v>
       </c>
@@ -3436,28 +3464,28 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="15"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="25"/>
-      <c r="U34" s="41"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="25"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="15"/>
-      <c r="X34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="15"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
-      <c r="AC34" s="15"/>
-      <c r="AD34" s="2"/>
-      <c r="AF34" s="41"/>
-      <c r="AG34" s="25"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="25"/>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="25"/>
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="25"/>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="40"/>
       <c r="C35" s="15">
         <v>2012</v>
       </c>
@@ -3470,7 +3498,7 @@
       <c r="J35" s="4">
         <v>2010</v>
       </c>
-      <c r="K35" s="46" t="s">
+      <c r="K35" s="25" t="s">
         <v>109</v>
       </c>
       <c r="L35" s="25" t="s">
@@ -3484,36 +3512,39 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="15"/>
-      <c r="S35" s="46"/>
+      <c r="S35" s="4">
+        <v>2000</v>
+      </c>
       <c r="T35" s="25"/>
-      <c r="U35" s="46"/>
+      <c r="U35" s="25"/>
       <c r="V35" s="25"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="4">
+      <c r="W35" s="25"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="4">
         <v>2006</v>
       </c>
-      <c r="Y35" s="25"/>
       <c r="Z35" s="25"/>
-      <c r="AA35" s="4">
+      <c r="AA35" s="25"/>
+      <c r="AB35" s="4">
         <v>2016</v>
       </c>
-      <c r="AB35" s="4">
+      <c r="AC35" s="4">
         <v>2014</v>
       </c>
-      <c r="AC35" s="27">
+      <c r="AD35" s="27">
         <v>2016</v>
       </c>
-      <c r="AD35" s="25"/>
-      <c r="AF35" s="46"/>
+      <c r="AE35" s="25"/>
       <c r="AG35" s="25"/>
       <c r="AH35" s="25"/>
       <c r="AI35" s="25"/>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ35" s="25"/>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="41">
+      <c r="B36" s="2">
         <v>2012</v>
       </c>
       <c r="F36" s="2"/>
@@ -3521,7 +3552,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="41">
+      <c r="K36" s="2">
         <v>2008</v>
       </c>
       <c r="L36" s="2"/>
@@ -3531,28 +3562,29 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="15"/>
-      <c r="S36" s="41"/>
+      <c r="S36" s="2"/>
       <c r="T36" s="2"/>
-      <c r="U36" s="41"/>
+      <c r="U36" s="2"/>
       <c r="V36" s="2"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="15"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
-      <c r="AC36" s="15"/>
-      <c r="AD36" s="25"/>
-      <c r="AF36" s="41"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="25"/>
       <c r="AG36" s="2"/>
-      <c r="AH36" s="25"/>
-      <c r="AI36" s="2"/>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="25"/>
+      <c r="AJ36" s="2"/>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="41">
+      <c r="B37" s="2">
         <v>2012</v>
       </c>
       <c r="F37" s="2"/>
@@ -3562,7 +3594,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="41">
+      <c r="K37" s="2">
         <v>2005</v>
       </c>
       <c r="L37" s="2"/>
@@ -3572,43 +3604,44 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="15"/>
-      <c r="S37" s="41"/>
+      <c r="S37" s="2"/>
       <c r="T37" s="2"/>
-      <c r="U37" s="42">
+      <c r="U37" s="2"/>
+      <c r="V37" s="4">
         <v>2001</v>
       </c>
-      <c r="V37" s="2"/>
-      <c r="W37" s="15"/>
-      <c r="X37" s="4">
+      <c r="W37" s="2"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="4">
         <v>2006</v>
       </c>
-      <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="25"/>
-      <c r="AF37" s="41"/>
-      <c r="AG37" s="25"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="25"/>
+      <c r="AG37" s="2"/>
       <c r="AH37" s="25"/>
       <c r="AI37" s="25"/>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+      <c r="AJ37" s="25"/>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="40"/>
       <c r="C38" s="17">
         <v>2016</v>
       </c>
-      <c r="L38"/>
-      <c r="S38" s="40"/>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S38" s="4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="41">
+      <c r="B39" s="2">
         <v>2012</v>
       </c>
       <c r="F39" s="4">
@@ -3620,7 +3653,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="46"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="2"/>
       <c r="M39" s="15"/>
       <c r="N39" s="25"/>
@@ -3628,75 +3661,67 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="15"/>
-      <c r="S39" s="41"/>
+      <c r="S39" s="4">
+        <v>2005</v>
+      </c>
       <c r="T39" s="2"/>
-      <c r="U39" s="42">
-        <v>2012</v>
-      </c>
-      <c r="V39" s="2"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="4">
+      <c r="U39" s="2"/>
+      <c r="V39" s="4">
+        <v>2012</v>
+      </c>
+      <c r="W39" s="2"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="4">
         <v>2004</v>
       </c>
-      <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
-      <c r="AC39" s="15"/>
-      <c r="AD39" s="25"/>
-      <c r="AF39" s="41"/>
-      <c r="AG39" s="25"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="15"/>
+      <c r="AE39" s="25"/>
+      <c r="AG39" s="2"/>
       <c r="AH39" s="25"/>
       <c r="AI39" s="25"/>
-    </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="AJ39" s="25"/>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="40"/>
       <c r="C40" s="17">
         <v>2015</v>
       </c>
-      <c r="L40"/>
-      <c r="S40" s="40"/>
-    </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="S40" s="2"/>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="40"/>
       <c r="C41" s="17">
         <v>2012</v>
       </c>
-      <c r="L41"/>
-      <c r="S41" s="40"/>
-    </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="43" t="s">
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="40"/>
       <c r="C42" s="17">
         <v>2017</v>
       </c>
-      <c r="L42"/>
-      <c r="S42" s="40"/>
-    </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="40"/>
       <c r="C43" s="17"/>
       <c r="E43" s="14"/>
-      <c r="L43"/>
-      <c r="S43" s="40"/>
-    </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="4">
         <v>2015</v>
       </c>
       <c r="C44" s="15">
@@ -3709,7 +3734,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="46"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="2"/>
       <c r="M44" s="15"/>
       <c r="N44" s="4">
@@ -3721,45 +3746,46 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="15"/>
-      <c r="S44" s="41"/>
-      <c r="T44" s="25" t="s">
+      <c r="S44" s="4">
+        <v>2002</v>
+      </c>
+      <c r="T44" s="2"/>
+      <c r="U44" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="U44" s="46"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="2"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="15"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="2"/>
-      <c r="AF44" s="41"/>
-      <c r="AG44" s="4">
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="4">
         <v>2010</v>
       </c>
-      <c r="AH44" s="2"/>
-      <c r="AI44" s="25" t="s">
+      <c r="AI44" s="2"/>
+      <c r="AJ44" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="40"/>
       <c r="C45" s="17">
         <v>2018</v>
       </c>
-      <c r="L45"/>
-      <c r="S45" s="40"/>
-    </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S45" s="2"/>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="41">
+      <c r="B46" s="2">
         <v>2012</v>
       </c>
       <c r="F46" s="2"/>
@@ -3769,7 +3795,7 @@
       <c r="H46" s="17"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="41"/>
+      <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="15"/>
       <c r="N46" s="2"/>
@@ -3777,38 +3803,38 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="15"/>
-      <c r="S46" s="41"/>
+      <c r="S46" s="2"/>
       <c r="T46" s="2"/>
-      <c r="U46" s="42">
+      <c r="U46" s="2"/>
+      <c r="V46" s="4">
         <v>2001</v>
       </c>
-      <c r="V46" s="2"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="4">
+      <c r="W46" s="2"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="4">
         <v>2004</v>
       </c>
-      <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="2"/>
-      <c r="AF46" s="41"/>
-      <c r="AG46" s="25" t="s">
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="15"/>
+      <c r="AE46" s="2"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="AH46" s="4">
+      <c r="AI46" s="4">
         <v>2003</v>
       </c>
-      <c r="AI46" s="4">
+      <c r="AJ46" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="40"/>
       <c r="C47" s="17"/>
       <c r="F47" s="4">
         <v>2003</v>
@@ -3819,7 +3845,7 @@
       <c r="H47" s="17"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
-      <c r="K47" s="41"/>
+      <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="15"/>
       <c r="N47" s="2"/>
@@ -3827,34 +3853,35 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="15"/>
-      <c r="S47" s="41"/>
+      <c r="S47" s="2"/>
       <c r="T47" s="2"/>
-      <c r="U47" s="42">
+      <c r="U47" s="2"/>
+      <c r="V47" s="4">
         <v>2004</v>
       </c>
-      <c r="V47" s="2"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="4">
+      <c r="W47" s="2"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="4">
         <v>2003</v>
       </c>
-      <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="2"/>
-      <c r="AF47" s="41"/>
-      <c r="AG47" s="25" t="s">
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="15"/>
+      <c r="AE47" s="2"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="AH47" s="25"/>
-      <c r="AI47" s="2"/>
-    </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI47" s="25"/>
+      <c r="AJ47" s="2"/>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="41">
+      <c r="B48" s="2">
         <v>2012</v>
       </c>
       <c r="F48" s="2"/>
@@ -3862,7 +3889,7 @@
       <c r="H48" s="17"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
-      <c r="K48" s="41"/>
+      <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="15"/>
       <c r="N48" s="2"/>
@@ -3870,39 +3897,42 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="15"/>
-      <c r="S48" s="41"/>
+      <c r="S48" s="4">
+        <v>2001</v>
+      </c>
       <c r="T48" s="2"/>
-      <c r="U48" s="41"/>
-      <c r="V48" s="25"/>
-      <c r="W48" s="17"/>
-      <c r="X48" s="4">
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="25"/>
+      <c r="X48" s="17"/>
+      <c r="Y48" s="4">
         <v>2002</v>
       </c>
-      <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
-      <c r="AC48" s="15"/>
-      <c r="AD48" s="2"/>
-      <c r="AF48" s="41"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="15"/>
+      <c r="AE48" s="2"/>
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
-    </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
+      <c r="AJ48" s="2"/>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="40"/>
       <c r="C49" s="17"/>
-      <c r="L49"/>
-      <c r="S49" s="40"/>
-    </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S49" s="4">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="2">
         <v>1999</v>
       </c>
       <c r="F50" s="2"/>
@@ -3910,7 +3940,7 @@
       <c r="H50" s="17"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="41"/>
+      <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="15"/>
       <c r="N50" s="2"/>
@@ -3918,30 +3948,30 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="15"/>
-      <c r="S50" s="41"/>
+      <c r="S50" s="2"/>
       <c r="T50" s="2"/>
-      <c r="U50" s="41"/>
+      <c r="U50" s="2"/>
       <c r="V50" s="2"/>
-      <c r="W50" s="15"/>
-      <c r="X50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="15"/>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
-      <c r="AC50" s="15"/>
-      <c r="AD50" s="2"/>
-      <c r="AF50" s="41"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="15"/>
+      <c r="AE50" s="2"/>
       <c r="AG50" s="2"/>
-      <c r="AH50" s="4">
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="4">
         <v>2003</v>
       </c>
-      <c r="AI50" s="2"/>
-    </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ50" s="2"/>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="40"/>
       <c r="C51" s="15">
         <v>2012</v>
       </c>
@@ -3950,7 +3980,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="41"/>
+      <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="15"/>
       <c r="N51" s="2"/>
@@ -3958,45 +3988,42 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="15"/>
-      <c r="S51" s="41"/>
+      <c r="S51" s="2"/>
       <c r="T51" s="2"/>
-      <c r="U51" s="42">
+      <c r="U51" s="2"/>
+      <c r="V51" s="4">
         <v>2000</v>
       </c>
-      <c r="V51" s="25" t="s">
+      <c r="W51" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="W51" s="15"/>
-      <c r="X51" s="2"/>
+      <c r="X51" s="15"/>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="2"/>
-      <c r="AF51" s="41"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="15"/>
+      <c r="AE51" s="2"/>
       <c r="AG51" s="2"/>
-      <c r="AH51" s="4">
+      <c r="AH51" s="2"/>
+      <c r="AI51" s="4">
         <v>2003</v>
       </c>
-      <c r="AI51" s="25"/>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="AJ51" s="25"/>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="40"/>
       <c r="C52" s="17">
         <v>2013</v>
       </c>
-      <c r="L52"/>
-      <c r="S52" s="40"/>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A53" s="45" t="s">
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="40"/>
       <c r="C53" s="17">
         <v>2015</v>
       </c>
@@ -4011,7 +4038,7 @@
       <c r="J53" s="4">
         <v>2005</v>
       </c>
-      <c r="K53" s="42">
+      <c r="K53" s="4">
         <v>2001</v>
       </c>
       <c r="L53" s="2"/>
@@ -4025,62 +4052,54 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="15"/>
-      <c r="S53" s="41"/>
+      <c r="S53" s="2"/>
       <c r="T53" s="2"/>
-      <c r="U53" s="42">
+      <c r="U53" s="2"/>
+      <c r="V53" s="4">
         <v>2003</v>
       </c>
-      <c r="V53" s="25"/>
-      <c r="W53" s="17"/>
-      <c r="X53" s="4">
+      <c r="W53" s="25"/>
+      <c r="X53" s="17"/>
+      <c r="Y53" s="4">
         <v>2005</v>
-      </c>
-      <c r="Y53" s="4">
-        <v>2006</v>
       </c>
       <c r="Z53" s="4">
         <v>2006</v>
       </c>
-      <c r="AA53" s="2"/>
+      <c r="AA53" s="4">
+        <v>2006</v>
+      </c>
       <c r="AB53" s="2"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="2"/>
-      <c r="AF53" s="42">
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="15"/>
+      <c r="AE53" s="2"/>
+      <c r="AG53" s="4">
         <v>2006</v>
       </c>
-      <c r="AG53" s="25" t="s">
+      <c r="AH53" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="AH53" s="25" t="s">
+      <c r="AI53" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="AI53" s="2"/>
-    </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B54" s="40"/>
-      <c r="L54"/>
-      <c r="S54" s="40"/>
-    </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ53" s="2"/>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="L55"/>
-      <c r="S55" s="40"/>
-    </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A56" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="40"/>
       <c r="C56" s="17"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="17"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="46"/>
+      <c r="K56" s="25"/>
       <c r="L56" s="4">
         <v>2004</v>
       </c>
@@ -4096,34 +4115,35 @@
         <v>2017</v>
       </c>
       <c r="R56" s="17"/>
-      <c r="S56" s="46"/>
+      <c r="S56" s="2"/>
       <c r="T56" s="25"/>
-      <c r="U56" s="46"/>
+      <c r="U56" s="25"/>
       <c r="V56" s="25"/>
-      <c r="W56" s="17"/>
-      <c r="X56" s="4">
+      <c r="W56" s="25"/>
+      <c r="X56" s="17"/>
+      <c r="Y56" s="4">
         <v>2006</v>
-      </c>
-      <c r="Y56" s="4">
-        <v>2005</v>
       </c>
       <c r="Z56" s="4">
         <v>2005</v>
       </c>
-      <c r="AA56" s="2"/>
+      <c r="AA56" s="4">
+        <v>2005</v>
+      </c>
       <c r="AB56" s="2"/>
-      <c r="AC56" s="15"/>
-      <c r="AD56" s="25"/>
-      <c r="AF56" s="46"/>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="15"/>
+      <c r="AE56" s="25"/>
       <c r="AG56" s="25"/>
       <c r="AH56" s="25"/>
       <c r="AI56" s="25"/>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ56" s="25"/>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="41">
+      <c r="B57" s="2">
         <v>2012</v>
       </c>
       <c r="D57" s="2">
@@ -4140,10 +4160,10 @@
       <c r="J57" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="K57" s="46" t="s">
+      <c r="K57" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="L57" s="46" t="s">
+      <c r="L57" s="25" t="s">
         <v>81</v>
       </c>
       <c r="M57" s="17" t="s">
@@ -4160,60 +4180,55 @@
       <c r="R57" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="S57" s="46" t="s">
-        <v>74</v>
-      </c>
+      <c r="S57" s="2"/>
       <c r="T57" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="U57" s="46" t="s">
+      <c r="U57" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="V57" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="V57" s="2"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="25" t="s">
+      <c r="W57" s="2"/>
+      <c r="X57" s="15"/>
+      <c r="Y57" s="25" t="s">
         <v>91</v>
-      </c>
-      <c r="Y57" s="25" t="s">
-        <v>97</v>
       </c>
       <c r="Z57" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="AA57" s="2"/>
+      <c r="AA57" s="25" t="s">
+        <v>97</v>
+      </c>
       <c r="AB57" s="2"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="25" t="s">
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="15"/>
+      <c r="AE57" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="AF57" s="46" t="s">
+      <c r="AG57" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="AG57" s="25"/>
       <c r="AH57" s="25"/>
       <c r="AI57" s="25"/>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B58" s="40"/>
-      <c r="S58" s="40"/>
-      <c r="V58" s="40"/>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B59" s="36" t="s">
+      <c r="AJ57" s="25"/>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B59" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="37"/>
-      <c r="D59" s="39" t="s">
+      <c r="C59" s="40"/>
+      <c r="D59" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="37"/>
-      <c r="V59" s="40"/>
+      <c r="E59" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:AC1"/>
-    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:R1"/>

</xml_diff>

<commit_message>
cleaned and filled historic stock indexes
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A08DD2D-B774-45DA-9A93-BB477EA09992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB13CC-387A-4B5E-A985-9B8B8A6EF410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
   <si>
     <t>United States</t>
   </si>
@@ -244,12 +244,6 @@
     <t>32 from 2012 + 3 from 2013</t>
   </si>
   <si>
-    <t>13 full &amp; 3 partial</t>
-  </si>
-  <si>
-    <t>32 full &amp; 3 partial</t>
-  </si>
-  <si>
     <t>12 from 2012 + 3 from 2013</t>
   </si>
   <si>
@@ -461,6 +455,9 @@
   </si>
   <si>
     <t>Policy Rates</t>
+  </si>
+  <si>
+    <t>Stock Index</t>
   </si>
 </sst>
 </file>
@@ -617,7 +614,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -625,12 +622,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -639,14 +630,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,28 +648,35 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1001,11 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6"/>
+      <selection pane="topRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,17 +1005,16 @@
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1032,995 +1023,904 @@
       <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="28" t="s">
+      <c r="F1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="G1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="H1" s="15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="13"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="7">
+      <c r="C4" s="36">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="2">
+      <c r="F4" s="9"/>
+      <c r="G4" s="2">
         <v>1999</v>
       </c>
-      <c r="J4" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="7">
+      <c r="C5" s="36">
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="2">
+      <c r="F5" s="9"/>
+      <c r="G5" s="2">
         <v>2008</v>
       </c>
-      <c r="J5" s="16">
+      <c r="H5" s="10">
         <v>41548</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="7">
+      <c r="C6" s="36">
         <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="2">
+      <c r="F6" s="9"/>
+      <c r="G6" s="2">
         <v>2008</v>
       </c>
-      <c r="J6" s="15">
+      <c r="H6" s="9">
         <v>2008</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="7">
+      <c r="C7" s="36">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7" s="9"/>
+      <c r="G7" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="7">
+      <c r="C8" s="36">
         <v>7</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="2">
+      <c r="F8" s="9"/>
+      <c r="G8" s="2">
         <v>2008</v>
       </c>
-      <c r="J8" s="15">
+      <c r="H8" s="9">
         <v>2008</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="36">
         <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J9" s="16">
+      <c r="F9" s="9"/>
+      <c r="G9" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H9" s="10">
         <v>41671</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="7">
+      <c r="C10" s="36">
         <v>4</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="2">
+      <c r="F10" s="9"/>
+      <c r="G10" s="2">
         <v>2008</v>
       </c>
-      <c r="J10" s="15">
+      <c r="H10" s="9">
         <v>2008</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="7">
+      <c r="C11" s="36">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="20">
+      <c r="F11" s="9"/>
+      <c r="G11" s="13">
         <v>41426</v>
       </c>
-      <c r="J11" s="16">
+      <c r="H11" s="10">
         <v>41395</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="36">
         <v>17</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="20">
+      <c r="F12" s="9"/>
+      <c r="G12" s="13">
         <v>41548</v>
       </c>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="7"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="37">
         <v>38</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G13" s="13">
+      <c r="F13" s="9"/>
+      <c r="G13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="4">
         <v>2001</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="38">
         <v>25</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="4">
-        <v>2008</v>
-      </c>
-      <c r="G14" s="13">
+      <c r="F14" s="9"/>
+      <c r="G14" s="2">
         <v>1999</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="2">
-        <v>1999</v>
-      </c>
-      <c r="J14" s="15">
+      <c r="H14" s="9">
         <v>2006</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="7">
+      <c r="C15" s="36">
         <v>15</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J15" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="37">
         <v>40</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="7"/>
+      <c r="G16" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="7">
+      <c r="C17" s="36">
         <v>8</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J17" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="38">
         <v>30</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="2">
+      <c r="F18" s="7"/>
+      <c r="G18" s="2">
         <v>1999</v>
       </c>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="39">
         <v>47</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="4">
-        <v>2013</v>
-      </c>
-      <c r="G19" s="13">
+      <c r="F19" s="9"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="4">
         <v>2001</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="38">
         <v>24</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="15"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="38">
         <v>28</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="4">
-        <v>2013</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="2">
+      <c r="F21" s="9"/>
+      <c r="G21" s="2">
         <v>2004</v>
       </c>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="7"/>
+      <c r="I21" s="13">
+        <v>36404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="38">
         <v>29</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+      <c r="G22" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="38">
         <v>26</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J23" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="G23" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H23" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="39">
         <v>51</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="4">
-        <v>2003</v>
-      </c>
-      <c r="G24" s="13">
+      <c r="F24" s="9"/>
+      <c r="G24" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H24" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I24" s="4">
         <v>2001</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J24" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="40">
         <v>31</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="G25" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="39">
         <v>50</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="4">
-        <v>2013</v>
-      </c>
-      <c r="G26" s="13">
+      <c r="F26" s="9"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="4">
         <v>2010</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="C27" s="39"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="27"/>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="19"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="4">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="41"/>
+      <c r="F28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="41"/>
+      <c r="F29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="5"/>
-      <c r="C30" s="7">
+      <c r="C30" s="36">
         <v>2</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="2">
+      <c r="F30" s="21"/>
+      <c r="G30" s="2">
         <v>2005</v>
       </c>
-      <c r="J30" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="H30" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="38">
         <v>21</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+      <c r="G31" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="7">
+      <c r="C32" s="36">
         <v>5</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J32" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32" s="21"/>
+      <c r="G32" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H32" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="7">
+      <c r="C33" s="36">
         <v>12</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="20">
+      <c r="E33" s="13">
         <v>36281</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J33" s="13"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="9"/>
+      <c r="G33" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="7">
+      <c r="C34" s="36">
         <v>10</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J34" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F34" s="24"/>
+      <c r="G34" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H34" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="7">
+      <c r="C35" s="36">
         <v>18</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="4">
         <v>2000</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="22"/>
+      <c r="G35" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="10">
+      <c r="C36" s="37">
         <v>39</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="4">
-        <v>2014</v>
-      </c>
-      <c r="G36" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H36" s="27"/>
-      <c r="I36" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J36" s="13"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="19"/>
+      <c r="G36" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="7">
+      <c r="C37" s="36">
         <v>14</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J37" s="13"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="F37" s="9"/>
+      <c r="G37" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="38">
         <v>27</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="4">
         <v>2000</v>
       </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="J38" s="13"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="5"/>
-      <c r="C39" s="7">
+      <c r="C39" s="36">
         <v>16</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="4">
         <v>2005</v>
       </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J39" s="13"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
+      <c r="F39" s="21"/>
+      <c r="G39" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="37">
         <v>35</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="J40" s="13"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
+      <c r="F40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="37">
         <v>33</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="G41" s="13">
-        <v>2004</v>
-      </c>
-      <c r="H41" s="13"/>
-      <c r="J41" s="13"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="F41" s="7"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="39">
         <v>54</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="G42" s="13">
-        <v>2001</v>
-      </c>
-      <c r="H42" s="13"/>
-      <c r="J42" s="13"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+      <c r="F42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="39">
         <v>57</v>
       </c>
       <c r="D43" s="4"/>
-      <c r="G43" s="13">
-        <v>2010</v>
-      </c>
-      <c r="H43" s="13"/>
-      <c r="J43" s="13"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="C44" s="7">
+      <c r="C44" s="36">
         <v>19</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="4">
         <v>2002</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J44" s="13"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="19"/>
+      <c r="G44" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H44" s="7"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="37">
         <v>36</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="J45" s="13"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="38">
         <v>22</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="G46" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J46" s="13"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="9"/>
+      <c r="G46" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="39">
         <v>43</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="4">
-        <v>2002</v>
-      </c>
-      <c r="G47" s="13"/>
-      <c r="H47" s="15"/>
-      <c r="J47" s="13"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="9"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="39">
         <v>53</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4">
         <v>2001</v>
       </c>
-      <c r="F48" s="2"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J48" s="13"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="21" t="s">
+      <c r="F48" s="9"/>
+      <c r="G48" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H48" s="7"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="39">
         <v>48</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="4">
         <v>2003</v>
       </c>
-      <c r="G49" s="13">
-        <v>2011</v>
-      </c>
-      <c r="H49" s="13"/>
-      <c r="J49" s="13"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="39">
         <v>56</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="G50" s="13">
-        <v>2011</v>
-      </c>
-      <c r="H50" s="15"/>
-      <c r="I50" s="2">
+      <c r="F50" s="9"/>
+      <c r="G50" s="2">
         <v>1999</v>
       </c>
-      <c r="J50" s="13"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H50" s="7"/>
+      <c r="I50" s="4">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="39">
         <v>46</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="G51" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H51" s="15"/>
-      <c r="I51" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J51" s="13"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+      <c r="F51" s="9"/>
+      <c r="G51" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="39">
         <v>41</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="G52" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H52" s="13"/>
-      <c r="J52" s="13"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
+      <c r="F52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="39">
         <v>45</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="4">
-        <v>2007</v>
-      </c>
-      <c r="G53" s="13">
+      <c r="F53" s="19"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="4">
         <v>2000</v>
       </c>
-      <c r="H53" s="27"/>
-      <c r="J53" s="13"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C54" s="9"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="J54" s="13"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="41"/>
+      <c r="F54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="J55" s="13"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+      <c r="C55" s="41"/>
+      <c r="F55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="C56" s="8">
+      <c r="C56" s="38">
         <v>23</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="31"/>
-      <c r="J56" s="13"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F56" s="23"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="5"/>
-      <c r="C57" s="7">
+      <c r="C57" s="36">
         <v>11</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="4">
-        <v>2013</v>
-      </c>
-      <c r="G57" s="13">
-        <v>1999</v>
-      </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="2">
-        <v>2012</v>
-      </c>
-      <c r="J57" s="15">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="J58" s="13"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="J59" s="22" t="s">
-        <v>68</v>
-      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="2">
+        <v>2012</v>
+      </c>
+      <c r="H57" s="9">
+        <v>2012</v>
+      </c>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="42"/>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2030,311 +1930,326 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:AJ59"/>
+  <dimension ref="A1:AM59"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S18" sqref="S18"/>
+      <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="13"/>
+    <col min="18" max="18" width="9.140625" style="7"/>
     <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
     <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="13" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" style="7" customWidth="1"/>
     <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="11.7109375" style="13" customWidth="1"/>
+    <col min="30" max="30" width="11.7109375" style="7" customWidth="1"/>
     <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" style="13" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" style="7" customWidth="1"/>
     <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B1" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="33"/>
+      <c r="P1" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="37" t="s">
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="40"/>
-      <c r="P1" s="37" t="s">
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG1" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH1" s="41"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="41"/>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AL1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="U2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" t="s">
+        <v>118</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="N3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="13" t="s">
+      <c r="P3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>122</v>
+      </c>
+      <c r="S3" t="s">
+        <v>138</v>
+      </c>
+      <c r="T3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" t="s">
         <v>119</v>
       </c>
-      <c r="S2" t="s">
-        <v>139</v>
-      </c>
-      <c r="T2" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" t="s">
-        <v>83</v>
-      </c>
-      <c r="V2" t="s">
-        <v>85</v>
-      </c>
-      <c r="W2" t="s">
-        <v>120</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="X3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE3" t="s">
         <v>92</v>
       </c>
-      <c r="Z2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" t="s">
-        <v>114</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="N3" t="s">
-        <v>88</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="P3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>124</v>
-      </c>
-      <c r="S3" t="s">
-        <v>140</v>
-      </c>
-      <c r="T3" t="s">
-        <v>80</v>
-      </c>
-      <c r="U3" t="s">
-        <v>84</v>
-      </c>
-      <c r="V3" t="s">
-        <v>84</v>
-      </c>
-      <c r="W3" t="s">
-        <v>121</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="AG3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" t="s">
         <v>129</v>
       </c>
-      <c r="Z3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>131</v>
-      </c>
       <c r="AI3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AJ3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM3" s="7"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2">
@@ -2345,37 +2260,39 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="15"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="15"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="15"/>
+      <c r="O4" s="9"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="15"/>
+      <c r="R4" s="9"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="15"/>
+      <c r="X4" s="9"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="15"/>
+      <c r="AD4" s="9"/>
       <c r="AE4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
-      <c r="AJ4" s="25"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="AJ4" s="17"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="7"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -2384,29 +2301,29 @@
       <c r="D5" s="4">
         <v>2019</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="10">
         <v>41548</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="4">
         <v>2007</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="15"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>91</v>
+      <c r="O5" s="9"/>
+      <c r="P5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -2415,21 +2332,23 @@
       </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="15"/>
+      <c r="X5" s="9"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="15"/>
+      <c r="AD5" s="9"/>
       <c r="AE5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="25"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="AJ5" s="17"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="7"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2">
@@ -2440,78 +2359,82 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="15"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="15"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="15"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="15"/>
+      <c r="R6" s="9"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="15"/>
+      <c r="X6" s="9"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="15"/>
+      <c r="AD6" s="9"/>
       <c r="AE6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="25"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="AJ6" s="17"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="7"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>2021</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="9">
         <v>2012</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="15"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="15"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="15"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="15"/>
+      <c r="R7" s="9"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="15"/>
+      <c r="X7" s="9"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="15"/>
+      <c r="AD7" s="9"/>
       <c r="AE7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="7"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2">
@@ -2522,80 +2445,84 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="15"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="15"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="9"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="11"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="15"/>
+      <c r="AD8" s="9"/>
       <c r="AE8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="25"/>
+      <c r="AI8" s="17"/>
       <c r="AJ8" s="2"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="7"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="15">
-        <v>2012</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="C9" s="9">
+        <v>2012</v>
+      </c>
+      <c r="E9" s="10">
         <v>41671</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="15"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="15"/>
+      <c r="R9" s="9"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="15"/>
+      <c r="X9" s="9"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="15"/>
+      <c r="AD9" s="9"/>
       <c r="AE9" s="4">
         <v>2011</v>
       </c>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="25"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="AJ9" s="17"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="7"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="2">
@@ -2606,108 +2533,112 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="15"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="9"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="15"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="15"/>
+      <c r="R10" s="9"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="11"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="15"/>
+      <c r="AD10" s="9"/>
       <c r="AE10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="7"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4">
         <v>2018</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="10">
         <v>41426</v>
       </c>
       <c r="D11" s="4">
         <v>2018</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="10">
         <v>41395</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="15"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="17"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="11"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="15"/>
+      <c r="X11" s="9"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="25"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="17"/>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="25"/>
+      <c r="AH11" s="17"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="7"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="10">
         <v>41548</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="15"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="15"/>
+      <c r="R12" s="9"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="11"/>
       <c r="Y12" s="4">
         <v>2003</v>
       </c>
@@ -2715,41 +2646,43 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="15"/>
+      <c r="AD12" s="9"/>
       <c r="AE12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="AJ12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="7"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="15"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="15"/>
+      <c r="O13" s="9"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="15"/>
+      <c r="R13" s="9"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="15"/>
+      <c r="X13" s="9"/>
       <c r="Y13" s="4">
         <v>2005</v>
       </c>
@@ -2757,15 +2690,18 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="15"/>
+      <c r="AD13" s="9"/>
       <c r="AE13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="25"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="AJ13" s="17"/>
+      <c r="AM13" s="19">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2">
@@ -2776,39 +2712,45 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="15"/>
+      <c r="M14" s="9"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="15"/>
+      <c r="O14" s="9"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="15"/>
+      <c r="R14" s="9"/>
       <c r="S14" s="2"/>
-      <c r="T14" s="25" t="s">
-        <v>81</v>
+      <c r="T14" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="15"/>
+      <c r="X14" s="9"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="15"/>
+      <c r="AD14" s="9"/>
       <c r="AE14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="AL14" s="4">
+        <v>2008</v>
+      </c>
+      <c r="AM14" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2">
@@ -2819,49 +2761,53 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="15"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="15"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="15"/>
+      <c r="R15" s="9"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="11"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="15"/>
+      <c r="AD15" s="9"/>
       <c r="AE15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="7"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2">
         <v>2012</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="24"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="16"/>
       <c r="S16" s="2"/>
-      <c r="V16" s="26"/>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="V16" s="18"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="7"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2">
@@ -2872,105 +2818,115 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="15"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="15"/>
+      <c r="O17" s="9"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="15"/>
+      <c r="R17" s="9"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="11"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="15"/>
+      <c r="AD17" s="9"/>
       <c r="AE17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="25"/>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="AJ17" s="17"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="7"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>1999</v>
       </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="24"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="N18" s="18"/>
+      <c r="O18" s="16"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="7"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="11"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="15"/>
+      <c r="M19" s="9"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="15"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="15"/>
+      <c r="R19" s="9"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="25"/>
-      <c r="X19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="11"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="15"/>
+      <c r="AD19" s="9"/>
       <c r="AE19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="AL19" s="4">
+        <v>2013</v>
+      </c>
+      <c r="AM19" s="19">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="11"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="15"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="2"/>
-      <c r="O20" s="15"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="15"/>
+      <c r="R20" s="9"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="25"/>
-      <c r="X20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="11"/>
       <c r="Y20" s="4">
         <v>2003</v>
       </c>
@@ -2978,87 +2934,92 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="15"/>
+      <c r="AD20" s="9"/>
       <c r="AE20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="7"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2">
         <v>2004</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="15"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="15"/>
+      <c r="O21" s="9"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="15"/>
+      <c r="R21" s="9"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="15"/>
+      <c r="X21" s="9"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="15"/>
+      <c r="AD21" s="9"/>
       <c r="AE21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="AM21" s="10">
+        <v>36404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="9">
         <v>2012</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="4">
         <v>2011</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="15"/>
+      <c r="M22" s="9"/>
       <c r="N22" s="4">
         <v>2012</v>
       </c>
-      <c r="O22" s="15"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="15"/>
+      <c r="R22" s="9"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="15"/>
+      <c r="X22" s="9"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="15"/>
+      <c r="AD22" s="9"/>
       <c r="AE22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
@@ -3066,9 +3027,11 @@
         <v>2004</v>
       </c>
       <c r="AJ22" s="2"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="7"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="2">
@@ -3079,23 +3042,23 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="15"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="15"/>
+      <c r="O23" s="9"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="15"/>
+      <c r="R23" s="9"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="11"/>
       <c r="Y23" s="4">
         <v>2002</v>
       </c>
@@ -3103,60 +3066,68 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="15"/>
+      <c r="AD23" s="9"/>
       <c r="AE23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="4">
         <v>2000</v>
       </c>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="25"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="AJ23" s="17"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="7"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="15">
-        <v>2012</v>
-      </c>
-      <c r="E24" s="15">
+      <c r="C24" s="9">
+        <v>2012</v>
+      </c>
+      <c r="E24" s="9">
         <v>2012</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="17"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="17"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="11"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="17" t="s">
-        <v>86</v>
+      <c r="X24" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="25"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="17"/>
       <c r="AG24" s="2"/>
-      <c r="AH24" s="25"/>
+      <c r="AH24" s="17"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="AL24" s="4">
+        <v>2003</v>
+      </c>
+      <c r="AM24" s="19">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="2">
@@ -3164,123 +3135,139 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="15"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="15"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="15"/>
+      <c r="R25" s="9"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="11"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="15"/>
+      <c r="AD25" s="9"/>
       <c r="AE25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="25"/>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="AJ25" s="17"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="7"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="11"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="15"/>
+      <c r="M26" s="9"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="15"/>
+      <c r="O26" s="9"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="15"/>
+      <c r="R26" s="9"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="11"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="15"/>
+      <c r="AD26" s="9"/>
       <c r="AE26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="2"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>71</v>
+      <c r="AL26" s="4">
+        <v>2013</v>
+      </c>
+      <c r="AM26" s="19">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B27" s="2">
         <v>2012</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="2">
         <v>2012</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="17"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="11"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="17"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="11"/>
       <c r="AE27" s="2"/>
-      <c r="AG27" s="25"/>
+      <c r="AG27" s="17"/>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="25" t="s">
-        <v>74</v>
+      <c r="AI27" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="AJ27" s="2"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="AL27" s="4">
+        <v>2007</v>
+      </c>
+      <c r="AM27" s="7"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM28" s="7"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="14"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="C29" s="8"/>
+      <c r="AM29" s="7"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="2">
@@ -3293,19 +3280,19 @@
         <v>2000</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="15"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="2"/>
       <c r="J30" s="4">
         <v>2011</v>
       </c>
-      <c r="K30" s="25"/>
+      <c r="K30" s="17"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="17"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="11"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="15"/>
+      <c r="R30" s="9"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -3313,31 +3300,35 @@
         <v>2014</v>
       </c>
       <c r="W30" s="2"/>
-      <c r="X30" s="15"/>
+      <c r="X30" s="9"/>
       <c r="Y30" s="2"/>
-      <c r="Z30" s="25"/>
-      <c r="AA30" s="25"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-      <c r="AD30" s="15"/>
-      <c r="AE30" s="25"/>
-      <c r="AG30" s="25"/>
-      <c r="AH30" s="25"/>
-      <c r="AI30" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ30" s="25"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="17"/>
+      <c r="AG30" s="17"/>
+      <c r="AH30" s="17"/>
+      <c r="AI30" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ30" s="17"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="7"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="2">
         <v>2012</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="7"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="2">
@@ -3349,24 +3340,24 @@
       <c r="F32" s="4">
         <v>2000</v>
       </c>
-      <c r="G32" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="15"/>
+      <c r="G32" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="9"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="N32" s="25"/>
-      <c r="O32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N32" s="17"/>
+      <c r="O32" s="11"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="15"/>
+      <c r="R32" s="9"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="4">
@@ -3376,25 +3367,27 @@
         <v>2011</v>
       </c>
       <c r="W32" s="2"/>
-      <c r="X32" s="15"/>
+      <c r="X32" s="9"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="15"/>
+      <c r="AD32" s="9"/>
       <c r="AE32" s="2"/>
       <c r="AG32" s="4">
         <v>2012</v>
       </c>
-      <c r="AH32" s="25"/>
-      <c r="AI32" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="AJ32" s="25"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="AH32" s="17"/>
+      <c r="AI32" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ32" s="17"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="7"/>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="2">
@@ -3402,18 +3395,18 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="15"/>
+      <c r="H33" s="9"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="15"/>
+      <c r="M33" s="9"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="15"/>
+      <c r="O33" s="9"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="20">
+      <c r="R33" s="9"/>
+      <c r="S33" s="13">
         <v>36281</v>
       </c>
       <c r="T33" s="2"/>
@@ -3422,24 +3415,26 @@
         <v>2000</v>
       </c>
       <c r="W33" s="2"/>
-      <c r="X33" s="15"/>
+      <c r="X33" s="9"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="15"/>
+      <c r="AD33" s="9"/>
       <c r="AE33" s="2"/>
       <c r="AG33" s="2"/>
-      <c r="AH33" s="25"/>
+      <c r="AH33" s="17"/>
       <c r="AI33" s="2"/>
-      <c r="AJ33" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>100</v>
+      <c r="AJ33" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="7"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="B34" s="2">
         <v>2012</v>
@@ -3449,99 +3444,103 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="15"/>
+      <c r="H34" s="9"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="N34" s="25"/>
-      <c r="O34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N34" s="17"/>
+      <c r="O34" s="11"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
-      <c r="R34" s="15"/>
+      <c r="R34" s="9"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
-      <c r="U34" s="25"/>
+      <c r="U34" s="17"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
-      <c r="X34" s="15"/>
+      <c r="X34" s="9"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="15"/>
+      <c r="AD34" s="9"/>
       <c r="AE34" s="2"/>
       <c r="AG34" s="2"/>
-      <c r="AH34" s="25"/>
+      <c r="AH34" s="17"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="25"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="AJ34" s="17"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="7"/>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="15">
-        <v>2012</v>
-      </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="17"/>
+      <c r="C35" s="9">
+        <v>2012</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="4">
         <v>2011</v>
       </c>
       <c r="J35" s="4">
         <v>2010</v>
       </c>
-      <c r="K35" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="L35" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="N35" s="25"/>
-      <c r="O35" s="17"/>
+      <c r="K35" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N35" s="17"/>
+      <c r="O35" s="11"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
-      <c r="R35" s="15"/>
+      <c r="R35" s="9"/>
       <c r="S35" s="4">
         <v>2000</v>
       </c>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="25"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="11"/>
       <c r="Y35" s="4">
         <v>2006</v>
       </c>
-      <c r="Z35" s="25"/>
-      <c r="AA35" s="25"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
       <c r="AB35" s="4">
         <v>2016</v>
       </c>
       <c r="AC35" s="4">
         <v>2014</v>
       </c>
-      <c r="AD35" s="27">
+      <c r="AD35" s="19">
         <v>2016</v>
       </c>
-      <c r="AE35" s="25"/>
-      <c r="AG35" s="25"/>
-      <c r="AH35" s="25"/>
-      <c r="AI35" s="25"/>
-      <c r="AJ35" s="25"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="AE35" s="17"/>
+      <c r="AG35" s="17"/>
+      <c r="AH35" s="17"/>
+      <c r="AI35" s="17"/>
+      <c r="AJ35" s="17"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="7"/>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="2">
@@ -3549,39 +3548,42 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="15"/>
+      <c r="H36" s="9"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2">
         <v>2008</v>
       </c>
       <c r="L36" s="2"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="17"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="11"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
-      <c r="R36" s="15"/>
+      <c r="R36" s="9"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="15"/>
+      <c r="X36" s="9"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="15"/>
-      <c r="AE36" s="25"/>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="17"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
-      <c r="AI36" s="25"/>
+      <c r="AI36" s="17"/>
       <c r="AJ36" s="2"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="AM36" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="2">
@@ -3591,19 +3593,19 @@
       <c r="G37" s="4">
         <v>2001</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="9"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2">
         <v>2005</v>
       </c>
       <c r="L37" s="2"/>
-      <c r="M37" s="15"/>
+      <c r="M37" s="9"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="15"/>
+      <c r="O37" s="9"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="15"/>
+      <c r="R37" s="9"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
@@ -3611,7 +3613,7 @@
         <v>2001</v>
       </c>
       <c r="W37" s="2"/>
-      <c r="X37" s="15"/>
+      <c r="X37" s="9"/>
       <c r="Y37" s="4">
         <v>2006</v>
       </c>
@@ -3619,26 +3621,30 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="25"/>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="17"/>
       <c r="AG37" s="2"/>
-      <c r="AH37" s="25"/>
-      <c r="AI37" s="25"/>
-      <c r="AJ37" s="25"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+      <c r="AH37" s="17"/>
+      <c r="AI37" s="17"/>
+      <c r="AJ37" s="17"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="7"/>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="11">
         <v>2016</v>
       </c>
       <c r="S38" s="4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="7"/>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="2">
@@ -3650,17 +3656,17 @@
       <c r="G39" s="4">
         <v>2001</v>
       </c>
-      <c r="H39" s="15"/>
+      <c r="H39" s="9"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="25"/>
+      <c r="K39" s="17"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="17"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="11"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="15"/>
+      <c r="R39" s="9"/>
       <c r="S39" s="4">
         <v>2005</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>2012</v>
       </c>
       <c r="W39" s="2"/>
-      <c r="X39" s="15"/>
+      <c r="X39" s="9"/>
       <c r="Y39" s="4">
         <v>2004</v>
       </c>
@@ -3678,111 +3684,128 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="15"/>
-      <c r="AE39" s="25"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="17"/>
       <c r="AG39" s="2"/>
-      <c r="AH39" s="25"/>
-      <c r="AI39" s="25"/>
-      <c r="AJ39" s="25"/>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="AH39" s="17"/>
+      <c r="AI39" s="17"/>
+      <c r="AJ39" s="17"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="7"/>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="11">
         <v>2015</v>
       </c>
       <c r="S40" s="2"/>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="7"/>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="17">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+      <c r="C41" s="11">
+        <v>2012</v>
+      </c>
+      <c r="AM41" s="7">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="11">
         <v>2017</v>
       </c>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="AM42" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="C43" s="11"/>
+      <c r="E43" s="8"/>
+      <c r="AM43" s="7">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B44" s="4">
         <v>2015</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="9">
         <v>2012</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="4">
         <v>2004</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="H44" s="9"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="25"/>
+      <c r="K44" s="17"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="15"/>
+      <c r="M44" s="9"/>
       <c r="N44" s="4">
         <v>2005</v>
       </c>
-      <c r="O44" s="27">
+      <c r="O44" s="19">
         <v>2005</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="15"/>
+      <c r="R44" s="9"/>
       <c r="S44" s="4">
         <v>2002</v>
       </c>
       <c r="T44" s="2"/>
-      <c r="U44" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="V44" s="25"/>
+      <c r="U44" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="V44" s="17"/>
       <c r="W44" s="2"/>
-      <c r="X44" s="15"/>
+      <c r="X44" s="9"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-      <c r="AD44" s="15"/>
+      <c r="AD44" s="9"/>
       <c r="AE44" s="2"/>
       <c r="AG44" s="2"/>
       <c r="AH44" s="4">
         <v>2010</v>
       </c>
       <c r="AI44" s="2"/>
-      <c r="AJ44" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="AJ44" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL44" s="2"/>
+      <c r="AM44" s="7"/>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="11">
         <v>2018</v>
       </c>
       <c r="S45" s="2"/>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="AL45" s="2"/>
+      <c r="AM45" s="7"/>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="2">
@@ -3792,17 +3815,17 @@
       <c r="G46" s="4">
         <v>2001</v>
       </c>
-      <c r="H46" s="17"/>
+      <c r="H46" s="11"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="15"/>
+      <c r="M46" s="9"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="15"/>
+      <c r="O46" s="9"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="15"/>
+      <c r="R46" s="9"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
@@ -3810,7 +3833,7 @@
         <v>2001</v>
       </c>
       <c r="W46" s="2"/>
-      <c r="X46" s="15"/>
+      <c r="X46" s="9"/>
       <c r="Y46" s="4">
         <v>2004</v>
       </c>
@@ -3818,11 +3841,11 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
-      <c r="AD46" s="15"/>
+      <c r="AD46" s="9"/>
       <c r="AE46" s="2"/>
       <c r="AG46" s="2"/>
-      <c r="AH46" s="25" t="s">
-        <v>86</v>
+      <c r="AH46" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="AI46" s="4">
         <v>2003</v>
@@ -3830,29 +3853,32 @@
       <c r="AJ46" s="4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
+      <c r="AM46" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="11"/>
       <c r="F47" s="4">
         <v>2003</v>
       </c>
       <c r="G47" s="4">
         <v>2002</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="15"/>
+      <c r="M47" s="9"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="15"/>
+      <c r="O47" s="9"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="15"/>
+      <c r="R47" s="9"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
@@ -3860,7 +3886,7 @@
         <v>2004</v>
       </c>
       <c r="W47" s="2"/>
-      <c r="X47" s="15"/>
+      <c r="X47" s="9"/>
       <c r="Y47" s="4">
         <v>2003</v>
       </c>
@@ -3868,17 +3894,20 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="15"/>
+      <c r="AD47" s="9"/>
       <c r="AE47" s="2"/>
       <c r="AG47" s="2"/>
-      <c r="AH47" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI47" s="25"/>
+      <c r="AH47" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI47" s="17"/>
       <c r="AJ47" s="2"/>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="AM47" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B48" s="2">
@@ -3886,25 +3915,25 @@
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="17"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="15"/>
+      <c r="M48" s="9"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="15"/>
+      <c r="O48" s="9"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="15"/>
+      <c r="R48" s="9"/>
       <c r="S48" s="4">
         <v>2001</v>
       </c>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-      <c r="W48" s="25"/>
-      <c r="X48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="11"/>
       <c r="Y48" s="4">
         <v>2002</v>
       </c>
@@ -3912,24 +3941,29 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
-      <c r="AD48" s="15"/>
+      <c r="AD48" s="9"/>
       <c r="AE48" s="2"/>
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
       <c r="AJ48" s="2"/>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="AL48" s="2"/>
+      <c r="AM48" s="7"/>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="11"/>
       <c r="S49" s="4">
         <v>2003</v>
       </c>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
+      <c r="AM49" s="7">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B50" s="2">
@@ -3937,29 +3971,29 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="17"/>
+      <c r="H50" s="11"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="15"/>
+      <c r="M50" s="9"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="15"/>
+      <c r="O50" s="9"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="15"/>
+      <c r="R50" s="9"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
-      <c r="X50" s="15"/>
+      <c r="X50" s="9"/>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
       <c r="AC50" s="2"/>
-      <c r="AD50" s="15"/>
+      <c r="AD50" s="9"/>
       <c r="AE50" s="2"/>
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
@@ -3967,71 +4001,80 @@
         <v>2003</v>
       </c>
       <c r="AJ50" s="2"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="AM50" s="19">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="9">
         <v>2012</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="17"/>
+      <c r="H51" s="11"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="15"/>
+      <c r="M51" s="9"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="15"/>
+      <c r="O51" s="9"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
-      <c r="R51" s="15"/>
+      <c r="R51" s="9"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="4">
         <v>2000</v>
       </c>
-      <c r="W51" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="X51" s="15"/>
+      <c r="W51" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="X51" s="9"/>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
       <c r="AC51" s="2"/>
-      <c r="AD51" s="15"/>
+      <c r="AD51" s="9"/>
       <c r="AE51" s="2"/>
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="4">
         <v>2003</v>
       </c>
-      <c r="AJ51" s="25"/>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="AJ51" s="17"/>
+      <c r="AM51" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="11">
         <v>2013</v>
       </c>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
+      <c r="AM52" s="7">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="17">
+      <c r="C53" s="11">
         <v>2015</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="4">
         <v>2001</v>
       </c>
-      <c r="H53" s="17"/>
+      <c r="H53" s="11"/>
       <c r="I53" s="4">
         <v>2006</v>
       </c>
@@ -4042,24 +4085,24 @@
         <v>2001</v>
       </c>
       <c r="L53" s="2"/>
-      <c r="M53" s="15"/>
+      <c r="M53" s="9"/>
       <c r="N53" s="4">
         <v>2007</v>
       </c>
-      <c r="O53" s="27">
+      <c r="O53" s="19">
         <v>2007</v>
       </c>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="15"/>
+      <c r="R53" s="9"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="4">
         <v>2003</v>
       </c>
-      <c r="W53" s="25"/>
-      <c r="X53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="11"/>
       <c r="Y53" s="4">
         <v>2005</v>
       </c>
@@ -4071,56 +4114,63 @@
       </c>
       <c r="AB53" s="2"/>
       <c r="AC53" s="2"/>
-      <c r="AD53" s="15"/>
+      <c r="AD53" s="9"/>
       <c r="AE53" s="2"/>
       <c r="AG53" s="4">
         <v>2006</v>
       </c>
-      <c r="AH53" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI53" s="25" t="s">
-        <v>103</v>
+      <c r="AH53" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI53" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="AJ53" s="2"/>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="AM53" s="19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM54" s="7"/>
+    </row>
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
+      <c r="AM55" s="7"/>
+    </row>
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A56" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="17"/>
+      <c r="C56" s="11"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="11"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="25"/>
+      <c r="K56" s="17"/>
       <c r="L56" s="4">
         <v>2004</v>
       </c>
-      <c r="M56" s="27">
+      <c r="M56" s="19">
         <v>2004</v>
       </c>
-      <c r="N56" s="25"/>
-      <c r="O56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="11"/>
       <c r="P56" s="4">
         <v>2017</v>
       </c>
       <c r="Q56" s="4">
         <v>2017</v>
       </c>
-      <c r="R56" s="17"/>
+      <c r="R56" s="11"/>
       <c r="S56" s="2"/>
-      <c r="T56" s="25"/>
-      <c r="U56" s="25"/>
-      <c r="V56" s="25"/>
-      <c r="W56" s="25"/>
-      <c r="X56" s="17"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="17"/>
+      <c r="X56" s="11"/>
       <c r="Y56" s="4">
         <v>2006</v>
       </c>
@@ -4132,15 +4182,17 @@
       </c>
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
-      <c r="AD56" s="15"/>
-      <c r="AE56" s="25"/>
-      <c r="AG56" s="25"/>
-      <c r="AH56" s="25"/>
-      <c r="AI56" s="25"/>
-      <c r="AJ56" s="25"/>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
+      <c r="AD56" s="9"/>
+      <c r="AE56" s="17"/>
+      <c r="AG56" s="17"/>
+      <c r="AH56" s="17"/>
+      <c r="AI56" s="17"/>
+      <c r="AJ56" s="17"/>
+      <c r="AL56" s="2"/>
+      <c r="AM56" s="7"/>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="2">
@@ -4149,94 +4201,104 @@
       <c r="D57" s="2">
         <v>2012</v>
       </c>
-      <c r="F57" s="25" t="s">
-        <v>74</v>
+      <c r="F57" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="K57" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L57" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="M57" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="N57" s="25"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q57" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="R57" s="17" t="s">
-        <v>74</v>
+      <c r="H57" s="11"/>
+      <c r="I57" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N57" s="17"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q57" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="R57" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="S57" s="2"/>
-      <c r="T57" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="U57" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="V57" s="25" t="s">
-        <v>86</v>
+      <c r="T57" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="U57" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="V57" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="W57" s="2"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z57" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA57" s="25" t="s">
-        <v>97</v>
+      <c r="X57" s="9"/>
+      <c r="Y57" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z57" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA57" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="AB57" s="2"/>
       <c r="AC57" s="2"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG57" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH57" s="25"/>
-      <c r="AI57" s="25"/>
-      <c r="AJ57" s="25"/>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B59" s="39" t="s">
+      <c r="AD57" s="9"/>
+      <c r="AE57" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG57" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH57" s="17"/>
+      <c r="AI57" s="17"/>
+      <c r="AJ57" s="17"/>
+      <c r="AL57" s="4">
+        <v>2013</v>
+      </c>
+      <c r="AM57" s="9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM58" s="7"/>
+    </row>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B59" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="40"/>
-      <c r="D59" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="E59" s="40"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E59" s="33"/>
+      <c r="AM59" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="Y1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first version of currency rates
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB13CC-387A-4B5E-A985-9B8B8A6EF410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66394F1-6FC8-455D-AF2F-A5350D9F68D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -614,7 +614,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -649,21 +649,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,8 +658,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1056,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="36">
+      <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
@@ -1075,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="36">
+      <c r="C5" s="31">
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
@@ -1094,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="36">
+      <c r="C6" s="31">
         <v>6</v>
       </c>
       <c r="D6" s="2"/>
@@ -1113,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="36">
+      <c r="C7" s="31">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
@@ -1130,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="36">
+      <c r="C8" s="31">
         <v>7</v>
       </c>
       <c r="D8" s="2"/>
@@ -1148,7 +1147,7 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="31">
         <v>20</v>
       </c>
       <c r="D9" s="2"/>
@@ -1167,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="36">
+      <c r="C10" s="31">
         <v>4</v>
       </c>
       <c r="D10" s="2"/>
@@ -1186,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="36">
+      <c r="C11" s="31">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
@@ -1204,7 +1203,7 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="31">
         <v>17</v>
       </c>
       <c r="D12" s="2"/>
@@ -1220,7 +1219,7 @@
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="32">
         <v>38</v>
       </c>
       <c r="D13" s="2"/>
@@ -1238,7 +1237,7 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="33">
         <v>25</v>
       </c>
       <c r="D14" s="2"/>
@@ -1257,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="36">
+      <c r="C15" s="31">
         <v>15</v>
       </c>
       <c r="D15" s="2"/>
@@ -1275,7 +1274,7 @@
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="32">
         <v>40</v>
       </c>
       <c r="D16" s="4"/>
@@ -1292,7 +1291,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="36">
+      <c r="C17" s="31">
         <v>8</v>
       </c>
       <c r="D17" s="2"/>
@@ -1310,7 +1309,7 @@
       <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="33">
         <v>30</v>
       </c>
       <c r="D18" s="2"/>
@@ -1325,7 +1324,7 @@
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="34">
         <v>47</v>
       </c>
       <c r="D19" s="2"/>
@@ -1340,7 +1339,7 @@
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="33">
         <v>24</v>
       </c>
       <c r="D20" s="2"/>
@@ -1353,7 +1352,7 @@
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="33">
         <v>28</v>
       </c>
       <c r="D21" s="2"/>
@@ -1371,7 +1370,7 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="33">
         <v>29</v>
       </c>
       <c r="D22" s="2"/>
@@ -1387,7 +1386,7 @@
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="33">
         <v>26</v>
       </c>
       <c r="D23" s="4"/>
@@ -1405,7 +1404,7 @@
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="39">
+      <c r="C24" s="34">
         <v>51</v>
       </c>
       <c r="D24" s="2"/>
@@ -1425,7 +1424,7 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="35">
         <v>31</v>
       </c>
       <c r="D25" s="4"/>
@@ -1441,7 +1440,7 @@
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="39">
+      <c r="C26" s="34">
         <v>50</v>
       </c>
       <c r="D26" s="2"/>
@@ -1456,7 +1455,7 @@
       <c r="A27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="39"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="19"/>
@@ -1466,7 +1465,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="41"/>
+      <c r="C28" s="36"/>
       <c r="F28" s="7"/>
       <c r="H28" s="7"/>
     </row>
@@ -1474,7 +1473,7 @@
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="41"/>
+      <c r="C29" s="36"/>
       <c r="F29" s="7"/>
       <c r="H29" s="7"/>
     </row>
@@ -1483,7 +1482,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="5"/>
-      <c r="C30" s="36">
+      <c r="C30" s="31">
         <v>2</v>
       </c>
       <c r="D30" s="2"/>
@@ -1501,7 +1500,7 @@
       <c r="A31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C31" s="33">
         <v>21</v>
       </c>
       <c r="F31" s="7"/>
@@ -1516,7 +1515,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="36">
+      <c r="C32" s="31">
         <v>5</v>
       </c>
       <c r="D32" s="2"/>
@@ -1535,7 +1534,7 @@
         <v>26</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="36">
+      <c r="C33" s="31">
         <v>12</v>
       </c>
       <c r="D33" s="2"/>
@@ -1554,7 +1553,7 @@
         <v>98</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="36">
+      <c r="C34" s="31">
         <v>10</v>
       </c>
       <c r="D34" s="2"/>
@@ -1573,7 +1572,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="36">
+      <c r="C35" s="31">
         <v>18</v>
       </c>
       <c r="D35" s="2"/>
@@ -1592,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="37">
+      <c r="C36" s="32">
         <v>39</v>
       </c>
       <c r="D36" s="2"/>
@@ -1609,7 +1608,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="36">
+      <c r="C37" s="31">
         <v>14</v>
       </c>
       <c r="D37" s="2"/>
@@ -1625,7 +1624,7 @@
       <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="33">
         <v>27</v>
       </c>
       <c r="D38" s="2"/>
@@ -1641,7 +1640,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="5"/>
-      <c r="C39" s="36">
+      <c r="C39" s="31">
         <v>16</v>
       </c>
       <c r="D39" s="2"/>
@@ -1659,7 +1658,7 @@
       <c r="A40" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="37">
+      <c r="C40" s="32">
         <v>35</v>
       </c>
       <c r="D40" s="2"/>
@@ -1672,7 +1671,7 @@
       <c r="A41" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="32">
         <v>33</v>
       </c>
       <c r="D41" s="4"/>
@@ -1683,7 +1682,7 @@
       <c r="A42" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="39">
+      <c r="C42" s="34">
         <v>54</v>
       </c>
       <c r="D42" s="4"/>
@@ -1694,7 +1693,7 @@
       <c r="A43" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="39">
+      <c r="C43" s="34">
         <v>57</v>
       </c>
       <c r="D43" s="4"/>
@@ -1706,7 +1705,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="C44" s="36">
+      <c r="C44" s="31">
         <v>19</v>
       </c>
       <c r="D44" s="2"/>
@@ -1724,7 +1723,7 @@
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="32">
         <v>36</v>
       </c>
       <c r="D45" s="2"/>
@@ -1737,7 +1736,7 @@
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="38">
+      <c r="C46" s="33">
         <v>22</v>
       </c>
       <c r="D46" s="2"/>
@@ -1753,7 +1752,7 @@
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="39">
+      <c r="C47" s="34">
         <v>43</v>
       </c>
       <c r="D47" s="2"/>
@@ -1766,7 +1765,7 @@
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="39">
+      <c r="C48" s="34">
         <v>53</v>
       </c>
       <c r="D48" s="4"/>
@@ -1784,7 +1783,7 @@
       <c r="A49" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="39">
+      <c r="C49" s="34">
         <v>48</v>
       </c>
       <c r="D49" s="2"/>
@@ -1798,7 +1797,7 @@
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="39">
+      <c r="C50" s="34">
         <v>56</v>
       </c>
       <c r="D50" s="2"/>
@@ -1816,7 +1815,7 @@
       <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="39">
+      <c r="C51" s="34">
         <v>46</v>
       </c>
       <c r="D51" s="2"/>
@@ -1832,7 +1831,7 @@
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="39">
+      <c r="C52" s="34">
         <v>41</v>
       </c>
       <c r="D52" s="2"/>
@@ -1843,7 +1842,7 @@
       <c r="A53" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="39">
+      <c r="C53" s="34">
         <v>45</v>
       </c>
       <c r="D53" s="2"/>
@@ -1855,7 +1854,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="41"/>
+      <c r="C54" s="36"/>
       <c r="F54" s="7"/>
       <c r="H54" s="7"/>
     </row>
@@ -1863,7 +1862,7 @@
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="41"/>
+      <c r="C55" s="36"/>
       <c r="F55" s="7"/>
       <c r="H55" s="7"/>
     </row>
@@ -1872,7 +1871,7 @@
         <v>44</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="C56" s="38">
+      <c r="C56" s="33">
         <v>23</v>
       </c>
       <c r="D56" s="4"/>
@@ -1886,7 +1885,7 @@
         <v>45</v>
       </c>
       <c r="B57" s="5"/>
-      <c r="C57" s="36">
+      <c r="C57" s="31">
         <v>11</v>
       </c>
       <c r="D57" s="2"/>
@@ -1900,27 +1899,9 @@
       </c>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-    </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="42"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1976,62 +1957,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="32" t="s">
+      <c r="O1" s="40"/>
+      <c r="P1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
       <c r="S1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32" t="s">
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="31"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="38"/>
       <c r="AE1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" s="32" t="s">
+      <c r="AG1" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
       <c r="AL1" s="1" t="s">
         <v>54</v>
       </c>
@@ -4276,29 +4257,29 @@
       <c r="AM58" s="7"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="35" t="s">
+      <c r="C59" s="40"/>
+      <c r="D59" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E59" s="33"/>
+      <c r="E59" s="40"/>
       <c r="AM59" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="Y1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
included all currency rates
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66394F1-6FC8-455D-AF2F-A5350D9F68D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEE112D-5FF1-4321-9D00-F3BE1C9C748A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="146">
   <si>
     <t>United States</t>
   </si>
@@ -457,7 +457,25 @@
     <t>Policy Rates</t>
   </si>
   <si>
-    <t>Stock Index</t>
+    <t xml:space="preserve">Currency </t>
+  </si>
+  <si>
+    <t>Rates</t>
+  </si>
+  <si>
+    <t>Currency Rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Yahoo y </t>
+  </si>
+  <si>
+    <t>Investing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock </t>
+  </si>
+  <si>
+    <t>Indices</t>
   </si>
 </sst>
 </file>
@@ -614,7 +632,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -658,24 +676,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -992,11 +1012,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K25" sqref="K25"/>
+      <selection pane="topRight" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1026,11 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
@@ -1032,17 +1053,26 @@
         <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="7"/>
       <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1050,7 +1080,7 @@
       <c r="F3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1098,9 @@
         <v>2012</v>
       </c>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1087,8 +1118,9 @@
         <v>41548</v>
       </c>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1106,8 +1138,9 @@
         <v>2008</v>
       </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1123,8 +1156,9 @@
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1142,8 +1176,9 @@
         <v>2008</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1160,8 +1195,9 @@
         <v>41671</v>
       </c>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1179,8 +1215,9 @@
         <v>2008</v>
       </c>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1198,8 +1235,9 @@
         <v>41395</v>
       </c>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1214,8 +1252,9 @@
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1232,8 +1271,9 @@
       <c r="I13" s="4">
         <v>2001</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1250,8 +1290,9 @@
         <v>2006</v>
       </c>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1269,8 +1310,9 @@
         <v>2012</v>
       </c>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -1285,8 +1327,9 @@
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1304,8 +1347,9 @@
         <v>2012</v>
       </c>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
@@ -1319,8 +1363,9 @@
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1334,8 +1379,9 @@
       <c r="I19" s="4">
         <v>2001</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1347,8 +1393,9 @@
       <c r="F20" s="9"/>
       <c r="H20" s="7"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1365,8 +1412,9 @@
       <c r="I21" s="13">
         <v>36404</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1381,8 +1429,9 @@
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1399,8 +1448,9 @@
         <v>2012</v>
       </c>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1419,8 +1469,9 @@
       <c r="I24" s="4">
         <v>2001</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1435,8 +1486,9 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1450,8 +1502,9 @@
       <c r="I26" s="4">
         <v>2010</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>69</v>
       </c>
@@ -1463,13 +1516,14 @@
       <c r="I27" s="4">
         <v>2007</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="36"/>
       <c r="F28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -1477,7 +1531,7 @@
       <c r="F29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1495,8 +1549,9 @@
         <v>2012</v>
       </c>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>24</v>
       </c>
@@ -1509,8 +1564,9 @@
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1528,8 +1584,9 @@
         <v>2012</v>
       </c>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1547,8 +1604,9 @@
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>98</v>
       </c>
@@ -1566,8 +1624,9 @@
         <v>2012</v>
       </c>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
@@ -1585,8 +1644,9 @@
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
@@ -1602,8 +1662,9 @@
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -1619,8 +1680,9 @@
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
@@ -1634,8 +1696,9 @@
       <c r="F38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
@@ -1653,8 +1716,9 @@
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>33</v>
       </c>
@@ -1666,8 +1730,9 @@
       <c r="F40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>49</v>
       </c>
@@ -1677,8 +1742,11 @@
       <c r="D41" s="4"/>
       <c r="F41" s="7"/>
       <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="13">
+        <v>36192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>34</v>
       </c>
@@ -1688,8 +1756,9 @@
       <c r="D42" s="4"/>
       <c r="F42" s="7"/>
       <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>35</v>
       </c>
@@ -1699,8 +1768,9 @@
       <c r="D43" s="4"/>
       <c r="F43" s="7"/>
       <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1718,8 +1788,9 @@
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
@@ -1731,8 +1802,9 @@
       <c r="F45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -1747,8 +1819,9 @@
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
@@ -1760,8 +1833,11 @@
       <c r="F47" s="9"/>
       <c r="H47" s="7"/>
       <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="4">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
@@ -1778,8 +1854,11 @@
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="4">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>40</v>
       </c>
@@ -1792,8 +1871,9 @@
       </c>
       <c r="F49" s="7"/>
       <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -1810,8 +1890,9 @@
       <c r="I50" s="4">
         <v>2001</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
@@ -1826,8 +1907,9 @@
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
@@ -1837,8 +1919,9 @@
       <c r="D52" s="2"/>
       <c r="F52" s="7"/>
       <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>43</v>
       </c>
@@ -1852,13 +1935,14 @@
       <c r="I53" s="4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C54" s="36"/>
       <c r="F54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
@@ -1866,7 +1950,7 @@
       <c r="F55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>44</v>
       </c>
@@ -1879,8 +1963,11 @@
       <c r="F56" s="23"/>
       <c r="H56" s="7"/>
       <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -1898,8 +1985,9 @@
         <v>2012</v>
       </c>
       <c r="I57" s="2"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="2"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G59" s="30"/>
       <c r="H59" s="30"/>
     </row>
@@ -1911,11 +1999,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:AM59"/>
+  <dimension ref="A1:AN59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP4" sqref="AP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,73 +2042,77 @@
     <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.7109375" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="38"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="37" t="s">
         <v>62</v>
       </c>
       <c r="E1" s="38"/>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="38"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
       <c r="M1" s="38"/>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="39" t="s">
         <v>111</v>
       </c>
       <c r="O1" s="40"/>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
       <c r="S1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
       <c r="X1" s="38"/>
-      <c r="Y1" s="37" t="s">
+      <c r="Y1" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
       <c r="AD1" s="38"/>
       <c r="AE1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AG1" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" s="41"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="41"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
       <c r="AL1" s="1" t="s">
         <v>54</v>
       </c>
       <c r="AM1" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN1" s="43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -2129,8 +2221,11 @@
       <c r="AM2" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN2" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>51</v>
       </c>
@@ -2228,8 +2323,11 @@
         <v>136</v>
       </c>
       <c r="AM3" s="7"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2271,8 +2369,9 @@
       <c r="AJ4" s="17"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="7"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN4" s="2"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2327,8 +2426,9 @@
       <c r="AJ5" s="17"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="7"/>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN5" s="2"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
@@ -2370,8 +2470,9 @@
       <c r="AJ6" s="17"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="7"/>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN6" s="2"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -2413,8 +2514,9 @@
       <c r="AJ7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="7"/>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN7" s="2"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
@@ -2456,8 +2558,9 @@
       <c r="AJ8" s="2"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="7"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN8" s="2"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -2501,8 +2604,9 @@
       <c r="AJ9" s="17"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="7"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN9" s="2"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2544,8 +2648,9 @@
       <c r="AJ10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="7"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN10" s="2"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
@@ -2593,8 +2698,9 @@
       <c r="AJ11" s="2"/>
       <c r="AL11" s="2"/>
       <c r="AM11" s="7"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN11" s="2"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
@@ -2637,8 +2743,9 @@
       </c>
       <c r="AL12" s="2"/>
       <c r="AM12" s="7"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN12" s="2"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
@@ -2680,8 +2787,9 @@
       <c r="AM13" s="19">
         <v>2001</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN13" s="2"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -2729,8 +2837,9 @@
       <c r="AM14" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN14" s="2"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -2772,8 +2881,9 @@
       <c r="AJ15" s="2"/>
       <c r="AL15" s="2"/>
       <c r="AM15" s="7"/>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN15" s="2"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
@@ -2786,8 +2896,9 @@
       <c r="V16" s="18"/>
       <c r="AL16" s="2"/>
       <c r="AM16" s="7"/>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
@@ -2829,8 +2940,9 @@
       <c r="AJ17" s="17"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="7"/>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN17" s="2"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>21</v>
       </c>
@@ -2841,8 +2953,9 @@
       <c r="O18" s="16"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="7"/>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN18" s="2"/>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>17</v>
       </c>
@@ -2883,8 +2996,9 @@
       <c r="AM19" s="19">
         <v>2001</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN19" s="2"/>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
@@ -2923,8 +3037,9 @@
       <c r="AJ20" s="2"/>
       <c r="AL20" s="2"/>
       <c r="AM20" s="7"/>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN20" s="2"/>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
@@ -2964,8 +3079,9 @@
       <c r="AM21" s="10">
         <v>36404</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN21" s="2"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -3010,8 +3126,9 @@
       <c r="AJ22" s="2"/>
       <c r="AL22" s="2"/>
       <c r="AM22" s="7"/>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN22" s="2"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
@@ -3057,8 +3174,9 @@
       <c r="AJ23" s="17"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="7"/>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN23" s="2"/>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
@@ -3106,8 +3224,9 @@
       <c r="AM24" s="19">
         <v>2001</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN24" s="2"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>13</v>
       </c>
@@ -3146,8 +3265,9 @@
       <c r="AJ25" s="17"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="7"/>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN25" s="2"/>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>18</v>
       </c>
@@ -3188,8 +3308,9 @@
       <c r="AM26" s="19">
         <v>2010</v>
       </c>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN26" s="2"/>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>69</v>
       </c>
@@ -3236,18 +3357,19 @@
         <v>2007</v>
       </c>
       <c r="AM27" s="7"/>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN27" s="2"/>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AM28" s="7"/>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="8"/>
       <c r="AM29" s="7"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
@@ -3297,8 +3419,9 @@
       <c r="AJ30" s="17"/>
       <c r="AL30" s="2"/>
       <c r="AM30" s="7"/>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN30" s="2"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>24</v>
       </c>
@@ -3307,8 +3430,9 @@
       </c>
       <c r="AL31" s="2"/>
       <c r="AM31" s="7"/>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN31" s="2"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
@@ -3366,8 +3490,9 @@
       <c r="AJ32" s="17"/>
       <c r="AL32" s="2"/>
       <c r="AM32" s="7"/>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN32" s="2"/>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
@@ -3412,8 +3537,9 @@
       </c>
       <c r="AL33" s="2"/>
       <c r="AM33" s="7"/>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN33" s="2"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>98</v>
       </c>
@@ -3459,8 +3585,9 @@
       <c r="AJ34" s="17"/>
       <c r="AL34" s="2"/>
       <c r="AM34" s="7"/>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN34" s="2"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
@@ -3519,8 +3646,9 @@
       <c r="AJ35" s="17"/>
       <c r="AL35" s="2"/>
       <c r="AM35" s="7"/>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN35" s="2"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>29</v>
       </c>
@@ -3562,8 +3690,9 @@
       <c r="AM36" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN36" s="2"/>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>30</v>
       </c>
@@ -3610,8 +3739,9 @@
       <c r="AJ37" s="17"/>
       <c r="AL37" s="2"/>
       <c r="AM37" s="7"/>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN37" s="2"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>31</v>
       </c>
@@ -3623,8 +3753,9 @@
       </c>
       <c r="AL38" s="2"/>
       <c r="AM38" s="7"/>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN38" s="2"/>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
@@ -3673,8 +3804,9 @@
       <c r="AJ39" s="17"/>
       <c r="AL39" s="2"/>
       <c r="AM39" s="7"/>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN39" s="2"/>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>33</v>
       </c>
@@ -3684,8 +3816,9 @@
       <c r="S40" s="2"/>
       <c r="AL40" s="2"/>
       <c r="AM40" s="7"/>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN40" s="2"/>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
@@ -3695,8 +3828,11 @@
       <c r="AM41" s="7">
         <v>2004</v>
       </c>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN41" s="13">
+        <v>36192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>34</v>
       </c>
@@ -3706,8 +3842,9 @@
       <c r="AM42" s="7">
         <v>2001</v>
       </c>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN42" s="2"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>35</v>
       </c>
@@ -3716,8 +3853,9 @@
       <c r="AM43" s="7">
         <v>2010</v>
       </c>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN43" s="2"/>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>48</v>
       </c>
@@ -3773,8 +3911,9 @@
       </c>
       <c r="AL44" s="2"/>
       <c r="AM44" s="7"/>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN44" s="2"/>
+    </row>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>36</v>
       </c>
@@ -3784,8 +3923,9 @@
       <c r="S45" s="2"/>
       <c r="AL45" s="2"/>
       <c r="AM45" s="7"/>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN45" s="2"/>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>37</v>
       </c>
@@ -3837,8 +3977,9 @@
       <c r="AM46" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN46" s="2"/>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>38</v>
       </c>
@@ -3886,8 +4027,11 @@
       <c r="AM47" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN47" s="4">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>39</v>
       </c>
@@ -3930,8 +4074,11 @@
       <c r="AJ48" s="2"/>
       <c r="AL48" s="2"/>
       <c r="AM48" s="7"/>
-    </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN48" s="4">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>40</v>
       </c>
@@ -3942,8 +4089,9 @@
       <c r="AM49" s="7">
         <v>2011</v>
       </c>
-    </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN49" s="2"/>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -3985,8 +4133,9 @@
       <c r="AM50" s="19">
         <v>2001</v>
       </c>
-    </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN50" s="2"/>
+    </row>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>47</v>
       </c>
@@ -4032,8 +4181,9 @@
       <c r="AM51" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN51" s="2"/>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>42</v>
       </c>
@@ -4043,8 +4193,9 @@
       <c r="AM52" s="7">
         <v>1999</v>
       </c>
-    </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN52" s="2"/>
+    </row>
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>43</v>
       </c>
@@ -4110,17 +4261,18 @@
       <c r="AM53" s="19">
         <v>2000</v>
       </c>
-    </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN53" s="2"/>
+    </row>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AM54" s="7"/>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>61</v>
       </c>
       <c r="AM55" s="7"/>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>44</v>
       </c>
@@ -4171,8 +4323,11 @@
       <c r="AJ56" s="17"/>
       <c r="AL56" s="2"/>
       <c r="AM56" s="7"/>
-    </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN56" s="4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>45</v>
       </c>
@@ -4252,12 +4407,13 @@
       <c r="AM57" s="9">
         <v>1999</v>
       </c>
-    </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN57" s="2"/>
+    </row>
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AM58" s="7"/>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B59" s="39" t="s">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="B59" s="41" t="s">
         <v>67</v>
       </c>
       <c r="C59" s="40"/>
@@ -4269,17 +4425,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="Y1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added index funds from IronIA
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD41B215-D43D-489F-B5DD-227A253FE906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128BE9CD-9AF7-4B4F-9CD7-C0401907DB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="359">
   <si>
     <t>United States</t>
   </si>
@@ -515,12 +515,6 @@
     <t>iShares MSCI Japan ETF</t>
   </si>
   <si>
-    <t>iShares MSCI Japan EUR Hedged UCITS ETF (Acc)</t>
-  </si>
-  <si>
-    <t>IJPE.L</t>
-  </si>
-  <si>
     <t>SXRW.DE</t>
   </si>
   <si>
@@ -539,9 +533,6 @@
     <t xml:space="preserve">iShares MSCI Canada UCITS ETF </t>
   </si>
   <si>
-    <t>ISF.L</t>
-  </si>
-  <si>
     <t>EWQ</t>
   </si>
   <si>
@@ -695,18 +686,12 @@
     <t>Lyxor BEL 20 TR (DR) UCITS ETF</t>
   </si>
   <si>
-    <t>Alternative option</t>
-  </si>
-  <si>
     <t>Global X MSCI Norway ETF</t>
   </si>
   <si>
     <t>NORW</t>
   </si>
   <si>
-    <t>OBXEDNB.OL</t>
-  </si>
-  <si>
     <t>DNB OBX ETF</t>
   </si>
   <si>
@@ -930,6 +915,207 @@
   </si>
   <si>
     <t>Global X MSCI Colombia ETF</t>
+  </si>
+  <si>
+    <t>ARGT</t>
+  </si>
+  <si>
+    <t>Global X MSCI Argentina ETF</t>
+  </si>
+  <si>
+    <t>ERUS</t>
+  </si>
+  <si>
+    <t>iShares MSCI Russia ETF</t>
+  </si>
+  <si>
+    <t>RUS.PA</t>
+  </si>
+  <si>
+    <t>Lyxor MSCI Russia UCITS ETF Acc</t>
+  </si>
+  <si>
+    <t>2008 to 2022</t>
+  </si>
+  <si>
+    <t>OBXD.OL</t>
+  </si>
+  <si>
+    <t>Index Fund (IronIA)</t>
+  </si>
+  <si>
+    <t>THD</t>
+  </si>
+  <si>
+    <t>iShares MSCI Thailand ETF</t>
+  </si>
+  <si>
+    <t>XCS4.DE</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI Thailand UCITS ETF</t>
+  </si>
+  <si>
+    <t>XCS3.DE</t>
+  </si>
+  <si>
+    <t>EWM</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI Malaysia UCITS ETF </t>
+  </si>
+  <si>
+    <t>iShares MSCI Malaysia ETF</t>
+  </si>
+  <si>
+    <t>iShares Core MSCI Japan IMI UCITS ETF</t>
+  </si>
+  <si>
+    <t>IJPA.AS</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>iShares MSCI UAE ETF</t>
+  </si>
+  <si>
+    <t>QAT</t>
+  </si>
+  <si>
+    <t>iShares MSCI Qatar ETF</t>
+  </si>
+  <si>
+    <t>KWT</t>
+  </si>
+  <si>
+    <t>iShares MSCI Kuwait ETF</t>
+  </si>
+  <si>
+    <t>EPHE</t>
+  </si>
+  <si>
+    <t>iShares MSCI Philippines ETF</t>
+  </si>
+  <si>
+    <t>XPQP.DE</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI Philippines UCITS ETF</t>
+  </si>
+  <si>
+    <t>EPU</t>
+  </si>
+  <si>
+    <t>iShares MSCI Peru ETF</t>
+  </si>
+  <si>
+    <t>EGPT</t>
+  </si>
+  <si>
+    <t>VanEck Egypt Index ETF</t>
+  </si>
+  <si>
+    <t>ETFs</t>
+  </si>
+  <si>
+    <t>LU1419797524</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>CSIF (LUX) EQUITY CAN "QB" (EUR)</t>
+  </si>
+  <si>
+    <t>IE0032126645</t>
+  </si>
+  <si>
+    <t>VANGUARD U.S. 500 STOCK INDEX (EUR) ACC</t>
+  </si>
+  <si>
+    <t>IE0008248803</t>
+  </si>
+  <si>
+    <t>VANGUARD EUROZONE STOCK INDEX (EUR) ACC</t>
+  </si>
+  <si>
+    <t>IE0007286036</t>
+  </si>
+  <si>
+    <t>VANGUARD JAPAN STOCK INDEX (EUR) ACC</t>
+  </si>
+  <si>
+    <t>LU0625737910</t>
+  </si>
+  <si>
+    <t>PICTET CHINA INDEX "P" (EUR)</t>
+  </si>
+  <si>
+    <t>LU0248271941</t>
+  </si>
+  <si>
+    <t>BGF INDIA "A2" (EUR)</t>
+  </si>
+  <si>
+    <t>LU0301637293</t>
+  </si>
+  <si>
+    <t>JPM KOREA EQUITY "A" (EUR) ACC</t>
+  </si>
+  <si>
+    <t>LU0616857586</t>
+  </si>
+  <si>
+    <t>DWS INVEST BRAZILIAN EQ "FC" (EUR) ACC</t>
+  </si>
+  <si>
+    <t>PICTET RUSSIA INDEX "I" (EUR)</t>
+  </si>
+  <si>
+    <t>LU0625742670</t>
+  </si>
+  <si>
+    <t>ES0149051007</t>
+  </si>
+  <si>
+    <t>LU0087656855</t>
+  </si>
+  <si>
+    <t>AXA WF ITALY EQUITY "F" (EUR)</t>
+  </si>
+  <si>
+    <t>LU0823428189</t>
+  </si>
+  <si>
+    <t>BNP GER MULTI-FACTOR EQ "P" (EUR) ACC</t>
+  </si>
+  <si>
+    <t>LU0823433775</t>
+  </si>
+  <si>
+    <t>BNP PARIBAS TURKEY EQUITY "I" (EUR) ACC</t>
+  </si>
+  <si>
+    <t>ABANCA IBEX 35 "D" (EUR)</t>
+  </si>
+  <si>
+    <t>IE00B7MSLV86</t>
+  </si>
+  <si>
+    <t>ISHARES UK INDEX (IE) "I" (EUR) ACC</t>
+  </si>
+  <si>
+    <t>LU1240788064</t>
+  </si>
+  <si>
+    <t>UBS (LUX) EQUITY SICA "Q" (EUR) A</t>
+  </si>
+  <si>
+    <t>FR0012806578</t>
+  </si>
+  <si>
+    <t>ODDO BHF AVENIR "CN" (EUR) ACC</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1272,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1130,22 +1316,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2451,11 +2644,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:AN59"/>
+  <dimension ref="A1:AP59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP4" sqref="AP4"/>
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO25" sqref="AO25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,69 +2685,71 @@
     <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" style="43" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.7109375" customWidth="1"/>
-    <col min="40" max="40" width="13.7109375" customWidth="1"/>
+    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.28515625" style="43" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="38"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="37" t="s">
         <v>62</v>
       </c>
       <c r="E1" s="38"/>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="38"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
       <c r="M1" s="38"/>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="39" t="s">
         <v>111</v>
       </c>
       <c r="O1" s="40"/>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
       <c r="S1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
       <c r="X1" s="38"/>
-      <c r="Y1" s="37" t="s">
+      <c r="Y1" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
       <c r="AD1" s="38"/>
       <c r="AE1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" s="37" t="s">
+      <c r="AG1" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" s="41"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="41"/>
-      <c r="AL1" s="1" t="s">
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AL1" s="29" t="s">
         <v>54</v>
       </c>
       <c r="AM1" s="20" t="s">
@@ -2563,8 +2758,12 @@
       <c r="AN1" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO1" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="AP1" s="47"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -2667,7 +2866,7 @@
       <c r="AJ2" t="s">
         <v>135</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL2" s="43" t="s">
         <v>55</v>
       </c>
       <c r="AM2" s="7" t="s">
@@ -2676,8 +2875,14 @@
       <c r="AN2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO2" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>51</v>
       </c>
@@ -2779,7 +2984,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -2819,11 +3024,17 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="17"/>
-      <c r="AL4" s="2"/>
+      <c r="AL4" s="44"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="2"/>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO4" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2876,11 +3087,17 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="17"/>
-      <c r="AL5" s="2"/>
+      <c r="AL5" s="44"/>
       <c r="AM5" s="7"/>
       <c r="AN5" s="2"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO5" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP5" s="2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
@@ -2920,11 +3137,17 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="17"/>
-      <c r="AL6" s="2"/>
+      <c r="AL6" s="44"/>
       <c r="AM6" s="7"/>
       <c r="AN6" s="2"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO6" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -2964,11 +3187,17 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
-      <c r="AL7" s="2"/>
+      <c r="AL7" s="44"/>
       <c r="AM7" s="7"/>
       <c r="AN7" s="2"/>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO7" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
@@ -3008,11 +3237,17 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="17"/>
       <c r="AJ8" s="2"/>
-      <c r="AL8" s="2"/>
+      <c r="AL8" s="44"/>
       <c r="AM8" s="7"/>
       <c r="AN8" s="2"/>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO8" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP8" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -3054,11 +3289,17 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="17"/>
-      <c r="AL9" s="2"/>
+      <c r="AL9" s="44"/>
       <c r="AM9" s="7"/>
       <c r="AN9" s="2"/>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO9" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -3098,11 +3339,17 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
-      <c r="AL10" s="2"/>
+      <c r="AL10" s="44"/>
       <c r="AM10" s="7"/>
       <c r="AN10" s="2"/>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO10" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
@@ -3148,11 +3395,17 @@
       <c r="AH11" s="17"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
-      <c r="AL11" s="2"/>
+      <c r="AL11" s="44"/>
       <c r="AM11" s="7"/>
       <c r="AN11" s="2"/>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO11" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
@@ -3193,11 +3446,17 @@
       <c r="AJ12" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL12" s="2"/>
+      <c r="AL12" s="44"/>
       <c r="AM12" s="7"/>
       <c r="AN12" s="2"/>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO12" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP12" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
@@ -3240,8 +3499,12 @@
         <v>2001</v>
       </c>
       <c r="AN13" s="2"/>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO13" s="46">
+        <v>2012</v>
+      </c>
+      <c r="AP13" s="17"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -3283,15 +3546,19 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
-      <c r="AL14" s="4">
+      <c r="AL14" s="46">
         <v>2008</v>
       </c>
       <c r="AM14" s="9">
         <v>1999</v>
       </c>
       <c r="AN14" s="2"/>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO14" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP14" s="17"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -3331,11 +3598,17 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
-      <c r="AL15" s="2"/>
+      <c r="AL15" s="44"/>
       <c r="AM15" s="7"/>
       <c r="AN15" s="2"/>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO15" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP15" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
@@ -3346,11 +3619,17 @@
       <c r="O16" s="16"/>
       <c r="S16" s="2"/>
       <c r="V16" s="18"/>
-      <c r="AL16" s="2"/>
+      <c r="AL16" s="44"/>
       <c r="AM16" s="7"/>
       <c r="AN16" s="2"/>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO16" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP16" s="17">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
@@ -3390,11 +3669,17 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="17"/>
-      <c r="AL17" s="2"/>
+      <c r="AL17" s="44"/>
       <c r="AM17" s="7"/>
       <c r="AN17" s="2"/>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO17" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP17" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>21</v>
       </c>
@@ -3403,11 +3688,17 @@
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="16"/>
-      <c r="AL18" s="2"/>
+      <c r="AL18" s="44"/>
       <c r="AM18" s="7"/>
       <c r="AN18" s="2"/>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO18" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP18" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>17</v>
       </c>
@@ -3442,15 +3733,21 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
-      <c r="AL19" s="4">
+      <c r="AL19" s="46">
         <v>2013</v>
       </c>
       <c r="AM19" s="19">
         <v>2001</v>
       </c>
       <c r="AN19" s="2"/>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO19" s="46">
+        <v>2012</v>
+      </c>
+      <c r="AP19" s="17">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
@@ -3487,11 +3784,17 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
-      <c r="AL20" s="2"/>
+      <c r="AL20" s="44"/>
       <c r="AM20" s="7"/>
       <c r="AN20" s="2"/>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO20" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP20" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
@@ -3532,8 +3835,14 @@
         <v>36404</v>
       </c>
       <c r="AN21" s="2"/>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO21" s="46">
+        <v>2009</v>
+      </c>
+      <c r="AP21" s="17">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -3576,11 +3885,15 @@
         <v>2004</v>
       </c>
       <c r="AJ22" s="2"/>
-      <c r="AL22" s="2"/>
+      <c r="AL22" s="44"/>
       <c r="AM22" s="7"/>
       <c r="AN22" s="2"/>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO22" s="46">
+        <v>2008</v>
+      </c>
+      <c r="AP22" s="17"/>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
@@ -3624,11 +3937,15 @@
       </c>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="17"/>
-      <c r="AL23" s="2"/>
+      <c r="AL23" s="44"/>
       <c r="AM23" s="7"/>
       <c r="AN23" s="2"/>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO23" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP23" s="17"/>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
@@ -3670,15 +3987,19 @@
       <c r="AH24" s="17"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
-      <c r="AL24" s="4">
+      <c r="AL24" s="46">
         <v>2003</v>
       </c>
       <c r="AM24" s="19">
         <v>2001</v>
       </c>
       <c r="AN24" s="2"/>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO24" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP24" s="17"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>13</v>
       </c>
@@ -3715,11 +4036,17 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="17"/>
-      <c r="AL25" s="2"/>
+      <c r="AL25" s="44"/>
       <c r="AM25" s="7"/>
       <c r="AN25" s="2"/>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO25" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP25" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>18</v>
       </c>
@@ -3754,15 +4081,19 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="2"/>
-      <c r="AL26" s="4">
+      <c r="AL26" s="46">
         <v>2013</v>
       </c>
       <c r="AM26" s="19">
         <v>2010</v>
       </c>
       <c r="AN26" s="2"/>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO26" s="46">
+        <v>2013</v>
+      </c>
+      <c r="AP26" s="17"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>69</v>
       </c>
@@ -3805,23 +4136,29 @@
         <v>72</v>
       </c>
       <c r="AJ27" s="2"/>
-      <c r="AL27" s="4">
+      <c r="AL27" s="46">
         <v>2007</v>
       </c>
       <c r="AM27" s="7"/>
       <c r="AN27" s="2"/>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO27" s="46">
+        <v>2002</v>
+      </c>
+      <c r="AP27" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AM28" s="7"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="8"/>
       <c r="AM29" s="7"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
@@ -3869,22 +4206,34 @@
         <v>133</v>
       </c>
       <c r="AJ30" s="17"/>
-      <c r="AL30" s="2"/>
+      <c r="AL30" s="44"/>
       <c r="AM30" s="7"/>
       <c r="AN30" s="2"/>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO30" s="46">
+        <v>2011</v>
+      </c>
+      <c r="AP30" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="2">
         <v>2012</v>
       </c>
-      <c r="AL31" s="2"/>
+      <c r="AL31" s="44"/>
       <c r="AM31" s="7"/>
       <c r="AN31" s="2"/>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO31" s="46">
+        <v>2000</v>
+      </c>
+      <c r="AP31" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
@@ -3940,11 +4289,17 @@
         <v>134</v>
       </c>
       <c r="AJ32" s="17"/>
-      <c r="AL32" s="2"/>
+      <c r="AL32" s="44"/>
       <c r="AM32" s="7"/>
       <c r="AN32" s="2"/>
-    </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO32" s="46">
+        <v>2012</v>
+      </c>
+      <c r="AP32" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
@@ -3987,11 +4342,17 @@
       <c r="AJ33" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL33" s="2"/>
+      <c r="AL33" s="44"/>
       <c r="AM33" s="7"/>
       <c r="AN33" s="2"/>
-    </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO33" s="46">
+        <v>2008</v>
+      </c>
+      <c r="AP33" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>98</v>
       </c>
@@ -4035,11 +4396,17 @@
       <c r="AH34" s="17"/>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="17"/>
-      <c r="AL34" s="2"/>
+      <c r="AL34" s="44"/>
       <c r="AM34" s="7"/>
       <c r="AN34" s="2"/>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO34" s="46">
+        <v>2000</v>
+      </c>
+      <c r="AP34" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
@@ -4096,11 +4463,17 @@
       <c r="AH35" s="17"/>
       <c r="AI35" s="17"/>
       <c r="AJ35" s="17"/>
-      <c r="AL35" s="2"/>
+      <c r="AL35" s="44"/>
       <c r="AM35" s="7"/>
       <c r="AN35" s="2"/>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO35" s="45">
+        <v>2015</v>
+      </c>
+      <c r="AP35" s="17">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>29</v>
       </c>
@@ -4143,8 +4516,14 @@
         <v>1999</v>
       </c>
       <c r="AN36" s="2"/>
-    </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO36" s="46">
+        <v>2003</v>
+      </c>
+      <c r="AP36" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>30</v>
       </c>
@@ -4189,11 +4568,17 @@
       <c r="AH37" s="17"/>
       <c r="AI37" s="17"/>
       <c r="AJ37" s="17"/>
-      <c r="AL37" s="2"/>
+      <c r="AL37" s="44"/>
       <c r="AM37" s="7"/>
       <c r="AN37" s="2"/>
-    </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO37" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP37" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>31</v>
       </c>
@@ -4203,11 +4588,17 @@
       <c r="S38" s="4">
         <v>2000</v>
       </c>
-      <c r="AL38" s="2"/>
+      <c r="AL38" s="44"/>
       <c r="AM38" s="7"/>
       <c r="AN38" s="2"/>
-    </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO38" s="46">
+        <v>2008</v>
+      </c>
+      <c r="AP38" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
@@ -4254,11 +4645,17 @@
       <c r="AH39" s="17"/>
       <c r="AI39" s="17"/>
       <c r="AJ39" s="17"/>
-      <c r="AL39" s="2"/>
+      <c r="AL39" s="44"/>
       <c r="AM39" s="7"/>
       <c r="AN39" s="2"/>
-    </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO39" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP39" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>33</v>
       </c>
@@ -4266,11 +4663,17 @@
         <v>2015</v>
       </c>
       <c r="S40" s="2"/>
-      <c r="AL40" s="2"/>
+      <c r="AL40" s="44"/>
       <c r="AM40" s="7"/>
       <c r="AN40" s="2"/>
-    </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO40" s="44">
+        <v>1999</v>
+      </c>
+      <c r="AP40" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
@@ -4283,8 +4686,12 @@
       <c r="AN41" s="13">
         <v>36192</v>
       </c>
-    </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO41" s="45">
+        <v>2014</v>
+      </c>
+      <c r="AP41" s="17"/>
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>34</v>
       </c>
@@ -4295,8 +4702,12 @@
         <v>2001</v>
       </c>
       <c r="AN42" s="2"/>
-    </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO42" s="45">
+        <v>2014</v>
+      </c>
+      <c r="AP42" s="17"/>
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>35</v>
       </c>
@@ -4306,8 +4717,12 @@
         <v>2010</v>
       </c>
       <c r="AN43" s="2"/>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO43" s="45">
+        <v>2020</v>
+      </c>
+      <c r="AP43" s="17"/>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>48</v>
       </c>
@@ -4361,11 +4776,17 @@
       <c r="AJ44" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL44" s="2"/>
+      <c r="AL44" s="44"/>
       <c r="AM44" s="7"/>
       <c r="AN44" s="2"/>
-    </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO44" s="46">
+        <v>2008</v>
+      </c>
+      <c r="AP44" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>36</v>
       </c>
@@ -4373,11 +4794,17 @@
         <v>2018</v>
       </c>
       <c r="S45" s="2"/>
-      <c r="AL45" s="2"/>
+      <c r="AL45" s="44"/>
       <c r="AM45" s="7"/>
       <c r="AN45" s="2"/>
-    </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO45" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP45" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>37</v>
       </c>
@@ -4430,8 +4857,14 @@
         <v>1999</v>
       </c>
       <c r="AN46" s="2"/>
-    </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO46" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP46" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>38</v>
       </c>
@@ -4482,8 +4915,12 @@
       <c r="AN47" s="4">
         <v>2002</v>
       </c>
-    </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO47" s="46">
+        <v>2007</v>
+      </c>
+      <c r="AP47" s="17"/>
+    </row>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>39</v>
       </c>
@@ -4524,13 +4961,19 @@
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
       <c r="AJ48" s="2"/>
-      <c r="AL48" s="2"/>
+      <c r="AL48" s="44"/>
       <c r="AM48" s="7"/>
       <c r="AN48" s="4">
         <v>2001</v>
       </c>
-    </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO48" s="46">
+        <v>2011</v>
+      </c>
+      <c r="AP48" s="2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>40</v>
       </c>
@@ -4542,8 +4985,12 @@
         <v>2011</v>
       </c>
       <c r="AN49" s="2"/>
-    </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO49" s="46">
+        <v>2009</v>
+      </c>
+      <c r="AP49" s="17"/>
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -4586,8 +5033,10 @@
         <v>2001</v>
       </c>
       <c r="AN50" s="2"/>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO50" s="45"/>
+      <c r="AP50" s="17"/>
+    </row>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>47</v>
       </c>
@@ -4634,8 +5083,12 @@
         <v>1999</v>
       </c>
       <c r="AN51" s="2"/>
-    </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO51" s="45"/>
+      <c r="AP51" s="17">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>42</v>
       </c>
@@ -4646,8 +5099,12 @@
         <v>1999</v>
       </c>
       <c r="AN52" s="2"/>
-    </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO52" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP52" s="17"/>
+    </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>43</v>
       </c>
@@ -4714,17 +5171,21 @@
         <v>2000</v>
       </c>
       <c r="AN53" s="2"/>
-    </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO53" s="46">
+        <v>2009</v>
+      </c>
+      <c r="AP53" s="17"/>
+    </row>
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AM54" s="7"/>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>61</v>
       </c>
       <c r="AM55" s="7"/>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>44</v>
       </c>
@@ -4773,13 +5234,17 @@
       <c r="AH56" s="17"/>
       <c r="AI56" s="17"/>
       <c r="AJ56" s="17"/>
-      <c r="AL56" s="2"/>
+      <c r="AL56" s="44"/>
       <c r="AM56" s="7"/>
       <c r="AN56" s="4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO56" s="46">
+        <v>2011</v>
+      </c>
+      <c r="AP56" s="17"/>
+    </row>
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>45</v>
       </c>
@@ -4853,19 +5318,25 @@
       <c r="AH57" s="17"/>
       <c r="AI57" s="17"/>
       <c r="AJ57" s="17"/>
-      <c r="AL57" s="4">
+      <c r="AL57" s="46">
         <v>2013</v>
       </c>
       <c r="AM57" s="9">
         <v>1999</v>
       </c>
       <c r="AN57" s="2"/>
-    </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO57" s="46">
+        <v>2010</v>
+      </c>
+      <c r="AP57" s="17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AM58" s="7"/>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B59" s="39" t="s">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="B59" s="41" t="s">
         <v>67</v>
       </c>
       <c r="C59" s="40"/>
@@ -4876,18 +5347,19 @@
       <c r="AM59" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="Y1:AD1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4897,8 +5369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC8819E-4998-4293-AE91-8A38F68283E5}">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4908,31 +5381,32 @@
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="H1" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="M1" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
@@ -4962,7 +5436,7 @@
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>146</v>
+        <v>327</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>147</v>
@@ -5007,6 +5481,18 @@
       <c r="K4">
         <v>2010</v>
       </c>
+      <c r="M4" t="s">
+        <v>329</v>
+      </c>
+      <c r="N4" t="s">
+        <v>330</v>
+      </c>
+      <c r="O4" t="s">
+        <v>150</v>
+      </c>
+      <c r="P4">
+        <v>2002</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -5025,16 +5511,28 @@
         <v>1999</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>310</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>309</v>
       </c>
       <c r="J5" t="s">
         <v>150</v>
       </c>
       <c r="K5">
-        <v>2010</v>
+        <v>2009</v>
+      </c>
+      <c r="M5" t="s">
+        <v>333</v>
+      </c>
+      <c r="N5" t="s">
+        <v>334</v>
+      </c>
+      <c r="O5" t="s">
+        <v>150</v>
+      </c>
+      <c r="P5">
+        <v>2006</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -5042,10 +5540,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
         <v>153</v>
@@ -5054,10 +5552,10 @@
         <v>1999</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J6" t="s">
         <v>150</v>
@@ -5066,16 +5564,16 @@
         <v>2010</v>
       </c>
       <c r="M6" t="s">
-        <v>166</v>
+        <v>353</v>
       </c>
       <c r="N6" t="s">
-        <v>161</v>
+        <v>354</v>
       </c>
       <c r="O6" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="P6">
-        <v>2008</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -5083,10 +5581,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
         <v>153</v>
@@ -5095,16 +5593,28 @@
         <v>1999</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J7" t="s">
         <v>150</v>
       </c>
       <c r="K7">
         <v>2010</v>
+      </c>
+      <c r="M7" t="s">
+        <v>326</v>
+      </c>
+      <c r="N7" t="s">
+        <v>328</v>
+      </c>
+      <c r="O7" t="s">
+        <v>150</v>
+      </c>
+      <c r="P7">
+        <v>2016</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -5112,10 +5622,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E8" t="s">
         <v>153</v>
@@ -5124,16 +5634,28 @@
         <v>1999</v>
       </c>
       <c r="H8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J8" t="s">
         <v>150</v>
       </c>
       <c r="K8">
         <v>2008</v>
+      </c>
+      <c r="M8" t="s">
+        <v>357</v>
+      </c>
+      <c r="N8" t="s">
+        <v>358</v>
+      </c>
+      <c r="O8" t="s">
+        <v>150</v>
+      </c>
+      <c r="P8">
+        <v>2015</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -5141,10 +5663,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
         <v>153</v>
@@ -5153,16 +5675,28 @@
         <v>1999</v>
       </c>
       <c r="H9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J9" t="s">
         <v>150</v>
       </c>
       <c r="K9">
         <v>2008</v>
+      </c>
+      <c r="M9" t="s">
+        <v>355</v>
+      </c>
+      <c r="N9" t="s">
+        <v>356</v>
+      </c>
+      <c r="O9" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9">
+        <v>2015</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5170,10 +5704,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E10" t="s">
         <v>153</v>
@@ -5182,16 +5716,28 @@
         <v>1999</v>
       </c>
       <c r="H10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J10" t="s">
         <v>150</v>
       </c>
       <c r="K10">
         <v>2008</v>
+      </c>
+      <c r="M10" t="s">
+        <v>348</v>
+      </c>
+      <c r="N10" t="s">
+        <v>349</v>
+      </c>
+      <c r="O10" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10">
+        <v>2013</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -5199,10 +5745,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E11" t="s">
         <v>153</v>
@@ -5211,13 +5757,13 @@
         <v>1999</v>
       </c>
       <c r="H11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K11">
         <v>2010</v>
@@ -5228,10 +5774,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
         <v>153</v>
@@ -5240,10 +5786,10 @@
         <v>1999</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J12" t="s">
         <v>150</v>
@@ -5257,10 +5803,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E13" t="s">
         <v>153</v>
@@ -5275,10 +5821,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
         <v>153</v>
@@ -5293,10 +5839,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E15" t="s">
         <v>153</v>
@@ -5305,16 +5851,28 @@
         <v>1999</v>
       </c>
       <c r="H15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J15" t="s">
         <v>150</v>
       </c>
       <c r="K15">
         <v>2011</v>
+      </c>
+      <c r="M15" t="s">
+        <v>345</v>
+      </c>
+      <c r="N15" t="s">
+        <v>352</v>
+      </c>
+      <c r="O15" t="s">
+        <v>150</v>
+      </c>
+      <c r="P15">
+        <v>2016</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -5322,10 +5880,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E16" t="s">
         <v>153</v>
@@ -5334,10 +5892,10 @@
         <v>1999</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>150</v>
@@ -5351,10 +5909,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E17" t="s">
         <v>153</v>
@@ -5363,16 +5921,28 @@
         <v>1999</v>
       </c>
       <c r="H17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J17" t="s">
         <v>150</v>
       </c>
       <c r="K17">
         <v>2008</v>
+      </c>
+      <c r="M17" t="s">
+        <v>346</v>
+      </c>
+      <c r="N17" t="s">
+        <v>347</v>
+      </c>
+      <c r="O17" t="s">
+        <v>150</v>
+      </c>
+      <c r="P17">
+        <v>1999</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -5380,10 +5950,10 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
         <v>153</v>
@@ -5392,10 +5962,10 @@
         <v>1999</v>
       </c>
       <c r="H18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J18" t="s">
         <v>150</v>
@@ -5409,10 +5979,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E19" t="s">
         <v>153</v>
@@ -5420,16 +5990,16 @@
       <c r="F19">
         <v>2012</v>
       </c>
-      <c r="H19" t="s">
-        <v>192</v>
-      </c>
-      <c r="I19" t="s">
-        <v>193</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="H19" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="17">
         <v>2008</v>
       </c>
     </row>
@@ -5438,10 +6008,10 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E20" t="s">
         <v>153</v>
@@ -5450,10 +6020,10 @@
         <v>1999</v>
       </c>
       <c r="H20" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J20" t="s">
         <v>150</v>
@@ -5467,10 +6037,10 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E21" t="s">
         <v>153</v>
@@ -5478,17 +6048,16 @@
       <c r="F21">
         <v>2009</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="M21" t="s">
-        <v>221</v>
-      </c>
-      <c r="N21" t="s">
-        <v>222</v>
-      </c>
-      <c r="O21" t="s">
-        <v>223</v>
-      </c>
-      <c r="P21">
+      <c r="H21" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="K21" s="17">
         <v>2008</v>
       </c>
     </row>
@@ -5497,10 +6066,10 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E22" t="s">
         <v>153</v>
@@ -5515,10 +6084,10 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E23" t="s">
         <v>153</v>
@@ -5533,10 +6102,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D24" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E24" t="s">
         <v>153</v>
@@ -5551,10 +6120,10 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D25" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E25" t="s">
         <v>153</v>
@@ -5563,10 +6132,10 @@
         <v>1999</v>
       </c>
       <c r="H25" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I25" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J25" t="s">
         <v>150</v>
@@ -5580,10 +6149,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
         <v>153</v>
@@ -5598,10 +6167,10 @@
         <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D27" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E27" t="s">
         <v>153</v>
@@ -5610,16 +6179,28 @@
         <v>2002</v>
       </c>
       <c r="H27" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I27" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="J27" t="s">
         <v>150</v>
       </c>
       <c r="K27">
         <v>2008</v>
+      </c>
+      <c r="M27" t="s">
+        <v>331</v>
+      </c>
+      <c r="N27" t="s">
+        <v>332</v>
+      </c>
+      <c r="O27" t="s">
+        <v>150</v>
+      </c>
+      <c r="P27">
+        <v>2001</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -5632,10 +6213,10 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E30" t="s">
         <v>153</v>
@@ -5644,15 +6225,27 @@
         <v>2011</v>
       </c>
       <c r="H30" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I30" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="J30" t="s">
         <v>150</v>
       </c>
       <c r="K30">
+        <v>2011</v>
+      </c>
+      <c r="M30" t="s">
+        <v>335</v>
+      </c>
+      <c r="N30" t="s">
+        <v>336</v>
+      </c>
+      <c r="O30" t="s">
+        <v>150</v>
+      </c>
+      <c r="P30">
         <v>2011</v>
       </c>
     </row>
@@ -5661,10 +6254,10 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D31" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E31" t="s">
         <v>153</v>
@@ -5673,10 +6266,10 @@
         <v>2000</v>
       </c>
       <c r="H31" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I31" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J31" t="s">
         <v>150</v>
@@ -5690,10 +6283,10 @@
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D32" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E32" t="s">
         <v>153</v>
@@ -5702,10 +6295,10 @@
         <v>2012</v>
       </c>
       <c r="H32" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I32" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="J32" t="s">
         <v>150</v>
@@ -5713,16 +6306,28 @@
       <c r="K32">
         <v>2008</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>337</v>
+      </c>
+      <c r="N32" t="s">
+        <v>338</v>
+      </c>
+      <c r="O32" t="s">
+        <v>150</v>
+      </c>
+      <c r="P32">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D33" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E33" t="s">
         <v>153</v>
@@ -5731,10 +6336,10 @@
         <v>2008</v>
       </c>
       <c r="H33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J33" t="s">
         <v>150</v>
@@ -5742,16 +6347,28 @@
       <c r="K33">
         <v>2008</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>339</v>
+      </c>
+      <c r="N33" t="s">
+        <v>340</v>
+      </c>
+      <c r="O33" t="s">
+        <v>150</v>
+      </c>
+      <c r="P33">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D34" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E34" t="s">
         <v>153</v>
@@ -5760,10 +6377,10 @@
         <v>2000</v>
       </c>
       <c r="H34" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I34" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="J34" t="s">
         <v>150</v>
@@ -5771,45 +6388,57 @@
       <c r="K34">
         <v>2008</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>341</v>
+      </c>
+      <c r="N34" t="s">
+        <v>342</v>
+      </c>
+      <c r="O34" t="s">
+        <v>150</v>
+      </c>
+      <c r="P34">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F35" s="17">
         <v>2015</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K35" s="17">
         <v>2019</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D36" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E36" t="s">
         <v>153</v>
@@ -5818,10 +6447,10 @@
         <v>2003</v>
       </c>
       <c r="H36" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I36" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J36" t="s">
         <v>150</v>
@@ -5830,15 +6459,15 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D37" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E37" t="s">
         <v>153</v>
@@ -5847,10 +6476,10 @@
         <v>1999</v>
       </c>
       <c r="H37" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I37" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="J37" t="s">
         <v>150</v>
@@ -5859,20 +6488,44 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38">
+        <v>2008</v>
+      </c>
+      <c r="H38" t="s">
+        <v>303</v>
+      </c>
+      <c r="I38" t="s">
+        <v>304</v>
+      </c>
+      <c r="J38" t="s">
+        <v>150</v>
+      </c>
+      <c r="K38">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D39" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E39" t="s">
         <v>153</v>
@@ -5881,10 +6534,10 @@
         <v>2010</v>
       </c>
       <c r="H39" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I39" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J39" t="s">
         <v>150</v>
@@ -5893,35 +6546,98 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>306</v>
+      </c>
+      <c r="D40" t="s">
+        <v>308</v>
+      </c>
+      <c r="E40" t="s">
+        <v>153</v>
+      </c>
+      <c r="F40">
+        <v>1999</v>
+      </c>
+      <c r="H40" t="s">
+        <v>305</v>
+      </c>
+      <c r="I40" t="s">
+        <v>307</v>
+      </c>
+      <c r="J40" t="s">
+        <v>150</v>
+      </c>
+      <c r="K40">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F41" s="17">
+        <v>2014</v>
+      </c>
+      <c r="H41" s="17"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="17">
+        <v>2014</v>
+      </c>
+      <c r="H42" s="17"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C43" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F43" s="17">
+        <v>2020</v>
+      </c>
+      <c r="H43" s="17"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D44" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E44" t="s">
         <v>153</v>
@@ -5930,10 +6646,10 @@
         <v>2008</v>
       </c>
       <c r="H44" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I44" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J44" t="s">
         <v>150</v>
@@ -5941,21 +6657,57 @@
       <c r="K44">
         <v>2008</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="M44" t="s">
+        <v>350</v>
+      </c>
+      <c r="N44" t="s">
+        <v>351</v>
+      </c>
+      <c r="O44" t="s">
+        <v>150</v>
+      </c>
+      <c r="P44">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>317</v>
+      </c>
+      <c r="D45" t="s">
+        <v>318</v>
+      </c>
+      <c r="E45" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45">
+        <v>2010</v>
+      </c>
+      <c r="H45" t="s">
+        <v>319</v>
+      </c>
+      <c r="I45" t="s">
+        <v>320</v>
+      </c>
+      <c r="J45" t="s">
+        <v>150</v>
+      </c>
+      <c r="K45">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D46" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E46" t="s">
         <v>153</v>
@@ -5964,10 +6716,10 @@
         <v>2010</v>
       </c>
       <c r="H46" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I46" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="J46" t="s">
         <v>150</v>
@@ -5976,15 +6728,15 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D47" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E47" t="s">
         <v>153</v>
@@ -5994,15 +6746,15 @@
       </c>
       <c r="H47" s="17"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E48" t="s">
         <v>153</v>
@@ -6011,10 +6763,10 @@
         <v>2011</v>
       </c>
       <c r="H48" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I48" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J48" t="s">
         <v>150</v>
@@ -6023,28 +6775,41 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>321</v>
+      </c>
+      <c r="D49" t="s">
+        <v>322</v>
+      </c>
+      <c r="E49" t="s">
+        <v>153</v>
+      </c>
+      <c r="F49">
+        <v>2009</v>
+      </c>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C50" s="17"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="17"/>
       <c r="H51" s="17" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="J51" s="17" t="s">
         <v>150</v>
@@ -6053,20 +6818,33 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>323</v>
+      </c>
+      <c r="D52" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F52">
+        <v>2010</v>
+      </c>
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E53" t="s">
         <v>153</v>
@@ -6076,19 +6854,68 @@
       </c>
       <c r="H53" s="17"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>292</v>
+      </c>
+      <c r="D56" t="s">
+        <v>293</v>
+      </c>
+      <c r="E56" t="s">
+        <v>259</v>
+      </c>
+      <c r="F56">
+        <v>2011</v>
+      </c>
+      <c r="H56" s="17"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>294</v>
+      </c>
+      <c r="D57" t="s">
+        <v>295</v>
+      </c>
+      <c r="E57" t="s">
+        <v>153</v>
+      </c>
+      <c r="F57">
+        <v>2010</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="I57" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="M57" t="s">
+        <v>344</v>
+      </c>
+      <c r="N57" t="s">
+        <v>343</v>
+      </c>
+      <c r="O57" t="s">
+        <v>150</v>
+      </c>
+      <c r="P57">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a few indicators and rounded values
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AAA6AC-B274-4BC6-879C-740BBCBF94A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8542091-9588-44DA-9CE5-430018722231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="375">
   <si>
     <t>United States</t>
   </si>
@@ -1134,6 +1134,36 @@
   </si>
   <si>
     <t>EUR ETFs</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Total industry</t>
+  </si>
+  <si>
+    <t>ex Construction</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>PPI</t>
+  </si>
+  <si>
+    <t>PPI Manufacture</t>
+  </si>
+  <si>
+    <t>of Food Products</t>
+  </si>
+  <si>
+    <t>to 2019</t>
+  </si>
+  <si>
+    <t>2001 to 2019</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1320,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1356,12 +1386,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1694,9 +1730,8 @@
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="48" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,13 +1762,13 @@
       <c r="J1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="1" t="s">
         <v>358</v>
       </c>
     </row>
@@ -1749,9 +1784,9 @@
       <c r="J2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K2" s="47"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="47" t="s">
+      <c r="M2" s="1" t="s">
         <v>359</v>
       </c>
     </row>
@@ -1782,11 +1817,11 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="49"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="4">
         <v>2010</v>
       </c>
-      <c r="M4" s="49">
+      <c r="M4" s="2">
         <v>2002</v>
       </c>
     </row>
@@ -1809,11 +1844,11 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="49"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="4">
         <v>2009</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="2">
         <v>2006</v>
       </c>
     </row>
@@ -1836,11 +1871,11 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="49"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="4">
         <v>2010</v>
       </c>
-      <c r="M6" s="51">
+      <c r="M6" s="17">
         <v>2011</v>
       </c>
     </row>
@@ -1861,11 +1896,11 @@
       <c r="H7" s="7"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="49"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="4">
         <v>2010</v>
       </c>
-      <c r="M7" s="50">
+      <c r="M7" s="4">
         <v>2016</v>
       </c>
     </row>
@@ -1888,7 +1923,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="49"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="2">
         <v>2008</v>
       </c>
@@ -1911,11 +1946,11 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="49"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2">
         <v>2008</v>
       </c>
-      <c r="M9" s="49">
+      <c r="M9" s="2">
         <v>2010</v>
       </c>
     </row>
@@ -1938,11 +1973,11 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="49"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2">
         <v>2008</v>
       </c>
-      <c r="M10" s="49">
+      <c r="M10" s="2">
         <v>2012</v>
       </c>
     </row>
@@ -1965,11 +2000,11 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="49"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="4">
         <v>2010</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="2">
         <v>2007</v>
       </c>
     </row>
@@ -1989,7 +2024,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="49"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2">
         <v>2008</v>
       </c>
@@ -2012,7 +2047,7 @@
         <v>2001</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="50">
+      <c r="K13" s="4">
         <v>2012</v>
       </c>
     </row>
@@ -2034,7 +2069,7 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="49"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -2055,11 +2090,11 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="49"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="4">
         <v>2011</v>
       </c>
-      <c r="M15" s="50">
+      <c r="M15" s="4">
         <v>2016</v>
       </c>
     </row>
@@ -2079,7 +2114,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="49"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="17">
         <v>2016</v>
       </c>
@@ -2103,11 +2138,11 @@
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="49"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="2">
         <v>2008</v>
       </c>
-      <c r="M17" s="49">
+      <c r="M17" s="2">
         <v>1999</v>
       </c>
     </row>
@@ -2126,7 +2161,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="49"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="4">
         <v>2011</v>
       </c>
@@ -2146,7 +2181,7 @@
         <v>2001</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="K19" s="50">
+      <c r="K19" s="4">
         <v>2012</v>
       </c>
       <c r="L19" s="17">
@@ -2166,7 +2201,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="49"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="2">
         <v>2008</v>
       </c>
@@ -2189,7 +2224,7 @@
         <v>36404</v>
       </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="50">
+      <c r="K21" s="4">
         <v>2009</v>
       </c>
       <c r="L21" s="17">
@@ -2212,7 +2247,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="50">
+      <c r="K22" s="4">
         <v>2008</v>
       </c>
     </row>
@@ -2234,7 +2269,7 @@
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="50">
+      <c r="K23" s="4">
         <v>2010</v>
       </c>
     </row>
@@ -2258,7 +2293,7 @@
         <v>2001</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="50">
+      <c r="K24" s="4">
         <v>2010</v>
       </c>
     </row>
@@ -2278,7 +2313,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="49"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2">
         <v>2008</v>
       </c>
@@ -2298,7 +2333,7 @@
         <v>2010</v>
       </c>
       <c r="J26" s="2"/>
-      <c r="K26" s="50">
+      <c r="K26" s="4">
         <v>2013</v>
       </c>
     </row>
@@ -2315,13 +2350,13 @@
         <v>2007</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="50">
+      <c r="K27" s="4">
         <v>2002</v>
       </c>
       <c r="L27" s="2">
         <v>2008</v>
       </c>
-      <c r="M27" s="49">
+      <c r="M27" s="2">
         <v>2001</v>
       </c>
     </row>
@@ -2357,13 +2392,13 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="50">
+      <c r="K30" s="4">
         <v>2011</v>
       </c>
       <c r="L30" s="4">
         <v>2011</v>
       </c>
-      <c r="M30" s="49">
+      <c r="M30" s="2">
         <v>2011</v>
       </c>
     </row>
@@ -2381,7 +2416,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="50">
+      <c r="K31" s="4">
         <v>2000</v>
       </c>
       <c r="L31" s="2">
@@ -2407,13 +2442,13 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="50">
+      <c r="K32" s="4">
         <v>2012</v>
       </c>
       <c r="L32" s="2">
         <v>2008</v>
       </c>
-      <c r="M32" s="49">
+      <c r="M32" s="2">
         <v>2005</v>
       </c>
     </row>
@@ -2436,13 +2471,13 @@
       <c r="H33" s="7"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="50">
+      <c r="K33" s="4">
         <v>2000</v>
       </c>
       <c r="L33" s="2">
         <v>2008</v>
       </c>
-      <c r="M33" s="49">
+      <c r="M33" s="2">
         <v>2007</v>
       </c>
     </row>
@@ -2465,13 +2500,13 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="50">
+      <c r="K34" s="4">
         <v>2000</v>
       </c>
       <c r="L34" s="2">
         <v>2008</v>
       </c>
-      <c r="M34" s="49">
+      <c r="M34" s="2">
         <v>2012</v>
       </c>
     </row>
@@ -2494,7 +2529,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="51">
+      <c r="K35" s="17">
         <v>2015</v>
       </c>
       <c r="L35" s="17">
@@ -2518,7 +2553,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="50">
+      <c r="K36" s="4">
         <v>2003</v>
       </c>
       <c r="L36" s="4">
@@ -2542,7 +2577,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="49"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="4">
         <v>2010</v>
       </c>
@@ -2562,7 +2597,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="50">
+      <c r="K38" s="4">
         <v>2008</v>
       </c>
       <c r="L38" s="4">
@@ -2588,7 +2623,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="50">
+      <c r="K39" s="4">
         <v>2010</v>
       </c>
       <c r="L39" s="4">
@@ -2608,7 +2643,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="49"/>
+      <c r="K40" s="2"/>
       <c r="L40" s="4">
         <v>2011</v>
       </c>
@@ -2626,7 +2661,7 @@
       <c r="J41" s="13">
         <v>36192</v>
       </c>
-      <c r="K41" s="51">
+      <c r="K41" s="17">
         <v>2014</v>
       </c>
     </row>
@@ -2641,7 +2676,7 @@
       <c r="F42" s="7"/>
       <c r="H42" s="7"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="51">
+      <c r="K42" s="17">
         <v>2014</v>
       </c>
     </row>
@@ -2656,7 +2691,7 @@
       <c r="F43" s="7"/>
       <c r="H43" s="7"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="51">
+      <c r="K43" s="17">
         <v>2020</v>
       </c>
     </row>
@@ -2679,13 +2714,13 @@
       <c r="H44" s="7"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="50">
+      <c r="K44" s="4">
         <v>2008</v>
       </c>
       <c r="L44" s="2">
         <v>2008</v>
       </c>
-      <c r="M44" s="49">
+      <c r="M44" s="2">
         <v>2012</v>
       </c>
     </row>
@@ -2702,7 +2737,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="50">
+      <c r="K45" s="4">
         <v>2010</v>
       </c>
       <c r="L45" s="4">
@@ -2725,7 +2760,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="50">
+      <c r="K46" s="4">
         <v>2010</v>
       </c>
       <c r="L46" s="4">
@@ -2747,7 +2782,7 @@
       <c r="J47" s="4">
         <v>2002</v>
       </c>
-      <c r="K47" s="50">
+      <c r="K47" s="4">
         <v>2007</v>
       </c>
     </row>
@@ -2771,7 +2806,7 @@
       <c r="J48" s="4">
         <v>2001</v>
       </c>
-      <c r="K48" s="50">
+      <c r="K48" s="4">
         <v>2011</v>
       </c>
       <c r="L48" s="2">
@@ -2792,7 +2827,7 @@
       <c r="F49" s="7"/>
       <c r="H49" s="7"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="50">
+      <c r="K49" s="4">
         <v>2009</v>
       </c>
     </row>
@@ -2814,7 +2849,7 @@
         <v>2001</v>
       </c>
       <c r="J50" s="2"/>
-      <c r="K50" s="51"/>
+      <c r="K50" s="17"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -2832,7 +2867,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="51"/>
+      <c r="K51" s="17"/>
       <c r="L51" s="17">
         <v>2018</v>
       </c>
@@ -2848,7 +2883,7 @@
       <c r="F52" s="7"/>
       <c r="H52" s="7"/>
       <c r="J52" s="2"/>
-      <c r="K52" s="50">
+      <c r="K52" s="4">
         <v>2010</v>
       </c>
     </row>
@@ -2867,7 +2902,7 @@
         <v>2000</v>
       </c>
       <c r="J53" s="2"/>
-      <c r="K53" s="50">
+      <c r="K53" s="4">
         <v>2009</v>
       </c>
     </row>
@@ -2900,7 +2935,7 @@
       <c r="J56" s="4">
         <v>2000</v>
       </c>
-      <c r="K56" s="50">
+      <c r="K56" s="4">
         <v>2011</v>
       </c>
     </row>
@@ -2923,13 +2958,13 @@
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="50">
+      <c r="K57" s="4">
         <v>2010</v>
       </c>
       <c r="L57" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="M57" s="51" t="s">
+      <c r="M57" s="17" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2945,11 +2980,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
-  <dimension ref="A1:AQ59"/>
+  <dimension ref="A1:AT59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS1" sqref="AS1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,33 +3004,37 @@
     <col min="15" max="15" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="7"/>
-    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.7109375" customWidth="1"/>
-    <col min="30" max="30" width="11.7109375" style="7" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" style="7" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.7109375" customWidth="1"/>
-    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.28515625" style="37" customWidth="1"/>
-    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="47" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" style="7" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="11.7109375" customWidth="1"/>
+    <col min="32" max="32" width="11.7109375" style="7" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="34" max="34" width="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" style="7" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" customWidth="1"/>
+    <col min="43" max="43" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.28515625" style="37" customWidth="1"/>
+    <col min="45" max="45" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B1" s="41" t="s">
         <v>63</v>
       </c>
@@ -3020,56 +3059,61 @@
         <v>111</v>
       </c>
       <c r="O1" s="45"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="29" t="s">
+      <c r="Q1" s="49"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="42" t="s">
+      <c r="V1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
       <c r="W1" s="42"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="41" t="s">
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
       <c r="AB1" s="42"/>
       <c r="AC1" s="42"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="12" t="s">
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="41" t="s">
         <v>70</v>
-      </c>
-      <c r="AG1" s="41" t="s">
-        <v>114</v>
       </c>
       <c r="AH1" s="42"/>
       <c r="AI1" s="42"/>
       <c r="AJ1" s="42"/>
-      <c r="AL1" s="29" t="s">
+      <c r="AK1" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL1" s="42"/>
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AM1" s="20" t="s">
+      <c r="AP1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AO1" s="41" t="s">
+      <c r="AR1" s="41" t="s">
         <v>322</v>
       </c>
-      <c r="AP1" s="42"/>
-      <c r="AQ1" s="20" t="s">
+      <c r="AS1" s="42"/>
+      <c r="AT1" s="20" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>59</v>
       </c>
@@ -3118,80 +3162,95 @@
       <c r="Q2" t="s">
         <v>88</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="53" t="s">
+        <v>371</v>
+      </c>
+      <c r="T2" s="56" t="s">
+        <v>370</v>
+      </c>
+      <c r="U2" t="s">
         <v>137</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>77</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>81</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>83</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>118</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>90</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>104</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>123</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>125</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>91</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>365</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>367</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="AK2" t="s">
         <v>93</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AL2" t="s">
         <v>128</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
         <v>131</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AN2" t="s">
         <v>135</v>
       </c>
-      <c r="AL2" s="37" t="s">
+      <c r="AO2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AP2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AQ2" t="s">
         <v>142</v>
       </c>
-      <c r="AO2" s="29" t="s">
+      <c r="AR2" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AQ2" s="20" t="s">
+      <c r="AT2" s="20" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>51</v>
       </c>
@@ -3237,72 +3296,87 @@
       <c r="Q3" t="s">
         <v>122</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="53" t="s">
+        <v>372</v>
+      </c>
+      <c r="T3" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="U3" t="s">
         <v>138</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>78</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>82</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>82</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>119</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>127</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>103</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>103</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>124</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AF3" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>92</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
+        <v>366</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>368</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="AK3" t="s">
         <v>94</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AL3" t="s">
         <v>129</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AM3" t="s">
         <v>132</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AN3" t="s">
         <v>136</v>
       </c>
-      <c r="AM3" s="7"/>
-      <c r="AN3" t="s">
+      <c r="AP3" s="7"/>
+      <c r="AQ3" t="s">
         <v>143</v>
       </c>
-      <c r="AO3" s="37" t="s">
+      <c r="AR3" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AS3" t="s">
         <v>55</v>
       </c>
-      <c r="AQ3" s="7" t="s">
+      <c r="AT3" s="7" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -3324,38 +3398,43 @@
       <c r="O4" s="9"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="9"/>
+      <c r="R4" s="51"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="T4" s="9"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="9"/>
+      <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="9"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="9"/>
+      <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
+      <c r="AF4" s="9"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
-      <c r="AJ4" s="17"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="38">
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="38">
         <v>1999</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AS4" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ4" s="9">
+      <c r="AT4" s="9">
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -3386,42 +3465,47 @@
       <c r="Q5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="4">
+      <c r="S5" s="17"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="4">
         <v>2002</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="9"/>
+      <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="9"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="9"/>
+      <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
+      <c r="AF5" s="9"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="17"/>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="2"/>
-      <c r="AO5" s="38">
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="38"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="38">
         <v>1999</v>
       </c>
-      <c r="AP5" s="4">
+      <c r="AS5" s="4">
         <v>2009</v>
       </c>
-      <c r="AQ5" s="9">
+      <c r="AT5" s="9">
         <v>2006</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
@@ -3443,38 +3527,49 @@
       <c r="O6" s="9"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="4">
+        <v>2008</v>
+      </c>
+      <c r="T6" s="19">
+        <v>2008</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="9"/>
+      <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
+      <c r="Z6" s="9"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="9"/>
+      <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
+      <c r="AF6" s="9"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="17"/>
-      <c r="AL6" s="38"/>
-      <c r="AM6" s="7"/>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="38">
+      <c r="AJ6" s="19">
+        <v>2010</v>
+      </c>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="38"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="38">
         <v>1999</v>
       </c>
-      <c r="AP6" s="4">
+      <c r="AS6" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ6" s="11">
+      <c r="AT6" s="11">
         <v>2011</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -3496,38 +3591,43 @@
       <c r="O7" s="9"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="9"/>
+      <c r="R7" s="51"/>
       <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
+      <c r="T7" s="9"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="9"/>
+      <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="Z7" s="9"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="9"/>
+      <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
+      <c r="AF7" s="9"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AL7" s="38"/>
-      <c r="AM7" s="7"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
-      <c r="AO7" s="38">
+      <c r="AO7" s="38"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="38">
         <v>1999</v>
       </c>
-      <c r="AP7" s="4">
+      <c r="AS7" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ7" s="19">
+      <c r="AT7" s="19">
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
@@ -3549,36 +3649,41 @@
       <c r="O8" s="9"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="9"/>
+      <c r="R8" s="51"/>
       <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="T8" s="9"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="19"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="9"/>
+      <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
+      <c r="AF8" s="9"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
-      <c r="AI8" s="17"/>
-      <c r="AJ8" s="2"/>
-      <c r="AL8" s="38"/>
-      <c r="AM8" s="7"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="17"/>
       <c r="AN8" s="2"/>
-      <c r="AO8" s="38">
+      <c r="AO8" s="38"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="38">
         <v>1999</v>
       </c>
-      <c r="AP8" s="2">
+      <c r="AS8" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ8" s="11"/>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT8" s="11"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -3600,40 +3705,53 @@
       <c r="O9" s="9"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="4">
+        <v>2002</v>
+      </c>
+      <c r="T9" s="19">
+        <v>2002</v>
+      </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="9"/>
+      <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
+      <c r="Z9" s="9"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="4">
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="4">
         <v>2011</v>
       </c>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="17"/>
-      <c r="AL9" s="38"/>
-      <c r="AM9" s="7"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="38">
+      <c r="AH9" s="4">
+        <v>2010</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>2010</v>
+      </c>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="17"/>
+      <c r="AO9" s="38"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="38">
         <v>1999</v>
       </c>
-      <c r="AP9" s="2">
+      <c r="AS9" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ9" s="9">
+      <c r="AT9" s="9">
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -3655,38 +3773,43 @@
       <c r="O10" s="9"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="9"/>
+      <c r="R10" s="51"/>
       <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="T10" s="9"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="19"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="9"/>
+      <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
+      <c r="AF10" s="9"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
-      <c r="AL10" s="38"/>
-      <c r="AM10" s="7"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
-      <c r="AO10" s="38">
+      <c r="AO10" s="38"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="38">
         <v>1999</v>
       </c>
-      <c r="AP10" s="2">
+      <c r="AS10" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ10" s="9">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT10" s="9">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
@@ -3714,38 +3837,43 @@
       <c r="O11" s="9"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="9"/>
+      <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
+      <c r="Z11" s="9"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="17"/>
-      <c r="AG11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="17"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AL11" s="38"/>
-      <c r="AM11" s="7"/>
+      <c r="AI11" s="17"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="17"/>
+      <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
-      <c r="AO11" s="38">
+      <c r="AO11" s="38"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="38">
         <v>1999</v>
       </c>
-      <c r="AP11" s="4">
+      <c r="AS11" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ11" s="9">
+      <c r="AT11" s="9">
         <v>2007</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
@@ -3764,40 +3892,47 @@
       <c r="O12" s="9"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="9"/>
+      <c r="R12" s="51"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
+      <c r="T12" s="9"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="4">
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="4">
         <v>2003</v>
       </c>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="9"/>
+      <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
+      <c r="AF12" s="9"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="17" t="s">
+      <c r="AJ12" s="19">
+        <v>2000</v>
+      </c>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL12" s="38"/>
-      <c r="AM12" s="7"/>
-      <c r="AN12" s="2"/>
-      <c r="AO12" s="38">
+      <c r="AO12" s="38"/>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="38">
         <v>1999</v>
       </c>
-      <c r="AP12" s="2">
+      <c r="AS12" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ12" s="11"/>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT12" s="11"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
@@ -3816,37 +3951,44 @@
       <c r="O13" s="9"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="T13" s="9"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="4">
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="4">
         <v>2005</v>
       </c>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="9"/>
+      <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
+      <c r="AF13" s="9"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="17"/>
-      <c r="AM13" s="19">
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="17"/>
+      <c r="AP13" s="19">
         <v>2001</v>
       </c>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="40">
-        <v>2012</v>
-      </c>
-      <c r="AP13" s="17"/>
-      <c r="AQ13" s="11"/>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="40">
+        <v>2012</v>
+      </c>
+      <c r="AS13" s="17"/>
+      <c r="AT13" s="11"/>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -3868,40 +4010,45 @@
       <c r="O14" s="9"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="17" t="s">
+      <c r="R14" s="51"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="9"/>
+      <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
+      <c r="Z14" s="9"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="9"/>
+      <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
+      <c r="AF14" s="9"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AL14" s="40">
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="40">
         <v>2008</v>
       </c>
-      <c r="AM14" s="9">
+      <c r="AP14" s="9">
         <v>1999</v>
       </c>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="38">
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="38">
         <v>1999</v>
       </c>
-      <c r="AP14" s="17"/>
-      <c r="AQ14" s="11"/>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS14" s="17"/>
+      <c r="AT14" s="11"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -3923,38 +4070,45 @@
       <c r="O15" s="9"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="19">
+        <v>2000</v>
+      </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="19"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="9"/>
+      <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
+      <c r="AF15" s="9"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AL15" s="38"/>
-      <c r="AM15" s="7"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
-      <c r="AO15" s="38">
+      <c r="AO15" s="38"/>
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="38">
         <v>1999</v>
       </c>
-      <c r="AP15" s="4">
+      <c r="AS15" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ15" s="19">
+      <c r="AT15" s="19">
         <v>2016</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
@@ -3963,20 +4117,20 @@
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="16"/>
-      <c r="S16" s="2"/>
-      <c r="V16" s="18"/>
-      <c r="AL16" s="38"/>
-      <c r="AM16" s="7"/>
-      <c r="AN16" s="2"/>
-      <c r="AO16" s="38">
+      <c r="U16" s="2"/>
+      <c r="X16" s="18"/>
+      <c r="AO16" s="38"/>
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="38">
         <v>1999</v>
       </c>
-      <c r="AP16" s="17">
+      <c r="AS16" s="17">
         <v>2016</v>
       </c>
-      <c r="AQ16" s="11"/>
-    </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT16" s="11"/>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
@@ -3998,38 +4152,47 @@
       <c r="O17" s="9"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="4">
+        <v>2000</v>
+      </c>
+      <c r="T17" s="19">
+        <v>2000</v>
+      </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="19"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="9"/>
+      <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
+      <c r="AF17" s="9"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="17"/>
-      <c r="AL17" s="38"/>
-      <c r="AM17" s="7"/>
-      <c r="AN17" s="2"/>
-      <c r="AO17" s="38">
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="17"/>
+      <c r="AO17" s="38"/>
+      <c r="AP17" s="7"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="38">
         <v>1999</v>
       </c>
-      <c r="AP17" s="2">
+      <c r="AS17" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ17" s="9">
+      <c r="AT17" s="9">
         <v>1999</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>21</v>
       </c>
@@ -4038,18 +4201,18 @@
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="16"/>
-      <c r="AL18" s="38"/>
-      <c r="AM18" s="7"/>
-      <c r="AN18" s="2"/>
-      <c r="AO18" s="38">
+      <c r="AO18" s="38"/>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="38">
         <v>1999</v>
       </c>
-      <c r="AP18" s="4">
+      <c r="AS18" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ18" s="11"/>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT18" s="11"/>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>17</v>
       </c>
@@ -4066,40 +4229,45 @@
       <c r="O19" s="9"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="9"/>
+      <c r="R19" s="51"/>
       <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
+      <c r="T19" s="9"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="19"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="9"/>
+      <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
+      <c r="AF19" s="9"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
-      <c r="AL19" s="40">
-        <v>2013</v>
-      </c>
-      <c r="AM19" s="19">
-        <v>2001</v>
-      </c>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="40">
-        <v>2012</v>
-      </c>
-      <c r="AP19" s="17">
+        <v>2013</v>
+      </c>
+      <c r="AP19" s="19">
+        <v>2001</v>
+      </c>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="40">
+        <v>2012</v>
+      </c>
+      <c r="AS19" s="17">
         <v>2008</v>
       </c>
-      <c r="AQ19" s="11"/>
-    </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT19" s="11"/>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>12</v>
       </c>
@@ -4116,38 +4284,49 @@
       <c r="O20" s="9"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="T20" s="19">
+        <v>2001</v>
+      </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="4">
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="4">
         <v>2003</v>
       </c>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="9"/>
+      <c r="AD20" s="2"/>
       <c r="AE20" s="2"/>
+      <c r="AF20" s="9"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
-      <c r="AL20" s="38"/>
-      <c r="AM20" s="7"/>
+      <c r="AJ20" s="19">
+        <v>2000</v>
+      </c>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
-      <c r="AO20" s="38">
+      <c r="AO20" s="38"/>
+      <c r="AP20" s="7"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="38">
         <v>1999</v>
       </c>
-      <c r="AP20" s="2">
+      <c r="AS20" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ20" s="11"/>
-    </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT20" s="11"/>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
@@ -4166,37 +4345,42 @@
       <c r="O21" s="9"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="9"/>
+      <c r="R21" s="51"/>
       <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
+      <c r="T21" s="9"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="9"/>
+      <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
+      <c r="Z21" s="9"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="9"/>
+      <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
+      <c r="AF21" s="9"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="2"/>
-      <c r="AM21" s="10">
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AP21" s="10">
         <v>36404</v>
       </c>
-      <c r="AN21" s="2"/>
-      <c r="AO21" s="40">
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="40">
         <v>2009</v>
       </c>
-      <c r="AP21" s="17">
+      <c r="AS21" s="17">
         <v>2008</v>
       </c>
-      <c r="AQ21" s="11"/>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT21" s="11"/>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -4219,36 +4403,41 @@
       <c r="O22" s="9"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="11"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="9"/>
+      <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
+      <c r="Z22" s="9"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="9"/>
+      <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
+      <c r="AF22" s="9"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
-      <c r="AI22" s="4">
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="4">
         <v>2004</v>
       </c>
-      <c r="AJ22" s="2"/>
-      <c r="AL22" s="38"/>
-      <c r="AM22" s="7"/>
       <c r="AN22" s="2"/>
-      <c r="AO22" s="40">
+      <c r="AO22" s="38"/>
+      <c r="AP22" s="7"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="40">
         <v>2008</v>
       </c>
-      <c r="AP22" s="17"/>
-      <c r="AQ22" s="11"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="11"/>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
@@ -4270,38 +4459,43 @@
       <c r="O23" s="9"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="9"/>
+      <c r="R23" s="51"/>
       <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
+      <c r="T23" s="9"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="17"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="4">
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="4">
         <v>2002</v>
       </c>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="9"/>
+      <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
+      <c r="AF23" s="9"/>
       <c r="AG23" s="2"/>
-      <c r="AH23" s="4">
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="4">
         <v>2000</v>
       </c>
-      <c r="AI23" s="2"/>
-      <c r="AJ23" s="17"/>
-      <c r="AL23" s="38"/>
-      <c r="AM23" s="7"/>
-      <c r="AN23" s="2"/>
-      <c r="AO23" s="40">
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="17"/>
+      <c r="AO23" s="38"/>
+      <c r="AP23" s="7"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="40">
         <v>2010</v>
       </c>
-      <c r="AP23" s="17"/>
-      <c r="AQ23" s="11"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS23" s="17"/>
+      <c r="AT23" s="11"/>
+    </row>
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
@@ -4323,40 +4517,45 @@
       <c r="O24" s="9"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="11" t="s">
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="17"/>
-      <c r="AG24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="17"/>
       <c r="AH24" s="17"/>
-      <c r="AI24" s="2"/>
-      <c r="AJ24" s="2"/>
-      <c r="AL24" s="40">
-        <v>2003</v>
-      </c>
-      <c r="AM24" s="19">
-        <v>2001</v>
-      </c>
+      <c r="AI24" s="17"/>
+      <c r="AJ24" s="11"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="17"/>
+      <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="40">
+        <v>2003</v>
+      </c>
+      <c r="AP24" s="19">
+        <v>2001</v>
+      </c>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="40">
         <v>2010</v>
       </c>
-      <c r="AP24" s="17"/>
-      <c r="AQ24" s="11"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS24" s="17"/>
+      <c r="AT24" s="11"/>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>13</v>
       </c>
@@ -4375,36 +4574,45 @@
       <c r="O25" s="9"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="4">
+        <v>2000</v>
+      </c>
+      <c r="T25" s="19">
+        <v>2000</v>
+      </c>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="19"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="9"/>
+      <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
+      <c r="AF25" s="9"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="17"/>
-      <c r="AL25" s="38"/>
-      <c r="AM25" s="7"/>
-      <c r="AN25" s="2"/>
-      <c r="AO25" s="38">
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="17"/>
+      <c r="AO25" s="38"/>
+      <c r="AP25" s="7"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="38">
         <v>1999</v>
       </c>
-      <c r="AP25" s="2">
+      <c r="AS25" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ25" s="11"/>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT25" s="11"/>
+    </row>
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>18</v>
       </c>
@@ -4421,38 +4629,45 @@
       <c r="O26" s="9"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="9"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="19"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="9"/>
+      <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
+      <c r="AF26" s="9"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="2"/>
-      <c r="AL26" s="40">
-        <v>2013</v>
-      </c>
-      <c r="AM26" s="19">
-        <v>2010</v>
-      </c>
+      <c r="AJ26" s="19">
+        <v>2000</v>
+      </c>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="40">
         <v>2013</v>
       </c>
-      <c r="AP26" s="17"/>
-      <c r="AQ26" s="11"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP26" s="19">
+        <v>2010</v>
+      </c>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="40">
+        <v>2013</v>
+      </c>
+      <c r="AS26" s="17"/>
+      <c r="AT26" s="11"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>69</v>
       </c>
@@ -4475,52 +4690,61 @@
       <c r="O27" s="11"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="4">
+        <v>2000</v>
+      </c>
+      <c r="T27" s="19">
+        <v>2000</v>
+      </c>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="9"/>
       <c r="AA27" s="17"/>
       <c r="AB27" s="17"/>
       <c r="AC27" s="17"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="2"/>
-      <c r="AG27" s="17"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="17"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="17" t="s">
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="17"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AJ27" s="2"/>
-      <c r="AL27" s="40">
-        <v>2007</v>
-      </c>
-      <c r="AM27" s="7"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="40">
+        <v>2007</v>
+      </c>
+      <c r="AP27" s="7"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="40">
         <v>2002</v>
       </c>
-      <c r="AP27" s="2">
+      <c r="AS27" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ27" s="9">
+      <c r="AT27" s="9">
         <v>2001</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AM28" s="7"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP28" s="7"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="AM29" s="7"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP29" s="7"/>
+    </row>
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>23</v>
       </c>
@@ -4546,60 +4770,65 @@
       <c r="O30" s="11"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="11"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="4">
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="4">
         <v>2014</v>
       </c>
-      <c r="W30" s="2"/>
-      <c r="X30" s="9"/>
       <c r="Y30" s="2"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="2"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="17"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="9"/>
       <c r="AG30" s="17"/>
       <c r="AH30" s="17"/>
-      <c r="AI30" s="17" t="s">
+      <c r="AI30" s="17"/>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="17"/>
+      <c r="AL30" s="17"/>
+      <c r="AM30" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="AJ30" s="17"/>
-      <c r="AL30" s="38"/>
-      <c r="AM30" s="7"/>
-      <c r="AN30" s="2"/>
-      <c r="AO30" s="40">
+      <c r="AN30" s="17"/>
+      <c r="AO30" s="38"/>
+      <c r="AP30" s="7"/>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="40">
         <v>2011</v>
       </c>
-      <c r="AP30" s="4">
+      <c r="AS30" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ30" s="9">
+      <c r="AT30" s="9">
         <v>2011</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="2">
         <v>2012</v>
       </c>
-      <c r="AL31" s="38"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="2"/>
-      <c r="AO31" s="40">
+      <c r="AO31" s="38"/>
+      <c r="AP31" s="7"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="40">
         <v>2000</v>
       </c>
-      <c r="AP31" s="2">
+      <c r="AS31" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ31" s="11"/>
-    </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT31" s="11"/>
+    </row>
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
@@ -4629,46 +4858,51 @@
       <c r="O32" s="11"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="4">
+      <c r="R32" s="51"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="4">
         <v>2011</v>
       </c>
-      <c r="V32" s="4">
+      <c r="X32" s="4">
         <v>2011</v>
       </c>
-      <c r="W32" s="2"/>
-      <c r="X32" s="9"/>
       <c r="Y32" s="2"/>
-      <c r="Z32" s="2"/>
+      <c r="Z32" s="9"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="9"/>
+      <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
-      <c r="AG32" s="4">
-        <v>2012</v>
-      </c>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17" t="s">
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="4">
+        <v>2012</v>
+      </c>
+      <c r="AL32" s="17"/>
+      <c r="AM32" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="AJ32" s="17"/>
-      <c r="AL32" s="38"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="2"/>
-      <c r="AO32" s="40">
-        <v>2012</v>
-      </c>
-      <c r="AP32" s="2">
+      <c r="AN32" s="17"/>
+      <c r="AO32" s="38"/>
+      <c r="AP32" s="7"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="40">
+        <v>2012</v>
+      </c>
+      <c r="AS32" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ32" s="9">
+      <c r="AT32" s="9">
         <v>2005</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>26</v>
       </c>
@@ -4687,44 +4921,51 @@
       <c r="O33" s="9"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="13">
+      <c r="R33" s="51"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="13">
         <v>36281</v>
       </c>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="4">
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="4">
         <v>2000</v>
       </c>
-      <c r="W33" s="2"/>
-      <c r="X33" s="9"/>
       <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
+      <c r="Z33" s="9"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="9"/>
+      <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
+      <c r="AF33" s="9"/>
       <c r="AG33" s="2"/>
-      <c r="AH33" s="17"/>
+      <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
-      <c r="AJ33" s="17" t="s">
+      <c r="AJ33" s="19">
+        <v>2000</v>
+      </c>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="17"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL33" s="38"/>
-      <c r="AM33" s="7"/>
-      <c r="AN33" s="2"/>
-      <c r="AO33" s="40">
+      <c r="AO33" s="38"/>
+      <c r="AP33" s="7"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="40">
         <v>2000</v>
       </c>
-      <c r="AP33" s="2">
+      <c r="AS33" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ33" s="9">
+      <c r="AT33" s="9">
         <v>2007</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>98</v>
       </c>
@@ -4750,38 +4991,43 @@
       <c r="O34" s="11"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="17"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="9"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
+      <c r="Z34" s="9"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="9"/>
+      <c r="AD34" s="2"/>
       <c r="AE34" s="2"/>
+      <c r="AF34" s="9"/>
       <c r="AG34" s="2"/>
-      <c r="AH34" s="17"/>
+      <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="17"/>
-      <c r="AL34" s="38"/>
-      <c r="AM34" s="7"/>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="40">
+      <c r="AJ34" s="9"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="17"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="38"/>
+      <c r="AP34" s="7"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="40">
         <v>2000</v>
       </c>
-      <c r="AP34" s="2">
+      <c r="AS34" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ34" s="9">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT34" s="9">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>28</v>
       </c>
@@ -4810,46 +5056,51 @@
       <c r="O35" s="11"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="4">
+      <c r="R35" s="51"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="4">
         <v>2000</v>
       </c>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
       <c r="V35" s="17"/>
       <c r="W35" s="17"/>
-      <c r="X35" s="11"/>
-      <c r="Y35" s="4">
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="4">
         <v>2006</v>
       </c>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="4">
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
+      <c r="AD35" s="4">
         <v>2016</v>
       </c>
-      <c r="AC35" s="4">
+      <c r="AE35" s="4">
         <v>2014</v>
       </c>
-      <c r="AD35" s="19">
+      <c r="AF35" s="19">
         <v>2016</v>
       </c>
-      <c r="AE35" s="17"/>
       <c r="AG35" s="17"/>
       <c r="AH35" s="17"/>
       <c r="AI35" s="17"/>
-      <c r="AJ35" s="17"/>
-      <c r="AL35" s="38"/>
-      <c r="AM35" s="7"/>
-      <c r="AN35" s="2"/>
-      <c r="AO35" s="39">
+      <c r="AJ35" s="11"/>
+      <c r="AK35" s="17"/>
+      <c r="AL35" s="17"/>
+      <c r="AM35" s="17"/>
+      <c r="AN35" s="17"/>
+      <c r="AO35" s="38"/>
+      <c r="AP35" s="7"/>
+      <c r="AQ35" s="2"/>
+      <c r="AR35" s="39">
         <v>2015</v>
       </c>
-      <c r="AP35" s="17">
+      <c r="AS35" s="17">
         <v>2019</v>
       </c>
-      <c r="AQ35" s="11"/>
-    </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT35" s="11"/>
+    </row>
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>29</v>
       </c>
@@ -4870,37 +5121,42 @@
       <c r="O36" s="11"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="11"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="9"/>
+      <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
+      <c r="Z36" s="9"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="9"/>
-      <c r="AE36" s="17"/>
-      <c r="AG36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="9"/>
+      <c r="AG36" s="17"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="17"/>
-      <c r="AJ36" s="2"/>
-      <c r="AM36" s="9">
+      <c r="AJ36" s="9"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="17"/>
+      <c r="AN36" s="2"/>
+      <c r="AP36" s="9">
         <v>1999</v>
       </c>
-      <c r="AN36" s="2"/>
-      <c r="AO36" s="40">
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="40">
         <v>2003</v>
       </c>
-      <c r="AP36" s="4">
+      <c r="AS36" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ36" s="11"/>
-    </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT36" s="11"/>
+    </row>
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>30</v>
       </c>
@@ -4923,61 +5179,68 @@
       <c r="O37" s="9"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="2"/>
-      <c r="V37" s="4">
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="4">
         <v>2001</v>
       </c>
-      <c r="W37" s="2"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="4">
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="9"/>
+      <c r="AA37" s="4">
         <v>2006</v>
       </c>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-      <c r="AD37" s="9"/>
-      <c r="AE37" s="17"/>
-      <c r="AG37" s="2"/>
-      <c r="AH37" s="17"/>
-      <c r="AI37" s="17"/>
-      <c r="AJ37" s="17"/>
-      <c r="AL37" s="38"/>
-      <c r="AM37" s="7"/>
-      <c r="AN37" s="2"/>
-      <c r="AO37" s="38">
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="9"/>
+      <c r="AG37" s="17"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ37" s="9"/>
+      <c r="AK37" s="2"/>
+      <c r="AL37" s="17"/>
+      <c r="AM37" s="17"/>
+      <c r="AN37" s="17"/>
+      <c r="AO37" s="38"/>
+      <c r="AP37" s="7"/>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="38">
         <v>1999</v>
       </c>
-      <c r="AP37" s="4">
+      <c r="AS37" s="4">
         <v>2010</v>
       </c>
-      <c r="AQ37" s="11"/>
-    </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT37" s="11"/>
+    </row>
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="11">
         <v>2016</v>
       </c>
-      <c r="S38" s="4">
+      <c r="U38" s="4">
         <v>2000</v>
       </c>
-      <c r="AL38" s="38"/>
-      <c r="AM38" s="7"/>
-      <c r="AN38" s="2"/>
-      <c r="AO38" s="40">
+      <c r="AO38" s="38"/>
+      <c r="AP38" s="7"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="40">
         <v>2008</v>
       </c>
-      <c r="AP38" s="4">
+      <c r="AS38" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ38" s="11"/>
-    </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT38" s="11"/>
+    </row>
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
@@ -5000,113 +5263,118 @@
       <c r="O39" s="11"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="4">
+      <c r="R39" s="51"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="4">
         <v>2005</v>
       </c>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="4">
-        <v>2012</v>
-      </c>
+      <c r="V39" s="2"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="4">
+      <c r="X39" s="4">
+        <v>2012</v>
+      </c>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="9"/>
+      <c r="AA39" s="4">
         <v>2004</v>
       </c>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="9"/>
-      <c r="AE39" s="17"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="17"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="17"/>
+      <c r="AH39" s="2"/>
       <c r="AI39" s="17"/>
-      <c r="AJ39" s="17"/>
-      <c r="AL39" s="38"/>
-      <c r="AM39" s="7"/>
-      <c r="AN39" s="2"/>
-      <c r="AO39" s="40">
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="17"/>
+      <c r="AM39" s="17"/>
+      <c r="AN39" s="17"/>
+      <c r="AO39" s="38"/>
+      <c r="AP39" s="7"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="40">
         <v>2010</v>
       </c>
-      <c r="AP39" s="4">
+      <c r="AS39" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ39" s="11"/>
-    </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT39" s="11"/>
+    </row>
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="11">
         <v>2015</v>
       </c>
-      <c r="S40" s="2"/>
-      <c r="AL40" s="38"/>
-      <c r="AM40" s="7"/>
-      <c r="AN40" s="2"/>
-      <c r="AO40" s="38">
+      <c r="U40" s="2"/>
+      <c r="AO40" s="38"/>
+      <c r="AP40" s="7"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="38">
         <v>1999</v>
       </c>
-      <c r="AP40" s="4">
+      <c r="AS40" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ40" s="11"/>
-    </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT40" s="11"/>
+    </row>
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="11">
         <v>2012</v>
       </c>
-      <c r="AM41" s="7">
+      <c r="AP41" s="7">
         <v>2004</v>
       </c>
-      <c r="AN41" s="13">
+      <c r="AQ41" s="13">
         <v>36192</v>
       </c>
-      <c r="AO41" s="39">
+      <c r="AR41" s="39">
         <v>2014</v>
       </c>
-      <c r="AP41" s="17"/>
-      <c r="AQ41" s="11"/>
-    </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS41" s="17"/>
+      <c r="AT41" s="11"/>
+    </row>
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="11">
         <v>2017</v>
       </c>
-      <c r="AM42" s="7">
+      <c r="AP42" s="7">
         <v>2001</v>
       </c>
-      <c r="AN42" s="2"/>
-      <c r="AO42" s="39">
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="39">
         <v>2014</v>
       </c>
-      <c r="AP42" s="17"/>
-      <c r="AQ42" s="11"/>
-    </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS42" s="17"/>
+      <c r="AT42" s="11"/>
+    </row>
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="11"/>
       <c r="E43" s="8"/>
-      <c r="AM43" s="7">
+      <c r="AP43" s="7">
         <v>2010</v>
       </c>
-      <c r="AN43" s="2"/>
-      <c r="AO43" s="39">
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="39">
         <v>2020</v>
       </c>
-      <c r="AP43" s="17"/>
-      <c r="AQ43" s="11"/>
-    </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS43" s="17"/>
+      <c r="AT43" s="11"/>
+    </row>
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>48</v>
       </c>
@@ -5134,65 +5402,70 @@
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="4">
+      <c r="R44" s="51"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="4">
         <v>2002</v>
       </c>
-      <c r="T44" s="2"/>
-      <c r="U44" s="17" t="s">
+      <c r="V44" s="2"/>
+      <c r="W44" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="V44" s="17"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="9"/>
+      <c r="X44" s="17"/>
       <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
+      <c r="Z44" s="9"/>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-      <c r="AD44" s="9"/>
+      <c r="AD44" s="2"/>
       <c r="AE44" s="2"/>
+      <c r="AF44" s="9"/>
       <c r="AG44" s="2"/>
-      <c r="AH44" s="4">
+      <c r="AH44" s="2"/>
+      <c r="AI44" s="2"/>
+      <c r="AJ44" s="11"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="4">
         <v>2010</v>
       </c>
-      <c r="AI44" s="2"/>
-      <c r="AJ44" s="17" t="s">
+      <c r="AM44" s="2"/>
+      <c r="AN44" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AL44" s="38"/>
-      <c r="AM44" s="7"/>
-      <c r="AN44" s="2"/>
-      <c r="AO44" s="40">
+      <c r="AO44" s="38"/>
+      <c r="AP44" s="7"/>
+      <c r="AQ44" s="2"/>
+      <c r="AR44" s="40">
         <v>2008</v>
       </c>
-      <c r="AP44" s="2">
+      <c r="AS44" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ44" s="9">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT44" s="9">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>36</v>
       </c>
       <c r="C45" s="11">
         <v>2018</v>
       </c>
-      <c r="S45" s="2"/>
-      <c r="AL45" s="38"/>
-      <c r="AM45" s="7"/>
-      <c r="AN45" s="2"/>
-      <c r="AO45" s="40">
+      <c r="U45" s="2"/>
+      <c r="AO45" s="38"/>
+      <c r="AP45" s="7"/>
+      <c r="AQ45" s="2"/>
+      <c r="AR45" s="40">
         <v>2010</v>
       </c>
-      <c r="AP45" s="4">
+      <c r="AS45" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ45" s="11"/>
-    </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT45" s="11"/>
+    </row>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>37</v>
       </c>
@@ -5213,47 +5486,54 @@
       <c r="O46" s="9"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
+      <c r="R46" s="51"/>
+      <c r="S46" s="4">
+        <v>2000</v>
+      </c>
+      <c r="T46" s="9"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="4">
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="4">
         <v>2001</v>
       </c>
-      <c r="W46" s="2"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="4">
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="9"/>
+      <c r="AA46" s="4">
         <v>2004</v>
       </c>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
-      <c r="AD46" s="9"/>
+      <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
+      <c r="AF46" s="9"/>
       <c r="AG46" s="2"/>
-      <c r="AH46" s="17" t="s">
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="2"/>
+      <c r="AJ46" s="9"/>
+      <c r="AK46" s="2"/>
+      <c r="AL46" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AI46" s="4">
+      <c r="AM46" s="4">
         <v>2003</v>
       </c>
-      <c r="AJ46" s="4">
+      <c r="AN46" s="4">
         <v>2000</v>
       </c>
-      <c r="AM46" s="9">
+      <c r="AP46" s="9">
         <v>1999</v>
       </c>
-      <c r="AN46" s="2"/>
-      <c r="AO46" s="40">
+      <c r="AQ46" s="2"/>
+      <c r="AR46" s="40">
         <v>2010</v>
       </c>
-      <c r="AP46" s="4">
+      <c r="AS46" s="4">
         <v>2011</v>
       </c>
-      <c r="AQ46" s="11"/>
-    </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT46" s="11"/>
+    </row>
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>38</v>
       </c>
@@ -5274,43 +5554,52 @@
       <c r="O47" s="9"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="4">
+        <v>2009</v>
+      </c>
+      <c r="T47" s="19">
+        <v>2003</v>
+      </c>
       <c r="U47" s="2"/>
-      <c r="V47" s="4">
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="4">
         <v>2004</v>
       </c>
-      <c r="W47" s="2"/>
-      <c r="X47" s="9"/>
-      <c r="Y47" s="4">
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="9"/>
+      <c r="AA47" s="4">
         <v>2003</v>
       </c>
-      <c r="Z47" s="2"/>
-      <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="9"/>
+      <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
+      <c r="AF47" s="9"/>
       <c r="AG47" s="2"/>
-      <c r="AH47" s="17" t="s">
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2"/>
+      <c r="AJ47" s="9"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="AI47" s="17"/>
-      <c r="AJ47" s="2"/>
-      <c r="AM47" s="9">
+      <c r="AM47" s="17"/>
+      <c r="AN47" s="2"/>
+      <c r="AP47" s="9">
         <v>1999</v>
       </c>
-      <c r="AN47" s="4">
+      <c r="AQ47" s="4">
         <v>2002</v>
       </c>
-      <c r="AO47" s="40">
+      <c r="AR47" s="40">
         <v>2007</v>
       </c>
-      <c r="AP47" s="17"/>
-      <c r="AQ47" s="11"/>
-    </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS47" s="17"/>
+      <c r="AT47" s="11"/>
+    </row>
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>39</v>
       </c>
@@ -5329,60 +5618,65 @@
       <c r="O48" s="9"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="4">
+      <c r="R48" s="51"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="4">
         <v>2001</v>
       </c>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-      <c r="W48" s="17"/>
-      <c r="X48" s="11"/>
-      <c r="Y48" s="4">
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="4">
         <v>2002</v>
       </c>
-      <c r="Z48" s="2"/>
-      <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
-      <c r="AD48" s="9"/>
+      <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
+      <c r="AF48" s="9"/>
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
-      <c r="AJ48" s="2"/>
-      <c r="AL48" s="38"/>
-      <c r="AM48" s="7"/>
-      <c r="AN48" s="4">
+      <c r="AJ48" s="11"/>
+      <c r="AK48" s="2"/>
+      <c r="AL48" s="2"/>
+      <c r="AM48" s="2"/>
+      <c r="AN48" s="2"/>
+      <c r="AO48" s="38"/>
+      <c r="AP48" s="7"/>
+      <c r="AQ48" s="4">
         <v>2001</v>
       </c>
-      <c r="AO48" s="40">
+      <c r="AR48" s="40">
         <v>2011</v>
       </c>
-      <c r="AP48" s="2">
+      <c r="AS48" s="2">
         <v>2008</v>
       </c>
-      <c r="AQ48" s="11"/>
-    </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT48" s="11"/>
+    </row>
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="S49" s="4">
+      <c r="U49" s="4">
         <v>2003</v>
       </c>
-      <c r="AM49" s="7">
+      <c r="AP49" s="7">
         <v>2011</v>
       </c>
-      <c r="AN49" s="2"/>
-      <c r="AO49" s="40">
+      <c r="AQ49" s="2"/>
+      <c r="AR49" s="40">
         <v>2009</v>
       </c>
-      <c r="AP49" s="17"/>
-      <c r="AQ49" s="11"/>
-    </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS49" s="17"/>
+      <c r="AT49" s="11"/>
+    </row>
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -5401,35 +5695,40 @@
       <c r="O50" s="9"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="9"/>
+      <c r="R50" s="51"/>
       <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
+      <c r="T50" s="9"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
-      <c r="X50" s="9"/>
+      <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
-      <c r="Z50" s="2"/>
+      <c r="Z50" s="9"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
       <c r="AC50" s="2"/>
-      <c r="AD50" s="9"/>
+      <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
+      <c r="AF50" s="9"/>
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
-      <c r="AI50" s="4">
+      <c r="AI50" s="2"/>
+      <c r="AJ50" s="9"/>
+      <c r="AK50" s="2"/>
+      <c r="AL50" s="2"/>
+      <c r="AM50" s="4">
         <v>2003</v>
       </c>
-      <c r="AJ50" s="2"/>
-      <c r="AM50" s="19">
+      <c r="AN50" s="2"/>
+      <c r="AP50" s="19">
         <v>2001</v>
       </c>
-      <c r="AN50" s="2"/>
-      <c r="AO50" s="39"/>
-      <c r="AP50" s="17"/>
-      <c r="AQ50" s="11"/>
-    </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AQ50" s="2"/>
+      <c r="AR50" s="39"/>
+      <c r="AS50" s="17"/>
+      <c r="AT50" s="11"/>
+    </row>
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>47</v>
       </c>
@@ -5448,58 +5747,63 @@
       <c r="O51" s="9"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
-      <c r="R51" s="9"/>
+      <c r="R51" s="51"/>
       <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
+      <c r="T51" s="9"/>
       <c r="U51" s="2"/>
-      <c r="V51" s="4">
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="4">
         <v>2000</v>
       </c>
-      <c r="W51" s="17" t="s">
+      <c r="Y51" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="2"/>
-      <c r="Z51" s="2"/>
+      <c r="Z51" s="9"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
       <c r="AC51" s="2"/>
-      <c r="AD51" s="9"/>
+      <c r="AD51" s="2"/>
       <c r="AE51" s="2"/>
+      <c r="AF51" s="9"/>
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
-      <c r="AI51" s="4">
+      <c r="AI51" s="2"/>
+      <c r="AJ51" s="9"/>
+      <c r="AK51" s="2"/>
+      <c r="AL51" s="2"/>
+      <c r="AM51" s="4">
         <v>2003</v>
       </c>
-      <c r="AJ51" s="17"/>
-      <c r="AM51" s="9">
+      <c r="AN51" s="17"/>
+      <c r="AP51" s="9">
         <v>1999</v>
       </c>
-      <c r="AN51" s="2"/>
-      <c r="AO51" s="39"/>
-      <c r="AP51" s="17">
+      <c r="AQ51" s="2"/>
+      <c r="AR51" s="39"/>
+      <c r="AS51" s="17">
         <v>2018</v>
       </c>
-      <c r="AQ51" s="11"/>
-    </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AT51" s="11"/>
+    </row>
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>42</v>
       </c>
       <c r="C52" s="11">
         <v>2013</v>
       </c>
-      <c r="AM52" s="7">
+      <c r="AP52" s="7">
         <v>1999</v>
       </c>
-      <c r="AN52" s="2"/>
-      <c r="AO52" s="40">
+      <c r="AQ52" s="2"/>
+      <c r="AR52" s="40">
         <v>2010</v>
       </c>
-      <c r="AP52" s="17"/>
-      <c r="AQ52" s="11"/>
-    </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS52" s="17"/>
+      <c r="AT52" s="11"/>
+    </row>
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>43</v>
       </c>
@@ -5530,58 +5834,63 @@
       </c>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
+      <c r="R53" s="51"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="9"/>
       <c r="U53" s="2"/>
-      <c r="V53" s="4">
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="4">
         <v>2003</v>
       </c>
-      <c r="W53" s="17"/>
-      <c r="X53" s="11"/>
-      <c r="Y53" s="4">
+      <c r="Y53" s="17"/>
+      <c r="Z53" s="11"/>
+      <c r="AA53" s="4">
         <v>2005</v>
       </c>
-      <c r="Z53" s="4">
+      <c r="AB53" s="4">
         <v>2006</v>
       </c>
-      <c r="AA53" s="4">
+      <c r="AC53" s="4">
         <v>2006</v>
       </c>
-      <c r="AB53" s="2"/>
-      <c r="AC53" s="2"/>
-      <c r="AD53" s="9"/>
+      <c r="AD53" s="2"/>
       <c r="AE53" s="2"/>
-      <c r="AG53" s="4">
+      <c r="AF53" s="9"/>
+      <c r="AG53" s="2"/>
+      <c r="AH53" s="2"/>
+      <c r="AI53" s="2"/>
+      <c r="AJ53" s="11"/>
+      <c r="AK53" s="4">
         <v>2006</v>
       </c>
-      <c r="AH53" s="17" t="s">
+      <c r="AL53" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="AI53" s="17" t="s">
+      <c r="AM53" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="AJ53" s="2"/>
-      <c r="AM53" s="19">
+      <c r="AN53" s="2"/>
+      <c r="AP53" s="19">
         <v>2000</v>
       </c>
-      <c r="AN53" s="2"/>
-      <c r="AO53" s="40">
+      <c r="AQ53" s="2"/>
+      <c r="AR53" s="40">
         <v>2009</v>
       </c>
-      <c r="AP53" s="17"/>
-      <c r="AQ53" s="11"/>
-    </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AM54" s="7"/>
-    </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS53" s="17"/>
+      <c r="AT53" s="11"/>
+    </row>
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP54" s="7"/>
+    </row>
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="AM55" s="7"/>
-    </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP55" s="7"/>
+    </row>
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>44</v>
       </c>
@@ -5606,42 +5915,47 @@
       <c r="Q56" s="4">
         <v>2017</v>
       </c>
-      <c r="R56" s="11"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="17"/>
-      <c r="U56" s="17"/>
+      <c r="R56" s="52"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="2"/>
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
-      <c r="X56" s="11"/>
-      <c r="Y56" s="4">
+      <c r="X56" s="17"/>
+      <c r="Y56" s="17"/>
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="4">
         <v>2006</v>
       </c>
-      <c r="Z56" s="4">
+      <c r="AB56" s="4">
         <v>2005</v>
       </c>
-      <c r="AA56" s="4">
+      <c r="AC56" s="4">
         <v>2005</v>
       </c>
-      <c r="AB56" s="2"/>
-      <c r="AC56" s="2"/>
-      <c r="AD56" s="9"/>
-      <c r="AE56" s="17"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="2"/>
+      <c r="AF56" s="9"/>
       <c r="AG56" s="17"/>
       <c r="AH56" s="17"/>
       <c r="AI56" s="17"/>
-      <c r="AJ56" s="17"/>
-      <c r="AL56" s="38"/>
-      <c r="AM56" s="7"/>
-      <c r="AN56" s="4">
+      <c r="AJ56" s="11"/>
+      <c r="AK56" s="17"/>
+      <c r="AL56" s="17"/>
+      <c r="AM56" s="17"/>
+      <c r="AN56" s="17"/>
+      <c r="AO56" s="38"/>
+      <c r="AP56" s="7"/>
+      <c r="AQ56" s="4">
         <v>2000</v>
       </c>
-      <c r="AO56" s="40">
+      <c r="AR56" s="40">
         <v>2011</v>
       </c>
-      <c r="AP56" s="17"/>
-      <c r="AQ56" s="11"/>
-    </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AS56" s="17"/>
+      <c r="AT56" s="11"/>
+    </row>
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>45</v>
       </c>
@@ -5679,63 +5993,72 @@
       <c r="Q57" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="R57" s="11" t="s">
+      <c r="R57" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="S57" s="2"/>
-      <c r="T57" s="17" t="s">
+      <c r="S57" s="17"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="U57" s="17" t="s">
+      <c r="W57" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="V57" s="17" t="s">
+      <c r="X57" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="W57" s="2"/>
-      <c r="X57" s="9"/>
-      <c r="Y57" s="17" t="s">
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="Z57" s="17" t="s">
+      <c r="AB57" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AA57" s="17" t="s">
+      <c r="AC57" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="2"/>
-      <c r="AD57" s="9"/>
-      <c r="AE57" s="17" t="s">
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+      <c r="AF57" s="9"/>
+      <c r="AG57" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="AG57" s="17" t="s">
+      <c r="AH57" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI57" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ57" s="11"/>
+      <c r="AK57" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AH57" s="17"/>
-      <c r="AI57" s="17"/>
-      <c r="AJ57" s="17"/>
-      <c r="AL57" s="40">
+      <c r="AL57" s="17"/>
+      <c r="AM57" s="17"/>
+      <c r="AN57" s="17"/>
+      <c r="AO57" s="40">
         <v>2013</v>
       </c>
-      <c r="AM57" s="9">
+      <c r="AP57" s="9">
         <v>1999</v>
       </c>
-      <c r="AN57" s="2"/>
-      <c r="AO57" s="40">
+      <c r="AQ57" s="2"/>
+      <c r="AR57" s="40">
         <v>2010</v>
       </c>
-      <c r="AP57" s="17" t="s">
+      <c r="AS57" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="AQ57" s="11" t="s">
+      <c r="AT57" s="11" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AM58" s="7"/>
-    </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP58" s="7"/>
+    </row>
+    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B59" s="44" t="s">
         <v>67</v>
       </c>
@@ -5744,22 +6067,22 @@
         <v>68</v>
       </c>
       <c r="E59" s="45"/>
-      <c r="AM59" s="7"/>
+      <c r="AP59" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AR1:AS1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AD1"/>
-    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AF1"/>
+    <mergeCell ref="AK1:AN1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="AG1:AJ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more indicators and rankings
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8229CD-9FBC-4D0C-97B8-85EF1E48D17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F68588D-E7EC-49F5-B6B7-E57C3B0B6026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="411">
   <si>
     <t>United States</t>
   </si>
@@ -1255,6 +1255,24 @@
   </si>
   <si>
     <t>Probably</t>
+  </si>
+  <si>
+    <t>Total stock</t>
+  </si>
+  <si>
+    <t>market cap</t>
+  </si>
+  <si>
+    <t>(% in 2020 by WB)</t>
+  </si>
+  <si>
+    <t>% of global GDP</t>
+  </si>
+  <si>
+    <t>MSCI ACWI</t>
+  </si>
+  <si>
+    <t>(% in 03/2023)</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1448,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1486,6 +1504,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1825,7 +1847,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,8 +2664,6 @@
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -2713,6 +2733,7 @@
         <v>2008</v>
       </c>
       <c r="M31" s="2"/>
+      <c r="O31" s="2"/>
       <c r="P31" s="2">
         <v>2012</v>
       </c>
@@ -2852,9 +2873,7 @@
         <v>2000</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="4">
-        <v>2011</v>
-      </c>
+      <c r="O35" s="4"/>
       <c r="P35" s="2">
         <v>2012</v>
       </c>
@@ -3396,9 +3415,7 @@
       <c r="N57" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="O57" s="16" t="s">
-        <v>95</v>
-      </c>
+      <c r="O57" s="2"/>
       <c r="P57" s="2">
         <v>2012</v>
       </c>
@@ -3410,10 +3427,10 @@
       <c r="P59" s="22"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="47" t="s">
         <v>403</v>
       </c>
-      <c r="C61" s="46"/>
+      <c r="C61" s="48"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3458,9 +3475,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B703FA39-2A94-42E5-99E2-495679D72086}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3469,10 +3488,12 @@
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="11" t="s">
         <v>58</v>
@@ -3487,10 +3508,16 @@
         <v>56</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -3503,10 +3530,16 @@
         <v>397</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -3515,8 +3548,11 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="45" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3533,8 +3569,14 @@
       <c r="F4" s="44">
         <v>59.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="44">
+        <v>40.43</v>
+      </c>
+      <c r="H4" s="44">
+        <v>25.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3551,8 +3593,14 @@
       <c r="F5" s="44">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="44">
+        <v>6.07</v>
+      </c>
+      <c r="H5" s="44">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3569,8 +3617,14 @@
       <c r="F6" s="44">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="44">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H6" s="44">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3587,8 +3641,14 @@
       <c r="F7" s="44">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="44">
+        <v>2.39</v>
+      </c>
+      <c r="H7" s="44">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -3605,8 +3665,14 @@
       <c r="F8" s="44">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="44">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H8" s="44">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -3622,8 +3688,14 @@
       <c r="F9" s="44">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="44">
+        <v>1.81</v>
+      </c>
+      <c r="H9" s="44">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -3640,8 +3712,14 @@
       <c r="F10" s="44">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="44">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H10" s="44">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -3658,8 +3736,14 @@
       <c r="F11" s="44">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="44">
+        <v>1.56</v>
+      </c>
+      <c r="H11" s="44">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3675,8 +3759,14 @@
       <c r="F12" s="44">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="44">
+        <v>1.44</v>
+      </c>
+      <c r="H12" s="44">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>14</v>
       </c>
@@ -3692,8 +3782,14 @@
       <c r="F13" s="44">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="44">
+        <v>0.61</v>
+      </c>
+      <c r="H13" s="44">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -3709,8 +3805,14 @@
       <c r="F14" s="44">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="44">
+        <v>0.83</v>
+      </c>
+      <c r="H14" s="44">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -3727,8 +3829,14 @@
       <c r="F15" s="44">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="44">
+        <v>0.82</v>
+      </c>
+      <c r="H15" s="44">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
@@ -3744,8 +3852,14 @@
       <c r="F16" s="44">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="44">
+        <v>5.54</v>
+      </c>
+      <c r="H16" s="44">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3762,8 +3876,14 @@
       <c r="F17" s="44">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="44">
+        <v>0.68</v>
+      </c>
+      <c r="H17" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
@@ -3779,8 +3899,14 @@
       <c r="F18" s="44">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="44">
+        <v>0.59</v>
+      </c>
+      <c r="H18" s="44">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>17</v>
       </c>
@@ -3796,8 +3922,14 @@
       <c r="F19" s="44">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="H19" s="44">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -3813,8 +3945,14 @@
       <c r="F20" s="44">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H20" s="44">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -3830,8 +3968,14 @@
       <c r="F21" s="44">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="44">
+        <v>0.27</v>
+      </c>
+      <c r="H21" s="44">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -3847,8 +3991,14 @@
       <c r="F22" s="44">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="44">
+        <v>0.24</v>
+      </c>
+      <c r="H22" s="44">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -3864,8 +4014,14 @@
       <c r="F23" s="44">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
@@ -3881,8 +4037,14 @@
       <c r="F24" s="44">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="44">
+        <v>0.12</v>
+      </c>
+      <c r="H24" s="44">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -3898,8 +4060,14 @@
       <c r="F25" s="44">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="44">
+        <v>0.12</v>
+      </c>
+      <c r="H25" s="44">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>18</v>
       </c>
@@ -3915,31 +4083,50 @@
       <c r="F26" s="44">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="44">
+        <v>0.06</v>
+      </c>
+      <c r="H26" s="44">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
       <c r="F27" s="44">
-        <v>8.48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <f>F8+F10+F12+F15+F17+F19+F20+F23+F25+F26+F48</f>
+        <v>8.4799999999999969</v>
+      </c>
+      <c r="G27" s="44">
+        <f>G8+G10+G12+G15+G17+G19+G20+G23+G25+G26+G48</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H27" s="44">
+        <f>H8+H10+H12+H15+H17+H19+H20+H23+H25+H26+H48</f>
+        <v>13.530000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="F28" s="44"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="36"/>
       <c r="D29" s="36"/>
       <c r="F29" s="44"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3956,8 +4143,14 @@
       <c r="F30" s="44">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="44">
+        <v>11.95</v>
+      </c>
+      <c r="H30" s="44">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>24</v>
       </c>
@@ -3967,8 +4160,14 @@
       <c r="F31" s="44">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="44">
+        <v>1.82</v>
+      </c>
+      <c r="H31" s="44">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3985,8 +4184,14 @@
       <c r="F32" s="44">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="44">
+        <v>3.27</v>
+      </c>
+      <c r="H32" s="44">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -4003,8 +4208,14 @@
       <c r="F33" s="44">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="44">
+        <v>1.97</v>
+      </c>
+      <c r="H33" s="44">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>98</v>
       </c>
@@ -4021,8 +4232,14 @@
       <c r="F34" s="44">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="44">
+        <v>0.89</v>
+      </c>
+      <c r="H34" s="44">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
@@ -4039,8 +4256,14 @@
       <c r="F35" s="44">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="44">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H35" s="44">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
@@ -4057,8 +4280,14 @@
       <c r="F36" s="44">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="44">
+        <v>0.95</v>
+      </c>
+      <c r="H36" s="44">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -4075,8 +4304,14 @@
       <c r="F37" s="44">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="44">
+        <v>0.36</v>
+      </c>
+      <c r="H37" s="44">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>31</v>
       </c>
@@ -4092,8 +4327,14 @@
       <c r="F38" s="44">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="44">
+        <v>0.49</v>
+      </c>
+      <c r="H38" s="44">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
@@ -4110,8 +4351,14 @@
       <c r="F39" s="44">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="44">
+        <v>0.45</v>
+      </c>
+      <c r="H39" s="44">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>33</v>
       </c>
@@ -4127,8 +4374,14 @@
       <c r="F40" s="44">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="44">
+        <v>0.39</v>
+      </c>
+      <c r="H40" s="44">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>49</v>
       </c>
@@ -4144,8 +4397,14 @@
       <c r="F41" s="44">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="44">
+        <v>0.27</v>
+      </c>
+      <c r="H41" s="44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>34</v>
       </c>
@@ -4161,8 +4420,14 @@
       <c r="F42" s="44">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="H42" s="44">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>35</v>
       </c>
@@ -4178,8 +4443,14 @@
       <c r="F43" s="44">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="44">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4196,8 +4467,14 @@
       <c r="F44" s="44">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="44">
+        <v>0.21</v>
+      </c>
+      <c r="H44" s="44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>36</v>
       </c>
@@ -4213,8 +4490,14 @@
       <c r="F45" s="44">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="44">
+        <v>0.25</v>
+      </c>
+      <c r="H45" s="44">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
@@ -4230,8 +4513,14 @@
       <c r="F46" s="44">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="44">
+        <v>0.16</v>
+      </c>
+      <c r="H46" s="44">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>38</v>
       </c>
@@ -4247,8 +4536,14 @@
       <c r="F47" s="44">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="44">
+        <v>0.17</v>
+      </c>
+      <c r="H47" s="44">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>39</v>
       </c>
@@ -4264,8 +4559,14 @@
       <c r="F48" s="44">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="H48" s="44">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>40</v>
       </c>
@@ -4281,8 +4582,14 @@
       <c r="F49" s="44">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="H49" s="44">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>41</v>
       </c>
@@ -4298,8 +4605,14 @@
       <c r="F50" s="44">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="44">
+        <v>0.03</v>
+      </c>
+      <c r="H50" s="44">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>47</v>
       </c>
@@ -4315,8 +4628,14 @@
       <c r="F51" s="44">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="H51" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>42</v>
       </c>
@@ -4332,8 +4651,14 @@
       <c r="F52" s="44">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="44">
+        <v>0.04</v>
+      </c>
+      <c r="H52" s="44">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>43</v>
       </c>
@@ -4349,21 +4674,43 @@
       <c r="F53" s="44">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="H53" s="44">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C54" s="36"/>
       <c r="D54" s="36"/>
-      <c r="F54" s="44"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F54" s="46">
+        <f>SUM(F4:F53)-F27</f>
+        <v>99.87</v>
+      </c>
+      <c r="G54" s="46">
+        <f>SUM(G4:G53)-G27</f>
+        <v>97.529999999999987</v>
+      </c>
+      <c r="H54" s="46">
+        <f>SUM(H4:H53)-H27</f>
+        <v>89.270000000000024</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="36"/>
       <c r="D55" s="36"/>
       <c r="F55" s="44"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>44</v>
       </c>
@@ -4380,8 +4727,14 @@
       <c r="F56" s="44">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="44">
+        <v>0.04</v>
+      </c>
+      <c r="H56" s="44">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -4398,6 +4751,15 @@
       <c r="F57" s="44">
         <v>0</v>
       </c>
+      <c r="G57" s="44">
+        <v>0.63</v>
+      </c>
+      <c r="H57" s="44">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G62" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4410,7 +4772,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4461,32 +4823,33 @@
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="21" t="s">
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="48"/>
       <c r="S1" s="1" t="s">
         <v>112</v>
       </c>
@@ -4497,33 +4860,33 @@
       <c r="X1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Y1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="47" t="s">
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="47" t="s">
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="45"/>
-      <c r="AL1" s="45"/>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="47" t="s">
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47"/>
+      <c r="AQ1" s="47"/>
       <c r="AR1" s="21" t="s">
         <v>54</v>
       </c>
@@ -4533,10 +4896,10 @@
       <c r="AT1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AU1" s="47" t="s">
+      <c r="AU1" s="49" t="s">
         <v>322</v>
       </c>
-      <c r="AV1" s="45"/>
+      <c r="AV1" s="47"/>
       <c r="AW1" s="19" t="s">
         <v>358</v>
       </c>
@@ -6359,6 +6722,7 @@
       </c>
       <c r="P31" s="16"/>
       <c r="Q31" s="16"/>
+      <c r="R31" s="8"/>
       <c r="AR31" s="24"/>
       <c r="AS31" s="6"/>
       <c r="AT31" s="2"/>
@@ -7737,18 +8101,18 @@
       <c r="AS58" s="6"/>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B59" s="48" t="s">
+      <c r="B59" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="50" t="s">
+      <c r="C59" s="51"/>
+      <c r="D59" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="E59" s="49"/>
+      <c r="E59" s="51"/>
       <c r="AS59" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="AU1:AV1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B59:C59"/>
@@ -7760,6 +8124,7 @@
     <mergeCell ref="AN1:AQ1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7795,26 +8160,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="47" t="s">
         <v>357</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>

</xml_diff>

<commit_message>
added GDP growth rate
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F68588D-E7EC-49F5-B6B7-E57C3B0B6026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D999AABF-DAC7-493E-BE9E-FCE4F9ACEC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="415">
   <si>
     <t>United States</t>
   </si>
@@ -1273,6 +1273,18 @@
   </si>
   <si>
     <t>(% in 03/2023)</t>
+  </si>
+  <si>
+    <t>GDP Annual</t>
+  </si>
+  <si>
+    <t>Growth Rate</t>
+  </si>
+  <si>
+    <t>GDP Growth</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
 </sst>
 </file>
@@ -1843,11 +1855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O35" sqref="O35"/>
+      <selection pane="topRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,12 +1876,13 @@
     <col min="12" max="12" width="11.140625" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="11" t="s">
         <v>56</v>
@@ -1911,16 +1924,19 @@
         <v>88</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>96</v>
+        <v>411</v>
       </c>
       <c r="P1" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="11" t="s">
         <v>57</v>
@@ -1952,16 +1968,19 @@
         <v>97</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>99</v>
+        <v>412</v>
       </c>
       <c r="P2" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q2" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1977,10 +1996,10 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
-      <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2006,12 +2025,13 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2">
         <v>1999</v>
       </c>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2039,12 +2059,13 @@
         <v>89</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="P5" s="2">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2">
         <v>2008</v>
       </c>
-      <c r="Q5" s="2"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2070,12 +2091,13 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2">
         <v>2008</v>
       </c>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2101,12 +2123,13 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2">
         <v>2012</v>
       </c>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2129,12 +2152,13 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2">
         <v>2008</v>
       </c>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2160,12 +2184,13 @@
       <c r="M9" s="4"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2">
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2">
         <v>2012</v>
       </c>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2191,12 +2216,13 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2">
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2">
         <v>2008</v>
       </c>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2222,12 +2248,13 @@
       <c r="M11" s="2"/>
       <c r="N11" s="16"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="12">
+      <c r="P11" s="2"/>
+      <c r="Q11" s="12">
         <v>41426</v>
       </c>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2250,12 +2277,13 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="12">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="12">
         <v>41548</v>
       </c>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>14</v>
       </c>
@@ -2279,12 +2307,13 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="42" t="s">
+      <c r="P13" s="2"/>
+      <c r="Q13" s="42" t="s">
         <v>402</v>
       </c>
-      <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2304,12 +2333,13 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="2">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2">
         <v>1999</v>
       </c>
-      <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -2335,12 +2365,13 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2">
         <v>2012</v>
       </c>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
@@ -2359,11 +2390,11 @@
         <v>2016</v>
       </c>
       <c r="L16" s="2"/>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -2389,12 +2420,13 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2">
         <v>2012</v>
       </c>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
@@ -2412,11 +2444,11 @@
       <c r="J18" s="4">
         <v>2011</v>
       </c>
-      <c r="P18" s="2">
+      <c r="Q18" s="2">
         <v>1999</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>17</v>
       </c>
@@ -2443,9 +2475,10 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -2468,9 +2501,10 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2497,12 +2531,13 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2">
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2">
         <v>2004</v>
       </c>
-      <c r="Q21" s="2"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -2524,12 +2559,13 @@
       <c r="M22" s="4"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2">
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2">
         <v>2012</v>
       </c>
-      <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -2551,12 +2587,13 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2">
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2">
         <v>2012</v>
       </c>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
@@ -2580,12 +2617,13 @@
       <c r="M24" s="4"/>
       <c r="N24" s="16"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2">
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2">
         <v>2012</v>
       </c>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2608,12 +2646,13 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2">
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2">
         <v>2012</v>
       </c>
-      <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>18</v>
       </c>
@@ -2637,9 +2676,10 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>69</v>
       </c>
@@ -2664,20 +2704,20 @@
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="36"/>
       <c r="C28" s="39"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="39"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2707,14 +2747,17 @@
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="2">
+      <c r="P30" s="4">
+        <v>2011</v>
+      </c>
+      <c r="Q30" s="2">
         <v>2005</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="R30" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>24</v>
       </c>
@@ -2734,11 +2777,12 @@
       </c>
       <c r="M31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2">
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2768,14 +2812,15 @@
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="2">
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2">
         <v>2012</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="R32" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2805,12 +2850,13 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="2">
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2">
         <v>2012</v>
       </c>
-      <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>98</v>
       </c>
@@ -2840,12 +2886,13 @@
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="2">
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2">
         <v>2012</v>
       </c>
-      <c r="Q34" s="2"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
@@ -2874,12 +2921,15 @@
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="2">
+      <c r="P35" s="4">
+        <v>2010</v>
+      </c>
+      <c r="Q35" s="2">
         <v>2012</v>
       </c>
-      <c r="Q35" s="16"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="16"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
@@ -2906,12 +2956,13 @@
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="2">
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2">
         <v>2012</v>
       </c>
-      <c r="Q36" s="2"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -2934,12 +2985,13 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2">
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2">
         <v>2012</v>
       </c>
-      <c r="Q37" s="2"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>31</v>
       </c>
@@ -2963,7 +3015,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
@@ -2992,14 +3044,15 @@
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="2">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2">
         <v>2012</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="R39" s="4">
         <v>2002</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>33</v>
       </c>
@@ -3019,7 +3072,7 @@
       </c>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>49</v>
       </c>
@@ -3038,7 +3091,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>34</v>
       </c>
@@ -3055,7 +3108,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>35</v>
       </c>
@@ -3072,7 +3125,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -3104,12 +3157,13 @@
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="2">
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2">
         <v>2012</v>
       </c>
-      <c r="Q44" s="2"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>36</v>
       </c>
@@ -3131,7 +3185,7 @@
       </c>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
@@ -3156,12 +3210,13 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="2">
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2">
         <v>2012</v>
       </c>
-      <c r="Q46" s="2"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>38</v>
       </c>
@@ -3185,11 +3240,12 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-      <c r="Q47" s="4">
+      <c r="P47" s="2"/>
+      <c r="R47" s="4">
         <v>2003</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>39</v>
       </c>
@@ -3218,12 +3274,13 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="2">
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2">
         <v>2012</v>
       </c>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>40</v>
       </c>
@@ -3243,7 +3300,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>41</v>
       </c>
@@ -3265,12 +3322,13 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="2">
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2">
         <v>1999</v>
       </c>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50" s="2"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>47</v>
       </c>
@@ -3293,12 +3351,13 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
-      <c r="P51" s="2">
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2">
         <v>2012</v>
       </c>
-      <c r="Q51" s="2"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" s="2"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>42</v>
       </c>
@@ -3315,7 +3374,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>43</v>
       </c>
@@ -3343,20 +3402,23 @@
       <c r="O53" s="4">
         <v>2006</v>
       </c>
-      <c r="Q53" s="2"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P53" s="4">
+        <v>2005</v>
+      </c>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B54" s="36"/>
       <c r="C54" s="39"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B55" s="36"/>
       <c r="C55" s="39"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>44</v>
       </c>
@@ -3384,9 +3446,10 @@
         <v>2017</v>
       </c>
       <c r="O56" s="2"/>
-      <c r="Q56" s="16"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P56" s="2"/>
+      <c r="R56" s="16"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -3416,23 +3479,26 @@
         <v>72</v>
       </c>
       <c r="O57" s="2"/>
-      <c r="P57" s="2">
+      <c r="P57" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q57" s="2">
         <v>2012</v>
       </c>
-      <c r="Q57" s="16" t="s">
+      <c r="R57" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P59" s="22"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q59" s="22"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B61" s="47" t="s">
         <v>403</v>
       </c>
       <c r="C61" s="48"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>395</v>
       </c>
@@ -3440,7 +3506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>404</v>
       </c>
@@ -3448,7 +3514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
         <v>393</v>
       </c>
@@ -4772,7 +4838,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I31" sqref="I31"/>
+      <selection pane="topRight" activeCell="J2" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cleaned World Bank folder
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE27FA6-0DCC-47E6-847C-4BC5FA01B218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84C7A7A-E990-4D8F-950B-0CEB2D8F0DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -1511,7 +1511,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1565,40 +1565,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="17" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3555,10 +3533,10 @@
       <c r="Q59" s="17"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="45" t="s">
         <v>399</v>
       </c>
-      <c r="C61" s="42"/>
+      <c r="C61" s="46"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -4905,22 +4883,20 @@
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="43" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="43" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="43" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.85546875" style="6" customWidth="1"/>
     <col min="19" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.42578125" style="6" customWidth="1"/>
     <col min="25" max="25" width="10.42578125" customWidth="1"/>
     <col min="26" max="26" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -4940,11 +4916,10 @@
     <col min="43" max="43" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19" style="43" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="12.140625" customWidth="1"/>
-    <col min="48" max="48" width="19" style="43" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="12" customWidth="1"/>
     <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
@@ -4958,110 +4933,110 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="41" t="s">
         <v>419</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="50" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
       <c r="R1" s="12"/>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="50"/>
-      <c r="Y1" s="50" t="s">
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="Y1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="51"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="42"/>
       <c r="AE1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="48" t="s">
+      <c r="AF1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="47" t="s">
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="51"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="42"/>
       <c r="AQ1" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="AS1" s="47" t="s">
+      <c r="AS1" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" s="50"/>
-      <c r="AU1" s="48" t="s">
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AV1" s="50"/>
-      <c r="AW1" s="50" t="s">
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AX1" s="50"/>
-      <c r="AY1" s="50"/>
-      <c r="AZ1" s="50"/>
-      <c r="BA1" s="50"/>
-      <c r="BB1" s="51"/>
-      <c r="BC1" s="49" t="s">
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="42"/>
+      <c r="BC1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="BD1" s="49"/>
-      <c r="BE1" s="49"/>
-      <c r="BF1" s="49"/>
-      <c r="BG1" s="49"/>
+      <c r="BD1" s="45"/>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="45"/>
+      <c r="BG1" s="45"/>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" t="s">
         <v>417</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" t="s">
         <v>418</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" t="s">
         <v>415</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="H2" t="s">
         <v>419</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" t="s">
         <v>421</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -5079,16 +5054,16 @@
       <c r="N2" t="s">
         <v>114</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" t="s">
         <v>114</v>
       </c>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="Q2" s="53" t="s">
+      <c r="Q2" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="43" t="s">
         <v>425</v>
       </c>
       <c r="S2" t="s">
@@ -5103,7 +5078,7 @@
       <c r="V2" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="W2" t="s">
         <v>384</v>
       </c>
       <c r="X2" s="6" t="s">
@@ -5172,19 +5147,19 @@
       <c r="AS2" t="s">
         <v>59</v>
       </c>
-      <c r="AT2" s="43" t="s">
+      <c r="AT2" t="s">
         <v>64</v>
       </c>
       <c r="AU2" t="s">
         <v>59</v>
       </c>
-      <c r="AV2" s="43" t="s">
+      <c r="AV2" t="s">
         <v>64</v>
       </c>
       <c r="AW2" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="43" t="s">
+      <c r="AX2" t="s">
         <v>75</v>
       </c>
       <c r="AY2" t="s">
@@ -5219,28 +5194,28 @@
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" t="s">
         <v>416</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" t="s">
         <v>420</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" t="s">
         <v>422</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -5258,16 +5233,16 @@
       <c r="N3" t="s">
         <v>111</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" t="s">
         <v>115</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="Q3" s="53" t="s">
+      <c r="Q3" s="17" t="s">
         <v>411</v>
       </c>
-      <c r="R3" s="54" t="s">
+      <c r="R3" s="43" t="s">
         <v>426</v>
       </c>
       <c r="S3" t="s">
@@ -5282,7 +5257,7 @@
       <c r="V3" t="s">
         <v>377</v>
       </c>
-      <c r="W3" s="43" t="s">
+      <c r="W3" t="s">
         <v>388</v>
       </c>
       <c r="Y3" t="s">
@@ -5336,22 +5311,22 @@
       <c r="AP3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="AQ3" s="59" t="s">
+      <c r="AQ3" t="s">
         <v>430</v>
       </c>
-      <c r="AR3" s="60" t="s">
+      <c r="AR3" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="AT3" s="43" t="s">
+      <c r="AT3" t="s">
         <v>66</v>
       </c>
-      <c r="AV3" s="43" t="s">
+      <c r="AV3" t="s">
         <v>66</v>
       </c>
       <c r="AW3" t="s">
         <v>71</v>
       </c>
-      <c r="AX3" s="43" t="s">
+      <c r="AX3" t="s">
         <v>76</v>
       </c>
       <c r="AY3" t="s">
@@ -5387,28 +5362,28 @@
         <v>0</v>
       </c>
       <c r="B4" s="19"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
         <v>1999</v>
       </c>
       <c r="F4" s="4">
         <v>2010</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="2">
         <v>2002</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="44"/>
+      <c r="W4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
@@ -5433,7 +5408,7 @@
         <v>2012</v>
       </c>
       <c r="AW4" s="2"/>
-      <c r="AX4" s="44"/>
+      <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
       <c r="AZ4" s="2"/>
       <c r="BA4" s="2"/>
@@ -5449,14 +5424,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
         <v>1999</v>
       </c>
       <c r="F5" s="4">
         <v>2009</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="2">
         <v>2006</v>
       </c>
       <c r="K5" s="2"/>
@@ -5465,14 +5440,14 @@
         <v>2007</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-      <c r="W5" s="44"/>
+      <c r="W5" s="2"/>
       <c r="Y5" s="13" t="s">
         <v>89</v>
       </c>
@@ -5504,11 +5479,11 @@
       <c r="AU5" s="4">
         <v>2019</v>
       </c>
-      <c r="AV5" s="52">
+      <c r="AV5" s="10">
         <v>41548</v>
       </c>
       <c r="AW5" s="2"/>
-      <c r="AX5" s="44"/>
+      <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="13"/>
@@ -5524,23 +5499,23 @@
         <v>3</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
         <v>1999</v>
       </c>
       <c r="F6" s="4">
         <v>2010</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="13">
         <v>2011</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="13" t="s">
@@ -5549,7 +5524,7 @@
       <c r="V6" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="W6" s="44"/>
+      <c r="W6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
@@ -5578,7 +5553,7 @@
         <v>2008</v>
       </c>
       <c r="AW6" s="2"/>
-      <c r="AX6" s="44"/>
+      <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
       <c r="AZ6" s="2"/>
       <c r="BA6" s="2"/>
@@ -5596,28 +5571,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
         <v>1999</v>
       </c>
       <c r="F7" s="4">
         <v>2010</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="4">
         <v>2016</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="44"/>
+      <c r="W7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
@@ -5638,11 +5613,11 @@
       <c r="AS7" s="4">
         <v>2021</v>
       </c>
-      <c r="AT7" s="44">
+      <c r="AT7" s="2">
         <v>2012</v>
       </c>
       <c r="AW7" s="2"/>
-      <c r="AX7" s="44"/>
+      <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2"/>
@@ -5658,28 +5633,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="19"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
         <v>1999</v>
       </c>
       <c r="F8" s="2">
         <v>2008</v>
       </c>
-      <c r="G8" s="45"/>
+      <c r="G8" s="13"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="4">
         <v>2003</v>
       </c>
-      <c r="W8" s="44"/>
+      <c r="W8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
@@ -5704,7 +5679,7 @@
         <v>2008</v>
       </c>
       <c r="AW8" s="2"/>
-      <c r="AX8" s="44"/>
+      <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="2"/>
@@ -5720,30 +5695,30 @@
         <v>10</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
         <v>1999</v>
       </c>
       <c r="F9" s="2">
         <v>2008</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="2">
         <v>2010</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
       <c r="S9" s="13"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="4">
         <v>2010</v>
       </c>
-      <c r="W9" s="46"/>
+      <c r="W9" s="4"/>
       <c r="Y9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -5765,14 +5740,14 @@
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
       <c r="AP9" s="7"/>
-      <c r="AT9" s="44">
+      <c r="AT9" s="2">
         <v>2012</v>
       </c>
-      <c r="AV9" s="52">
+      <c r="AV9" s="10">
         <v>41671</v>
       </c>
       <c r="AW9" s="2"/>
-      <c r="AX9" s="45"/>
+      <c r="AX9" s="13"/>
       <c r="AY9" s="4">
         <v>2011</v>
       </c>
@@ -5794,30 +5769,30 @@
         <v>2</v>
       </c>
       <c r="B10" s="19"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>1999</v>
       </c>
       <c r="F10" s="2">
         <v>2008</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="2">
         <v>2012</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="4">
         <v>2005</v>
       </c>
-      <c r="W10" s="44"/>
+      <c r="W10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
@@ -5842,7 +5817,7 @@
         <v>2008</v>
       </c>
       <c r="AW10" s="2"/>
-      <c r="AX10" s="44"/>
+      <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
@@ -5858,28 +5833,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
         <v>1999</v>
       </c>
       <c r="F11" s="4">
         <v>2010</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="2">
         <v>2007</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="44"/>
+      <c r="W11" s="2"/>
       <c r="Y11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
@@ -5900,17 +5875,17 @@
       <c r="AS11" s="4">
         <v>2018</v>
       </c>
-      <c r="AT11" s="52">
+      <c r="AT11" s="10">
         <v>41426</v>
       </c>
       <c r="AU11" s="4">
         <v>2018</v>
       </c>
-      <c r="AV11" s="52">
+      <c r="AV11" s="10">
         <v>41395</v>
       </c>
       <c r="AW11" s="2"/>
-      <c r="AX11" s="44"/>
+      <c r="AX11" s="2"/>
       <c r="AY11" s="13"/>
       <c r="AZ11" s="13"/>
       <c r="BA11" s="13"/>
@@ -5926,26 +5901,26 @@
         <v>8</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
         <v>1999</v>
       </c>
       <c r="F12" s="2">
         <v>2008</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="13"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="44"/>
+      <c r="W12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
@@ -5965,11 +5940,11 @@
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="7"/>
-      <c r="AT12" s="52">
+      <c r="AT12" s="10">
         <v>41548</v>
       </c>
       <c r="AW12" s="2"/>
-      <c r="AX12" s="45"/>
+      <c r="AX12" s="13"/>
       <c r="AY12" s="2"/>
       <c r="AZ12" s="2"/>
       <c r="BA12" s="2"/>
@@ -5988,27 +5963,27 @@
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="4">
         <v>2001</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="46">
+      <c r="D13" s="2"/>
+      <c r="E13" s="4">
         <v>2012</v>
       </c>
       <c r="F13" s="13"/>
-      <c r="G13" s="45"/>
+      <c r="G13" s="13"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="44"/>
+      <c r="W13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
@@ -6030,11 +6005,11 @@
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="7"/>
-      <c r="AT13" s="52" t="s">
+      <c r="AT13" s="10" t="s">
         <v>65</v>
       </c>
       <c r="AW13" s="2"/>
-      <c r="AX13" s="45"/>
+      <c r="AX13" s="13"/>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
@@ -6052,27 +6027,27 @@
       <c r="B14" s="20">
         <v>2008</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="2">
         <v>1999</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
         <v>1999</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="45"/>
+      <c r="G14" s="13"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="44"/>
+      <c r="W14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
@@ -6099,7 +6074,7 @@
         <v>2006</v>
       </c>
       <c r="AW14" s="2"/>
-      <c r="AX14" s="45"/>
+      <c r="AX14" s="13"/>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2"/>
@@ -6115,28 +6090,28 @@
         <v>7</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>1999</v>
       </c>
       <c r="F15" s="4">
         <v>2011</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="4">
         <v>2016</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="44"/>
+      <c r="W15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
@@ -6163,7 +6138,7 @@
         <v>2012</v>
       </c>
       <c r="AW15" s="2"/>
-      <c r="AX15" s="44"/>
+      <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
       <c r="AZ15" s="2"/>
       <c r="BA15" s="2"/>
@@ -6179,14 +6154,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
         <v>1999</v>
       </c>
       <c r="F16" s="13">
         <v>2016</v>
       </c>
-      <c r="G16" s="45"/>
+      <c r="G16" s="13"/>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
       <c r="U16" s="2"/>
@@ -6202,28 +6177,28 @@
         <v>5</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
         <v>1999</v>
       </c>
       <c r="F17" s="2">
         <v>2008</v>
       </c>
-      <c r="G17" s="44">
+      <c r="G17" s="2">
         <v>1999</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="44"/>
+      <c r="W17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
@@ -6252,7 +6227,7 @@
         <v>2012</v>
       </c>
       <c r="AW17" s="2"/>
-      <c r="AX17" s="44"/>
+      <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2"/>
       <c r="BA17" s="2"/>
@@ -6268,14 +6243,14 @@
         <v>21</v>
       </c>
       <c r="B18" s="19"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
         <v>1999</v>
       </c>
       <c r="F18" s="4">
         <v>2011</v>
       </c>
-      <c r="G18" s="45"/>
+      <c r="G18" s="13"/>
       <c r="S18" s="14"/>
       <c r="T18" s="14"/>
       <c r="U18" s="13" t="s">
@@ -6295,29 +6270,29 @@
       <c r="B19" s="20">
         <v>2013</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="4">
         <v>2001</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="46">
+      <c r="D19" s="2"/>
+      <c r="E19" s="4">
         <v>2012</v>
       </c>
       <c r="F19" s="13">
         <v>2008</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="13"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="44"/>
+      <c r="W19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
@@ -6335,9 +6310,9 @@
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
       <c r="AP19" s="7"/>
-      <c r="AT19" s="45"/>
+      <c r="AT19" s="13"/>
       <c r="AW19" s="2"/>
-      <c r="AX19" s="45"/>
+      <c r="AX19" s="13"/>
       <c r="AY19" s="2"/>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="2"/>
@@ -6353,26 +6328,26 @@
         <v>12</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
         <v>1999</v>
       </c>
       <c r="F20" s="2">
         <v>2008</v>
       </c>
-      <c r="G20" s="45"/>
+      <c r="G20" s="13"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="44"/>
+      <c r="W20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
@@ -6396,9 +6371,9 @@
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
       <c r="AP20" s="7"/>
-      <c r="AT20" s="45"/>
+      <c r="AT20" s="13"/>
       <c r="AW20" s="2"/>
-      <c r="AX20" s="45"/>
+      <c r="AX20" s="13"/>
       <c r="AY20" s="2"/>
       <c r="AZ20" s="2"/>
       <c r="BA20" s="2"/>
@@ -6415,29 +6390,29 @@
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="52">
+      <c r="C21" s="10">
         <v>36404</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="46">
+      <c r="D21" s="2"/>
+      <c r="E21" s="4">
         <v>2009</v>
       </c>
       <c r="F21" s="13">
         <v>2008</v>
       </c>
-      <c r="G21" s="45"/>
+      <c r="G21" s="13"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="44"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="44"/>
+      <c r="W21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
@@ -6459,7 +6434,7 @@
         <v>2004</v>
       </c>
       <c r="AW21" s="2"/>
-      <c r="AX21" s="45"/>
+      <c r="AX21" s="13"/>
       <c r="AY21" s="2"/>
       <c r="AZ21" s="2"/>
       <c r="BA21" s="2"/>
@@ -6475,19 +6450,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="19"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="46">
+      <c r="D22" s="2"/>
+      <c r="E22" s="4">
         <v>2008</v>
       </c>
       <c r="F22" s="13"/>
-      <c r="G22" s="45"/>
+      <c r="G22" s="13"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
       <c r="S22" s="4">
         <v>2012</v>
       </c>
@@ -6498,7 +6473,7 @@
       <c r="V22" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="W22" s="46"/>
+      <c r="W22" s="4"/>
       <c r="Y22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
@@ -6516,11 +6491,11 @@
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
       <c r="AP22" s="7"/>
-      <c r="AT22" s="44">
+      <c r="AT22" s="2">
         <v>2012</v>
       </c>
       <c r="AW22" s="2"/>
-      <c r="AX22" s="45"/>
+      <c r="AX22" s="13"/>
       <c r="AY22" s="2"/>
       <c r="AZ22" s="2"/>
       <c r="BA22" s="2"/>
@@ -6540,24 +6515,24 @@
         <v>20</v>
       </c>
       <c r="B23" s="19"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="46">
+      <c r="D23" s="2"/>
+      <c r="E23" s="4">
         <v>2010</v>
       </c>
       <c r="F23" s="13"/>
-      <c r="G23" s="45"/>
+      <c r="G23" s="13"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44"/>
-      <c r="Q23" s="44"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="44"/>
+      <c r="W23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
@@ -6584,7 +6559,7 @@
         <v>2012</v>
       </c>
       <c r="AW23" s="2"/>
-      <c r="AX23" s="45"/>
+      <c r="AX23" s="13"/>
       <c r="AY23" s="2"/>
       <c r="AZ23" s="2"/>
       <c r="BA23" s="2"/>
@@ -6604,27 +6579,27 @@
       <c r="B24" s="20">
         <v>2003</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24" s="4">
         <v>2001</v>
       </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="46">
+      <c r="D24" s="2"/>
+      <c r="E24" s="4">
         <v>2010</v>
       </c>
       <c r="F24" s="13"/>
-      <c r="G24" s="45"/>
+      <c r="G24" s="13"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
-      <c r="Q24" s="44"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
       <c r="S24" s="13"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="46"/>
+      <c r="W24" s="4"/>
       <c r="Y24" s="13"/>
       <c r="AA24" s="13"/>
       <c r="AB24" s="13"/>
@@ -6644,14 +6619,14 @@
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
       <c r="AP24" s="7"/>
-      <c r="AT24" s="44">
+      <c r="AT24" s="2">
         <v>2012</v>
       </c>
-      <c r="AV24" s="44">
+      <c r="AV24" s="2">
         <v>2012</v>
       </c>
       <c r="AW24" s="2"/>
-      <c r="AX24" s="45"/>
+      <c r="AX24" s="13"/>
       <c r="AY24" s="13"/>
       <c r="AZ24" s="13"/>
       <c r="BA24" s="13"/>
@@ -6667,26 +6642,26 @@
         <v>13</v>
       </c>
       <c r="B25" s="19"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
         <v>1999</v>
       </c>
       <c r="F25" s="2">
         <v>2008</v>
       </c>
-      <c r="G25" s="45"/>
+      <c r="G25" s="13"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="44"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="44"/>
+      <c r="W25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
@@ -6712,7 +6687,7 @@
         <v>2012</v>
       </c>
       <c r="AW25" s="2"/>
-      <c r="AX25" s="45"/>
+      <c r="AX25" s="13"/>
       <c r="AY25" s="2"/>
       <c r="AZ25" s="2"/>
       <c r="BA25" s="2"/>
@@ -6730,27 +6705,27 @@
       <c r="B26" s="20">
         <v>2013</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="4">
         <v>2010</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="46">
+      <c r="D26" s="2"/>
+      <c r="E26" s="4">
         <v>2013</v>
       </c>
       <c r="F26" s="13"/>
-      <c r="G26" s="45"/>
+      <c r="G26" s="13"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-      <c r="W26" s="44"/>
+      <c r="W26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
@@ -6768,9 +6743,9 @@
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
       <c r="AP26" s="7"/>
-      <c r="AT26" s="45"/>
+      <c r="AT26" s="13"/>
       <c r="AW26" s="2"/>
-      <c r="AX26" s="45"/>
+      <c r="AX26" s="13"/>
       <c r="AY26" s="2"/>
       <c r="AZ26" s="2"/>
       <c r="BA26" s="2"/>
@@ -6790,26 +6765,26 @@
       <c r="B27" s="20">
         <v>2007</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="46">
+      <c r="D27" s="2"/>
+      <c r="E27" s="4">
         <v>2002</v>
       </c>
       <c r="F27" s="2">
         <v>2008</v>
       </c>
-      <c r="G27" s="44">
+      <c r="G27" s="2">
         <v>2001</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="44"/>
+      <c r="O27" s="2"/>
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
-      <c r="W27" s="44"/>
+      <c r="W27" s="2"/>
       <c r="Y27" s="13"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="13"/>
@@ -6834,12 +6809,12 @@
       <c r="AS27" s="2">
         <v>2012</v>
       </c>
-      <c r="AT27" s="61"/>
+      <c r="AT27" s="14"/>
       <c r="AU27" s="2">
         <v>2012</v>
       </c>
       <c r="AW27" s="2"/>
-      <c r="AX27" s="45"/>
+      <c r="AX27" s="13"/>
       <c r="AY27" s="2"/>
       <c r="AZ27" s="2"/>
       <c r="BA27" s="2"/>
@@ -6856,21 +6831,21 @@
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AT29" s="62"/>
+      <c r="AT29" s="44"/>
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="19"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="46">
+      <c r="D30" s="2"/>
+      <c r="E30" s="4">
         <v>2011</v>
       </c>
       <c r="F30" s="4">
         <v>2011</v>
       </c>
-      <c r="G30" s="44">
+      <c r="G30" s="2">
         <v>2011</v>
       </c>
       <c r="K30" s="2"/>
@@ -6879,16 +6854,16 @@
       </c>
       <c r="M30" s="13"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="44"/>
-      <c r="P30" s="46">
+      <c r="O30" s="2"/>
+      <c r="P30" s="4">
         <v>2011</v>
       </c>
-      <c r="Q30" s="44"/>
+      <c r="Q30" s="2"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
       <c r="V30" s="13"/>
-      <c r="W30" s="46">
+      <c r="W30" s="4">
         <v>2002</v>
       </c>
       <c r="Y30" s="2"/>
@@ -6919,7 +6894,7 @@
       <c r="AW30" s="4">
         <v>2000</v>
       </c>
-      <c r="AX30" s="44"/>
+      <c r="AX30" s="2"/>
       <c r="AY30" s="13"/>
       <c r="AZ30" s="13"/>
       <c r="BA30" s="13"/>
@@ -6937,19 +6912,19 @@
         <v>24</v>
       </c>
       <c r="B31" s="19"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="46">
+      <c r="D31" s="2"/>
+      <c r="E31" s="4">
         <v>2000</v>
       </c>
       <c r="F31" s="2">
         <v>2008</v>
       </c>
-      <c r="G31" s="45"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
+      <c r="G31" s="13"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
-      <c r="W31" s="44"/>
+      <c r="W31" s="2"/>
       <c r="AS31" s="2">
         <v>2012</v>
       </c>
@@ -6959,14 +6934,14 @@
         <v>25</v>
       </c>
       <c r="B32" s="19"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="46">
+      <c r="D32" s="2"/>
+      <c r="E32" s="4">
         <v>2012</v>
       </c>
       <c r="F32" s="2">
         <v>2008</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="2">
         <v>2005</v>
       </c>
       <c r="K32" s="2"/>
@@ -6975,11 +6950,11 @@
       <c r="N32" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="O32" s="45" t="s">
+      <c r="O32" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
       <c r="U32" s="4">
@@ -6988,7 +6963,7 @@
       <c r="V32" s="4">
         <v>2017</v>
       </c>
-      <c r="W32" s="46">
+      <c r="W32" s="4">
         <v>2018</v>
       </c>
       <c r="Y32" s="2"/>
@@ -7021,7 +6996,7 @@
       <c r="AW32" s="4">
         <v>2000</v>
       </c>
-      <c r="AX32" s="44"/>
+      <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
       <c r="AZ32" s="2"/>
       <c r="BA32" s="2"/>
@@ -7043,28 +7018,28 @@
         <v>26</v>
       </c>
       <c r="B33" s="19"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="46">
+      <c r="D33" s="2"/>
+      <c r="E33" s="4">
         <v>2000</v>
       </c>
       <c r="F33" s="2">
         <v>2008</v>
       </c>
-      <c r="G33" s="44">
+      <c r="G33" s="2">
         <v>2007</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="44"/>
+      <c r="W33" s="2"/>
       <c r="Y33" s="2"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
@@ -7090,7 +7065,7 @@
         <v>2012</v>
       </c>
       <c r="AW33" s="2"/>
-      <c r="AX33" s="44"/>
+      <c r="AX33" s="2"/>
       <c r="AY33" s="2"/>
       <c r="AZ33" s="2"/>
       <c r="BA33" s="2"/>
@@ -7110,14 +7085,14 @@
         <v>98</v>
       </c>
       <c r="B34" s="19"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="46">
+      <c r="D34" s="2"/>
+      <c r="E34" s="4">
         <v>2000</v>
       </c>
       <c r="F34" s="2">
         <v>2008</v>
       </c>
-      <c r="G34" s="44">
+      <c r="G34" s="2">
         <v>2012</v>
       </c>
       <c r="K34" s="2"/>
@@ -7126,11 +7101,11 @@
       <c r="N34" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="O34" s="45" t="s">
+      <c r="O34" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P34" s="44"/>
-      <c r="Q34" s="44"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
       <c r="U34" s="13" t="s">
@@ -7139,7 +7114,7 @@
       <c r="V34" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="W34" s="46">
+      <c r="W34" s="4">
         <v>2012</v>
       </c>
       <c r="Y34" s="2"/>
@@ -7166,7 +7141,7 @@
         <v>2012</v>
       </c>
       <c r="AW34" s="2"/>
-      <c r="AX34" s="44"/>
+      <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
       <c r="AZ34" s="2"/>
       <c r="BA34" s="2"/>
@@ -7182,14 +7157,14 @@
         <v>28</v>
       </c>
       <c r="B35" s="19"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="45">
+      <c r="D35" s="2"/>
+      <c r="E35" s="13">
         <v>2015</v>
       </c>
       <c r="F35" s="13">
         <v>2019</v>
       </c>
-      <c r="G35" s="45"/>
+      <c r="G35" s="13"/>
       <c r="K35" s="4">
         <v>2011</v>
       </c>
@@ -7202,13 +7177,13 @@
       <c r="N35" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="O35" s="45" t="s">
+      <c r="O35" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="P35" s="46">
+      <c r="P35" s="4">
         <v>2010</v>
       </c>
-      <c r="Q35" s="46"/>
+      <c r="Q35" s="4"/>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13" t="s">
@@ -7217,7 +7192,7 @@
       <c r="V35" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="W35" s="46">
+      <c r="W35" s="4">
         <v>2000</v>
       </c>
       <c r="Y35" s="2"/>
@@ -7247,11 +7222,11 @@
       <c r="AP35" s="15">
         <v>2016</v>
       </c>
-      <c r="AT35" s="44">
+      <c r="AT35" s="2">
         <v>2012</v>
       </c>
       <c r="AW35" s="13"/>
-      <c r="AX35" s="45"/>
+      <c r="AX35" s="13"/>
       <c r="AY35" s="13"/>
       <c r="AZ35" s="13"/>
       <c r="BA35" s="13"/>
@@ -7266,26 +7241,26 @@
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="44">
+      <c r="C36" s="2">
         <v>1999</v>
       </c>
-      <c r="D36" s="44"/>
-      <c r="E36" s="46">
+      <c r="D36" s="2"/>
+      <c r="E36" s="4">
         <v>2003</v>
       </c>
       <c r="F36" s="4">
         <v>2010</v>
       </c>
-      <c r="G36" s="45"/>
+      <c r="G36" s="13"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2">
         <v>2008</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
-      <c r="Q36" s="44"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
       <c r="U36" s="4">
@@ -7294,7 +7269,7 @@
       <c r="V36" s="4">
         <v>2008</v>
       </c>
-      <c r="W36" s="46">
+      <c r="W36" s="4">
         <v>2000</v>
       </c>
       <c r="Y36" s="2"/>
@@ -7318,7 +7293,7 @@
         <v>2012</v>
       </c>
       <c r="AW36" s="2"/>
-      <c r="AX36" s="44"/>
+      <c r="AX36" s="2"/>
       <c r="AY36" s="13"/>
       <c r="AZ36" s="2"/>
       <c r="BA36" s="13"/>
@@ -7334,23 +7309,23 @@
         <v>30</v>
       </c>
       <c r="B37" s="19"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2">
         <v>1999</v>
       </c>
       <c r="F37" s="4">
         <v>2010</v>
       </c>
-      <c r="G37" s="45"/>
+      <c r="G37" s="13"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2">
         <v>2005</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="44"/>
-      <c r="P37" s="44"/>
-      <c r="Q37" s="44"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="13" t="s">
@@ -7359,7 +7334,7 @@
       <c r="V37" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="W37" s="44"/>
+      <c r="W37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
@@ -7385,7 +7360,7 @@
         <v>2012</v>
       </c>
       <c r="AW37" s="2"/>
-      <c r="AX37" s="44"/>
+      <c r="AX37" s="2"/>
       <c r="AY37" s="13"/>
       <c r="AZ37" s="2"/>
       <c r="BA37" s="13" t="s">
@@ -7405,14 +7380,14 @@
         <v>31</v>
       </c>
       <c r="B38" s="19"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="46">
+      <c r="D38" s="2"/>
+      <c r="E38" s="4">
         <v>2008</v>
       </c>
       <c r="F38" s="4">
         <v>2011</v>
       </c>
-      <c r="G38" s="45"/>
+      <c r="G38" s="13"/>
       <c r="U38" s="13" t="s">
         <v>374</v>
       </c>
@@ -7422,7 +7397,7 @@
       <c r="AE38" s="4">
         <v>2000</v>
       </c>
-      <c r="AT38" s="45">
+      <c r="AT38" s="13">
         <v>2016</v>
       </c>
     </row>
@@ -7431,28 +7406,28 @@
         <v>32</v>
       </c>
       <c r="B39" s="19"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="46">
+      <c r="D39" s="2"/>
+      <c r="E39" s="4">
         <v>2010</v>
       </c>
       <c r="F39" s="4">
         <v>2011</v>
       </c>
-      <c r="G39" s="45"/>
+      <c r="G39" s="13"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="13"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="44"/>
-      <c r="Q39" s="44"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="4">
         <v>2009</v>
       </c>
       <c r="V39" s="2"/>
-      <c r="W39" s="46">
+      <c r="W39" s="4">
         <v>2000</v>
       </c>
       <c r="Y39" s="2"/>
@@ -7484,7 +7459,7 @@
       <c r="AW39" s="4">
         <v>2002</v>
       </c>
-      <c r="AX39" s="44"/>
+      <c r="AX39" s="2"/>
       <c r="AY39" s="13"/>
       <c r="AZ39" s="2"/>
       <c r="BA39" s="13"/>
@@ -7502,14 +7477,14 @@
         <v>33</v>
       </c>
       <c r="B40" s="19"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2">
         <v>1999</v>
       </c>
       <c r="F40" s="4">
         <v>2011</v>
       </c>
-      <c r="G40" s="45"/>
+      <c r="G40" s="13"/>
       <c r="U40" s="13" t="s">
         <v>89</v>
       </c>
@@ -7517,7 +7492,7 @@
         <v>89</v>
       </c>
       <c r="AE40" s="2"/>
-      <c r="AT40" s="45">
+      <c r="AT40" s="13">
         <v>2015</v>
       </c>
     </row>
@@ -7525,20 +7500,20 @@
       <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41">
         <v>2004</v>
       </c>
-      <c r="D41" s="52">
+      <c r="D41" s="10">
         <v>36192</v>
       </c>
-      <c r="E41" s="45">
+      <c r="E41" s="13">
         <v>2014</v>
       </c>
       <c r="F41" s="13"/>
-      <c r="G41" s="45"/>
+      <c r="G41" s="13"/>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
-      <c r="AT41" s="45">
+      <c r="AT41" s="13">
         <v>2012</v>
       </c>
     </row>
@@ -7546,22 +7521,22 @@
       <c r="A42" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42">
         <v>2001</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45">
+      <c r="D42" s="2"/>
+      <c r="E42" s="13">
         <v>2014</v>
       </c>
       <c r="F42" s="13"/>
-      <c r="G42" s="45"/>
+      <c r="G42" s="13"/>
       <c r="U42" s="13" t="s">
         <v>375</v>
       </c>
       <c r="V42" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="AT42" s="45">
+      <c r="AT42" s="13">
         <v>2017</v>
       </c>
     </row>
@@ -7569,42 +7544,42 @@
       <c r="A43" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43">
         <v>2010</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="45">
+      <c r="D43" s="2"/>
+      <c r="E43" s="13">
         <v>2020</v>
       </c>
       <c r="F43" s="13"/>
-      <c r="G43" s="45"/>
+      <c r="G43" s="13"/>
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
-      <c r="AT43" s="45"/>
-      <c r="AV43" s="62"/>
+      <c r="AT43" s="13"/>
+      <c r="AV43" s="44"/>
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B44" s="19"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="46">
+      <c r="D44" s="2"/>
+      <c r="E44" s="4">
         <v>2008</v>
       </c>
       <c r="F44" s="2">
         <v>2008</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G44" s="2">
         <v>2012</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="13"/>
       <c r="N44" s="2"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
       <c r="S44" s="4">
         <v>2005</v>
       </c>
@@ -7615,7 +7590,7 @@
       <c r="V44" s="4">
         <v>2000</v>
       </c>
-      <c r="W44" s="46">
+      <c r="W44" s="4">
         <v>2005</v>
       </c>
       <c r="Y44" s="2"/>
@@ -7642,11 +7617,11 @@
       <c r="AS44" s="4">
         <v>2015</v>
       </c>
-      <c r="AT44" s="44">
+      <c r="AT44" s="2">
         <v>2012</v>
       </c>
       <c r="AW44" s="2"/>
-      <c r="AX44" s="44"/>
+      <c r="AX44" s="2"/>
       <c r="AY44" s="2"/>
       <c r="AZ44" s="2"/>
       <c r="BA44" s="2"/>
@@ -7668,18 +7643,18 @@
         <v>36</v>
       </c>
       <c r="B45" s="19"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="46">
+      <c r="D45" s="2"/>
+      <c r="E45" s="4">
         <v>2010</v>
       </c>
       <c r="F45" s="4">
         <v>2011</v>
       </c>
-      <c r="G45" s="45"/>
+      <c r="G45" s="13"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
       <c r="AE45" s="2"/>
-      <c r="AT45" s="45">
+      <c r="AT45" s="13">
         <v>2018</v>
       </c>
     </row>
@@ -7687,29 +7662,29 @@
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="2">
         <v>1999</v>
       </c>
-      <c r="D46" s="44"/>
-      <c r="E46" s="46">
+      <c r="D46" s="2"/>
+      <c r="E46" s="4">
         <v>2010</v>
       </c>
       <c r="F46" s="4">
         <v>2011</v>
       </c>
-      <c r="G46" s="45"/>
+      <c r="G46" s="13"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="44"/>
-      <c r="P46" s="44"/>
-      <c r="Q46" s="44"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
-      <c r="W46" s="44"/>
+      <c r="W46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
@@ -7737,7 +7712,7 @@
         <v>2012</v>
       </c>
       <c r="AW46" s="2"/>
-      <c r="AX46" s="45"/>
+      <c r="AX46" s="13"/>
       <c r="AY46" s="2"/>
       <c r="AZ46" s="2"/>
       <c r="BA46" s="2"/>
@@ -7760,24 +7735,24 @@
       <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="44">
+      <c r="C47" s="2">
         <v>1999</v>
       </c>
-      <c r="D47" s="46">
+      <c r="D47" s="4">
         <v>2002</v>
       </c>
-      <c r="E47" s="46">
+      <c r="E47" s="4">
         <v>2007</v>
       </c>
       <c r="F47" s="13"/>
-      <c r="G47" s="45"/>
+      <c r="G47" s="13"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="44"/>
-      <c r="P47" s="44"/>
-      <c r="Q47" s="44"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="13" t="s">
@@ -7786,7 +7761,7 @@
       <c r="V47" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="W47" s="44"/>
+      <c r="W47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
@@ -7812,11 +7787,11 @@
       <c r="AN47" s="2"/>
       <c r="AO47" s="2"/>
       <c r="AP47" s="7"/>
-      <c r="AT47" s="45"/>
+      <c r="AT47" s="13"/>
       <c r="AW47" s="4">
         <v>2003</v>
       </c>
-      <c r="AX47" s="45"/>
+      <c r="AX47" s="13"/>
       <c r="AY47" s="2"/>
       <c r="AZ47" s="2"/>
       <c r="BA47" s="2"/>
@@ -7836,28 +7811,28 @@
         <v>39</v>
       </c>
       <c r="B48" s="19"/>
-      <c r="D48" s="46">
+      <c r="D48" s="4">
         <v>2001</v>
       </c>
-      <c r="E48" s="46">
+      <c r="E48" s="4">
         <v>2011</v>
       </c>
       <c r="F48" s="2">
         <v>2008</v>
       </c>
-      <c r="G48" s="45"/>
+      <c r="G48" s="13"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="44"/>
-      <c r="P48" s="44"/>
-      <c r="Q48" s="44"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-      <c r="W48" s="44"/>
+      <c r="W48" s="2"/>
       <c r="Y48" s="2"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
@@ -7883,7 +7858,7 @@
         <v>2012</v>
       </c>
       <c r="AW48" s="2"/>
-      <c r="AX48" s="45"/>
+      <c r="AX48" s="13"/>
       <c r="AY48" s="2"/>
       <c r="AZ48" s="2"/>
       <c r="BA48" s="2"/>
@@ -7898,15 +7873,15 @@
       <c r="A49" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49">
         <v>2011</v>
       </c>
-      <c r="D49" s="44"/>
-      <c r="E49" s="46">
+      <c r="D49" s="2"/>
+      <c r="E49" s="4">
         <v>2009</v>
       </c>
       <c r="F49" s="13"/>
-      <c r="G49" s="45"/>
+      <c r="G49" s="13"/>
       <c r="U49" s="13" t="s">
         <v>376</v>
       </c>
@@ -7916,31 +7891,31 @@
       <c r="AE49" s="4">
         <v>2003</v>
       </c>
-      <c r="AT49" s="45"/>
+      <c r="AT49" s="13"/>
     </row>
     <row r="50" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="46">
+      <c r="C50" s="4">
         <v>2001</v>
       </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="45"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="13"/>
-      <c r="G50" s="45"/>
+      <c r="G50" s="13"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="44"/>
-      <c r="P50" s="44"/>
-      <c r="Q50" s="44"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
-      <c r="W50" s="44"/>
+      <c r="W50" s="2"/>
       <c r="Y50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
@@ -7962,7 +7937,7 @@
         <v>1999</v>
       </c>
       <c r="AW50" s="2"/>
-      <c r="AX50" s="45"/>
+      <c r="AX50" s="13"/>
       <c r="AY50" s="2"/>
       <c r="AZ50" s="2"/>
       <c r="BA50" s="2"/>
@@ -7979,27 +7954,27 @@
       <c r="A51" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="44">
+      <c r="C51" s="2">
         <v>1999</v>
       </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="45"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="13">
         <v>2018</v>
       </c>
-      <c r="G51" s="45"/>
+      <c r="G51" s="13"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="44"/>
-      <c r="P51" s="44"/>
-      <c r="Q51" s="44"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
-      <c r="W51" s="44"/>
+      <c r="W51" s="2"/>
       <c r="Y51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
@@ -8021,11 +7996,11 @@
       <c r="AN51" s="2"/>
       <c r="AO51" s="2"/>
       <c r="AP51" s="7"/>
-      <c r="AT51" s="44">
+      <c r="AT51" s="2">
         <v>2012</v>
       </c>
       <c r="AW51" s="2"/>
-      <c r="AX51" s="45"/>
+      <c r="AX51" s="13"/>
       <c r="AY51" s="2"/>
       <c r="AZ51" s="2"/>
       <c r="BA51" s="2"/>
@@ -8042,22 +8017,22 @@
       <c r="A52" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52">
         <v>1999</v>
       </c>
-      <c r="D52" s="44"/>
-      <c r="E52" s="46">
+      <c r="D52" s="2"/>
+      <c r="E52" s="4">
         <v>2010</v>
       </c>
       <c r="F52" s="13"/>
-      <c r="G52" s="45"/>
+      <c r="G52" s="13"/>
       <c r="U52" s="13" t="s">
         <v>95</v>
       </c>
       <c r="V52" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="AT52" s="45">
+      <c r="AT52" s="13">
         <v>2013</v>
       </c>
     </row>
@@ -8065,15 +8040,15 @@
       <c r="A53" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="46">
+      <c r="C53" s="4">
         <v>2000</v>
       </c>
-      <c r="D53" s="44"/>
-      <c r="E53" s="46">
+      <c r="D53" s="2"/>
+      <c r="E53" s="4">
         <v>2009</v>
       </c>
       <c r="F53" s="13"/>
-      <c r="G53" s="45"/>
+      <c r="G53" s="13"/>
       <c r="K53" s="4">
         <v>2006</v>
       </c>
@@ -8084,11 +8059,11 @@
         <v>2001</v>
       </c>
       <c r="N53" s="2"/>
-      <c r="O53" s="44"/>
-      <c r="P53" s="46">
+      <c r="O53" s="2"/>
+      <c r="P53" s="4">
         <v>2005</v>
       </c>
-      <c r="Q53" s="46">
+      <c r="Q53" s="4">
         <v>2006</v>
       </c>
       <c r="S53" s="4">
@@ -8103,7 +8078,7 @@
       <c r="V53" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="W53" s="46">
+      <c r="W53" s="4">
         <v>2001</v>
       </c>
       <c r="Y53" s="2"/>
@@ -8131,11 +8106,11 @@
       <c r="AN53" s="2"/>
       <c r="AO53" s="2"/>
       <c r="AP53" s="7"/>
-      <c r="AT53" s="45">
+      <c r="AT53" s="13">
         <v>2015</v>
       </c>
       <c r="AW53" s="2"/>
-      <c r="AX53" s="45"/>
+      <c r="AX53" s="13"/>
       <c r="AY53" s="2"/>
       <c r="AZ53" s="2"/>
       <c r="BA53" s="2"/>
@@ -8164,25 +8139,25 @@
         <v>44</v>
       </c>
       <c r="B56" s="19"/>
-      <c r="D56" s="46">
+      <c r="D56" s="4">
         <v>2000</v>
       </c>
-      <c r="E56" s="46">
+      <c r="E56" s="4">
         <v>2011</v>
       </c>
       <c r="F56" s="13"/>
-      <c r="G56" s="45"/>
+      <c r="G56" s="13"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="13"/>
       <c r="N56" s="4">
         <v>2004</v>
       </c>
-      <c r="O56" s="46">
+      <c r="O56" s="4">
         <v>2004</v>
       </c>
-      <c r="P56" s="44"/>
-      <c r="Q56" s="44"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
       <c r="S56" s="13"/>
       <c r="T56" s="13"/>
       <c r="U56" s="4">
@@ -8191,7 +8166,7 @@
       <c r="V56" s="4">
         <v>2003</v>
       </c>
-      <c r="W56" s="46">
+      <c r="W56" s="4">
         <v>2002</v>
       </c>
       <c r="Y56" s="4">
@@ -8221,9 +8196,9 @@
       <c r="AN56" s="2"/>
       <c r="AO56" s="2"/>
       <c r="AP56" s="7"/>
-      <c r="AT56" s="45"/>
+      <c r="AT56" s="13"/>
       <c r="AW56" s="13"/>
-      <c r="AX56" s="45"/>
+      <c r="AX56" s="13"/>
       <c r="AY56" s="13"/>
       <c r="AZ56" s="13"/>
       <c r="BA56" s="13"/>
@@ -8241,17 +8216,17 @@
       <c r="B57" s="20">
         <v>2013</v>
       </c>
-      <c r="C57" s="44">
+      <c r="C57" s="2">
         <v>1999</v>
       </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="46">
+      <c r="D57" s="2"/>
+      <c r="E57" s="4">
         <v>2010</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="G57" s="45" t="s">
+      <c r="G57" s="13" t="s">
         <v>352</v>
       </c>
       <c r="K57" s="13" t="s">
@@ -8266,18 +8241,18 @@
       <c r="N57" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="O57" s="45" t="s">
+      <c r="O57" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="P57" s="45" t="s">
+      <c r="P57" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="Q57" s="44"/>
+      <c r="Q57" s="2"/>
       <c r="S57" s="13"/>
       <c r="T57" s="13"/>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
-      <c r="W57" s="44"/>
+      <c r="W57" s="2"/>
       <c r="Y57" s="13" t="s">
         <v>72</v>
       </c>
@@ -8322,7 +8297,7 @@
       <c r="AW57" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AX57" s="45"/>
+      <c r="AX57" s="13"/>
       <c r="AY57" s="13" t="s">
         <v>89</v>
       </c>
@@ -8342,14 +8317,12 @@
       <c r="BG57" s="13"/>
     </row>
     <row r="59" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS59" s="63" t="s">
+      <c r="AS59" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AT59" s="64"/>
-      <c r="AU59" s="64" t="s">
+      <c r="AU59" t="s">
         <v>68</v>
       </c>
-      <c r="AV59" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8389,26 +8362,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="45" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -9974,7 +9947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32A262C-BF3B-4D84-B60A-8947EF3BFC30}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cataloged indicators into categories
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84C7A7A-E990-4D8F-950B-0CEB2D8F0DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DF176D-0E4D-406A-91C8-ED1B587686B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -4945,7 +4945,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="42"/>
       <c r="K1" s="1" t="s">
-        <v>108</v>
+        <v>425</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -9947,7 +9947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32A262C-BF3B-4D84-B60A-8947EF3BFC30}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added economic calendar from investing.com
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080252E9-0701-4C90-9293-2329B51C2EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603B4679-70BC-4E33-B0FE-D122D0DAE4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="449">
   <si>
     <t>United States</t>
   </si>
@@ -1381,6 +1381,12 @@
   </si>
   <si>
     <t>Inventories</t>
+  </si>
+  <si>
+    <t>Investing</t>
+  </si>
+  <si>
+    <t>Calendar</t>
   </si>
 </sst>
 </file>
@@ -1622,12 +1628,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1945,11 +1955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
-  <dimension ref="A1:R65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,22 +1968,23 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="9" t="s">
         <v>55</v>
@@ -1987,47 +1998,50 @@
       <c r="E1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="47" t="s">
         <v>382</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="52" t="s">
+        <v>447</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="9" t="s">
         <v>56</v>
@@ -2037,41 +2051,44 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="47"/>
+      <c r="G2" s="42" t="s">
+        <v>448</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -2079,18 +2096,18 @@
       <c r="C3" s="12"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="47"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="12"/>
-      <c r="N3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="12"/>
+      <c r="O3" s="9"/>
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2102,27 +2119,28 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="4">
+      <c r="J4" s="2"/>
+      <c r="K4" s="4">
         <v>2010</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="7">
         <v>2002</v>
       </c>
-      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2">
         <v>1999</v>
       </c>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2134,27 +2152,28 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="4">
+      <c r="J5" s="2"/>
+      <c r="K5" s="4">
         <v>2009</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L5" s="7">
         <v>2006</v>
       </c>
-      <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2">
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2">
         <v>2008</v>
       </c>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2166,27 +2185,28 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="4">
+      <c r="J6" s="2"/>
+      <c r="K6" s="4">
         <v>2010</v>
       </c>
-      <c r="K6" s="8">
+      <c r="L6" s="8">
         <v>2011</v>
       </c>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2">
         <v>2008</v>
       </c>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2198,27 +2218,28 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="4">
+      <c r="J7" s="2"/>
+      <c r="K7" s="4">
         <v>2010</v>
       </c>
-      <c r="K7" s="15">
+      <c r="L7" s="15">
         <v>2016</v>
       </c>
-      <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2">
         <v>2012</v>
       </c>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2230,24 +2251,25 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
         <v>2008</v>
       </c>
-      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2">
         <v>2008</v>
       </c>
-      <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2259,27 +2281,28 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
         <v>2008</v>
       </c>
-      <c r="K9" s="7">
+      <c r="L9" s="7">
         <v>2010</v>
       </c>
-      <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="4"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="2">
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2">
         <v>2012</v>
       </c>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2291,27 +2314,28 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
         <v>2008</v>
       </c>
-      <c r="K10" s="7">
+      <c r="L10" s="7">
         <v>2012</v>
       </c>
-      <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2">
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2">
         <v>2008</v>
       </c>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2323,27 +2347,28 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="4">
+      <c r="J11" s="2"/>
+      <c r="K11" s="4">
         <v>2010</v>
       </c>
-      <c r="K11" s="7">
+      <c r="L11" s="7">
         <v>2007</v>
       </c>
-      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="10">
+      <c r="O11" s="2"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="10">
         <v>41426</v>
       </c>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2355,24 +2380,24 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="48"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
         <v>2008</v>
       </c>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="10">
+      <c r="Q12" s="2"/>
+      <c r="R12" s="10">
         <v>41548</v>
       </c>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -2384,25 +2409,25 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="4">
+      <c r="F13" s="48"/>
+      <c r="H13" s="4">
         <v>2001</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="4">
+      <c r="I13" s="2"/>
+      <c r="J13" s="4">
         <v>2012</v>
       </c>
-      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="36" t="s">
+      <c r="Q13" s="2"/>
+      <c r="R13" s="36" t="s">
         <v>397</v>
       </c>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2414,21 +2439,21 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="48"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="2">
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2">
         <v>1999</v>
       </c>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -2440,27 +2465,28 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="4">
+      <c r="J15" s="2"/>
+      <c r="K15" s="4">
         <v>2011</v>
       </c>
-      <c r="K15" s="15">
+      <c r="L15" s="15">
         <v>2016</v>
       </c>
-      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="2">
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2">
         <v>2012</v>
       </c>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
@@ -2471,19 +2497,20 @@
         <v>0.7</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="13">
+      <c r="J16" s="2"/>
+      <c r="K16" s="13">
         <v>2016</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2">
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -2495,27 +2522,28 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="2"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
         <v>2008</v>
       </c>
-      <c r="K17" s="7">
+      <c r="L17" s="7">
         <v>1999</v>
       </c>
-      <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
-      <c r="Q17" s="2">
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2">
         <v>2012</v>
       </c>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>21</v>
       </c>
@@ -2526,18 +2554,19 @@
         <v>0.43</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="4">
+      <c r="J18" s="2"/>
+      <c r="K18" s="4">
         <v>2011</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="R18" s="2">
         <v>1999</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>17</v>
       </c>
@@ -2549,25 +2578,25 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="4">
+      <c r="F19" s="48"/>
+      <c r="H19" s="4">
         <v>2001</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="4">
+      <c r="I19" s="2"/>
+      <c r="J19" s="4">
         <v>2012</v>
       </c>
-      <c r="J19" s="13">
+      <c r="K19" s="13">
         <v>2008</v>
       </c>
-      <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -2579,21 +2608,21 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="48"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2">
         <v>2008</v>
       </c>
-      <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2605,28 +2634,28 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="10">
+      <c r="F21" s="48"/>
+      <c r="H21" s="10">
         <v>36404</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="4">
+      <c r="I21" s="2"/>
+      <c r="J21" s="4">
         <v>2009</v>
       </c>
-      <c r="J21" s="13">
+      <c r="K21" s="13">
         <v>2008</v>
       </c>
-      <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
-      <c r="Q21" s="2">
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2">
         <v>2004</v>
       </c>
-      <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
@@ -2638,23 +2667,23 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="49"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="4">
+      <c r="I22" s="2"/>
+      <c r="J22" s="4">
         <v>2008</v>
       </c>
-      <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="4"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="2">
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2">
         <v>2012</v>
       </c>
-      <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -2666,23 +2695,23 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="48"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="4">
+      <c r="I23" s="2"/>
+      <c r="J23" s="4">
         <v>2010</v>
       </c>
-      <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="2">
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2">
         <v>2012</v>
       </c>
-      <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
@@ -2694,25 +2723,26 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="4">
+      <c r="F24" s="48"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="4">
         <v>2001</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="4">
+      <c r="I24" s="2"/>
+      <c r="J24" s="4">
         <v>2010</v>
       </c>
-      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="4"/>
+      <c r="N24" s="2"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2">
+      <c r="P24" s="4"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2">
         <v>2012</v>
       </c>
-      <c r="R24" s="2"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2724,24 +2754,24 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="48"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2">
         <v>2008</v>
       </c>
-      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-      <c r="Q25" s="2">
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2">
         <v>2012</v>
       </c>
-      <c r="R25" s="2"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>18</v>
       </c>
@@ -2753,22 +2783,22 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="4">
+      <c r="F26" s="48"/>
+      <c r="H26" s="4">
         <v>2010</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="4">
+      <c r="I26" s="2"/>
+      <c r="J26" s="4">
         <v>2013</v>
       </c>
-      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="R26" s="2"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q26" s="2"/>
+      <c r="S26" s="2"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>68</v>
       </c>
@@ -2778,35 +2808,36 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="2"/>
-      <c r="G27" s="4">
+      <c r="G27" s="7"/>
+      <c r="H27" s="4">
         <v>2007</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="4">
+      <c r="I27" s="2"/>
+      <c r="J27" s="4">
         <v>2002</v>
       </c>
-      <c r="J27" s="2">
+      <c r="K27" s="2">
         <v>2008</v>
       </c>
-      <c r="K27" s="7">
+      <c r="L27" s="7">
         <v>2001</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="R27" s="2"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="S27" s="2"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="C28" s="33"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="33"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2818,35 +2849,36 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="2"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="4">
-        <v>2011</v>
-      </c>
+      <c r="I30" s="2"/>
       <c r="J30" s="4">
         <v>2011</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="4">
         <v>2011</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="7">
         <v>2011</v>
       </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="4">
+      <c r="M30" s="4">
+        <v>2011</v>
+      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="4">
         <v>2002</v>
       </c>
-      <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-      <c r="Q30" s="2">
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2">
         <v>2005</v>
       </c>
-      <c r="R30" s="4">
+      <c r="S30" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>24</v>
       </c>
@@ -2856,23 +2888,23 @@
       <c r="C31" s="33">
         <v>1.8</v>
       </c>
-      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="4">
+      <c r="I31" s="2"/>
+      <c r="J31" s="4">
         <v>2000</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>2008</v>
       </c>
-      <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="Q31" s="2">
+      <c r="P31" s="2"/>
+      <c r="R31" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2884,33 +2916,34 @@
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="2"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="7"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="4">
+      <c r="I32" s="2"/>
+      <c r="J32" s="4">
         <v>2012</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>2008</v>
       </c>
-      <c r="K32" s="7">
+      <c r="L32" s="7">
         <v>2005</v>
       </c>
-      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="13">
+      <c r="N32" s="2"/>
+      <c r="O32" s="13">
         <v>2018</v>
       </c>
-      <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2">
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2">
         <v>2012</v>
       </c>
-      <c r="R32" s="4">
+      <c r="S32" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2922,31 +2955,32 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="2"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="4">
+      <c r="I33" s="2"/>
+      <c r="J33" s="4">
         <v>2000</v>
       </c>
-      <c r="J33" s="2">
+      <c r="K33" s="2">
         <v>2008</v>
       </c>
-      <c r="K33" s="7">
+      <c r="L33" s="7">
         <v>2007</v>
       </c>
-      <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="10">
+      <c r="P33" s="2"/>
+      <c r="Q33" s="10">
         <v>36281</v>
       </c>
-      <c r="Q33" s="2">
+      <c r="R33" s="2">
         <v>2012</v>
       </c>
-      <c r="R33" s="2"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>97</v>
       </c>
@@ -2958,31 +2992,32 @@
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="4">
+      <c r="I34" s="2"/>
+      <c r="J34" s="4">
         <v>2000</v>
       </c>
-      <c r="J34" s="2">
+      <c r="K34" s="2">
         <v>2008</v>
       </c>
-      <c r="K34" s="7">
+      <c r="L34" s="7">
         <v>2012</v>
       </c>
-      <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="4">
+      <c r="N34" s="2"/>
+      <c r="O34" s="4">
         <v>2012</v>
       </c>
-      <c r="O34" s="2"/>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2">
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2">
         <v>2012</v>
       </c>
-      <c r="R34" s="2"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>28</v>
       </c>
@@ -2994,32 +3029,32 @@
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="2"/>
+      <c r="F35" s="51"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="13">
+      <c r="I35" s="2"/>
+      <c r="J35" s="13">
         <v>2015</v>
       </c>
-      <c r="J35" s="13">
+      <c r="K35" s="13">
         <v>2019</v>
       </c>
-      <c r="L35" s="4">
+      <c r="M35" s="4">
         <v>2010</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4">
+      <c r="N35" s="4"/>
+      <c r="O35" s="4">
         <v>2000</v>
       </c>
-      <c r="O35" s="2"/>
-      <c r="P35" s="4">
+      <c r="P35" s="2"/>
+      <c r="Q35" s="4">
         <v>2000</v>
       </c>
-      <c r="Q35" s="2">
+      <c r="R35" s="2">
         <v>2012</v>
       </c>
-      <c r="R35" s="13"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="13"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
@@ -3031,28 +3066,29 @@
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="2"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="7"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="4">
+      <c r="I36" s="2"/>
+      <c r="J36" s="4">
         <v>2003</v>
       </c>
-      <c r="J36" s="4">
+      <c r="K36" s="4">
         <v>2010</v>
       </c>
-      <c r="L36" s="2"/>
       <c r="M36" s="2"/>
-      <c r="N36" s="4">
+      <c r="N36" s="2"/>
+      <c r="O36" s="4">
         <v>2000</v>
       </c>
-      <c r="O36" s="2"/>
       <c r="P36" s="2"/>
-      <c r="Q36" s="2">
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2">
         <v>2012</v>
       </c>
-      <c r="R36" s="2"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="2"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -3064,24 +3100,24 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="2"/>
+      <c r="F37" s="49"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="4">
+      <c r="J37" s="2"/>
+      <c r="K37" s="4">
         <v>2010</v>
       </c>
-      <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
-      <c r="Q37" s="2">
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2">
         <v>2012</v>
       </c>
-      <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>31</v>
       </c>
@@ -3092,20 +3128,20 @@
         <v>0.27</v>
       </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="2"/>
+      <c r="F38" s="49"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="4">
+      <c r="I38" s="2"/>
+      <c r="J38" s="4">
         <v>2008</v>
       </c>
-      <c r="J38" s="4">
+      <c r="K38" s="4">
         <v>2011</v>
       </c>
-      <c r="P38" s="4">
+      <c r="Q38" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
@@ -3117,32 +3153,32 @@
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="2"/>
+      <c r="F39" s="49"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="4">
+      <c r="I39" s="2"/>
+      <c r="J39" s="4">
         <v>2010</v>
       </c>
-      <c r="J39" s="4">
+      <c r="K39" s="4">
         <v>2011</v>
       </c>
-      <c r="L39" s="2"/>
       <c r="M39" s="2"/>
-      <c r="N39" s="4">
+      <c r="N39" s="2"/>
+      <c r="O39" s="4">
         <v>2000</v>
       </c>
-      <c r="O39" s="2"/>
-      <c r="P39" s="4">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="4">
         <v>2005</v>
       </c>
-      <c r="Q39" s="2">
+      <c r="R39" s="2">
         <v>2012</v>
       </c>
-      <c r="R39" s="4">
+      <c r="S39" s="4">
         <v>2002</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>33</v>
       </c>
@@ -3153,16 +3189,16 @@
         <v>0.18</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="2"/>
+      <c r="F40" s="49"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="4">
+      <c r="J40" s="2"/>
+      <c r="K40" s="4">
         <v>2011</v>
       </c>
-      <c r="P40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
@@ -3173,15 +3209,15 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="8"/>
-      <c r="H41" s="10">
+      <c r="F41" s="51"/>
+      <c r="I41" s="10">
         <v>36192</v>
       </c>
-      <c r="I41" s="13">
+      <c r="J41" s="13">
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>34</v>
       </c>
@@ -3192,13 +3228,13 @@
         <v>0.1</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="8"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="13">
+      <c r="F42" s="51"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="13">
         <v>2014</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>35</v>
       </c>
@@ -3209,13 +3245,13 @@
         <v>0.1</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="8"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="13">
+      <c r="F43" s="51"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="13">
         <v>2020</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -3227,33 +3263,33 @@
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="2"/>
+      <c r="F44" s="48"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="4">
+      <c r="I44" s="2"/>
+      <c r="J44" s="4">
         <v>2008</v>
       </c>
-      <c r="J44" s="2">
+      <c r="K44" s="2">
         <v>2008</v>
       </c>
-      <c r="K44" s="7">
+      <c r="L44" s="7">
         <v>2012</v>
       </c>
-      <c r="L44" s="2"/>
       <c r="M44" s="2"/>
-      <c r="N44" s="4">
+      <c r="N44" s="2"/>
+      <c r="O44" s="4">
         <v>2005</v>
       </c>
-      <c r="O44" s="2"/>
-      <c r="P44" s="4">
+      <c r="P44" s="2"/>
+      <c r="Q44" s="4">
         <v>2002</v>
       </c>
-      <c r="Q44" s="2">
+      <c r="R44" s="2">
         <v>2012</v>
       </c>
-      <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="2"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>36</v>
       </c>
@@ -3264,18 +3300,18 @@
         <v>0.09</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="2"/>
+      <c r="F45" s="48"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="4">
+      <c r="I45" s="2"/>
+      <c r="J45" s="4">
         <v>2010</v>
       </c>
-      <c r="J45" s="4">
+      <c r="K45" s="4">
         <v>2011</v>
       </c>
-      <c r="P45" s="2"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
@@ -3287,26 +3323,26 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="2"/>
+      <c r="F46" s="48"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="4">
+      <c r="I46" s="2"/>
+      <c r="J46" s="4">
         <v>2010</v>
       </c>
-      <c r="J46" s="4">
+      <c r="K46" s="4">
         <v>2011</v>
       </c>
-      <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
-      <c r="Q46" s="2">
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2">
         <v>2012</v>
       </c>
-      <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
@@ -3318,24 +3354,24 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="4">
+      <c r="F47" s="49"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="4">
         <v>2002</v>
       </c>
-      <c r="I47" s="4">
+      <c r="J47" s="4">
         <v>2007</v>
       </c>
-      <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
-      <c r="R47" s="4">
+      <c r="Q47" s="2"/>
+      <c r="S47" s="4">
         <v>2003</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>39</v>
       </c>
@@ -3347,30 +3383,30 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="4">
+      <c r="F48" s="48"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="4">
         <v>2001</v>
       </c>
-      <c r="I48" s="4">
+      <c r="J48" s="4">
         <v>2011</v>
       </c>
-      <c r="J48" s="2">
+      <c r="K48" s="2">
         <v>2008</v>
       </c>
-      <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="4">
+      <c r="P48" s="2"/>
+      <c r="Q48" s="4">
         <v>2001</v>
       </c>
-      <c r="Q48" s="2">
+      <c r="R48" s="2">
         <v>2012</v>
       </c>
-      <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48" s="2"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>40</v>
       </c>
@@ -3381,16 +3417,16 @@
         <v>0.03</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="15"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="4">
+      <c r="F49" s="49"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="4">
         <v>2009</v>
       </c>
-      <c r="P49" s="4">
+      <c r="Q49" s="4">
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>41</v>
       </c>
@@ -3402,23 +3438,23 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="4">
+      <c r="F50" s="48"/>
+      <c r="H50" s="4">
         <v>2001</v>
       </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="13"/>
-      <c r="L50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="13"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
-      <c r="Q50" s="2">
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2">
         <v>1999</v>
       </c>
-      <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50" s="2"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
         <v>47</v>
       </c>
@@ -3430,24 +3466,24 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="48"/>
       <c r="H51" s="2"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13">
+      <c r="I51" s="2"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13">
         <v>2018</v>
       </c>
-      <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
-      <c r="Q51" s="2">
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2">
         <v>2012</v>
       </c>
-      <c r="R51" s="2"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51" s="2"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>42</v>
       </c>
@@ -3458,13 +3494,13 @@
         <v>0.01</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="15"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="4">
+      <c r="F52" s="49"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="4">
         <v>2010</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>43</v>
       </c>
@@ -3476,39 +3512,39 @@
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="4">
+      <c r="F53" s="49"/>
+      <c r="H53" s="4">
         <v>2000</v>
       </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="4">
+      <c r="I53" s="2"/>
+      <c r="J53" s="4">
         <v>2009</v>
       </c>
-      <c r="L53" s="4">
+      <c r="M53" s="4">
         <v>2005</v>
       </c>
-      <c r="M53" s="4">
+      <c r="N53" s="4">
         <v>2006</v>
       </c>
-      <c r="N53" s="4">
+      <c r="O53" s="4">
         <v>2001</v>
       </c>
-      <c r="O53" s="2"/>
       <c r="P53" s="2"/>
-      <c r="R53" s="2"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q53" s="2"/>
+      <c r="S53" s="2"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B54" s="30"/>
       <c r="C54" s="33"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="33"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>44</v>
       </c>
@@ -3520,24 +3556,24 @@
       </c>
       <c r="D56" s="24"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="4">
+      <c r="F56" s="49"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="4">
         <v>2000</v>
       </c>
-      <c r="I56" s="4">
+      <c r="J56" s="4">
         <v>2011</v>
       </c>
-      <c r="L56" s="2"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="4">
+      <c r="N56" s="2"/>
+      <c r="O56" s="4">
         <v>2002</v>
       </c>
-      <c r="O56" s="4"/>
-      <c r="P56" s="2"/>
-      <c r="R56" s="13"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P56" s="4"/>
+      <c r="Q56" s="2"/>
+      <c r="S56" s="13"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>45</v>
       </c>
@@ -3549,42 +3585,43 @@
       </c>
       <c r="D57" s="23"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="7"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="4">
+      <c r="I57" s="2"/>
+      <c r="J57" s="4">
         <v>2010</v>
       </c>
-      <c r="J57" s="13" t="s">
+      <c r="K57" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="K57" s="8" t="s">
+      <c r="L57" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="L57" s="13" t="s">
+      <c r="M57" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
-      <c r="Q57" s="2">
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2">
         <v>2012</v>
       </c>
-      <c r="R57" s="13" t="s">
+      <c r="S57" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q59" s="17"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R59" s="17"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="45" t="s">
         <v>398</v>
       </c>
       <c r="C61" s="46"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>390</v>
       </c>
@@ -3592,7 +3629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>399</v>
       </c>
@@ -3600,7 +3637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="13" t="s">
         <v>388</v>
       </c>
@@ -4974,7 +5011,7 @@
     <col min="56" max="56" width="12" customWidth="1"/>
     <col min="57" max="57" width="14" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="15" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="15" style="48" customWidth="1"/>
+    <col min="59" max="59" width="15" customWidth="1"/>
     <col min="60" max="60" width="15" style="6" customWidth="1"/>
     <col min="61" max="62" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -5056,7 +5093,7 @@
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
       <c r="BF1" s="1"/>
-      <c r="BG1" s="47"/>
+      <c r="BG1" s="1"/>
       <c r="BI1" s="45" t="s">
         <v>112</v>
       </c>
@@ -5238,10 +5275,10 @@
       <c r="BF2" t="s">
         <v>362</v>
       </c>
-      <c r="BG2" s="48" t="s">
+      <c r="BG2" t="s">
         <v>360</v>
       </c>
-      <c r="BH2" s="52" t="s">
+      <c r="BH2" s="6" t="s">
         <v>445</v>
       </c>
       <c r="BI2" t="s">
@@ -5426,10 +5463,10 @@
       <c r="BF3" t="s">
         <v>363</v>
       </c>
-      <c r="BG3" s="48" t="s">
+      <c r="BG3" t="s">
         <v>364</v>
       </c>
-      <c r="BH3" s="52" t="s">
+      <c r="BH3" s="6" t="s">
         <v>446</v>
       </c>
       <c r="BI3" t="s">
@@ -5516,7 +5553,7 @@
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
       <c r="BF4" s="2"/>
-      <c r="BG4" s="49"/>
+      <c r="BG4" s="2"/>
       <c r="BH4" s="7"/>
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
@@ -5611,7 +5648,7 @@
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
       <c r="BF5" s="13"/>
-      <c r="BG5" s="50"/>
+      <c r="BG5" s="13"/>
       <c r="BH5" s="7"/>
       <c r="BI5" s="2"/>
       <c r="BJ5" s="2"/>
@@ -5701,7 +5738,7 @@
       <c r="BD6" s="2"/>
       <c r="BE6" s="2"/>
       <c r="BF6" s="2"/>
-      <c r="BG6" s="51">
+      <c r="BG6" s="4">
         <v>2010</v>
       </c>
       <c r="BH6" s="7"/>
@@ -5779,7 +5816,7 @@
       <c r="BD7" s="2"/>
       <c r="BE7" s="2"/>
       <c r="BF7" s="2"/>
-      <c r="BG7" s="49"/>
+      <c r="BG7" s="2"/>
       <c r="BH7" s="7"/>
       <c r="BI7" s="13"/>
       <c r="BJ7" s="2"/>
@@ -5861,7 +5898,7 @@
       <c r="BD8" s="2"/>
       <c r="BE8" s="2"/>
       <c r="BF8" s="2"/>
-      <c r="BG8" s="49"/>
+      <c r="BG8" s="2"/>
       <c r="BH8" s="7"/>
       <c r="BI8" s="2"/>
       <c r="BJ8" s="2"/>
@@ -5949,7 +5986,7 @@
       <c r="BF9" s="4">
         <v>2010</v>
       </c>
-      <c r="BG9" s="50"/>
+      <c r="BG9" s="13"/>
       <c r="BH9" s="7"/>
       <c r="BI9" s="2"/>
       <c r="BJ9" s="2"/>
@@ -6027,7 +6064,7 @@
       <c r="BD10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BF10" s="2"/>
-      <c r="BG10" s="49"/>
+      <c r="BG10" s="2"/>
       <c r="BH10" s="7"/>
       <c r="BI10" s="2"/>
       <c r="BJ10" s="2"/>
@@ -6109,7 +6146,7 @@
       <c r="BD11" s="13"/>
       <c r="BE11" s="13"/>
       <c r="BF11" s="13"/>
-      <c r="BG11" s="50"/>
+      <c r="BG11" s="13"/>
       <c r="BH11" s="7"/>
       <c r="BI11" s="2"/>
       <c r="BJ11" s="2"/>
@@ -6188,7 +6225,7 @@
       <c r="BD12" s="2"/>
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
-      <c r="BG12" s="51">
+      <c r="BG12" s="4">
         <v>2000</v>
       </c>
       <c r="BH12" s="7"/>
@@ -6273,7 +6310,7 @@
       <c r="BD13" s="2"/>
       <c r="BE13" s="2"/>
       <c r="BF13" s="2"/>
-      <c r="BG13" s="50"/>
+      <c r="BG13" s="13"/>
       <c r="BH13" s="7"/>
       <c r="BI13" s="2"/>
       <c r="BJ13" s="2"/>
@@ -6358,7 +6395,7 @@
       <c r="BD14" s="2"/>
       <c r="BE14" s="2"/>
       <c r="BF14" s="2"/>
-      <c r="BG14" s="49"/>
+      <c r="BG14" s="2"/>
       <c r="BH14" s="7"/>
       <c r="BI14" s="2"/>
       <c r="BJ14" s="2"/>
@@ -6438,7 +6475,7 @@
       <c r="BD15" s="2"/>
       <c r="BE15" s="2"/>
       <c r="BF15" s="2"/>
-      <c r="BG15" s="49"/>
+      <c r="BG15" s="2"/>
       <c r="BH15" s="7"/>
       <c r="BI15" s="2"/>
       <c r="BJ15" s="2"/>
@@ -6555,7 +6592,7 @@
       <c r="BD17" s="2"/>
       <c r="BE17" s="2"/>
       <c r="BF17" s="2"/>
-      <c r="BG17" s="49"/>
+      <c r="BG17" s="2"/>
       <c r="BH17" s="7"/>
       <c r="BI17" s="2"/>
       <c r="BJ17" s="2"/>
@@ -6668,7 +6705,7 @@
       <c r="BD19" s="2"/>
       <c r="BE19" s="2"/>
       <c r="BF19" s="2"/>
-      <c r="BG19" s="49"/>
+      <c r="BG19" s="2"/>
       <c r="BH19" s="7"/>
       <c r="BI19" s="2"/>
       <c r="BJ19" s="2"/>
@@ -6751,7 +6788,7 @@
       <c r="BD20" s="2"/>
       <c r="BE20" s="2"/>
       <c r="BF20" s="2"/>
-      <c r="BG20" s="51">
+      <c r="BG20" s="4">
         <v>2000</v>
       </c>
       <c r="BH20" s="7"/>
@@ -6832,7 +6869,7 @@
       <c r="BD21" s="2"/>
       <c r="BE21" s="2"/>
       <c r="BF21" s="2"/>
-      <c r="BG21" s="50"/>
+      <c r="BG21" s="13"/>
       <c r="BH21" s="7"/>
       <c r="BI21" s="13"/>
       <c r="BJ21" s="2"/>
@@ -6909,7 +6946,7 @@
       <c r="BD22" s="2"/>
       <c r="BE22" s="2"/>
       <c r="BF22" s="2"/>
-      <c r="BG22" s="50"/>
+      <c r="BG22" s="13"/>
       <c r="BH22" s="8"/>
       <c r="BI22" s="4">
         <v>2011</v>
@@ -6995,7 +7032,7 @@
       <c r="BD23" s="2"/>
       <c r="BE23" s="2"/>
       <c r="BF23" s="2"/>
-      <c r="BG23" s="50"/>
+      <c r="BG23" s="13"/>
       <c r="BH23" s="7"/>
       <c r="BI23" s="2"/>
       <c r="BJ23" s="2"/>
@@ -7082,7 +7119,7 @@
       <c r="BD24" s="13"/>
       <c r="BE24" s="13"/>
       <c r="BF24" s="13"/>
-      <c r="BG24" s="50"/>
+      <c r="BG24" s="13"/>
       <c r="BH24" s="7"/>
       <c r="BI24" s="2"/>
       <c r="BJ24" s="2"/>
@@ -7159,7 +7196,7 @@
       <c r="BD25" s="2"/>
       <c r="BE25" s="2"/>
       <c r="BF25" s="2"/>
-      <c r="BG25" s="49"/>
+      <c r="BG25" s="2"/>
       <c r="BH25" s="7"/>
       <c r="BI25" s="2"/>
       <c r="BJ25" s="2"/>
@@ -7236,7 +7273,7 @@
       <c r="BD26" s="2"/>
       <c r="BE26" s="2"/>
       <c r="BF26" s="2"/>
-      <c r="BG26" s="51">
+      <c r="BG26" s="4">
         <v>2000</v>
       </c>
       <c r="BH26" s="7"/>
@@ -7324,7 +7361,7 @@
       <c r="BD27" s="2"/>
       <c r="BE27" s="2"/>
       <c r="BF27" s="2"/>
-      <c r="BG27" s="49"/>
+      <c r="BG27" s="2"/>
       <c r="BH27" s="8"/>
       <c r="BI27" s="2"/>
       <c r="BJ27" s="13"/>
@@ -7424,7 +7461,7 @@
       <c r="BD30" s="13"/>
       <c r="BE30" s="13"/>
       <c r="BF30" s="13"/>
-      <c r="BG30" s="49"/>
+      <c r="BG30" s="2"/>
       <c r="BH30" s="8"/>
       <c r="BI30" s="2"/>
       <c r="BJ30" s="13"/>
@@ -7552,7 +7589,7 @@
       <c r="BD32" s="2"/>
       <c r="BE32" s="2"/>
       <c r="BF32" s="2"/>
-      <c r="BG32" s="49"/>
+      <c r="BG32" s="2"/>
       <c r="BH32" s="15">
         <v>2004</v>
       </c>
@@ -7639,7 +7676,7 @@
       <c r="BD33" s="2"/>
       <c r="BE33" s="2"/>
       <c r="BF33" s="2"/>
-      <c r="BG33" s="51">
+      <c r="BG33" s="4">
         <v>2000</v>
       </c>
       <c r="BH33" s="7"/>
@@ -7743,7 +7780,7 @@
       <c r="BD34" s="2"/>
       <c r="BE34" s="2"/>
       <c r="BF34" s="2"/>
-      <c r="BG34" s="49"/>
+      <c r="BG34" s="2"/>
       <c r="BH34" s="7"/>
       <c r="BI34" s="2"/>
       <c r="BJ34" s="2"/>
@@ -7850,7 +7887,7 @@
       <c r="BD35" s="13"/>
       <c r="BE35" s="13"/>
       <c r="BF35" s="13"/>
-      <c r="BG35" s="50"/>
+      <c r="BG35" s="13"/>
       <c r="BH35" s="7"/>
       <c r="BI35" s="13"/>
       <c r="BJ35" s="13"/>
@@ -7931,7 +7968,7 @@
       <c r="BD36" s="13"/>
       <c r="BE36" s="2"/>
       <c r="BF36" s="13"/>
-      <c r="BG36" s="49"/>
+      <c r="BG36" s="2"/>
       <c r="BH36" s="8"/>
       <c r="BI36" s="2"/>
       <c r="BJ36" s="2"/>
@@ -8020,7 +8057,7 @@
       <c r="BF37" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="BG37" s="49"/>
+      <c r="BG37" s="2"/>
       <c r="BH37" s="7"/>
       <c r="BI37" s="4">
         <v>2001</v>
@@ -8145,7 +8182,7 @@
       <c r="BD39" s="13"/>
       <c r="BE39" s="2"/>
       <c r="BF39" s="13"/>
-      <c r="BG39" s="50"/>
+      <c r="BG39" s="13"/>
       <c r="BH39" s="15">
         <v>2008</v>
       </c>
@@ -8379,7 +8416,7 @@
       <c r="BD44" s="2"/>
       <c r="BE44" s="2"/>
       <c r="BF44" s="2"/>
-      <c r="BG44" s="50"/>
+      <c r="BG44" s="13"/>
       <c r="BH44" s="7"/>
       <c r="BI44" s="4">
         <v>2004</v>
@@ -8494,7 +8531,7 @@
       <c r="BD46" s="2"/>
       <c r="BE46" s="2"/>
       <c r="BF46" s="2"/>
-      <c r="BG46" s="49"/>
+      <c r="BG46" s="2"/>
       <c r="BH46" s="7"/>
       <c r="BI46" s="4">
         <v>2001</v>
@@ -8595,7 +8632,7 @@
       <c r="BD47" s="2"/>
       <c r="BE47" s="2"/>
       <c r="BF47" s="2"/>
-      <c r="BG47" s="49"/>
+      <c r="BG47" s="2"/>
       <c r="BH47" s="7"/>
       <c r="BI47" s="4">
         <v>2002</v>
@@ -8682,7 +8719,7 @@
       <c r="BD48" s="2"/>
       <c r="BE48" s="2"/>
       <c r="BF48" s="2"/>
-      <c r="BG48" s="50"/>
+      <c r="BG48" s="13"/>
       <c r="BH48" s="8"/>
       <c r="BI48" s="2"/>
       <c r="BJ48" s="2"/>
@@ -8789,7 +8826,7 @@
       <c r="BD50" s="2"/>
       <c r="BE50" s="2"/>
       <c r="BF50" s="2"/>
-      <c r="BG50" s="49"/>
+      <c r="BG50" s="2"/>
       <c r="BH50" s="7"/>
       <c r="BI50" s="2"/>
       <c r="BJ50" s="2"/>
@@ -8872,7 +8909,7 @@
       <c r="BD51" s="2"/>
       <c r="BE51" s="2"/>
       <c r="BF51" s="2"/>
-      <c r="BG51" s="49"/>
+      <c r="BG51" s="2"/>
       <c r="BH51" s="7"/>
       <c r="BI51" s="2"/>
       <c r="BJ51" s="2"/>
@@ -9012,7 +9049,7 @@
       <c r="BD53" s="2"/>
       <c r="BE53" s="2"/>
       <c r="BF53" s="2"/>
-      <c r="BG53" s="50"/>
+      <c r="BG53" s="13"/>
       <c r="BH53" s="8"/>
       <c r="BI53" s="4">
         <v>2001</v>
@@ -9120,7 +9157,7 @@
       <c r="BD56" s="13"/>
       <c r="BE56" s="13"/>
       <c r="BF56" s="13"/>
-      <c r="BG56" s="50"/>
+      <c r="BG56" s="13"/>
       <c r="BH56" s="8"/>
       <c r="BI56" s="13"/>
       <c r="BJ56" s="13"/>
@@ -9251,7 +9288,7 @@
       <c r="BF57" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="BG57" s="50"/>
+      <c r="BG57" s="13"/>
       <c r="BH57" s="8" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
improved investing calendar web scrapping
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6C286-D844-4EDC-9979-68C2049E5640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B54DC26-338D-4052-9FFC-5029048A2EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -2371,6 +2371,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2430,6 +2431,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2599,6 +2601,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2625,6 +2628,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="10">
         <v>36404</v>
       </c>
@@ -2658,6 +2662,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="4"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="4">
@@ -2686,6 +2691,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="4">
@@ -2745,6 +2751,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2878,6 +2885,7 @@
       <c r="C31" s="33">
         <v>1.8</v>
       </c>
+      <c r="G31" s="7"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="4">
@@ -3020,6 +3028,7 @@
       <c r="D35" s="23"/>
       <c r="E35" s="2"/>
       <c r="F35" s="13"/>
+      <c r="G35" s="7"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="13">
@@ -3091,6 +3100,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -3144,6 +3154,7 @@
       <c r="D39" s="21"/>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
+      <c r="G39" s="7"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="4">
@@ -3254,6 +3265,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
+      <c r="G44" s="7"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="4">
@@ -3314,6 +3326,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="4">
@@ -3547,6 +3560,7 @@
       <c r="D56" s="24"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
+      <c r="G56" s="7"/>
       <c r="H56" s="2"/>
       <c r="I56" s="4">
         <v>2000</v>

</xml_diff>

<commit_message>
refactored investing calendar preprocessing
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDC5B87-AB02-4C06-BFB4-2AD2B2E8C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62162CFB-84BA-4A17-A705-D7CC67E25F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -1949,7 +1949,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A44" sqref="A44:XFD44"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2371,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2601,7 +2601,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2628,7 +2628,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="10">
         <v>36404</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="7"/>
+      <c r="G22" s="15"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="4">
@@ -2691,7 +2691,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="15"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="4">
@@ -2751,7 +2751,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2885,7 +2885,7 @@
       <c r="C31" s="33">
         <v>1.8</v>
       </c>
-      <c r="G31" s="7"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="4">
@@ -3028,7 +3028,7 @@
       <c r="D35" s="23"/>
       <c r="E35" s="2"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="7"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="13">
@@ -3154,7 +3154,7 @@
       <c r="D39" s="21"/>
       <c r="E39" s="2"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="7"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="4">
@@ -3560,7 +3560,7 @@
       <c r="D56" s="24"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="7"/>
+      <c r="G56" s="15"/>
       <c r="H56" s="2"/>
       <c r="I56" s="4">
         <v>2000</v>

</xml_diff>

<commit_message>
extended web scrapping from 1999 for 50 countries
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62162CFB-84BA-4A17-A705-D7CC67E25F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E850D87-4D17-4447-9F06-3E605764F203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -1393,7 +1393,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1447,6 +1447,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1562,7 +1569,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1628,10 +1635,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1649,7 +1659,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1952,7 +1962,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -2401,6 +2411,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="4">
         <v>2001</v>
       </c>
@@ -2571,6 +2582,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="4">
         <v>2001</v>
       </c>
@@ -2601,7 +2613,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="15"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2781,6 +2793,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
+      <c r="G26" s="47"/>
       <c r="H26" s="4">
         <v>2010</v>
       </c>
@@ -3129,6 +3142,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="4"/>
+      <c r="G38" s="15"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="4">
@@ -3191,6 +3205,7 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="4"/>
+      <c r="G40" s="15"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -3211,6 +3226,7 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="13"/>
+      <c r="G41" s="8"/>
       <c r="I41" s="10">
         <v>36192</v>
       </c>
@@ -3230,6 +3246,7 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="13"/>
+      <c r="G42" s="8"/>
       <c r="I42" s="2"/>
       <c r="J42" s="13">
         <v>2014</v>
@@ -3247,6 +3264,7 @@
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="13"/>
+      <c r="G43" s="8"/>
       <c r="I43" s="2"/>
       <c r="J43" s="13">
         <v>2020</v>
@@ -3303,6 +3321,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
+      <c r="G45" s="15"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="4">
@@ -3358,6 +3377,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="4"/>
+      <c r="G47" s="15"/>
       <c r="H47" s="2"/>
       <c r="I47" s="4">
         <v>2002</v>
@@ -3387,6 +3407,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
       <c r="F48" s="2"/>
+      <c r="G48" s="8"/>
       <c r="H48" s="2"/>
       <c r="I48" s="4">
         <v>2001</v>
@@ -3421,6 +3442,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="4"/>
+      <c r="G49" s="8"/>
       <c r="I49" s="2"/>
       <c r="J49" s="4">
         <v>2009</v>
@@ -3442,6 +3464,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="4">
         <v>2001</v>
       </c>
@@ -3470,6 +3493,7 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="13"/>
@@ -3498,6 +3522,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="4"/>
+      <c r="G52" s="8"/>
       <c r="I52" s="2"/>
       <c r="J52" s="4">
         <v>2010</v>
@@ -3516,6 +3541,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="2"/>
       <c r="F53" s="4"/>
+      <c r="G53" s="15"/>
       <c r="H53" s="4">
         <v>2000</v>
       </c>
@@ -3546,6 +3572,7 @@
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="33"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
@@ -3672,7 +3699,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4966,7 +4993,7 @@
       <selection pane="topRight" activeCell="AZ31" sqref="AZ31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -9327,7 +9354,7 @@
       <selection pane="topRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
@@ -10937,7 +10964,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
cataloged and cleaned indicators from economic calendar
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E850D87-4D17-4447-9F06-3E605764F203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF31A5B-5D46-47E5-AA65-5583AA7858AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="452">
   <si>
     <t>United States</t>
   </si>
@@ -1387,6 +1387,15 @@
   </si>
   <si>
     <t>Calendar</t>
+  </si>
+  <si>
+    <t>With 15 countries</t>
+  </si>
+  <si>
+    <t>With 30 countries</t>
+  </si>
+  <si>
+    <t>With ACWI 50</t>
   </si>
 </sst>
 </file>
@@ -1629,19 +1638,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bueno" xfId="2" builtinId="26"/>
-    <cellStyle name="Incorrecto" xfId="3" builtinId="27"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1659,7 +1668,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1962,7 +1971,7 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -2411,7 +2420,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="47"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="4">
         <v>2001</v>
       </c>
@@ -2582,7 +2591,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="49"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="4">
         <v>2001</v>
       </c>
@@ -2793,7 +2802,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="47"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="4">
         <v>2010</v>
       </c>
@@ -3572,7 +3581,7 @@
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="33"/>
-      <c r="G55" s="48"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
@@ -3647,10 +3656,10 @@
       <c r="R59" s="17"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="48" t="s">
         <v>398</v>
       </c>
-      <c r="C61" s="46"/>
+      <c r="C61" s="49"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -3695,11 +3704,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B703FA39-2A94-42E5-99E2-495679D72086}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3709,9 +3718,12 @@
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="9" t="s">
         <v>57</v>
@@ -3734,8 +3746,14 @@
       <c r="H1" s="9" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L1" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
@@ -3756,8 +3774,14 @@
       <c r="H2" s="9" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L2" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -3769,8 +3793,11 @@
       <c r="G3" s="39" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" s="39" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3793,8 +3820,19 @@
       <c r="H4" s="38">
         <v>25.32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="L4" s="38">
+        <f>G4+G5+G6+G7+G8+G9+G10+G12+G11+G15+G17+G30+G32+G33+G37</f>
+        <v>79.919999999999987</v>
+      </c>
+      <c r="M4" s="38">
+        <f>H4+H5+H6+H7+H8+H9+H10+H12+H11+H15+H17+H30+H32+H33+H37</f>
+        <v>72.680000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3817,8 +3855,19 @@
       <c r="H5" s="38">
         <v>4.21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="L5" s="38">
+        <f>L4+G14+G20+G21+G22+G23+G25+G31+G34+G35+G36+G39+G44+G46+G56+G57</f>
+        <v>89.119999999999976</v>
+      </c>
+      <c r="M5" s="38">
+        <f>M4+H14+H20+H21+H22+H23+H25+H31+H34+H35+H36+H39+H44+H46+H56+H57</f>
+        <v>85.890000000000015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -3841,8 +3890,19 @@
       <c r="H6" s="38">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="L6" s="40">
+        <f>SUM(G4:G53)-G27+G56+G57</f>
+        <v>98.199999999999989</v>
+      </c>
+      <c r="M6" s="40">
+        <f>SUM(H4:H53)-H27+H56+H57</f>
+        <v>92.130000000000024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3865,8 +3925,9 @@
       <c r="H7" s="38">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M7" s="44"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -3890,7 +3951,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -3913,7 +3974,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -3937,7 +3998,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -3961,7 +4022,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -3984,7 +4045,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>14</v>
       </c>
@@ -4007,7 +4068,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -4030,7 +4091,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -4054,7 +4115,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
@@ -4981,6 +5042,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4993,7 +5055,7 @@
       <selection pane="topRight" activeCell="AZ31" sqref="AZ31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -5123,13 +5185,13 @@
       <c r="BE1" s="1"/>
       <c r="BF1" s="1"/>
       <c r="BG1" s="1"/>
-      <c r="BI1" s="45" t="s">
+      <c r="BI1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="BJ1" s="45"/>
-      <c r="BK1" s="45"/>
-      <c r="BL1" s="45"/>
-      <c r="BM1" s="45"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -9354,7 +9416,7 @@
       <selection pane="topRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
@@ -9375,26 +9437,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -10964,7 +11026,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
updated and saved remaining market data
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7A71DD-5ABA-440B-8D12-11E8284E7742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CE37B1-D0B0-4587-887F-4B513D632D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="435">
   <si>
     <t>United States</t>
   </si>
@@ -597,12 +597,6 @@
     <t>iShares MSCI Denmark ETF</t>
   </si>
   <si>
-    <t>SLG-OMXH25.HE</t>
-  </si>
-  <si>
-    <t>Seligson &amp; Co OMX Helsinki 25 ETF</t>
-  </si>
-  <si>
     <t>EWD</t>
   </si>
   <si>
@@ -886,12 +880,6 @@
   </si>
   <si>
     <t>Global X MSCI Greece ETF</t>
-  </si>
-  <si>
-    <t>CZX.DE</t>
-  </si>
-  <si>
-    <t>Expat Czech PX UCITS ETF</t>
   </si>
   <si>
     <t>GXG</t>
@@ -1959,7 +1947,7 @@
         <v>55</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>46</v>
@@ -1968,7 +1956,7 @@
         <v>50</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>140</v>
@@ -1977,34 +1965,34 @@
         <v>137</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>87</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2013,12 +2001,12 @@
         <v>56</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="42" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>141</v>
@@ -2029,25 +2017,25 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="12" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>70</v>
@@ -2379,7 +2367,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="36" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="R13" s="2"/>
     </row>
@@ -2538,9 +2526,6 @@
       <c r="I19" s="4">
         <v>2012</v>
       </c>
-      <c r="J19" s="13">
-        <v>2008</v>
-      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3413,9 +3398,6 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="13"/>
-      <c r="J50" s="13">
-        <v>2018</v>
-      </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3532,10 +3514,10 @@
         <v>2010</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="L55" s="13" t="s">
         <v>88</v>
@@ -3556,13 +3538,13 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B59" s="48" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C59" s="49"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C60" s="6">
         <v>15</v>
@@ -3570,7 +3552,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C61" s="6">
         <v>15</v>
@@ -3578,7 +3560,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B62" s="13" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C62" s="6">
         <v>10</v>
@@ -3586,7 +3568,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B63" s="35" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C63" s="6">
         <v>10</v>
@@ -3637,19 +3619,19 @@
         <v>55</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3659,25 +3641,25 @@
         <v>56</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3690,10 +3672,10 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="39" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="L3" s="39" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3720,7 +3702,7 @@
         <v>25.32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="L4" s="38">
         <f>G4+G5+G6+G7+G8+G9+G10+G12+G11+G15+G17+G29+G31+G32+G36</f>
@@ -3755,7 +3737,7 @@
         <v>4.21</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="L5" s="38">
         <f>L4+G14+G20+G21+G22+G23+G25+G30+G33+G34+G35+G38+G43+G45+G54+G55</f>
@@ -3790,7 +3772,7 @@
         <v>3.05</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="L6" s="40">
         <f>SUM(G4:G52)-G27+G54+G55</f>
@@ -4987,7 +4969,7 @@
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="41" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4998,7 +4980,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="42"/>
       <c r="K1" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -5036,7 +5018,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AQ1" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
@@ -5076,22 +5058,22 @@
         <v>139</v>
       </c>
       <c r="E2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" t="s">
+        <v>400</v>
+      </c>
+      <c r="G2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H2" t="s">
+        <v>401</v>
+      </c>
+      <c r="I2" t="s">
         <v>403</v>
       </c>
-      <c r="F2" t="s">
-        <v>404</v>
-      </c>
-      <c r="G2" t="s">
-        <v>401</v>
-      </c>
-      <c r="H2" t="s">
-        <v>405</v>
-      </c>
-      <c r="I2" t="s">
-        <v>407</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="K2" t="s">
         <v>95</v>
@@ -5109,16 +5091,16 @@
         <v>113</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="S2" s="43" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="T2" t="s">
         <v>84</v>
@@ -5127,10 +5109,10 @@
         <v>84</v>
       </c>
       <c r="V2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="X2" t="s">
         <v>87</v>
@@ -5142,13 +5124,13 @@
         <v>115</v>
       </c>
       <c r="AA2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="AB2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="AD2" t="s">
         <v>135</v>
@@ -5187,22 +5169,22 @@
         <v>124</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="AQ2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AR2" t="s">
         <v>413</v>
       </c>
-      <c r="AR2" t="s">
-        <v>417</v>
-      </c>
       <c r="AS2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AT2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="AV2" t="s">
         <v>58</v>
@@ -5226,16 +5208,16 @@
         <v>90</v>
       </c>
       <c r="BC2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="BD2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="BE2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="BF2" s="6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="BG2" t="s">
         <v>72</v>
@@ -5264,7 +5246,7 @@
         <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -5273,16 +5255,16 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="K3" t="s">
         <v>98</v>
@@ -5300,16 +5282,16 @@
         <v>114</v>
       </c>
       <c r="P3" s="17" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="S3" s="43" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="T3" t="s">
         <v>85</v>
@@ -5318,10 +5300,10 @@
         <v>86</v>
       </c>
       <c r="V3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="X3" t="s">
         <v>96</v>
@@ -5330,13 +5312,13 @@
         <v>120</v>
       </c>
       <c r="AA3" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AB3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="AD3" t="s">
         <v>136</v>
@@ -5375,22 +5357,22 @@
         <v>122</v>
       </c>
       <c r="AP3" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>410</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AR3" t="s">
         <v>414</v>
       </c>
-      <c r="AR3" t="s">
-        <v>418</v>
-      </c>
       <c r="AS3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="AT3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AU3" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="AW3" t="s">
         <v>65</v>
@@ -5408,16 +5390,16 @@
         <v>91</v>
       </c>
       <c r="BC3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="BD3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="BE3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="BG3" t="s">
         <v>70</v>
@@ -5618,13 +5600,13 @@
         <v>2011</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -6092,13 +6074,13 @@
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="4" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -6173,13 +6155,13 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -6195,7 +6177,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="13" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AB13" s="2"/>
       <c r="AC13"/>
@@ -6252,13 +6234,13 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -6441,13 +6423,13 @@
         <v>1999</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -6550,18 +6532,16 @@
       <c r="E19" s="4">
         <v>2012</v>
       </c>
-      <c r="F19" s="13">
-        <v>2008</v>
-      </c>
+      <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -6650,7 +6630,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="13" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="AB20" s="4">
         <v>2001</v>
@@ -6710,13 +6690,13 @@
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -7612,13 +7592,13 @@
       <c r="AP33" s="7"/>
       <c r="AQ33" s="13"/>
       <c r="AR33" s="13" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AS33" s="13" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AT33" s="13" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AU33" s="15">
         <v>2010</v>
@@ -8200,13 +8180,13 @@
         <v>2010</v>
       </c>
       <c r="AR43" s="13" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AS43" s="13" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AT43" s="13" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AU43" s="15">
         <v>2008</v>
@@ -8623,9 +8603,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="13">
-        <v>2018</v>
-      </c>
+      <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="4">
         <v>2005</v>
@@ -8782,7 +8760,7 @@
       <c r="AO52" s="2"/>
       <c r="AP52" s="7"/>
       <c r="AQ52" s="13" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AR52" s="4">
         <v>2005</v>
@@ -8837,13 +8815,13 @@
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -8927,10 +8905,10 @@
         <v>2010</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H55" s="4">
         <v>2009</v>
@@ -9005,13 +8983,13 @@
       <c r="AP55" s="7"/>
       <c r="AQ55" s="13"/>
       <c r="AR55" s="13" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AS55" s="13" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AT55" s="13" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AU55" s="7"/>
       <c r="AV55" s="2">
@@ -9092,21 +9070,21 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="C1" s="48" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
       <c r="G1" s="1"/>
       <c r="H1" s="48" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I1" s="48"/>
       <c r="J1" s="48"/>
       <c r="K1" s="48"/>
       <c r="L1" s="1"/>
       <c r="M1" s="48" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="N1" s="48"/>
       <c r="O1" s="48"/>
@@ -9141,7 +9119,7 @@
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>143</v>
@@ -9184,14 +9162,14 @@
       <c r="J4" t="s">
         <v>146</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>2010</v>
       </c>
       <c r="M4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N4" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="O4" t="s">
         <v>146</v>
@@ -9217,22 +9195,22 @@
         <v>1999</v>
       </c>
       <c r="H5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="I5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J5" t="s">
         <v>146</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>2009</v>
       </c>
       <c r="M5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="N5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="O5" t="s">
         <v>146</v>
@@ -9266,19 +9244,19 @@
       <c r="J6" t="s">
         <v>146</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>2010</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>346</v>
+      <c r="M6" t="s">
+        <v>341</v>
+      </c>
+      <c r="N6" t="s">
+        <v>342</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6">
         <v>2011</v>
       </c>
     </row>
@@ -9307,16 +9285,16 @@
       <c r="J7" t="s">
         <v>146</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <v>2010</v>
       </c>
-      <c r="M7" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="O7" s="13" t="s">
+      <c r="M7" t="s">
+        <v>338</v>
+      </c>
+      <c r="N7" t="s">
+        <v>315</v>
+      </c>
+      <c r="O7" t="s">
         <v>146</v>
       </c>
       <c r="P7" s="13">
@@ -9382,10 +9360,10 @@
         <v>2008</v>
       </c>
       <c r="M9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="N9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="O9" t="s">
         <v>146</v>
@@ -9423,10 +9401,10 @@
         <v>2008</v>
       </c>
       <c r="M10" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="N10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="O10" t="s">
         <v>146</v>
@@ -9460,14 +9438,14 @@
       <c r="J11" t="s">
         <v>178</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>2010</v>
       </c>
       <c r="M11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="N11" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="O11" t="s">
         <v>146</v>
@@ -9522,18 +9500,16 @@
       <c r="F13">
         <v>2012</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
         <v>149</v>
@@ -9549,10 +9525,10 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E15" t="s">
         <v>149</v>
@@ -9561,24 +9537,24 @@
         <v>1999</v>
       </c>
       <c r="H15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J15" t="s">
         <v>146</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>2011</v>
       </c>
-      <c r="M15" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="O15" s="13" t="s">
+      <c r="M15" t="s">
+        <v>330</v>
+      </c>
+      <c r="N15" t="s">
+        <v>335</v>
+      </c>
+      <c r="O15" t="s">
         <v>146</v>
       </c>
       <c r="P15" s="13">
@@ -9590,10 +9566,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E16" t="s">
         <v>149</v>
@@ -9601,29 +9577,28 @@
       <c r="F16">
         <v>1999</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="H16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I16" t="s">
+        <v>193</v>
+      </c>
+      <c r="J16" t="s">
         <v>146</v>
       </c>
       <c r="K16" s="13">
         <v>2016</v>
       </c>
-      <c r="M16" s="13"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
         <v>149</v>
@@ -9632,10 +9607,10 @@
         <v>1999</v>
       </c>
       <c r="H17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J17" t="s">
         <v>146</v>
@@ -9644,10 +9619,10 @@
         <v>2008</v>
       </c>
       <c r="M17" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="N17" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="O17" t="s">
         <v>146</v>
@@ -9661,10 +9636,10 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E18" t="s">
         <v>149</v>
@@ -9673,10 +9648,10 @@
         <v>1999</v>
       </c>
       <c r="H18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J18" t="s">
         <v>146</v>
@@ -9684,17 +9659,16 @@
       <c r="K18">
         <v>2011</v>
       </c>
-      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E19" t="s">
         <v>149</v>
@@ -9702,29 +9676,16 @@
       <c r="F19">
         <v>2012</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="K19" s="13">
-        <v>2008</v>
-      </c>
-      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
         <v>149</v>
@@ -9733,10 +9694,10 @@
         <v>1999</v>
       </c>
       <c r="H20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J20" t="s">
         <v>146</v>
@@ -9751,27 +9712,27 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E21" t="s">
         <v>149</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="4">
         <v>2009</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>213</v>
+      <c r="H21" t="s">
+        <v>289</v>
+      </c>
+      <c r="I21" t="s">
+        <v>211</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="K21" s="13">
+        <v>212</v>
+      </c>
+      <c r="K21">
         <v>2008</v>
       </c>
       <c r="M21" s="13"/>
@@ -9781,15 +9742,15 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E22" t="s">
         <v>149</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="4">
         <v>2008</v>
       </c>
       <c r="H22" s="13"/>
@@ -9800,15 +9761,15 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E23" t="s">
         <v>149</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>2010</v>
       </c>
       <c r="H23" s="13"/>
@@ -9819,10 +9780,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E24" t="s">
         <v>149</v>
@@ -9830,18 +9791,16 @@
       <c r="F24">
         <v>2010</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E25" t="s">
         <v>149</v>
@@ -9850,10 +9809,10 @@
         <v>1999</v>
       </c>
       <c r="H25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I25" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J25" t="s">
         <v>146</v>
@@ -9868,10 +9827,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E26" t="s">
         <v>149</v>
@@ -9879,18 +9838,16 @@
       <c r="F26">
         <v>2013</v>
       </c>
-      <c r="H26" s="13"/>
-      <c r="M26" s="13"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E27" t="s">
         <v>149</v>
@@ -9899,10 +9856,10 @@
         <v>2002</v>
       </c>
       <c r="H27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J27" t="s">
         <v>146</v>
@@ -9911,10 +9868,10 @@
         <v>2008</v>
       </c>
       <c r="M27" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="N27" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="O27" t="s">
         <v>146</v>
@@ -9933,34 +9890,34 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E29" t="s">
         <v>149</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="4">
         <v>2011</v>
       </c>
       <c r="H29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J29" t="s">
         <v>146</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="4">
         <v>2011</v>
       </c>
       <c r="M29" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="N29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="O29" t="s">
         <v>146</v>
@@ -9974,22 +9931,22 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E30" t="s">
         <v>149</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="4">
         <v>2000</v>
       </c>
       <c r="H30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J30" t="s">
         <v>146</v>
@@ -10004,22 +9961,22 @@
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D31" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E31" t="s">
         <v>149</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="4">
         <v>2012</v>
       </c>
       <c r="H31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I31" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J31" t="s">
         <v>146</v>
@@ -10028,10 +9985,10 @@
         <v>2008</v>
       </c>
       <c r="M31" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="N31" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="O31" t="s">
         <v>146</v>
@@ -10045,22 +10002,22 @@
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D32" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E32" t="s">
         <v>149</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="4">
         <v>2000</v>
       </c>
       <c r="H32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J32" t="s">
         <v>146</v>
@@ -10069,10 +10026,10 @@
         <v>2008</v>
       </c>
       <c r="M32" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="N32" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="O32" t="s">
         <v>146</v>
@@ -10086,22 +10043,22 @@
         <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D33" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E33" t="s">
         <v>149</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="4">
         <v>2000</v>
       </c>
       <c r="H33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J33" t="s">
         <v>146</v>
@@ -10110,10 +10067,10 @@
         <v>2008</v>
       </c>
       <c r="M33" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="N33" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="O33" t="s">
         <v>146</v>
@@ -10126,25 +10083,25 @@
       <c r="A34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" t="s">
+        <v>250</v>
+      </c>
+      <c r="E34" t="s">
         <v>251</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>253</v>
       </c>
       <c r="F34" s="13">
         <v>2015</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="J34" s="13" t="s">
+      <c r="H34" t="s">
+        <v>253</v>
+      </c>
+      <c r="I34" t="s">
+        <v>252</v>
+      </c>
+      <c r="J34" t="s">
         <v>178</v>
       </c>
       <c r="K34" s="13">
@@ -10157,27 +10114,27 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D35" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E35" t="s">
         <v>149</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="4">
         <v>2003</v>
       </c>
       <c r="H35" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I35" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J35" t="s">
         <v>146</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="4">
         <v>2010</v>
       </c>
       <c r="M35" s="13"/>
@@ -10187,10 +10144,10 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E36" t="s">
         <v>149</v>
@@ -10199,15 +10156,15 @@
         <v>1999</v>
       </c>
       <c r="H36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I36" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J36" t="s">
         <v>146</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="4">
         <v>2010</v>
       </c>
       <c r="M36" s="13"/>
@@ -10217,10 +10174,10 @@
         <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E37" t="s">
         <v>149</v>
@@ -10229,10 +10186,10 @@
         <v>2008</v>
       </c>
       <c r="H37" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I37" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J37" t="s">
         <v>146</v>
@@ -10240,34 +10197,33 @@
       <c r="K37">
         <v>2011</v>
       </c>
-      <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E38" t="s">
         <v>149</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="4">
         <v>2010</v>
       </c>
       <c r="H38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I38" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J38" t="s">
         <v>146</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="4">
         <v>2011</v>
       </c>
       <c r="M38" s="13"/>
@@ -10277,10 +10233,10 @@
         <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D39" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E39" t="s">
         <v>149</v>
@@ -10289,10 +10245,10 @@
         <v>1999</v>
       </c>
       <c r="H39" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I39" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J39" t="s">
         <v>146</v>
@@ -10300,86 +10256,79 @@
       <c r="K39">
         <v>2011</v>
       </c>
-      <c r="M39" s="13"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="E40" s="13" t="s">
+      <c r="C40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E40" t="s">
         <v>149</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40">
         <v>2014</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="M40" s="13"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="E41" s="13" t="s">
+      <c r="C41" t="s">
+        <v>302</v>
+      </c>
+      <c r="D41" t="s">
+        <v>303</v>
+      </c>
+      <c r="E41" t="s">
         <v>149</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41">
         <v>2014</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="M41" s="13"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="E42" s="13" t="s">
+      <c r="C42" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42" t="s">
+        <v>305</v>
+      </c>
+      <c r="E42" t="s">
         <v>149</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42">
         <v>2020</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="M42" s="13"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D43" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E43" t="s">
         <v>149</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="4">
         <v>2008</v>
       </c>
       <c r="H43" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I43" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J43" t="s">
         <v>146</v>
@@ -10388,10 +10337,10 @@
         <v>2008</v>
       </c>
       <c r="M43" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="N43" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O43" t="s">
         <v>146</v>
@@ -10405,10 +10354,10 @@
         <v>36</v>
       </c>
       <c r="C44" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D44" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E44" t="s">
         <v>149</v>
@@ -10417,10 +10366,10 @@
         <v>2010</v>
       </c>
       <c r="H44" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="I44" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="J44" t="s">
         <v>146</v>
@@ -10428,34 +10377,33 @@
       <c r="K44">
         <v>2011</v>
       </c>
-      <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E45" t="s">
         <v>149</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="4">
         <v>2010</v>
       </c>
       <c r="H45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I45" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J45" t="s">
         <v>146</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="4">
         <v>2011</v>
       </c>
       <c r="M45" s="13"/>
@@ -10465,10 +10413,10 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E46" t="s">
         <v>149</v>
@@ -10476,18 +10424,16 @@
       <c r="F46">
         <v>2007</v>
       </c>
-      <c r="H46" s="13"/>
-      <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D47" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E47" t="s">
         <v>149</v>
@@ -10496,10 +10442,10 @@
         <v>2011</v>
       </c>
       <c r="H47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I47" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J47" t="s">
         <v>146</v>
@@ -10507,17 +10453,16 @@
       <c r="K47">
         <v>2008</v>
       </c>
-      <c r="M47" s="13"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D48" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E48" t="s">
         <v>149</v>
@@ -10525,45 +10470,26 @@
       <c r="F48">
         <v>2009</v>
       </c>
-      <c r="H48" s="13"/>
-      <c r="M48" s="13"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="M49" s="13"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="H50" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="J50" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="K50" s="13">
-        <v>2018</v>
-      </c>
-      <c r="M50" s="13"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D51" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E51" t="s">
         <v>149</v>
@@ -10571,18 +10497,16 @@
       <c r="F51">
         <v>2010</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="M51" s="13"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D52" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E52" t="s">
         <v>149</v>
@@ -10590,8 +10514,6 @@
       <c r="F52">
         <v>2009</v>
       </c>
-      <c r="H52" s="13"/>
-      <c r="M52" s="13"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -10603,15 +10525,15 @@
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D54" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E54" t="s">
-        <v>253</v>
-      </c>
-      <c r="F54">
+        <v>251</v>
+      </c>
+      <c r="F54" s="4">
         <v>2011</v>
       </c>
       <c r="H54" s="13"/>
@@ -10622,40 +10544,40 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D55" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E55" t="s">
         <v>149</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="4">
         <v>2010</v>
       </c>
-      <c r="H55" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="I55" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="J55" s="13" t="s">
+      <c r="H55" t="s">
+        <v>286</v>
+      </c>
+      <c r="I55" t="s">
+        <v>287</v>
+      </c>
+      <c r="J55" t="s">
         <v>146</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="M55" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="N55" s="13" t="s">
-        <v>350</v>
-      </c>
-      <c r="O55" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="M55" t="s">
+        <v>345</v>
+      </c>
+      <c r="N55" t="s">
+        <v>346</v>
+      </c>
+      <c r="O55" t="s">
         <v>149</v>
       </c>
       <c r="P55" s="13" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combined, cleaned and saved to db PMI indicators
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CF225C-F7DF-4256-B7D1-E1A5C1DD5463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC8C85C-9BEF-4CEE-87B3-21E0BBC2B4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -1617,9 +1617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1657,7 +1657,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1763,7 +1763,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1905,7 +1905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1915,7 +1915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -4905,9 +4905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
   <dimension ref="A1:BK57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AV24" sqref="AV24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added country weights in ACWI
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC8C85C-9BEF-4CEE-87B3-21E0BBC2B4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA230CA-230F-4184-A73F-D8D745A9273D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Detailed indices" sheetId="3" r:id="rId3"/>
     <sheet name="ETFs" sheetId="4" r:id="rId4"/>
     <sheet name="Sorted countries" sheetId="2" r:id="rId5"/>
+    <sheet name="Country weights" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="455">
   <si>
     <t>United States</t>
   </si>
@@ -1345,6 +1346,66 @@
   </si>
   <si>
     <t>UBS (Lux) MSCI Hong Kong UCITS ETF</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Marocco</t>
+  </si>
+  <si>
+    <t>Total EM</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Significant</t>
+  </si>
+  <si>
+    <t>Notable</t>
+  </si>
+  <si>
+    <t>Marginal</t>
+  </si>
+  <si>
+    <t>0.8 - 2.0%</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>&gt; 40%</t>
+  </si>
+  <si>
+    <t>Japan and UK</t>
+  </si>
+  <si>
+    <t>4 - 10%</t>
+  </si>
+  <si>
+    <t>2 - 4%</t>
+  </si>
+  <si>
+    <t>MSCI EM:</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>0.3 - 0.8%</t>
+  </si>
+  <si>
+    <t>&lt;= 0.3%</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1478,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1493,6 +1554,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1527,7 +1606,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1590,12 +1669,21 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1617,9 +1705,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1657,7 +1745,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1763,7 +1851,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1905,7 +1993,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1917,7 +2005,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,10 +3625,10 @@
       <c r="Q57" s="17"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="48" t="s">
+      <c r="B59" s="49" t="s">
         <v>379</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="50"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
@@ -4905,8 +4993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EBD188-E2E0-4927-8EED-FFEB431050C3}">
   <dimension ref="A1:BK57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AV24" sqref="AV24"/>
     </sheetView>
   </sheetViews>
@@ -5038,13 +5126,13 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BG1" s="48" t="s">
+      <c r="BG1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
+      <c r="BH1" s="49"/>
+      <c r="BI1" s="49"/>
+      <c r="BJ1" s="49"/>
+      <c r="BK1" s="49"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -9045,7 +9133,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9069,26 +9157,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="49" t="s">
         <v>246</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="49" t="s">
         <v>346</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -10860,4 +10948,3515 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE8DE30-8CF4-49FE-905A-5BDCBDCD0F61}">
+  <dimension ref="A1:AL73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="18"/>
+    <col min="37" max="37" width="9.140625" style="48"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1">
+        <f>1988</f>
+        <v>1988</v>
+      </c>
+      <c r="C1">
+        <f t="shared" ref="C1:AL1" si="0">B1+1</f>
+        <v>1989</v>
+      </c>
+      <c r="D1">
+        <f t="shared" si="0"/>
+        <v>1990</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>1991</v>
+      </c>
+      <c r="F1">
+        <f t="shared" si="0"/>
+        <v>1992</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
+        <v>1993</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>1994</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>1995</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>1996</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>1997</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>1998</v>
+      </c>
+      <c r="M1" s="18">
+        <f t="shared" si="0"/>
+        <v>1999</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="O1">
+        <f t="shared" si="0"/>
+        <v>2001</v>
+      </c>
+      <c r="P1">
+        <f t="shared" si="0"/>
+        <v>2002</v>
+      </c>
+      <c r="Q1">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="R1">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="S1">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="T1">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="U1">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="V1">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="W1">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="X1">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="Y1">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="Z1">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="AA1">
+        <f>Z1+1</f>
+        <v>2013</v>
+      </c>
+      <c r="AB1">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="AC1">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="AD1">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="AE1">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="AF1">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="AG1">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="AH1">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="AI1">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="AJ1">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="AK1" s="48">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="AL1">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38">
+        <v>32.75</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38">
+        <v>40.44</v>
+      </c>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38">
+        <v>46.56</v>
+      </c>
+      <c r="M4" s="55"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38">
+        <v>53.99</v>
+      </c>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38">
+        <v>41.8</v>
+      </c>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38">
+        <v>47.45</v>
+      </c>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="38">
+        <v>58.6</v>
+      </c>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="38">
+        <v>59.3</v>
+      </c>
+      <c r="AL4">
+        <v>63.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="38">
+        <v>40.15</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38">
+        <v>22.69</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38">
+        <v>11.26</v>
+      </c>
+      <c r="M5" s="55"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38">
+        <v>8.44</v>
+      </c>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38">
+        <v>8.6</v>
+      </c>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38">
+        <v>7.5</v>
+      </c>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38">
+        <v>6.2</v>
+      </c>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="38">
+        <v>6.1</v>
+      </c>
+      <c r="AL5">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="52">
+        <v>10.4</v>
+      </c>
+      <c r="M6" s="55"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="52">
+        <v>11.5</v>
+      </c>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="52">
+        <v>9.6</v>
+      </c>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="52">
+        <v>7.9</v>
+      </c>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AI6" s="38">
+        <v>4</v>
+      </c>
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="38">
+        <v>3.9</v>
+      </c>
+      <c r="AL6">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="38">
+        <v>2.42</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38">
+        <v>2.29</v>
+      </c>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38">
+        <v>2.29</v>
+      </c>
+      <c r="M7" s="55"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38">
+        <v>3.67</v>
+      </c>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="38">
+        <v>4.3</v>
+      </c>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="38"/>
+      <c r="AI7" s="38">
+        <v>2.9</v>
+      </c>
+      <c r="AJ7" s="38"/>
+      <c r="AK7" s="38">
+        <v>3</v>
+      </c>
+      <c r="AL7">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="52">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M8" s="55"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="52">
+        <v>3.1</v>
+      </c>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="52">
+        <v>4.2</v>
+      </c>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="52">
+        <v>3.1</v>
+      </c>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="AJ8" s="38"/>
+      <c r="AK8" s="38">
+        <v>3</v>
+      </c>
+      <c r="AL8">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="52">
+        <v>3.4</v>
+      </c>
+      <c r="M9" s="55"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="52">
+        <v>3.1</v>
+      </c>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="52">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="52">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="38"/>
+      <c r="AH9" s="38"/>
+      <c r="AI9" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="AJ9" s="38"/>
+      <c r="AK9" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="AL9">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="52">
+        <v>4.2</v>
+      </c>
+      <c r="M10" s="55"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="52">
+        <v>2.6</v>
+      </c>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="52">
+        <v>3.7</v>
+      </c>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="52">
+        <v>2.9</v>
+      </c>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="38">
+        <v>2.1</v>
+      </c>
+      <c r="AL10">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38">
+        <v>1.48</v>
+      </c>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38">
+        <v>1.22</v>
+      </c>
+      <c r="M11" s="55"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38">
+        <v>1.88</v>
+      </c>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38">
+        <v>2.79</v>
+      </c>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38">
+        <v>3.31</v>
+      </c>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="38">
+        <v>1.9</v>
+      </c>
+      <c r="AJ11" s="38"/>
+      <c r="AK11" s="38">
+        <v>2</v>
+      </c>
+      <c r="AL11">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="Q12" s="52">
+        <v>1.6</v>
+      </c>
+      <c r="V12" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="AA12" s="52">
+        <v>0.8</v>
+      </c>
+      <c r="AI12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AK12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AL12">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="52">
+        <v>1.2</v>
+      </c>
+      <c r="M13" s="55"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="52">
+        <v>1.2</v>
+      </c>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="38"/>
+      <c r="V13" s="52">
+        <v>1.3</v>
+      </c>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="52">
+        <v>1.2</v>
+      </c>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
+      <c r="AI13" s="38">
+        <v>1.2</v>
+      </c>
+      <c r="AJ13" s="38"/>
+      <c r="AK13" s="38">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="52">
+        <v>1.2</v>
+      </c>
+      <c r="M14" s="55"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="52">
+        <v>1.9</v>
+      </c>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="52">
+        <v>0.96</v>
+      </c>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AI14" s="38">
+        <v>0.61</v>
+      </c>
+      <c r="AJ14" s="38"/>
+      <c r="AK14" s="38">
+        <v>0.66</v>
+      </c>
+      <c r="AL14">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="38">
+        <v>0.76</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38">
+        <v>1.56</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38">
+        <v>1.25</v>
+      </c>
+      <c r="M15" s="55"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38">
+        <v>0.64</v>
+      </c>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38">
+        <v>1.05</v>
+      </c>
+      <c r="W15" s="38"/>
+      <c r="X15" s="38"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="38">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AB15" s="38"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="38"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="38"/>
+      <c r="AG15" s="38"/>
+      <c r="AH15" s="38"/>
+      <c r="AI15" s="38">
+        <v>0.79</v>
+      </c>
+      <c r="AJ15" s="38"/>
+      <c r="AK15" s="38">
+        <v>0.7</v>
+      </c>
+      <c r="AL15">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="52">
+        <v>1.9</v>
+      </c>
+      <c r="M16" s="55"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="52">
+        <v>1.8</v>
+      </c>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="52">
+        <v>0.79</v>
+      </c>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="38"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="38"/>
+      <c r="AG16" s="38"/>
+      <c r="AH16" s="38"/>
+      <c r="AI16" s="38">
+        <v>0.67</v>
+      </c>
+      <c r="AJ16" s="38"/>
+      <c r="AK16" s="38">
+        <v>0.69</v>
+      </c>
+      <c r="AL16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="38">
+        <v>0.49</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38">
+        <v>0.77</v>
+      </c>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="M17" s="55"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38">
+        <v>0.33</v>
+      </c>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38">
+        <v>0.48</v>
+      </c>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38">
+        <v>0.71</v>
+      </c>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="38">
+        <v>0.32</v>
+      </c>
+      <c r="AJ17" s="38"/>
+      <c r="AK17" s="38">
+        <v>0.43</v>
+      </c>
+      <c r="AL17">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="M18" s="55"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="52">
+        <v>0.37</v>
+      </c>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
+      <c r="AI18" s="38">
+        <v>0.68</v>
+      </c>
+      <c r="AJ18" s="38"/>
+      <c r="AK18" s="38">
+        <v>0.77</v>
+      </c>
+      <c r="AL18">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="52">
+        <v>0.45</v>
+      </c>
+      <c r="M19" s="55"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="52">
+        <v>0.45</v>
+      </c>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="52">
+        <v>0.27</v>
+      </c>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38">
+        <v>0.33</v>
+      </c>
+      <c r="AJ19" s="38"/>
+      <c r="AK19" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="AL19">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="M20" s="55"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="52">
+        <v>0.49</v>
+      </c>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
+      <c r="AI20" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="AJ20" s="38"/>
+      <c r="AK20" s="38">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AL20">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="M21" s="55"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="52">
+        <v>0.6</v>
+      </c>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="52">
+        <v>0.34</v>
+      </c>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38">
+        <v>0.24</v>
+      </c>
+      <c r="AJ21" s="38"/>
+      <c r="AK21" s="38">
+        <v>0.24</v>
+      </c>
+      <c r="AL21">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="38">
+        <v>0.17</v>
+      </c>
+      <c r="M22" s="55"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38">
+        <v>0.13</v>
+      </c>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38">
+        <v>0.24</v>
+      </c>
+      <c r="W22" s="38"/>
+      <c r="X22" s="38"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="38">
+        <v>0.21</v>
+      </c>
+      <c r="AB22" s="38"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="38"/>
+      <c r="AG22" s="38"/>
+      <c r="AH22" s="38"/>
+      <c r="AI22" s="38">
+        <v>0.26</v>
+      </c>
+      <c r="AJ22" s="38"/>
+      <c r="AK22" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="AL22">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="M23" s="55"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
+      <c r="U23" s="38"/>
+      <c r="V23" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="52">
+        <v>0.19</v>
+      </c>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="38"/>
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="38"/>
+      <c r="AI23" s="38">
+        <v>0.18</v>
+      </c>
+      <c r="AJ23" s="38"/>
+      <c r="AK23" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="AL23">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.19</v>
+      </c>
+      <c r="G24">
+        <v>0.17</v>
+      </c>
+      <c r="L24" s="38">
+        <v>0.13</v>
+      </c>
+      <c r="M24" s="55"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="W24" s="38"/>
+      <c r="X24" s="38"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="AB24" s="38"/>
+      <c r="AC24" s="38"/>
+      <c r="AD24" s="38"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="38"/>
+      <c r="AG24" s="38"/>
+      <c r="AH24" s="38"/>
+      <c r="AI24" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="AJ24" s="38"/>
+      <c r="AK24" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="AL24">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="M25" s="55"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="52">
+        <v>0.08</v>
+      </c>
+      <c r="AB25" s="38"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="38"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AG25" s="38"/>
+      <c r="AH25" s="38"/>
+      <c r="AI25" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="AJ25" s="38"/>
+      <c r="AK25" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="AL25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>0.08</v>
+      </c>
+      <c r="G26">
+        <v>0.09</v>
+      </c>
+      <c r="L26" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="M26" s="55"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="52">
+        <v>0.06</v>
+      </c>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="38"/>
+      <c r="AE26" s="38"/>
+      <c r="AF26" s="38"/>
+      <c r="AG26" s="38"/>
+      <c r="AH26" s="38"/>
+      <c r="AI26" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="AJ26" s="38"/>
+      <c r="AK26" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="AL26">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="55"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="38"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="38"/>
+      <c r="AG27" s="38"/>
+      <c r="AH27" s="38"/>
+      <c r="AI27" s="38"/>
+      <c r="AJ27" s="38"/>
+      <c r="AK27" s="38"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="M28" s="55"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38">
+        <v>0.26</v>
+      </c>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="W28" s="38"/>
+      <c r="X28" s="38"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="38">
+        <v>2.23</v>
+      </c>
+      <c r="AB28" s="38"/>
+      <c r="AD28" s="38"/>
+      <c r="AE28" s="38"/>
+      <c r="AF28" s="51"/>
+      <c r="AH28" s="38"/>
+      <c r="AI28" s="38">
+        <v>3.8</v>
+      </c>
+      <c r="AJ28" s="38"/>
+      <c r="AK28" s="38">
+        <v>3.3</v>
+      </c>
+      <c r="AL28">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M29" s="55"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38">
+        <v>0.51</v>
+      </c>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="W29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Z29" s="38"/>
+      <c r="AA29" s="38">
+        <v>1.34</v>
+      </c>
+      <c r="AB29" s="38"/>
+      <c r="AD29" s="38"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="38"/>
+      <c r="AG29" s="38"/>
+      <c r="AH29" s="38"/>
+      <c r="AI29" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="AJ29" s="38"/>
+      <c r="AK29" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="AL29">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="M30" s="55"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38">
+        <v>0.94</v>
+      </c>
+      <c r="W30" s="38"/>
+      <c r="X30" s="38"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30">
+        <v>0.79</v>
+      </c>
+      <c r="AB30" s="38"/>
+      <c r="AD30" s="38"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="38"/>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="38"/>
+      <c r="AI30" s="38">
+        <v>1.4</v>
+      </c>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="38">
+        <v>1.6</v>
+      </c>
+      <c r="AL30">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="38">
+        <v>0.72</v>
+      </c>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="M31" s="55"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38">
+        <v>0.86</v>
+      </c>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="38"/>
+      <c r="V31" s="38">
+        <v>1.62</v>
+      </c>
+      <c r="W31" s="38"/>
+      <c r="X31" s="38"/>
+      <c r="Z31" s="38"/>
+      <c r="AA31">
+        <v>1.94</v>
+      </c>
+      <c r="AB31" s="38"/>
+      <c r="AD31" s="38"/>
+      <c r="AE31" s="38"/>
+      <c r="AF31" s="38"/>
+      <c r="AG31" s="38"/>
+      <c r="AH31" s="38"/>
+      <c r="AI31" s="38">
+        <v>1.7</v>
+      </c>
+      <c r="AJ31" s="38"/>
+      <c r="AK31" s="38">
+        <v>1.4</v>
+      </c>
+      <c r="AL31">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="51">
+        <v>0.19</v>
+      </c>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38">
+        <v>0.47</v>
+      </c>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38">
+        <v>1.02</v>
+      </c>
+      <c r="M32" s="55"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="38"/>
+      <c r="V32" s="38">
+        <v>1.51</v>
+      </c>
+      <c r="W32" s="38"/>
+      <c r="X32" s="38"/>
+      <c r="Z32" s="38"/>
+      <c r="AA32">
+        <v>1.64</v>
+      </c>
+      <c r="AB32" s="38"/>
+      <c r="AD32" s="38"/>
+      <c r="AE32" s="38"/>
+      <c r="AF32" s="38"/>
+      <c r="AG32" s="38"/>
+      <c r="AH32" s="38"/>
+      <c r="AI32" s="38">
+        <v>0.65</v>
+      </c>
+      <c r="AJ32" s="38"/>
+      <c r="AK32" s="38">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AL32">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="38">
+        <v>0.37</v>
+      </c>
+      <c r="M33" s="55"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="38"/>
+      <c r="U33" s="38"/>
+      <c r="V33" s="38">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="W33" s="38"/>
+      <c r="X33" s="38"/>
+      <c r="Z33" s="38"/>
+      <c r="AA33" s="38">
+        <v>0.76</v>
+      </c>
+      <c r="AB33" s="38"/>
+      <c r="AC33" s="38"/>
+      <c r="AD33" s="38"/>
+      <c r="AE33" s="38"/>
+      <c r="AF33" s="38"/>
+      <c r="AG33" s="38"/>
+      <c r="AH33" s="38"/>
+      <c r="AI33" s="38">
+        <v>0.38</v>
+      </c>
+      <c r="AJ33" s="57">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="53"/>
+      <c r="AL33" s="54"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38">
+        <v>0.67</v>
+      </c>
+      <c r="M34" s="55"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
+      <c r="T34" s="38"/>
+      <c r="U34" s="38"/>
+      <c r="V34" s="38">
+        <v>0.76</v>
+      </c>
+      <c r="W34" s="38"/>
+      <c r="X34" s="38"/>
+      <c r="Z34" s="38"/>
+      <c r="AA34">
+        <v>1.01</v>
+      </c>
+      <c r="AB34" s="38"/>
+      <c r="AD34" s="38"/>
+      <c r="AE34" s="38"/>
+      <c r="AF34" s="38"/>
+      <c r="AG34" s="38"/>
+      <c r="AH34" s="38"/>
+      <c r="AI34" s="38">
+        <v>0.44</v>
+      </c>
+      <c r="AJ34" s="38"/>
+      <c r="AK34" s="38">
+        <v>0.39</v>
+      </c>
+      <c r="AL34">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="51">
+        <v>0.08</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38">
+        <v>1.19</v>
+      </c>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38">
+        <v>0.81</v>
+      </c>
+      <c r="M35" s="55"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38">
+        <v>0.31</v>
+      </c>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="38"/>
+      <c r="U35" s="38"/>
+      <c r="V35" s="38">
+        <v>0.51</v>
+      </c>
+      <c r="W35" s="38"/>
+      <c r="X35" s="38"/>
+      <c r="Z35" s="38"/>
+      <c r="AA35">
+        <v>0.63</v>
+      </c>
+      <c r="AB35" s="38"/>
+      <c r="AD35" s="38"/>
+      <c r="AE35" s="38"/>
+      <c r="AF35" s="38"/>
+      <c r="AG35" s="38"/>
+      <c r="AH35" s="38"/>
+      <c r="AI35" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="AJ35" s="38"/>
+      <c r="AK35" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="AL35">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="51">
+        <v>0.08</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="M36" s="55"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R36" s="38"/>
+      <c r="S36" s="38"/>
+      <c r="T36" s="38"/>
+      <c r="U36" s="38"/>
+      <c r="V36" s="38">
+        <v>0.15</v>
+      </c>
+      <c r="W36" s="38"/>
+      <c r="X36" s="38"/>
+      <c r="Z36" s="38"/>
+      <c r="AA36">
+        <v>0.27</v>
+      </c>
+      <c r="AB36" s="38"/>
+      <c r="AD36" s="38"/>
+      <c r="AE36" s="38"/>
+      <c r="AF36" s="38"/>
+      <c r="AG36" s="38"/>
+      <c r="AH36" s="38"/>
+      <c r="AI36" s="38">
+        <v>0.22</v>
+      </c>
+      <c r="AJ36" s="38"/>
+      <c r="AK36" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="AL36">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="38"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38">
+        <v>0.11</v>
+      </c>
+      <c r="M37" s="55"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38">
+        <v>0.04</v>
+      </c>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="38"/>
+      <c r="U37" s="38"/>
+      <c r="V37" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="W37" s="38"/>
+      <c r="X37" s="38"/>
+      <c r="Z37" s="38"/>
+      <c r="AA37">
+        <v>0.36</v>
+      </c>
+      <c r="AB37" s="38"/>
+      <c r="AD37" s="38"/>
+      <c r="AE37" s="38"/>
+      <c r="AF37" s="38"/>
+      <c r="AG37" s="38"/>
+      <c r="AH37" s="38"/>
+      <c r="AI37" s="38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AJ37" s="38"/>
+      <c r="AK37" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="AL37">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="51">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38">
+        <v>0.82</v>
+      </c>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38">
+        <v>0.36</v>
+      </c>
+      <c r="M38" s="55"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38">
+        <v>0.22</v>
+      </c>
+      <c r="R38" s="38"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38"/>
+      <c r="U38" s="38"/>
+      <c r="V38" s="38">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W38" s="38"/>
+      <c r="X38" s="38"/>
+      <c r="Z38" s="38"/>
+      <c r="AA38">
+        <v>0.46</v>
+      </c>
+      <c r="AB38" s="38"/>
+      <c r="AD38" s="38"/>
+      <c r="AE38" s="38"/>
+      <c r="AF38" s="38"/>
+      <c r="AG38" s="38"/>
+      <c r="AH38" s="38"/>
+      <c r="AI38" s="38">
+        <v>0.18</v>
+      </c>
+      <c r="AJ38" s="38"/>
+      <c r="AK38" s="38">
+        <v>0.18</v>
+      </c>
+      <c r="AL38">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="M39" s="55"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="38"/>
+      <c r="U39" s="38"/>
+      <c r="V39" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="W39" s="38"/>
+      <c r="X39" s="38"/>
+      <c r="Z39" s="38"/>
+      <c r="AA39">
+        <v>0.21</v>
+      </c>
+      <c r="AB39" s="38"/>
+      <c r="AD39" s="38"/>
+      <c r="AE39" s="38"/>
+      <c r="AF39" s="38"/>
+      <c r="AG39" s="38"/>
+      <c r="AH39" s="38"/>
+      <c r="AI39" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="AJ39" s="38"/>
+      <c r="AK39" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="AL39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="51">
+        <v>0.08</v>
+      </c>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38">
+        <v>0.34</v>
+      </c>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="M40" s="55"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
+      <c r="T40" s="38"/>
+      <c r="U40" s="38"/>
+      <c r="V40" s="38">
+        <v>0.13</v>
+      </c>
+      <c r="W40" s="38"/>
+      <c r="X40" s="38"/>
+      <c r="Z40" s="38"/>
+      <c r="AA40">
+        <v>0.24</v>
+      </c>
+      <c r="AB40" s="38"/>
+      <c r="AD40" s="38"/>
+      <c r="AE40" s="38"/>
+      <c r="AF40" s="38"/>
+      <c r="AG40" s="38"/>
+      <c r="AH40" s="38"/>
+      <c r="AI40" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="AJ40" s="38"/>
+      <c r="AK40" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AL40">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="M41" s="55"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
+      <c r="T41" s="38"/>
+      <c r="U41" s="38"/>
+      <c r="V41" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="W41" s="38"/>
+      <c r="X41" s="38"/>
+      <c r="Z41" s="38"/>
+      <c r="AA41">
+        <v>0.17</v>
+      </c>
+      <c r="AB41" s="38"/>
+      <c r="AD41" s="38"/>
+      <c r="AE41" s="38"/>
+      <c r="AF41" s="38"/>
+      <c r="AG41" s="38"/>
+      <c r="AH41" s="38"/>
+      <c r="AI41" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="AJ41" s="38"/>
+      <c r="AK41" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="AL41" s="38">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A42" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M42" s="55"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="R42" s="38"/>
+      <c r="S42" s="38"/>
+      <c r="T42" s="38"/>
+      <c r="U42" s="38"/>
+      <c r="V42" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="W42" s="38"/>
+      <c r="X42" s="57">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="53"/>
+      <c r="Z42" s="53"/>
+      <c r="AA42" s="53"/>
+      <c r="AB42" s="53"/>
+      <c r="AC42" s="53"/>
+      <c r="AD42" s="53"/>
+      <c r="AE42" s="53"/>
+      <c r="AF42" s="53"/>
+      <c r="AG42" s="51">
+        <v>0.05</v>
+      </c>
+      <c r="AH42" s="38"/>
+      <c r="AI42" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AJ42" s="57">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="53"/>
+      <c r="AL42" s="54"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38">
+        <v>0</v>
+      </c>
+      <c r="M43" s="56"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53">
+        <v>0</v>
+      </c>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53">
+        <v>0</v>
+      </c>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="53"/>
+      <c r="Z43" s="53"/>
+      <c r="AA43" s="53">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="53"/>
+      <c r="AC43" s="54"/>
+      <c r="AD43" s="53"/>
+      <c r="AE43" s="53"/>
+      <c r="AF43" s="53"/>
+      <c r="AG43" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="AH43" s="38"/>
+      <c r="AI43" s="38">
+        <v>0.36</v>
+      </c>
+      <c r="AJ43" s="38"/>
+      <c r="AK43" s="38">
+        <v>0.43</v>
+      </c>
+      <c r="AL43" s="52">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38">
+        <v>0</v>
+      </c>
+      <c r="M44" s="56"/>
+      <c r="N44" s="54"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53">
+        <v>0</v>
+      </c>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="53">
+        <v>0</v>
+      </c>
+      <c r="W44" s="53"/>
+      <c r="X44" s="53"/>
+      <c r="Y44" s="53"/>
+      <c r="Z44" s="53"/>
+      <c r="AA44" s="53">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="51">
+        <v>0.06</v>
+      </c>
+      <c r="AD44" s="38"/>
+      <c r="AE44" s="38"/>
+      <c r="AF44" s="38"/>
+      <c r="AG44" s="38"/>
+      <c r="AH44" s="38"/>
+      <c r="AI44" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="AJ44" s="38"/>
+      <c r="AK44" s="38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL44" s="52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38">
+        <v>0</v>
+      </c>
+      <c r="M45" s="56"/>
+      <c r="N45" s="54"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53">
+        <v>0</v>
+      </c>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53">
+        <v>0</v>
+      </c>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
+      <c r="Y45" s="53"/>
+      <c r="Z45" s="53"/>
+      <c r="AA45" s="53">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="51">
+        <v>0.06</v>
+      </c>
+      <c r="AD45" s="38"/>
+      <c r="AE45" s="38"/>
+      <c r="AF45" s="38"/>
+      <c r="AG45" s="38"/>
+      <c r="AH45" s="38"/>
+      <c r="AI45" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="AJ45" s="38"/>
+      <c r="AK45" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="AL45" s="52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38">
+        <v>0</v>
+      </c>
+      <c r="M46" s="56"/>
+      <c r="N46" s="54"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="53">
+        <v>0</v>
+      </c>
+      <c r="R46" s="53"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="53"/>
+      <c r="U46" s="53"/>
+      <c r="V46" s="53">
+        <v>0</v>
+      </c>
+      <c r="W46" s="53"/>
+      <c r="X46" s="53"/>
+      <c r="Y46" s="53"/>
+      <c r="Z46" s="53"/>
+      <c r="AA46" s="53">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="53"/>
+      <c r="AC46" s="54"/>
+      <c r="AD46" s="53"/>
+      <c r="AE46" s="53"/>
+      <c r="AF46" s="53"/>
+      <c r="AG46" s="53"/>
+      <c r="AH46" s="51">
+        <v>0.06</v>
+      </c>
+      <c r="AI46" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ46" s="38"/>
+      <c r="AK46" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="AL46" s="52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="M47" s="55"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="R47" s="38"/>
+      <c r="S47" s="38"/>
+      <c r="T47" s="38"/>
+      <c r="U47" s="38"/>
+      <c r="V47" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="W47" s="38"/>
+      <c r="X47" s="38"/>
+      <c r="Z47" s="38"/>
+      <c r="AA47">
+        <v>0.12</v>
+      </c>
+      <c r="AB47" s="38"/>
+      <c r="AD47" s="38"/>
+      <c r="AE47" s="38"/>
+      <c r="AF47" s="38"/>
+      <c r="AG47" s="38"/>
+      <c r="AH47" s="38"/>
+      <c r="AI47" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AJ47" s="38"/>
+      <c r="AK47" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="AL47">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38">
+        <v>0.17</v>
+      </c>
+      <c r="M48" s="55"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38">
+        <v>0</v>
+      </c>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+      <c r="V48" s="38">
+        <v>0</v>
+      </c>
+      <c r="W48" s="38"/>
+      <c r="X48" s="38"/>
+      <c r="Z48" s="38"/>
+      <c r="AA48" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="38"/>
+      <c r="AD48" s="38"/>
+      <c r="AE48" s="38"/>
+      <c r="AF48" s="38"/>
+      <c r="AG48" s="38"/>
+      <c r="AH48" s="38"/>
+      <c r="AI48" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="AJ48" s="38"/>
+      <c r="AK48" s="38">
+        <v>0.04</v>
+      </c>
+      <c r="AL48">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="M49" s="55"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="R49" s="38"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W49" s="38"/>
+      <c r="X49" s="38"/>
+      <c r="Z49" s="38"/>
+      <c r="AA49">
+        <v>0.08</v>
+      </c>
+      <c r="AB49" s="38"/>
+      <c r="AD49" s="38"/>
+      <c r="AE49" s="38"/>
+      <c r="AF49" s="38"/>
+      <c r="AG49" s="38"/>
+      <c r="AH49" s="38"/>
+      <c r="AI49" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AJ49" s="38"/>
+      <c r="AK49" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="AL49">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="M50" s="55"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="R50" s="38"/>
+      <c r="S50" s="38"/>
+      <c r="T50" s="38"/>
+      <c r="U50" s="38"/>
+      <c r="V50" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="W50" s="38"/>
+      <c r="X50" s="38"/>
+      <c r="Z50" s="38"/>
+      <c r="AA50">
+        <v>0.04</v>
+      </c>
+      <c r="AB50" s="38"/>
+      <c r="AD50" s="38"/>
+      <c r="AE50" s="38"/>
+      <c r="AF50" s="38"/>
+      <c r="AG50" s="38"/>
+      <c r="AH50" s="38"/>
+      <c r="AI50" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="AJ50" s="38"/>
+      <c r="AK50" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AL50">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="M51" s="55"/>
+      <c r="O51" s="38"/>
+      <c r="P51" s="38"/>
+      <c r="Q51" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="R51" s="38"/>
+      <c r="S51" s="38"/>
+      <c r="T51" s="38"/>
+      <c r="U51" s="38"/>
+      <c r="V51" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="W51" s="38"/>
+      <c r="X51" s="38"/>
+      <c r="Z51" s="38"/>
+      <c r="AA51">
+        <v>0.04</v>
+      </c>
+      <c r="AB51" s="38"/>
+      <c r="AD51" s="38"/>
+      <c r="AE51" s="38"/>
+      <c r="AF51" s="38"/>
+      <c r="AG51" s="38"/>
+      <c r="AH51" s="38"/>
+      <c r="AI51" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AJ51" s="38"/>
+      <c r="AK51" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AL51">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38">
+        <v>0</v>
+      </c>
+      <c r="M52" s="56"/>
+      <c r="N52" s="54"/>
+      <c r="O52" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="R52" s="38"/>
+      <c r="S52" s="38"/>
+      <c r="T52" s="38"/>
+      <c r="U52" s="38"/>
+      <c r="V52" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="W52" s="38"/>
+      <c r="X52" s="38"/>
+      <c r="Z52" s="38"/>
+      <c r="AA52">
+        <v>0.04</v>
+      </c>
+      <c r="AB52" s="38"/>
+      <c r="AD52" s="38"/>
+      <c r="AE52" s="38"/>
+      <c r="AF52" s="38"/>
+      <c r="AG52" s="38"/>
+      <c r="AH52" s="38"/>
+      <c r="AI52" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AJ52" s="38"/>
+      <c r="AK52" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AL52" s="52">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A53" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="M53" s="55"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="38">
+        <v>0</v>
+      </c>
+      <c r="R53" s="38"/>
+      <c r="S53" s="38"/>
+      <c r="T53" s="38"/>
+      <c r="U53" s="38"/>
+      <c r="V53" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="W53" s="38"/>
+      <c r="X53" s="38"/>
+      <c r="Z53" s="38"/>
+      <c r="AA53">
+        <v>0.16</v>
+      </c>
+      <c r="AB53" s="38"/>
+      <c r="AD53" s="38"/>
+      <c r="AE53" s="38"/>
+      <c r="AF53" s="38"/>
+      <c r="AG53" s="38"/>
+      <c r="AH53" s="38"/>
+      <c r="AI53" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="AJ53" s="38"/>
+      <c r="AK53" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AL53" s="52">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>435</v>
+      </c>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="M54" s="55"/>
+      <c r="O54" s="38"/>
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="R54" s="38"/>
+      <c r="S54" s="38"/>
+      <c r="T54" s="38"/>
+      <c r="U54" s="38"/>
+      <c r="V54" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="W54" s="57">
+        <v>0</v>
+      </c>
+      <c r="X54" s="53"/>
+      <c r="Y54" s="53"/>
+      <c r="Z54" s="53"/>
+      <c r="AA54" s="53"/>
+      <c r="AB54" s="53"/>
+      <c r="AC54" s="53"/>
+      <c r="AD54" s="53"/>
+      <c r="AE54" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="AF54" s="38"/>
+      <c r="AG54" s="38"/>
+      <c r="AH54" s="38"/>
+      <c r="AI54" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AJ54" s="57">
+        <v>0</v>
+      </c>
+      <c r="AK54" s="53"/>
+      <c r="AL54" s="54"/>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>436</v>
+      </c>
+      <c r="B55" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="M55" s="55"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="R55" s="38"/>
+      <c r="S55" s="38"/>
+      <c r="T55" s="38"/>
+      <c r="U55" s="38"/>
+      <c r="V55" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="W55" s="57">
+        <v>0</v>
+      </c>
+      <c r="X55" s="53"/>
+      <c r="Y55" s="53"/>
+      <c r="Z55" s="53"/>
+      <c r="AA55" s="53"/>
+      <c r="AB55" s="53"/>
+      <c r="AC55" s="53"/>
+      <c r="AD55" s="53"/>
+      <c r="AE55" s="53"/>
+      <c r="AF55" s="53"/>
+      <c r="AG55" s="53"/>
+      <c r="AH55" s="53"/>
+      <c r="AI55" s="53"/>
+      <c r="AJ55" s="53"/>
+      <c r="AK55" s="53"/>
+      <c r="AL55" s="54"/>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>437</v>
+      </c>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="M56" s="55"/>
+      <c r="O56" s="57">
+        <v>0</v>
+      </c>
+      <c r="P56" s="53"/>
+      <c r="Q56" s="53">
+        <v>0</v>
+      </c>
+      <c r="R56" s="53"/>
+      <c r="S56" s="53"/>
+      <c r="T56" s="53"/>
+      <c r="U56" s="53"/>
+      <c r="V56" s="53">
+        <v>0</v>
+      </c>
+      <c r="W56" s="53"/>
+      <c r="X56" s="53"/>
+      <c r="Y56" s="53"/>
+      <c r="Z56" s="53"/>
+      <c r="AA56" s="53"/>
+      <c r="AB56" s="53"/>
+      <c r="AC56" s="53"/>
+      <c r="AD56" s="53"/>
+      <c r="AE56" s="53"/>
+      <c r="AF56" s="53"/>
+      <c r="AG56" s="53"/>
+      <c r="AH56" s="53"/>
+      <c r="AI56" s="53"/>
+      <c r="AJ56" s="53"/>
+      <c r="AK56" s="53"/>
+      <c r="AL56" s="54"/>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
+        <v>438</v>
+      </c>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="M57" s="55"/>
+      <c r="N57" s="38"/>
+      <c r="O57" s="38"/>
+      <c r="P57" s="38"/>
+      <c r="Q57" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="R57" s="38"/>
+      <c r="S57" s="38"/>
+      <c r="T57" s="57">
+        <v>0</v>
+      </c>
+      <c r="U57" s="53"/>
+      <c r="V57" s="53">
+        <v>0</v>
+      </c>
+      <c r="W57" s="53"/>
+      <c r="X57" s="53"/>
+      <c r="Y57" s="53"/>
+      <c r="Z57" s="53"/>
+      <c r="AA57" s="53"/>
+      <c r="AB57" s="53"/>
+      <c r="AC57" s="53"/>
+      <c r="AD57" s="53"/>
+      <c r="AE57" s="53"/>
+      <c r="AF57" s="53"/>
+      <c r="AG57" s="53"/>
+      <c r="AH57" s="53"/>
+      <c r="AI57" s="53"/>
+      <c r="AJ57" s="53"/>
+      <c r="AK57" s="53"/>
+      <c r="AL57" s="54"/>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A58" s="35" t="s">
+        <v>439</v>
+      </c>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
+      <c r="L58" s="38">
+        <v>0</v>
+      </c>
+      <c r="M58" s="56"/>
+      <c r="N58" s="53"/>
+      <c r="O58" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="P58" s="38"/>
+      <c r="Q58" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="R58" s="38"/>
+      <c r="S58" s="38"/>
+      <c r="T58" s="38"/>
+      <c r="U58" s="38"/>
+      <c r="V58" s="38">
+        <v>0.03</v>
+      </c>
+      <c r="W58" s="38"/>
+      <c r="X58" s="38"/>
+      <c r="Y58" s="38"/>
+      <c r="Z58" s="38"/>
+      <c r="AA58" s="38">
+        <v>0.01</v>
+      </c>
+      <c r="AB58" s="57">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="53"/>
+      <c r="AD58" s="53"/>
+      <c r="AE58" s="53"/>
+      <c r="AF58" s="53"/>
+      <c r="AG58" s="53"/>
+      <c r="AH58" s="53"/>
+      <c r="AI58" s="53"/>
+      <c r="AJ58" s="53"/>
+      <c r="AK58" s="53"/>
+      <c r="AL58" s="54"/>
+    </row>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B60" s="38">
+        <f>SUM(B4:B58)</f>
+        <v>78.860000000000014</v>
+      </c>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38">
+        <f>SUM(G4:G58)</f>
+        <v>73.989999999999995</v>
+      </c>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="38">
+        <f>SUM(L4:L58)</f>
+        <v>99.630000000000024</v>
+      </c>
+      <c r="M60" s="55"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="38"/>
+      <c r="Q60" s="38">
+        <f>SUM(Q4:Q58)</f>
+        <v>99.859999999999971</v>
+      </c>
+      <c r="R60" s="38"/>
+      <c r="S60" s="38"/>
+      <c r="T60" s="38"/>
+      <c r="U60" s="38"/>
+      <c r="V60" s="38">
+        <f>SUM(V4:V58)</f>
+        <v>99.67000000000003</v>
+      </c>
+      <c r="W60" s="38"/>
+      <c r="X60" s="38"/>
+      <c r="Y60" s="38"/>
+      <c r="Z60" s="38"/>
+      <c r="AA60" s="38">
+        <f>SUM(AA4:AA58)</f>
+        <v>99.610000000000014</v>
+      </c>
+      <c r="AB60" s="38"/>
+      <c r="AC60" s="38"/>
+      <c r="AD60" s="38"/>
+      <c r="AE60" s="38"/>
+      <c r="AF60" s="38"/>
+      <c r="AG60" s="38"/>
+      <c r="AH60" s="38"/>
+      <c r="AI60" s="38">
+        <f>SUM(AI4:AI58)</f>
+        <v>99.940000000000012</v>
+      </c>
+      <c r="AJ60" s="38"/>
+      <c r="AK60" s="38">
+        <f>SUM(AK4:AK58)</f>
+        <v>99.86999999999999</v>
+      </c>
+      <c r="AL60" s="38">
+        <f>SUM(AL4:AL58)</f>
+        <v>99.989999999999981</v>
+      </c>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B61" s="38">
+        <f>SUM(B28:B58)</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38">
+        <f t="shared" ref="C61:AL61" si="1">SUM(G28:G58)</f>
+        <v>4.4999999999999991</v>
+      </c>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38">
+        <f t="shared" si="1"/>
+        <v>6.6899999999999995</v>
+      </c>
+      <c r="M61" s="55"/>
+      <c r="N61" s="38"/>
+      <c r="O61" s="38"/>
+      <c r="P61" s="38"/>
+      <c r="Q61" s="38">
+        <f t="shared" si="1"/>
+        <v>3.8299999999999987</v>
+      </c>
+      <c r="R61" s="38"/>
+      <c r="S61" s="38"/>
+      <c r="T61" s="38"/>
+      <c r="U61" s="38"/>
+      <c r="V61" s="38">
+        <f t="shared" si="1"/>
+        <v>11.079999999999998</v>
+      </c>
+      <c r="W61" s="38"/>
+      <c r="X61" s="38"/>
+      <c r="Y61" s="38"/>
+      <c r="Z61" s="38"/>
+      <c r="AA61" s="38">
+        <f t="shared" si="1"/>
+        <v>12.54</v>
+      </c>
+      <c r="AB61" s="38"/>
+      <c r="AC61" s="38"/>
+      <c r="AD61" s="38"/>
+      <c r="AE61" s="38"/>
+      <c r="AF61" s="38"/>
+      <c r="AG61" s="38"/>
+      <c r="AH61" s="38"/>
+      <c r="AI61" s="38">
+        <f t="shared" si="1"/>
+        <v>11.969999999999999</v>
+      </c>
+      <c r="AJ61" s="38"/>
+      <c r="AK61" s="38">
+        <f t="shared" si="1"/>
+        <v>11.249999999999998</v>
+      </c>
+      <c r="AL61" s="38">
+        <f t="shared" si="1"/>
+        <v>10.009999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B63" t="s">
+        <v>447</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="L63" s="38">
+        <f>L4</f>
+        <v>46.56</v>
+      </c>
+      <c r="Q63" s="38">
+        <f>Q4</f>
+        <v>53.99</v>
+      </c>
+      <c r="V63" s="38">
+        <f>V4</f>
+        <v>41.8</v>
+      </c>
+      <c r="AA63" s="38">
+        <f>AA4</f>
+        <v>47.45</v>
+      </c>
+      <c r="AI63" s="38">
+        <f>AI4</f>
+        <v>58.6</v>
+      </c>
+      <c r="AK63" s="38">
+        <f>AK4</f>
+        <v>59.3</v>
+      </c>
+      <c r="AL63" s="38">
+        <f>AL4</f>
+        <v>63.23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B64" t="s">
+        <v>449</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="L64" s="38">
+        <f>L5+L6</f>
+        <v>21.66</v>
+      </c>
+      <c r="Q64" s="38">
+        <f>Q5+Q6</f>
+        <v>19.939999999999998</v>
+      </c>
+      <c r="V64" s="38">
+        <f>V5+V6</f>
+        <v>18.2</v>
+      </c>
+      <c r="AA64" s="38">
+        <f>AA5+AA6</f>
+        <v>15.4</v>
+      </c>
+      <c r="AI64" s="38">
+        <f>AI5+AI6</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AK64" s="38">
+        <f>AK5+AK6</f>
+        <v>10</v>
+      </c>
+      <c r="AL64" s="38">
+        <f>AL5+AL6</f>
+        <v>8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B65" t="s">
+        <v>450</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="L65" s="38">
+        <f>SUM(L7:L11)+L28</f>
+        <v>15.239999999999998</v>
+      </c>
+      <c r="Q65" s="38">
+        <f>SUM(Q7:Q11)+Q28</f>
+        <v>13.139999999999999</v>
+      </c>
+      <c r="V65" s="38">
+        <f>SUM(V7:V11)+V28</f>
+        <v>20.259999999999998</v>
+      </c>
+      <c r="AA65" s="38">
+        <f>SUM(AA7:AA11)+AA28</f>
+        <v>18.84</v>
+      </c>
+      <c r="AI65" s="38">
+        <f>SUM(AI7:AI11)+AI28</f>
+        <v>16.099999999999998</v>
+      </c>
+      <c r="AK65" s="38">
+        <f>SUM(AK7:AK11)+AK28</f>
+        <v>15.8</v>
+      </c>
+      <c r="AL65" s="38">
+        <f>SUM(AL7:AL11)+AL28</f>
+        <v>14.350000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B66" t="s">
+        <v>445</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="L66" s="38">
+        <f>SUM(L12:L16)+SUM(L29:L33)</f>
+        <v>10.18</v>
+      </c>
+      <c r="Q66" s="38">
+        <f>SUM(Q12:Q16)+SUM(Q29:Q33)</f>
+        <v>8.77</v>
+      </c>
+      <c r="V66" s="38">
+        <f>SUM(V12:V16)+SUM(V29:V33)</f>
+        <v>13.39</v>
+      </c>
+      <c r="AA66" s="38">
+        <f>SUM(AA12:AA16)+SUM(AA29:AA33)</f>
+        <v>11.309999999999999</v>
+      </c>
+      <c r="AI66" s="38">
+        <f>SUM(AI12:AI16)+SUM(AI29:AI33)</f>
+        <v>10.3</v>
+      </c>
+      <c r="AK66" s="38">
+        <f>SUM(AK12:AK16)+SUM(AK29:AK33)</f>
+        <v>9.5</v>
+      </c>
+      <c r="AL66" s="38">
+        <f>SUM(AL12:AL16)+SUM(AL29:AL33)</f>
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="B67" t="s">
+        <v>453</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="L67" s="38">
+        <f>SUM(L17:L21)+SUM(L34:L35)</f>
+        <v>3.34</v>
+      </c>
+      <c r="Q67" s="38">
+        <f>SUM(Q17:Q21)+SUM(Q34:Q35)</f>
+        <v>2.85</v>
+      </c>
+      <c r="V67" s="38">
+        <f>SUM(V17:V21)+SUM(V34:V35)</f>
+        <v>3.65</v>
+      </c>
+      <c r="AA67" s="38">
+        <f>SUM(AA17:AA21)+SUM(AA34:AA35)</f>
+        <v>3.8200000000000003</v>
+      </c>
+      <c r="AI67" s="38">
+        <f>SUM(AI17:AI21)+SUM(AI34:AI35)</f>
+        <v>2.5100000000000002</v>
+      </c>
+      <c r="AK67" s="38">
+        <f>SUM(AK17:AK21)+SUM(AK34:AK35)</f>
+        <v>2.69</v>
+      </c>
+      <c r="AL67" s="38">
+        <f>SUM(AL17:AL21)+SUM(AL34:AL35)</f>
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A68" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="B68" t="s">
+        <v>454</v>
+      </c>
+      <c r="C68">
+        <v>28</v>
+      </c>
+      <c r="L68" s="38">
+        <f>SUM(L22:L26)+SUM(L36:L58)</f>
+        <v>2.6500000000000004</v>
+      </c>
+      <c r="Q68" s="38">
+        <f>SUM(Q22:Q26)+SUM(Q36:Q58)</f>
+        <v>1.1700000000000002</v>
+      </c>
+      <c r="V68" s="38">
+        <f>SUM(V22:V26)+SUM(V36:V58)</f>
+        <v>2.3700000000000006</v>
+      </c>
+      <c r="AA68" s="38">
+        <f>SUM(AA22:AA26)+SUM(AA36:AA58)</f>
+        <v>2.79</v>
+      </c>
+      <c r="AI68" s="38">
+        <f>SUM(AI22:AI26)+SUM(AI36:AI58)</f>
+        <v>2.2300000000000004</v>
+      </c>
+      <c r="AK68" s="38">
+        <f>SUM(AK22:AK26)+SUM(AK36:AK58)</f>
+        <v>2.58</v>
+      </c>
+      <c r="AL68" s="38">
+        <f>SUM(AL22:AL26)+SUM(AL36:AL58)</f>
+        <v>2.0000000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f>SUM(C63:C68)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AI73" t="s">
+        <v>452</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
filled acwi country weights since 1999
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA230CA-230F-4184-A73F-D8D745A9273D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F2F3BA-89DB-444C-ADD4-D410133C6DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Data coverage" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="457">
   <si>
     <t>United States</t>
   </si>
@@ -1405,7 +1405,13 @@
     <t>0.3 - 0.8%</t>
   </si>
   <si>
-    <t>&lt;= 0.3%</t>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>0.1 - 0.3</t>
+  </si>
+  <si>
+    <t>&lt;= 0.1%</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1612,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1670,12 +1676,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1684,6 +1684,15 @@
     <xf numFmtId="2" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2003,9 +2012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD81D1A-35C6-4C9D-B55B-751553A65962}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C13" sqref="C13"/>
+      <selection pane="topRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,10 +3634,10 @@
       <c r="Q57" s="17"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="60" t="s">
         <v>379</v>
       </c>
-      <c r="C59" s="50"/>
+      <c r="C59" s="61"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
@@ -3675,7 +3684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B703FA39-2A94-42E5-99E2-495679D72086}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4995,7 +5006,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AV24" sqref="AV24"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,13 +5137,13 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BG1" s="49" t="s">
+      <c r="BG1" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="BH1" s="49"/>
-      <c r="BI1" s="49"/>
-      <c r="BJ1" s="49"/>
-      <c r="BK1" s="49"/>
+      <c r="BH1" s="60"/>
+      <c r="BI1" s="60"/>
+      <c r="BJ1" s="60"/>
+      <c r="BK1" s="60"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -9133,7 +9144,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9157,26 +9168,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="60" t="s">
         <v>245</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="60" t="s">
         <v>246</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="60" t="s">
         <v>346</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -10952,10 +10963,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE8DE30-8CF4-49FE-905A-5BDCBDCD0F61}">
-  <dimension ref="A1:AL73"/>
+  <dimension ref="A1:AL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -11146,7 +11157,7 @@
       <c r="L4" s="38">
         <v>46.56</v>
       </c>
-      <c r="M4" s="55"/>
+      <c r="M4" s="53"/>
       <c r="N4" s="38"/>
       <c r="O4" s="38"/>
       <c r="P4" s="38"/>
@@ -11205,7 +11216,7 @@
       <c r="L5" s="38">
         <v>11.26</v>
       </c>
-      <c r="M5" s="55"/>
+      <c r="M5" s="53"/>
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
       <c r="P5" s="38"/>
@@ -11257,27 +11268,27 @@
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
-      <c r="L6" s="52">
+      <c r="L6" s="50">
         <v>10.4</v>
       </c>
-      <c r="M6" s="55"/>
+      <c r="M6" s="53"/>
       <c r="N6" s="38"/>
       <c r="O6" s="38"/>
       <c r="P6" s="38"/>
-      <c r="Q6" s="52">
+      <c r="Q6" s="50">
         <v>11.5</v>
       </c>
       <c r="R6" s="38"/>
       <c r="S6" s="38"/>
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
-      <c r="V6" s="52">
+      <c r="V6" s="50">
         <v>9.6</v>
       </c>
       <c r="W6" s="38"/>
       <c r="X6" s="38"/>
       <c r="Z6" s="38"/>
-      <c r="AA6" s="52">
+      <c r="AA6" s="50">
         <v>7.9</v>
       </c>
       <c r="AB6" s="38"/>
@@ -11319,7 +11330,7 @@
       <c r="L7" s="38">
         <v>2.29</v>
       </c>
-      <c r="M7" s="55"/>
+      <c r="M7" s="53"/>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
@@ -11371,27 +11382,27 @@
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
-      <c r="L8" s="52">
+      <c r="L8" s="50">
         <v>4.0999999999999996</v>
       </c>
-      <c r="M8" s="55"/>
+      <c r="M8" s="53"/>
       <c r="N8" s="38"/>
       <c r="O8" s="38"/>
       <c r="P8" s="38"/>
-      <c r="Q8" s="52">
+      <c r="Q8" s="50">
         <v>3.1</v>
       </c>
       <c r="R8" s="38"/>
       <c r="S8" s="38"/>
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
-      <c r="V8" s="52">
+      <c r="V8" s="50">
         <v>4.2</v>
       </c>
       <c r="W8" s="38"/>
       <c r="X8" s="38"/>
       <c r="Z8" s="38"/>
-      <c r="AA8" s="52">
+      <c r="AA8" s="50">
         <v>3.1</v>
       </c>
       <c r="AB8" s="38"/>
@@ -11426,27 +11437,27 @@
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
-      <c r="L9" s="52">
+      <c r="L9" s="50">
         <v>3.4</v>
       </c>
-      <c r="M9" s="55"/>
+      <c r="M9" s="53"/>
       <c r="N9" s="38"/>
       <c r="O9" s="38"/>
       <c r="P9" s="38"/>
-      <c r="Q9" s="52">
+      <c r="Q9" s="50">
         <v>3.1</v>
       </c>
       <c r="R9" s="38"/>
       <c r="S9" s="38"/>
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
-      <c r="V9" s="52">
+      <c r="V9" s="50">
         <v>4.0999999999999996</v>
       </c>
       <c r="W9" s="38"/>
       <c r="X9" s="38"/>
       <c r="Z9" s="38"/>
-      <c r="AA9" s="52">
+      <c r="AA9" s="50">
         <v>3</v>
       </c>
       <c r="AB9" s="38"/>
@@ -11481,27 +11492,27 @@
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="52">
+      <c r="L10" s="50">
         <v>4.2</v>
       </c>
-      <c r="M10" s="55"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
       <c r="P10" s="38"/>
-      <c r="Q10" s="52">
+      <c r="Q10" s="50">
         <v>2.6</v>
       </c>
       <c r="R10" s="38"/>
       <c r="S10" s="38"/>
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
-      <c r="V10" s="52">
+      <c r="V10" s="50">
         <v>3.7</v>
       </c>
       <c r="W10" s="38"/>
       <c r="X10" s="38"/>
       <c r="Z10" s="38"/>
-      <c r="AA10" s="52">
+      <c r="AA10" s="50">
         <v>2.9</v>
       </c>
       <c r="AB10" s="38"/>
@@ -11543,7 +11554,7 @@
       <c r="L11" s="38">
         <v>1.22</v>
       </c>
-      <c r="M11" s="55"/>
+      <c r="M11" s="53"/>
       <c r="N11" s="38"/>
       <c r="O11" s="38"/>
       <c r="P11" s="38"/>
@@ -11585,16 +11596,16 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="52">
+      <c r="L12" s="50">
         <v>1.5</v>
       </c>
-      <c r="Q12" s="52">
+      <c r="Q12" s="50">
         <v>1.6</v>
       </c>
-      <c r="V12" s="52">
+      <c r="V12" s="50">
         <v>1.3</v>
       </c>
-      <c r="AA12" s="52">
+      <c r="AA12" s="50">
         <v>0.8</v>
       </c>
       <c r="AI12">
@@ -11621,27 +11632,27 @@
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
-      <c r="L13" s="52">
+      <c r="L13" s="50">
         <v>1.2</v>
       </c>
-      <c r="M13" s="55"/>
+      <c r="M13" s="53"/>
       <c r="N13" s="38"/>
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
-      <c r="Q13" s="52">
+      <c r="Q13" s="50">
         <v>1.2</v>
       </c>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
-      <c r="V13" s="52">
+      <c r="V13" s="50">
         <v>1.3</v>
       </c>
       <c r="W13" s="38"/>
       <c r="X13" s="38"/>
       <c r="Z13" s="38"/>
-      <c r="AA13" s="52">
+      <c r="AA13" s="50">
         <v>1.2</v>
       </c>
       <c r="AB13" s="38"/>
@@ -11676,27 +11687,27 @@
       <c r="I14" s="38"/>
       <c r="J14" s="38"/>
       <c r="K14" s="38"/>
-      <c r="L14" s="52">
+      <c r="L14" s="50">
         <v>1.2</v>
       </c>
-      <c r="M14" s="55"/>
+      <c r="M14" s="53"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
-      <c r="Q14" s="52">
+      <c r="Q14" s="50">
         <v>1.5</v>
       </c>
       <c r="R14" s="38"/>
       <c r="S14" s="38"/>
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
-      <c r="V14" s="52">
+      <c r="V14" s="50">
         <v>1.9</v>
       </c>
       <c r="W14" s="38"/>
       <c r="X14" s="38"/>
       <c r="Z14" s="38"/>
-      <c r="AA14" s="52">
+      <c r="AA14" s="50">
         <v>0.96</v>
       </c>
       <c r="AB14" s="38"/>
@@ -11738,7 +11749,7 @@
       <c r="L15" s="38">
         <v>1.25</v>
       </c>
-      <c r="M15" s="55"/>
+      <c r="M15" s="53"/>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
@@ -11790,27 +11801,27 @@
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
-      <c r="L16" s="52">
+      <c r="L16" s="50">
         <v>1.9</v>
       </c>
-      <c r="M16" s="55"/>
+      <c r="M16" s="53"/>
       <c r="N16" s="38"/>
       <c r="O16" s="38"/>
       <c r="P16" s="38"/>
-      <c r="Q16" s="52">
+      <c r="Q16" s="50">
         <v>1.8</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="38"/>
       <c r="T16" s="38"/>
       <c r="U16" s="38"/>
-      <c r="V16" s="52">
+      <c r="V16" s="50">
         <v>1.5</v>
       </c>
       <c r="W16" s="38"/>
       <c r="X16" s="38"/>
       <c r="Z16" s="38"/>
-      <c r="AA16" s="52">
+      <c r="AA16" s="50">
         <v>0.79</v>
       </c>
       <c r="AB16" s="38"/>
@@ -11852,7 +11863,7 @@
       <c r="L17" s="38">
         <v>0.41</v>
       </c>
-      <c r="M17" s="55"/>
+      <c r="M17" s="53"/>
       <c r="N17" s="38"/>
       <c r="O17" s="38"/>
       <c r="P17" s="38"/>
@@ -11904,27 +11915,27 @@
       <c r="I18" s="38"/>
       <c r="J18" s="38"/>
       <c r="K18" s="38"/>
-      <c r="L18" s="52">
+      <c r="L18" s="50">
         <v>0.3</v>
       </c>
-      <c r="M18" s="55"/>
+      <c r="M18" s="53"/>
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
       <c r="P18" s="38"/>
-      <c r="Q18" s="52">
+      <c r="Q18" s="50">
         <v>0.3</v>
       </c>
       <c r="R18" s="38"/>
       <c r="S18" s="38"/>
       <c r="T18" s="38"/>
       <c r="U18" s="38"/>
-      <c r="V18" s="52">
+      <c r="V18" s="50">
         <v>0.4</v>
       </c>
       <c r="W18" s="38"/>
       <c r="X18" s="38"/>
       <c r="Z18" s="38"/>
-      <c r="AA18" s="52">
+      <c r="AA18" s="50">
         <v>0.37</v>
       </c>
       <c r="AB18" s="38"/>
@@ -11959,27 +11970,27 @@
       <c r="I19" s="38"/>
       <c r="J19" s="38"/>
       <c r="K19" s="38"/>
-      <c r="L19" s="52">
+      <c r="L19" s="50">
         <v>0.45</v>
       </c>
-      <c r="M19" s="55"/>
+      <c r="M19" s="53"/>
       <c r="N19" s="38"/>
       <c r="O19" s="38"/>
       <c r="P19" s="38"/>
-      <c r="Q19" s="52">
+      <c r="Q19" s="50">
         <v>0.45</v>
       </c>
       <c r="R19" s="38"/>
       <c r="S19" s="38"/>
       <c r="T19" s="38"/>
       <c r="U19" s="38"/>
-      <c r="V19" s="52">
+      <c r="V19" s="50">
         <v>0.4</v>
       </c>
       <c r="W19" s="38"/>
       <c r="X19" s="38"/>
       <c r="Z19" s="38"/>
-      <c r="AA19" s="52">
+      <c r="AA19" s="50">
         <v>0.27</v>
       </c>
       <c r="AB19" s="38"/>
@@ -12014,27 +12025,27 @@
       <c r="I20" s="38"/>
       <c r="J20" s="38"/>
       <c r="K20" s="38"/>
-      <c r="L20" s="52">
+      <c r="L20" s="50">
         <v>0.3</v>
       </c>
-      <c r="M20" s="55"/>
+      <c r="M20" s="53"/>
       <c r="N20" s="38"/>
       <c r="O20" s="38"/>
       <c r="P20" s="38"/>
-      <c r="Q20" s="52">
+      <c r="Q20" s="50">
         <v>0.5</v>
       </c>
       <c r="R20" s="38"/>
       <c r="S20" s="38"/>
       <c r="T20" s="38"/>
       <c r="U20" s="38"/>
-      <c r="V20" s="52">
+      <c r="V20" s="50">
         <v>0.5</v>
       </c>
       <c r="W20" s="38"/>
       <c r="X20" s="38"/>
       <c r="Z20" s="38"/>
-      <c r="AA20" s="52">
+      <c r="AA20" s="50">
         <v>0.49</v>
       </c>
       <c r="AB20" s="38"/>
@@ -12059,27 +12070,27 @@
       <c r="A21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="52">
+      <c r="L21" s="50">
         <v>0.4</v>
       </c>
-      <c r="M21" s="55"/>
+      <c r="M21" s="53"/>
       <c r="N21" s="38"/>
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
-      <c r="Q21" s="52">
+      <c r="Q21" s="50">
         <v>0.4</v>
       </c>
       <c r="R21" s="38"/>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
       <c r="U21" s="38"/>
-      <c r="V21" s="52">
+      <c r="V21" s="50">
         <v>0.6</v>
       </c>
       <c r="W21" s="38"/>
       <c r="X21" s="38"/>
       <c r="Z21" s="38"/>
-      <c r="AA21" s="52">
+      <c r="AA21" s="50">
         <v>0.34</v>
       </c>
       <c r="AB21" s="38"/>
@@ -12101,13 +12112,13 @@
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="52" t="s">
         <v>19</v>
       </c>
       <c r="L22" s="38">
         <v>0.17</v>
       </c>
-      <c r="M22" s="55"/>
+      <c r="M22" s="53"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
       <c r="P22" s="38"/>
@@ -12146,30 +12157,30 @@
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="52">
+      <c r="L23" s="50">
         <v>0.1</v>
       </c>
-      <c r="M23" s="55"/>
+      <c r="M23" s="53"/>
       <c r="N23" s="38"/>
       <c r="O23" s="38"/>
       <c r="P23" s="38"/>
-      <c r="Q23" s="52">
+      <c r="Q23" s="50">
         <v>0.1</v>
       </c>
       <c r="R23" s="38"/>
       <c r="S23" s="38"/>
       <c r="T23" s="38"/>
       <c r="U23" s="38"/>
-      <c r="V23" s="52">
+      <c r="V23" s="50">
         <v>0.2</v>
       </c>
       <c r="W23" s="38"/>
       <c r="X23" s="38"/>
       <c r="Z23" s="38"/>
-      <c r="AA23" s="52">
+      <c r="AA23" s="50">
         <v>0.19</v>
       </c>
       <c r="AB23" s="38"/>
@@ -12203,7 +12214,7 @@
       <c r="L24" s="38">
         <v>0.13</v>
       </c>
-      <c r="M24" s="55"/>
+      <c r="M24" s="53"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
       <c r="P24" s="38"/>
@@ -12245,27 +12256,27 @@
       <c r="A25" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="50">
         <v>0.1</v>
       </c>
-      <c r="M25" s="55"/>
+      <c r="M25" s="53"/>
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
       <c r="P25" s="38"/>
-      <c r="Q25" s="52">
+      <c r="Q25" s="50">
         <v>0.1</v>
       </c>
       <c r="R25" s="38"/>
       <c r="S25" s="38"/>
       <c r="T25" s="38"/>
       <c r="U25" s="38"/>
-      <c r="V25" s="52">
+      <c r="V25" s="50">
         <v>0.1</v>
       </c>
       <c r="W25" s="38"/>
       <c r="X25" s="38"/>
       <c r="Z25" s="38"/>
-      <c r="AA25" s="52">
+      <c r="AA25" s="50">
         <v>0.08</v>
       </c>
       <c r="AB25" s="38"/>
@@ -12296,26 +12307,26 @@
       <c r="G26">
         <v>0.09</v>
       </c>
-      <c r="L26" s="52">
+      <c r="L26" s="50">
         <v>0.1</v>
       </c>
-      <c r="M26" s="55"/>
+      <c r="M26" s="53"/>
       <c r="O26" s="38"/>
       <c r="P26" s="38"/>
-      <c r="Q26" s="52">
+      <c r="Q26" s="50">
         <v>0.1</v>
       </c>
       <c r="R26" s="38"/>
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
       <c r="U26" s="38"/>
-      <c r="V26" s="52">
+      <c r="V26" s="50">
         <v>0.1</v>
       </c>
       <c r="W26" s="38"/>
       <c r="X26" s="38"/>
       <c r="Z26" s="38"/>
-      <c r="AA26" s="52">
+      <c r="AA26" s="50">
         <v>0.06</v>
       </c>
       <c r="AB26" s="38"/>
@@ -12351,7 +12362,7 @@
       <c r="J27" s="38"/>
       <c r="K27" s="38"/>
       <c r="L27" s="38"/>
-      <c r="M27" s="55"/>
+      <c r="M27" s="53"/>
       <c r="O27" s="38"/>
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
@@ -12388,12 +12399,12 @@
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
       <c r="I28" s="38"/>
-      <c r="J28" s="51"/>
+      <c r="J28" s="49"/>
       <c r="K28" s="38"/>
       <c r="L28" s="38">
         <v>0.03</v>
       </c>
-      <c r="M28" s="55"/>
+      <c r="M28" s="53"/>
       <c r="O28" s="38"/>
       <c r="P28" s="38"/>
       <c r="Q28" s="38">
@@ -12415,7 +12426,7 @@
       <c r="AB28" s="38"/>
       <c r="AD28" s="38"/>
       <c r="AE28" s="38"/>
-      <c r="AF28" s="51"/>
+      <c r="AF28" s="49"/>
       <c r="AH28" s="38"/>
       <c r="AI28" s="38">
         <v>3.8</v>
@@ -12440,12 +12451,12 @@
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
-      <c r="J29" s="51"/>
+      <c r="J29" s="49"/>
       <c r="K29" s="38"/>
       <c r="L29" s="38">
         <v>1.1399999999999999</v>
       </c>
-      <c r="M29" s="55"/>
+      <c r="M29" s="53"/>
       <c r="O29" s="38"/>
       <c r="P29" s="38"/>
       <c r="Q29" s="38">
@@ -12490,7 +12501,7 @@
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
-      <c r="G30" s="51"/>
+      <c r="G30" s="49"/>
       <c r="H30" s="38"/>
       <c r="I30" s="38"/>
       <c r="J30" s="38"/>
@@ -12498,7 +12509,7 @@
       <c r="L30" s="38">
         <v>0.4</v>
       </c>
-      <c r="M30" s="55"/>
+      <c r="M30" s="53"/>
       <c r="O30" s="38"/>
       <c r="P30" s="38"/>
       <c r="Q30" s="38">
@@ -12542,7 +12553,7 @@
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="51"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="38">
         <v>0.72</v>
       </c>
@@ -12553,7 +12564,7 @@
       <c r="L31" s="38">
         <v>0.2</v>
       </c>
-      <c r="M31" s="55"/>
+      <c r="M31" s="53"/>
       <c r="O31" s="38"/>
       <c r="P31" s="38"/>
       <c r="Q31" s="38">
@@ -12593,7 +12604,7 @@
       <c r="A32" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="51">
+      <c r="B32" s="49">
         <v>0.19</v>
       </c>
       <c r="C32" s="38"/>
@@ -12610,7 +12621,7 @@
       <c r="L32" s="38">
         <v>1.02</v>
       </c>
-      <c r="M32" s="55"/>
+      <c r="M32" s="53"/>
       <c r="O32" s="38"/>
       <c r="P32" s="38"/>
       <c r="Q32" s="38">
@@ -12659,11 +12670,11 @@
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
       <c r="J33" s="38"/>
-      <c r="K33" s="51"/>
+      <c r="K33" s="49"/>
       <c r="L33" s="38">
         <v>0.37</v>
       </c>
-      <c r="M33" s="55"/>
+      <c r="M33" s="53"/>
       <c r="O33" s="38"/>
       <c r="P33" s="38"/>
       <c r="Q33" s="38">
@@ -12692,11 +12703,11 @@
       <c r="AI33" s="38">
         <v>0.38</v>
       </c>
-      <c r="AJ33" s="57">
+      <c r="AJ33" s="55">
         <v>0</v>
       </c>
-      <c r="AK33" s="53"/>
-      <c r="AL33" s="54"/>
+      <c r="AK33" s="51"/>
+      <c r="AL33" s="52"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
@@ -12709,13 +12720,13 @@
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
-      <c r="I34" s="51"/>
+      <c r="I34" s="49"/>
       <c r="J34" s="38"/>
       <c r="K34" s="38"/>
       <c r="L34" s="38">
         <v>0.67</v>
       </c>
-      <c r="M34" s="55"/>
+      <c r="M34" s="53"/>
       <c r="O34" s="38"/>
       <c r="P34" s="38"/>
       <c r="Q34" s="38">
@@ -12755,7 +12766,7 @@
       <c r="A35" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="51">
+      <c r="B35" s="49">
         <v>0.08</v>
       </c>
       <c r="C35" s="38"/>
@@ -12772,7 +12783,7 @@
       <c r="L35" s="38">
         <v>0.81</v>
       </c>
-      <c r="M35" s="55"/>
+      <c r="M35" s="53"/>
       <c r="O35" s="38"/>
       <c r="P35" s="38"/>
       <c r="Q35" s="38">
@@ -12809,44 +12820,44 @@
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="51">
-        <v>0.08</v>
+      <c r="A36" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="49">
+        <v>0.28999999999999998</v>
       </c>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38">
-        <v>0.41</v>
+        <v>0.82</v>
       </c>
       <c r="H36" s="38"/>
       <c r="I36" s="38"/>
       <c r="J36" s="38"/>
       <c r="K36" s="38"/>
       <c r="L36" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="M36" s="55"/>
+        <v>0.36</v>
+      </c>
+      <c r="M36" s="53"/>
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
       <c r="Q36" s="38">
-        <v>7.0000000000000007E-2</v>
+        <v>0.22</v>
       </c>
       <c r="R36" s="38"/>
       <c r="S36" s="38"/>
       <c r="T36" s="38"/>
       <c r="U36" s="38"/>
       <c r="V36" s="38">
-        <v>0.15</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="W36" s="38"/>
       <c r="X36" s="38"/>
       <c r="Z36" s="38"/>
       <c r="AA36">
-        <v>0.27</v>
+        <v>0.46</v>
       </c>
       <c r="AB36" s="38"/>
       <c r="AD36" s="38"/>
@@ -12855,53 +12866,55 @@
       <c r="AG36" s="38"/>
       <c r="AH36" s="38"/>
       <c r="AI36" s="38">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="AJ36" s="38"/>
       <c r="AK36" s="38">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="AL36">
         <v>0.16</v>
       </c>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="38"/>
-      <c r="C37" s="51"/>
+      <c r="A37" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="49">
+        <v>0.08</v>
+      </c>
+      <c r="C37" s="38"/>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38">
-        <v>0.09</v>
+        <v>0.41</v>
       </c>
       <c r="H37" s="38"/>
       <c r="I37" s="38"/>
       <c r="J37" s="38"/>
       <c r="K37" s="38"/>
       <c r="L37" s="38">
-        <v>0.11</v>
-      </c>
-      <c r="M37" s="55"/>
+        <v>0.1</v>
+      </c>
+      <c r="M37" s="53"/>
       <c r="O37" s="38"/>
       <c r="P37" s="38"/>
       <c r="Q37" s="38">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="R37" s="38"/>
       <c r="S37" s="38"/>
       <c r="T37" s="38"/>
       <c r="U37" s="38"/>
       <c r="V37" s="38">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="W37" s="38"/>
       <c r="X37" s="38"/>
       <c r="Z37" s="38"/>
       <c r="AA37">
-        <v>0.36</v>
+        <v>0.27</v>
       </c>
       <c r="AB37" s="38"/>
       <c r="AD37" s="38"/>
@@ -12910,55 +12923,53 @@
       <c r="AG37" s="38"/>
       <c r="AH37" s="38"/>
       <c r="AI37" s="38">
-        <v>0.14000000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="AJ37" s="38"/>
       <c r="AK37" s="38">
-        <v>0.23</v>
+        <v>0.27</v>
       </c>
       <c r="AL37">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="51">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="C38" s="38"/>
+      <c r="A38" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38">
-        <v>0.82</v>
+        <v>0.09</v>
       </c>
       <c r="H38" s="38"/>
       <c r="I38" s="38"/>
       <c r="J38" s="38"/>
       <c r="K38" s="38"/>
       <c r="L38" s="38">
-        <v>0.36</v>
-      </c>
-      <c r="M38" s="55"/>
+        <v>0.11</v>
+      </c>
+      <c r="M38" s="53"/>
       <c r="O38" s="38"/>
       <c r="P38" s="38"/>
       <c r="Q38" s="38">
-        <v>0.22</v>
+        <v>0.04</v>
       </c>
       <c r="R38" s="38"/>
       <c r="S38" s="38"/>
       <c r="T38" s="38"/>
       <c r="U38" s="38"/>
       <c r="V38" s="38">
-        <v>0.28000000000000003</v>
+        <v>0.19</v>
       </c>
       <c r="W38" s="38"/>
       <c r="X38" s="38"/>
       <c r="Z38" s="38"/>
       <c r="AA38">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="AB38" s="38"/>
       <c r="AD38" s="38"/>
@@ -12967,22 +12978,22 @@
       <c r="AG38" s="38"/>
       <c r="AH38" s="38"/>
       <c r="AI38" s="38">
-        <v>0.18</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AJ38" s="38"/>
       <c r="AK38" s="38">
-        <v>0.18</v>
+        <v>0.23</v>
       </c>
       <c r="AL38">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="38"/>
-      <c r="C39" s="51"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
@@ -12996,7 +13007,7 @@
       <c r="L39" s="38">
         <v>0.2</v>
       </c>
-      <c r="M39" s="55"/>
+      <c r="M39" s="53"/>
       <c r="O39" s="38"/>
       <c r="P39" s="38"/>
       <c r="Q39" s="38">
@@ -13033,10 +13044,10 @@
       </c>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="51">
+      <c r="B40" s="49">
         <v>0.08</v>
       </c>
       <c r="C40" s="38"/>
@@ -13053,7 +13064,7 @@
       <c r="L40" s="38">
         <v>0.25</v>
       </c>
-      <c r="M40" s="55"/>
+      <c r="M40" s="53"/>
       <c r="O40" s="38"/>
       <c r="P40" s="38"/>
       <c r="Q40" s="38">
@@ -13090,7 +13101,7 @@
       </c>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="52" t="s">
         <v>37</v>
       </c>
       <c r="B41" s="38"/>
@@ -13100,13 +13111,13 @@
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
       <c r="H41" s="38"/>
-      <c r="I41" s="51"/>
+      <c r="I41" s="49"/>
       <c r="J41" s="38"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38">
         <v>0.03</v>
       </c>
-      <c r="M41" s="55"/>
+      <c r="M41" s="53"/>
       <c r="O41" s="38"/>
       <c r="P41" s="38"/>
       <c r="Q41" s="38">
@@ -13146,7 +13157,7 @@
       <c r="A42" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="51">
+      <c r="B42" s="49">
         <v>0.01</v>
       </c>
       <c r="C42" s="38"/>
@@ -13163,7 +13174,7 @@
       <c r="L42" s="38">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M42" s="55"/>
+      <c r="M42" s="53"/>
       <c r="O42" s="38"/>
       <c r="P42" s="38"/>
       <c r="Q42" s="38">
@@ -13177,32 +13188,32 @@
         <v>0.05</v>
       </c>
       <c r="W42" s="38"/>
-      <c r="X42" s="57">
+      <c r="X42" s="55">
         <v>0</v>
       </c>
-      <c r="Y42" s="53"/>
-      <c r="Z42" s="53"/>
-      <c r="AA42" s="53"/>
-      <c r="AB42" s="53"/>
-      <c r="AC42" s="53"/>
-      <c r="AD42" s="53"/>
-      <c r="AE42" s="53"/>
-      <c r="AF42" s="53"/>
-      <c r="AG42" s="51">
+      <c r="Y42" s="51"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="51"/>
+      <c r="AB42" s="51"/>
+      <c r="AC42" s="51"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="51"/>
+      <c r="AG42" s="49">
         <v>0.05</v>
       </c>
       <c r="AH42" s="38"/>
       <c r="AI42" s="38">
         <v>0.02</v>
       </c>
-      <c r="AJ42" s="57">
+      <c r="AJ42" s="55">
         <v>0</v>
       </c>
-      <c r="AK42" s="53"/>
-      <c r="AL42" s="54"/>
+      <c r="AK42" s="51"/>
+      <c r="AL42" s="52"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="52" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="38"/>
@@ -13218,33 +13229,33 @@
       <c r="L43" s="38">
         <v>0</v>
       </c>
-      <c r="M43" s="56"/>
-      <c r="N43" s="54"/>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53">
+      <c r="M43" s="54"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="51"/>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="51">
         <v>0</v>
       </c>
-      <c r="R43" s="53"/>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
-      <c r="U43" s="53"/>
-      <c r="V43" s="53">
+      <c r="R43" s="51"/>
+      <c r="S43" s="51"/>
+      <c r="T43" s="51"/>
+      <c r="U43" s="51"/>
+      <c r="V43" s="51">
         <v>0</v>
       </c>
-      <c r="W43" s="53"/>
-      <c r="X43" s="53"/>
-      <c r="Y43" s="53"/>
-      <c r="Z43" s="53"/>
-      <c r="AA43" s="53">
+      <c r="W43" s="51"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="51"/>
+      <c r="Z43" s="51"/>
+      <c r="AA43" s="51">
         <v>0</v>
       </c>
-      <c r="AB43" s="53"/>
-      <c r="AC43" s="54"/>
-      <c r="AD43" s="53"/>
-      <c r="AE43" s="53"/>
-      <c r="AF43" s="53"/>
-      <c r="AG43" s="51">
+      <c r="AB43" s="51"/>
+      <c r="AC43" s="52"/>
+      <c r="AD43" s="51"/>
+      <c r="AE43" s="51"/>
+      <c r="AF43" s="51"/>
+      <c r="AG43" s="49">
         <v>0.3</v>
       </c>
       <c r="AH43" s="38"/>
@@ -13255,70 +13266,70 @@
       <c r="AK43" s="38">
         <v>0.43</v>
       </c>
-      <c r="AL43" s="52">
+      <c r="AL43" s="50">
         <v>0.4</v>
       </c>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="38"/>
+      <c r="A44" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="49">
+        <v>0.04</v>
+      </c>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
+      <c r="G44" s="38">
+        <v>0.09</v>
+      </c>
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
       <c r="L44" s="38">
+        <v>0.17</v>
+      </c>
+      <c r="M44" s="53"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38">
         <v>0</v>
       </c>
-      <c r="M44" s="56"/>
-      <c r="N44" s="54"/>
-      <c r="O44" s="53"/>
-      <c r="P44" s="53"/>
-      <c r="Q44" s="53">
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
+      <c r="T44" s="38"/>
+      <c r="U44" s="38"/>
+      <c r="V44" s="38">
         <v>0</v>
       </c>
-      <c r="R44" s="53"/>
-      <c r="S44" s="53"/>
-      <c r="T44" s="53"/>
-      <c r="U44" s="53"/>
-      <c r="V44" s="53">
+      <c r="W44" s="38"/>
+      <c r="X44" s="38"/>
+      <c r="Z44" s="38"/>
+      <c r="AA44" s="38">
         <v>0</v>
       </c>
-      <c r="W44" s="53"/>
-      <c r="X44" s="53"/>
-      <c r="Y44" s="53"/>
-      <c r="Z44" s="53"/>
-      <c r="AA44" s="53">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="51">
-        <v>0.06</v>
-      </c>
+      <c r="AB44" s="38"/>
       <c r="AD44" s="38"/>
       <c r="AE44" s="38"/>
       <c r="AF44" s="38"/>
       <c r="AG44" s="38"/>
       <c r="AH44" s="38"/>
       <c r="AI44" s="38">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="AJ44" s="38"/>
       <c r="AK44" s="38">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="AL44" s="52">
-        <v>0.1</v>
+        <v>0.04</v>
+      </c>
+      <c r="AL44">
+        <v>0.04</v>
       </c>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B45" s="38"/>
       <c r="C45" s="38"/>
@@ -13333,28 +13344,28 @@
       <c r="L45" s="38">
         <v>0</v>
       </c>
-      <c r="M45" s="56"/>
-      <c r="N45" s="54"/>
-      <c r="O45" s="53"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="53">
+      <c r="M45" s="54"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="51">
         <v>0</v>
       </c>
-      <c r="R45" s="53"/>
-      <c r="S45" s="53"/>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
-      <c r="V45" s="53">
+      <c r="R45" s="51"/>
+      <c r="S45" s="51"/>
+      <c r="T45" s="51"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="51">
         <v>0</v>
       </c>
-      <c r="W45" s="53"/>
-      <c r="X45" s="53"/>
-      <c r="Y45" s="53"/>
-      <c r="Z45" s="53"/>
-      <c r="AA45" s="53">
+      <c r="W45" s="51"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="51"/>
+      <c r="Z45" s="51"/>
+      <c r="AA45" s="51">
         <v>0</v>
       </c>
-      <c r="AB45" s="51">
+      <c r="AB45" s="49">
         <v>0.06</v>
       </c>
       <c r="AD45" s="38"/>
@@ -13363,19 +13374,19 @@
       <c r="AG45" s="38"/>
       <c r="AH45" s="38"/>
       <c r="AI45" s="38">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="AJ45" s="38"/>
       <c r="AK45" s="38">
-        <v>0.1</v>
-      </c>
-      <c r="AL45" s="52">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL45" s="50">
         <v>0.1</v>
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B46" s="38"/>
       <c r="C46" s="38"/>
@@ -13390,110 +13401,110 @@
       <c r="L46" s="38">
         <v>0</v>
       </c>
-      <c r="M46" s="56"/>
-      <c r="N46" s="54"/>
-      <c r="O46" s="53"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="53">
+      <c r="M46" s="54"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51">
         <v>0</v>
       </c>
-      <c r="R46" s="53"/>
-      <c r="S46" s="53"/>
-      <c r="T46" s="53"/>
-      <c r="U46" s="53"/>
-      <c r="V46" s="53">
+      <c r="R46" s="51"/>
+      <c r="S46" s="51"/>
+      <c r="T46" s="51"/>
+      <c r="U46" s="51"/>
+      <c r="V46" s="51">
         <v>0</v>
       </c>
-      <c r="W46" s="53"/>
-      <c r="X46" s="53"/>
-      <c r="Y46" s="53"/>
-      <c r="Z46" s="53"/>
-      <c r="AA46" s="53">
+      <c r="W46" s="51"/>
+      <c r="X46" s="51"/>
+      <c r="Y46" s="51"/>
+      <c r="Z46" s="51"/>
+      <c r="AA46" s="51">
         <v>0</v>
       </c>
-      <c r="AB46" s="53"/>
-      <c r="AC46" s="54"/>
-      <c r="AD46" s="53"/>
-      <c r="AE46" s="53"/>
-      <c r="AF46" s="53"/>
-      <c r="AG46" s="53"/>
-      <c r="AH46" s="51">
+      <c r="AB46" s="49">
         <v>0.06</v>
       </c>
+      <c r="AD46" s="38"/>
+      <c r="AE46" s="38"/>
+      <c r="AF46" s="38"/>
+      <c r="AG46" s="38"/>
+      <c r="AH46" s="38"/>
       <c r="AI46" s="38">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="AJ46" s="38"/>
       <c r="AK46" s="38">
         <v>0.1</v>
       </c>
-      <c r="AL46" s="52">
+      <c r="AL46" s="50">
         <v>0.1</v>
       </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="51">
-        <v>0.03</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B47" s="38"/>
       <c r="C47" s="38"/>
       <c r="D47" s="38"/>
       <c r="E47" s="38"/>
       <c r="F47" s="38"/>
-      <c r="G47" s="38">
-        <v>0.09</v>
-      </c>
+      <c r="G47" s="38"/>
       <c r="H47" s="38"/>
       <c r="I47" s="38"/>
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38">
-        <v>0.09</v>
-      </c>
-      <c r="M47" s="55"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="38">
-        <v>0.02</v>
-      </c>
-      <c r="R47" s="38"/>
-      <c r="S47" s="38"/>
-      <c r="T47" s="38"/>
-      <c r="U47" s="38"/>
-      <c r="V47" s="38">
+        <v>0</v>
+      </c>
+      <c r="M47" s="54"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51">
+        <v>0</v>
+      </c>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="51"/>
+      <c r="V47" s="51">
+        <v>0</v>
+      </c>
+      <c r="W47" s="51"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="51"/>
+      <c r="Z47" s="51"/>
+      <c r="AA47" s="51">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="51"/>
+      <c r="AC47" s="52"/>
+      <c r="AD47" s="51"/>
+      <c r="AE47" s="51"/>
+      <c r="AF47" s="51"/>
+      <c r="AG47" s="51"/>
+      <c r="AH47" s="49">
         <v>0.06</v>
       </c>
-      <c r="W47" s="38"/>
-      <c r="X47" s="38"/>
-      <c r="Z47" s="38"/>
-      <c r="AA47">
-        <v>0.12</v>
-      </c>
-      <c r="AB47" s="38"/>
-      <c r="AD47" s="38"/>
-      <c r="AE47" s="38"/>
-      <c r="AF47" s="38"/>
-      <c r="AG47" s="38"/>
-      <c r="AH47" s="38"/>
       <c r="AI47" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ47" s="38"/>
       <c r="AK47" s="38">
-        <v>0.09</v>
-      </c>
-      <c r="AL47">
-        <v>0.08</v>
+        <v>0.1</v>
+      </c>
+      <c r="AL47" s="50">
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="51">
-        <v>0.04</v>
+      <c r="A48" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="49">
+        <v>0.03</v>
       </c>
       <c r="C48" s="38"/>
       <c r="D48" s="38"/>
@@ -13507,26 +13518,26 @@
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38">
-        <v>0.17</v>
-      </c>
-      <c r="M48" s="55"/>
+        <v>0.09</v>
+      </c>
+      <c r="M48" s="53"/>
       <c r="O48" s="38"/>
       <c r="P48" s="38"/>
       <c r="Q48" s="38">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="R48" s="38"/>
       <c r="S48" s="38"/>
       <c r="T48" s="38"/>
       <c r="U48" s="38"/>
       <c r="V48" s="38">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="W48" s="38"/>
       <c r="X48" s="38"/>
       <c r="Z48" s="38"/>
-      <c r="AA48" s="38">
-        <v>0</v>
+      <c r="AA48">
+        <v>0.12</v>
       </c>
       <c r="AB48" s="38"/>
       <c r="AD48" s="38"/>
@@ -13535,14 +13546,14 @@
       <c r="AG48" s="38"/>
       <c r="AH48" s="38"/>
       <c r="AI48" s="38">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ48" s="38"/>
       <c r="AK48" s="38">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="AL48">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.25">
@@ -13554,7 +13565,7 @@
       <c r="D49" s="38"/>
       <c r="E49" s="38"/>
       <c r="F49" s="38"/>
-      <c r="G49" s="51"/>
+      <c r="G49" s="49"/>
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
       <c r="J49" s="38"/>
@@ -13562,7 +13573,7 @@
       <c r="L49" s="38">
         <v>0.08</v>
       </c>
-      <c r="M49" s="55"/>
+      <c r="M49" s="53"/>
       <c r="O49" s="38"/>
       <c r="P49" s="38"/>
       <c r="Q49" s="38">
@@ -13610,12 +13621,12 @@
       <c r="G50" s="38"/>
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
-      <c r="J50" s="51"/>
+      <c r="J50" s="49"/>
       <c r="K50" s="38"/>
       <c r="L50" s="38">
         <v>0.08</v>
       </c>
-      <c r="M50" s="55"/>
+      <c r="M50" s="53"/>
       <c r="O50" s="38"/>
       <c r="P50" s="38"/>
       <c r="Q50" s="38">
@@ -13663,12 +13674,12 @@
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
       <c r="I51" s="38"/>
-      <c r="J51" s="51"/>
+      <c r="J51" s="49"/>
       <c r="K51" s="38"/>
       <c r="L51" s="38">
         <v>0.06</v>
       </c>
-      <c r="M51" s="55"/>
+      <c r="M51" s="53"/>
       <c r="O51" s="38"/>
       <c r="P51" s="38"/>
       <c r="Q51" s="38">
@@ -13721,9 +13732,9 @@
       <c r="L52" s="38">
         <v>0</v>
       </c>
-      <c r="M52" s="56"/>
-      <c r="N52" s="54"/>
-      <c r="O52" s="51">
+      <c r="M52" s="54"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="49">
         <v>0.01</v>
       </c>
       <c r="P52" s="38"/>
@@ -13756,12 +13767,12 @@
       <c r="AK52" s="38">
         <v>0.01</v>
       </c>
-      <c r="AL52" s="52">
+      <c r="AL52" s="50">
         <v>0.01</v>
       </c>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A53" s="58" t="s">
+      <c r="A53" s="56" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="38"/>
@@ -13769,7 +13780,7 @@
       <c r="D53" s="38"/>
       <c r="E53" s="38"/>
       <c r="F53" s="38"/>
-      <c r="G53" s="51"/>
+      <c r="G53" s="49"/>
       <c r="H53" s="38"/>
       <c r="I53" s="38"/>
       <c r="J53" s="38"/>
@@ -13777,7 +13788,7 @@
       <c r="L53" s="38">
         <v>0.06</v>
       </c>
-      <c r="M53" s="55"/>
+      <c r="M53" s="53"/>
       <c r="O53" s="38"/>
       <c r="P53" s="38"/>
       <c r="Q53" s="38">
@@ -13809,7 +13820,7 @@
       <c r="AK53" s="38">
         <v>0.01</v>
       </c>
-      <c r="AL53" s="52">
+      <c r="AL53" s="50">
         <v>0.01</v>
       </c>
     </row>
@@ -13822,7 +13833,7 @@
       <c r="D54" s="38"/>
       <c r="E54" s="38"/>
       <c r="F54" s="38"/>
-      <c r="G54" s="51"/>
+      <c r="G54" s="49"/>
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
       <c r="J54" s="38"/>
@@ -13830,7 +13841,7 @@
       <c r="L54" s="38">
         <v>0.05</v>
       </c>
-      <c r="M54" s="55"/>
+      <c r="M54" s="53"/>
       <c r="O54" s="38"/>
       <c r="P54" s="38"/>
       <c r="Q54" s="38">
@@ -13843,17 +13854,17 @@
       <c r="V54" s="38">
         <v>0.02</v>
       </c>
-      <c r="W54" s="57">
+      <c r="W54" s="55">
         <v>0</v>
       </c>
-      <c r="X54" s="53"/>
-      <c r="Y54" s="53"/>
-      <c r="Z54" s="53"/>
-      <c r="AA54" s="53"/>
-      <c r="AB54" s="53"/>
-      <c r="AC54" s="53"/>
-      <c r="AD54" s="53"/>
-      <c r="AE54" s="51">
+      <c r="X54" s="51"/>
+      <c r="Y54" s="51"/>
+      <c r="Z54" s="51"/>
+      <c r="AA54" s="51"/>
+      <c r="AB54" s="51"/>
+      <c r="AC54" s="51"/>
+      <c r="AD54" s="51"/>
+      <c r="AE54" s="49">
         <v>0.02</v>
       </c>
       <c r="AF54" s="38"/>
@@ -13862,17 +13873,17 @@
       <c r="AI54" s="38">
         <v>0.01</v>
       </c>
-      <c r="AJ54" s="57">
+      <c r="AJ54" s="55">
         <v>0</v>
       </c>
-      <c r="AK54" s="53"/>
-      <c r="AL54" s="54"/>
+      <c r="AK54" s="51"/>
+      <c r="AL54" s="52"/>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
         <v>436</v>
       </c>
-      <c r="B55" s="51">
+      <c r="B55" s="49">
         <v>0.02</v>
       </c>
       <c r="C55" s="38"/>
@@ -13889,7 +13900,7 @@
       <c r="L55" s="38">
         <v>0.01</v>
       </c>
-      <c r="M55" s="55"/>
+      <c r="M55" s="53"/>
       <c r="O55" s="38"/>
       <c r="P55" s="38"/>
       <c r="Q55" s="38">
@@ -13902,24 +13913,24 @@
       <c r="V55" s="38">
         <v>0.01</v>
       </c>
-      <c r="W55" s="57">
+      <c r="W55" s="55">
         <v>0</v>
       </c>
-      <c r="X55" s="53"/>
-      <c r="Y55" s="53"/>
-      <c r="Z55" s="53"/>
-      <c r="AA55" s="53"/>
-      <c r="AB55" s="53"/>
-      <c r="AC55" s="53"/>
-      <c r="AD55" s="53"/>
-      <c r="AE55" s="53"/>
-      <c r="AF55" s="53"/>
-      <c r="AG55" s="53"/>
-      <c r="AH55" s="53"/>
-      <c r="AI55" s="53"/>
-      <c r="AJ55" s="53"/>
-      <c r="AK55" s="53"/>
-      <c r="AL55" s="54"/>
+      <c r="X55" s="51"/>
+      <c r="Y55" s="51"/>
+      <c r="Z55" s="51"/>
+      <c r="AA55" s="51"/>
+      <c r="AB55" s="51"/>
+      <c r="AC55" s="51"/>
+      <c r="AD55" s="51"/>
+      <c r="AE55" s="51"/>
+      <c r="AF55" s="51"/>
+      <c r="AG55" s="51"/>
+      <c r="AH55" s="51"/>
+      <c r="AI55" s="51"/>
+      <c r="AJ55" s="51"/>
+      <c r="AK55" s="51"/>
+      <c r="AL55" s="52"/>
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
@@ -13930,7 +13941,7 @@
       <c r="D56" s="38"/>
       <c r="E56" s="38"/>
       <c r="F56" s="38"/>
-      <c r="G56" s="51"/>
+      <c r="G56" s="49"/>
       <c r="H56" s="38"/>
       <c r="I56" s="38"/>
       <c r="J56" s="38"/>
@@ -13938,37 +13949,37 @@
       <c r="L56" s="38">
         <v>0.01</v>
       </c>
-      <c r="M56" s="55"/>
-      <c r="O56" s="57">
+      <c r="M56" s="53"/>
+      <c r="O56" s="55">
         <v>0</v>
       </c>
-      <c r="P56" s="53"/>
-      <c r="Q56" s="53">
+      <c r="P56" s="51"/>
+      <c r="Q56" s="51">
         <v>0</v>
       </c>
-      <c r="R56" s="53"/>
-      <c r="S56" s="53"/>
-      <c r="T56" s="53"/>
-      <c r="U56" s="53"/>
-      <c r="V56" s="53">
+      <c r="R56" s="51"/>
+      <c r="S56" s="51"/>
+      <c r="T56" s="51"/>
+      <c r="U56" s="51"/>
+      <c r="V56" s="51">
         <v>0</v>
       </c>
-      <c r="W56" s="53"/>
-      <c r="X56" s="53"/>
-      <c r="Y56" s="53"/>
-      <c r="Z56" s="53"/>
-      <c r="AA56" s="53"/>
-      <c r="AB56" s="53"/>
-      <c r="AC56" s="53"/>
-      <c r="AD56" s="53"/>
-      <c r="AE56" s="53"/>
-      <c r="AF56" s="53"/>
-      <c r="AG56" s="53"/>
-      <c r="AH56" s="53"/>
-      <c r="AI56" s="53"/>
-      <c r="AJ56" s="53"/>
-      <c r="AK56" s="53"/>
-      <c r="AL56" s="54"/>
+      <c r="W56" s="51"/>
+      <c r="X56" s="51"/>
+      <c r="Y56" s="51"/>
+      <c r="Z56" s="51"/>
+      <c r="AA56" s="51"/>
+      <c r="AB56" s="51"/>
+      <c r="AC56" s="51"/>
+      <c r="AD56" s="51"/>
+      <c r="AE56" s="51"/>
+      <c r="AF56" s="51"/>
+      <c r="AG56" s="51"/>
+      <c r="AH56" s="51"/>
+      <c r="AI56" s="51"/>
+      <c r="AJ56" s="51"/>
+      <c r="AK56" s="51"/>
+      <c r="AL56" s="52"/>
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
@@ -13979,7 +13990,7 @@
       <c r="D57" s="38"/>
       <c r="E57" s="38"/>
       <c r="F57" s="38"/>
-      <c r="G57" s="51"/>
+      <c r="G57" s="49"/>
       <c r="H57" s="38"/>
       <c r="I57" s="38"/>
       <c r="J57" s="38"/>
@@ -13987,7 +13998,7 @@
       <c r="L57" s="38">
         <v>0.1</v>
       </c>
-      <c r="M57" s="55"/>
+      <c r="M57" s="53"/>
       <c r="N57" s="38"/>
       <c r="O57" s="38"/>
       <c r="P57" s="38"/>
@@ -13996,29 +14007,29 @@
       </c>
       <c r="R57" s="38"/>
       <c r="S57" s="38"/>
-      <c r="T57" s="57">
+      <c r="T57" s="55">
         <v>0</v>
       </c>
-      <c r="U57" s="53"/>
-      <c r="V57" s="53">
+      <c r="U57" s="51"/>
+      <c r="V57" s="51">
         <v>0</v>
       </c>
-      <c r="W57" s="53"/>
-      <c r="X57" s="53"/>
-      <c r="Y57" s="53"/>
-      <c r="Z57" s="53"/>
-      <c r="AA57" s="53"/>
-      <c r="AB57" s="53"/>
-      <c r="AC57" s="53"/>
-      <c r="AD57" s="53"/>
-      <c r="AE57" s="53"/>
-      <c r="AF57" s="53"/>
-      <c r="AG57" s="53"/>
-      <c r="AH57" s="53"/>
-      <c r="AI57" s="53"/>
-      <c r="AJ57" s="53"/>
-      <c r="AK57" s="53"/>
-      <c r="AL57" s="54"/>
+      <c r="W57" s="51"/>
+      <c r="X57" s="51"/>
+      <c r="Y57" s="51"/>
+      <c r="Z57" s="51"/>
+      <c r="AA57" s="51"/>
+      <c r="AB57" s="51"/>
+      <c r="AC57" s="51"/>
+      <c r="AD57" s="51"/>
+      <c r="AE57" s="51"/>
+      <c r="AF57" s="51"/>
+      <c r="AG57" s="51"/>
+      <c r="AH57" s="51"/>
+      <c r="AI57" s="51"/>
+      <c r="AJ57" s="51"/>
+      <c r="AK57" s="51"/>
+      <c r="AL57" s="52"/>
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
@@ -14036,9 +14047,9 @@
       <c r="L58" s="38">
         <v>0</v>
       </c>
-      <c r="M58" s="56"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="51">
+      <c r="M58" s="54"/>
+      <c r="N58" s="51"/>
+      <c r="O58" s="49">
         <v>0.01</v>
       </c>
       <c r="P58" s="38"/>
@@ -14059,19 +14070,19 @@
       <c r="AA58" s="38">
         <v>0.01</v>
       </c>
-      <c r="AB58" s="57">
+      <c r="AB58" s="55">
         <v>0</v>
       </c>
-      <c r="AC58" s="53"/>
-      <c r="AD58" s="53"/>
-      <c r="AE58" s="53"/>
-      <c r="AF58" s="53"/>
-      <c r="AG58" s="53"/>
-      <c r="AH58" s="53"/>
-      <c r="AI58" s="53"/>
-      <c r="AJ58" s="53"/>
-      <c r="AK58" s="53"/>
-      <c r="AL58" s="54"/>
+      <c r="AC58" s="51"/>
+      <c r="AD58" s="51"/>
+      <c r="AE58" s="51"/>
+      <c r="AF58" s="51"/>
+      <c r="AG58" s="51"/>
+      <c r="AH58" s="51"/>
+      <c r="AI58" s="51"/>
+      <c r="AJ58" s="51"/>
+      <c r="AK58" s="51"/>
+      <c r="AL58" s="52"/>
     </row>
     <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -14097,7 +14108,7 @@
         <f>SUM(L4:L58)</f>
         <v>99.630000000000024</v>
       </c>
-      <c r="M60" s="55"/>
+      <c r="M60" s="53"/>
       <c r="N60" s="38"/>
       <c r="O60" s="38"/>
       <c r="P60" s="38"/>
@@ -14155,7 +14166,7 @@
       <c r="E61" s="38"/>
       <c r="F61" s="38"/>
       <c r="G61" s="38">
-        <f t="shared" ref="C61:AL61" si="1">SUM(G28:G58)</f>
+        <f t="shared" ref="G61:AL61" si="1">SUM(G28:G58)</f>
         <v>4.4999999999999991</v>
       </c>
       <c r="H61" s="38"/>
@@ -14166,7 +14177,7 @@
         <f t="shared" si="1"/>
         <v>6.6899999999999995</v>
       </c>
-      <c r="M61" s="55"/>
+      <c r="M61" s="53"/>
       <c r="N61" s="38"/>
       <c r="O61" s="38"/>
       <c r="P61" s="38"/>
@@ -14375,84 +14386,123 @@
         <v>453</v>
       </c>
       <c r="C67">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L67" s="38">
-        <f>SUM(L17:L21)+SUM(L34:L35)</f>
-        <v>3.34</v>
+        <f>SUM(L17:L21)+SUM(L34:L36)</f>
+        <v>3.6999999999999997</v>
       </c>
       <c r="Q67" s="38">
-        <f>SUM(Q17:Q21)+SUM(Q34:Q35)</f>
-        <v>2.85</v>
+        <f>SUM(Q17:Q21)+SUM(Q34:Q36)</f>
+        <v>3.0700000000000003</v>
       </c>
       <c r="V67" s="38">
-        <f>SUM(V17:V21)+SUM(V34:V35)</f>
-        <v>3.65</v>
+        <f>SUM(V17:V21)+SUM(V34:V36)</f>
+        <v>3.9299999999999997</v>
       </c>
       <c r="AA67" s="38">
-        <f>SUM(AA17:AA21)+SUM(AA34:AA35)</f>
-        <v>3.8200000000000003</v>
+        <f>SUM(AA17:AA21)+SUM(AA34:AA36)</f>
+        <v>4.28</v>
       </c>
       <c r="AI67" s="38">
-        <f>SUM(AI17:AI21)+SUM(AI34:AI35)</f>
-        <v>2.5100000000000002</v>
+        <f>SUM(AI17:AI21)+SUM(AI34:AI36)</f>
+        <v>2.6900000000000004</v>
       </c>
       <c r="AK67" s="38">
-        <f>SUM(AK17:AK21)+SUM(AK34:AK35)</f>
-        <v>2.69</v>
+        <f>SUM(AK17:AK21)+SUM(AK34:AK36)</f>
+        <v>2.87</v>
       </c>
       <c r="AL67" s="38">
-        <f>SUM(AL17:AL21)+SUM(AL34:AL35)</f>
-        <v>2.37</v>
+        <f>SUM(AL17:AL21)+SUM(AL34:AL36)</f>
+        <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B68" t="s">
+        <v>455</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="L68" s="38">
+        <f>SUM(L22:L23)+SUM(L37:L44)</f>
+        <v>1.42</v>
+      </c>
+      <c r="Q68" s="38">
+        <f>SUM(Q22:Q23)+SUM(Q37:Q44)</f>
+        <v>0.52</v>
+      </c>
+      <c r="V68" s="38">
+        <f>SUM(V22:V23)+SUM(V37:V44)</f>
+        <v>1.34</v>
+      </c>
+      <c r="AA68" s="38">
+        <f>SUM(AA22:AA23)+SUM(AA37:AA44)</f>
+        <v>1.65</v>
+      </c>
+      <c r="AI68" s="38">
+        <f>SUM(AI22:AI23)+SUM(AI37:AI44)</f>
+        <v>1.42</v>
+      </c>
+      <c r="AK68" s="38">
+        <f>SUM(AK22:AK23)+SUM(AK37:AK44)</f>
+        <v>1.65</v>
+      </c>
+      <c r="AL68" s="38">
+        <f>SUM(AL22:AL23)+SUM(AL37:AL44)</f>
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
         <v>444</v>
       </c>
-      <c r="B68" t="s">
-        <v>454</v>
-      </c>
-      <c r="C68">
-        <v>28</v>
-      </c>
-      <c r="L68" s="38">
-        <f>SUM(L22:L26)+SUM(L36:L58)</f>
-        <v>2.6500000000000004</v>
-      </c>
-      <c r="Q68" s="38">
-        <f>SUM(Q22:Q26)+SUM(Q36:Q58)</f>
-        <v>1.1700000000000002</v>
-      </c>
-      <c r="V68" s="38">
-        <f>SUM(V22:V26)+SUM(V36:V58)</f>
-        <v>2.3700000000000006</v>
-      </c>
-      <c r="AA68" s="38">
-        <f>SUM(AA22:AA26)+SUM(AA36:AA58)</f>
-        <v>2.79</v>
-      </c>
-      <c r="AI68" s="38">
-        <f>SUM(AI22:AI26)+SUM(AI36:AI58)</f>
-        <v>2.2300000000000004</v>
-      </c>
-      <c r="AK68" s="38">
-        <f>SUM(AK22:AK26)+SUM(AK36:AK58)</f>
-        <v>2.58</v>
-      </c>
-      <c r="AL68" s="38">
-        <f>SUM(AL22:AL26)+SUM(AL36:AL58)</f>
-        <v>2.0000000000000004</v>
-      </c>
-    </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>456</v>
+      </c>
       <c r="C69">
-        <f>SUM(C63:C68)</f>
+        <v>17</v>
+      </c>
+      <c r="L69" s="38">
+        <f>SUM(L24:L26)+SUM(L45:L58)</f>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="Q69" s="38">
+        <f>SUM(Q24:Q26)+SUM(Q45:Q58)</f>
+        <v>0.43000000000000005</v>
+      </c>
+      <c r="V69" s="38">
+        <f>SUM(V24:V26)+SUM(V45:V58)</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="AA69" s="38">
+        <f>SUM(AA24:AA26)+SUM(AA45:AA58)</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="AI69" s="38">
+        <f>SUM(AI24:AI26)+SUM(AI45:AI58)</f>
+        <v>0.63</v>
+      </c>
+      <c r="AK69" s="38">
+        <f>SUM(AK24:AK26)+SUM(AK45:AK58)</f>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="AL69" s="38">
+        <f>SUM(AL24:AL26)+SUM(AL45:AL58)</f>
+        <v>0.63000000000000012</v>
+      </c>
+    </row>
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f>SUM(C63:C69)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI73" t="s">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AI74" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
portfolio optimization with quadratic programming
</commit_message>
<xml_diff>
--- a/Data/Data Sources Coverage_ACWI.xlsx
+++ b/Data/Data Sources Coverage_ACWI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Master mAI-X\TFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB564FC-2BE9-455E-BA24-0E5CB48478AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD674685-BA94-47B7-995D-3AE8AD3312D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D7359AC-8169-4D64-B280-A03E914C2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Country weights" sheetId="6" r:id="rId1"/>
@@ -1698,9 +1698,6 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1711,6 +1708,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1732,9 +1732,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1772,7 +1772,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1878,7 +1878,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2020,7 +2020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2030,9 +2030,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE8DE30-8CF4-49FE-905A-5BDCBDCD0F61}">
   <dimension ref="A1:AL74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q29" sqref="Q29:Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7801,32 +7801,32 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="60">
+      <c r="B29" s="59">
         <v>35</v>
       </c>
-      <c r="C29" s="61">
+      <c r="C29" s="60">
         <v>0.18</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="64">
+      <c r="D29" s="59"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="63">
         <v>2011</v>
       </c>
-      <c r="K29" s="65"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="60"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C30"/>
@@ -8645,13 +8645,13 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BG1" s="58" t="s">
+      <c r="BG1" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="BH1" s="58"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="58"/>
-      <c r="BK1" s="58"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="68"/>
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
@@ -11044,34 +11044,34 @@
       <c r="BJ29" s="13"/>
       <c r="BK29" s="13"/>
     </row>
-    <row r="30" spans="1:63" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="s">
+    <row r="30" spans="1:63" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62">
+      <c r="B30" s="66"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61">
         <v>1999</v>
       </c>
-      <c r="F30" s="64">
+      <c r="F30" s="63">
         <v>2011</v>
       </c>
-      <c r="G30" s="66"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="68"/>
-      <c r="R30" s="62"/>
-      <c r="S30" s="68"/>
-      <c r="W30" s="68"/>
-      <c r="AC30" s="65"/>
-      <c r="AD30" s="62"/>
-      <c r="AI30" s="65"/>
-      <c r="AP30" s="68"/>
-      <c r="AU30" s="68"/>
-      <c r="AW30" s="66">
+      <c r="G30" s="65"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="67"/>
+      <c r="R30" s="61"/>
+      <c r="S30" s="67"/>
+      <c r="W30" s="67"/>
+      <c r="AC30" s="64"/>
+      <c r="AD30" s="61"/>
+      <c r="AI30" s="64"/>
+      <c r="AP30" s="67"/>
+      <c r="AU30" s="67"/>
+      <c r="AW30" s="65">
         <v>2015</v>
       </c>
-      <c r="BF30" s="65"/>
+      <c r="BF30" s="64"/>
     </row>
     <row r="31" spans="1:63" x14ac:dyDescent="0.25">
       <c r="B31"/>
@@ -12667,7 +12667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC8819E-4998-4293-AE91-8A38F68283E5}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -12693,26 +12693,26 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="68" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="68" t="s">
         <v>343</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>

</xml_diff>